<commit_message>
Working with mismatched headers
</commit_message>
<xml_diff>
--- a/info/apinet_survey (2).xlsx
+++ b/info/apinet_survey (2).xlsx
@@ -3615,7 +3615,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3681,6 +3681,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
@@ -3739,8 +3747,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4B01A6"/>
-        <bgColor rgb="FF800080"/>
+        <fgColor rgb="FFC00000"/>
+        <bgColor rgb="FF800000"/>
       </patternFill>
     </fill>
     <fill>
@@ -3753,12 +3761,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFA6A6"/>
         <bgColor rgb="FFF5BBFE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor rgb="FF800000"/>
       </patternFill>
     </fill>
     <fill>
@@ -3787,8 +3789,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FFC99C00"/>
+        <fgColor rgb="FF4B01A6"/>
+        <bgColor rgb="FF800080"/>
       </patternFill>
     </fill>
     <fill>
@@ -3801,6 +3803,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF0C5201"/>
         <bgColor rgb="FF333300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFC99C00"/>
       </patternFill>
     </fill>
   </fills>
@@ -3848,7 +3856,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3937,11 +3945,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3949,11 +3957,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3961,7 +3969,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3969,19 +3977,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="10" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4013,7 +4021,39 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="14" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4021,35 +4061,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="15" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4057,59 +4093,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4197,11 +4209,11 @@
   </sheetPr>
   <dimension ref="A1:AK339"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q288" activeCellId="0" sqref="Q288"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L303" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q323" activeCellId="0" sqref="Q323"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.12"/>
@@ -11126,7 +11138,7 @@
       <c r="M187" s="11" t="s">
         <v>541</v>
       </c>
-      <c r="N187" s="13" t="s">
+      <c r="N187" s="15" t="s">
         <v>542</v>
       </c>
       <c r="O187" s="13" t="s">
@@ -14298,7 +14310,7 @@
       <c r="M275" s="11" t="s">
         <v>710</v>
       </c>
-      <c r="N275" s="13" t="s">
+      <c r="N275" s="15" t="s">
         <v>711</v>
       </c>
       <c r="O275" s="13" t="s">
@@ -14570,7 +14582,7 @@
       <c r="M282" s="15" t="s">
         <v>736</v>
       </c>
-      <c r="N282" s="13" t="s">
+      <c r="N282" s="15" t="s">
         <v>737</v>
       </c>
       <c r="O282" s="13" t="s">
@@ -14653,7 +14665,7 @@
       <c r="M284" s="15" t="s">
         <v>749</v>
       </c>
-      <c r="N284" s="13" t="s">
+      <c r="N284" s="15" t="s">
         <v>750</v>
       </c>
       <c r="O284" s="13" t="s">
@@ -14745,7 +14757,7 @@
       <c r="M286" s="15" t="s">
         <v>766</v>
       </c>
-      <c r="N286" s="13" t="s">
+      <c r="N286" s="15" t="s">
         <v>767</v>
       </c>
     </row>
@@ -14821,7 +14833,7 @@
       <c r="M288" s="15" t="s">
         <v>769</v>
       </c>
-      <c r="N288" s="13" t="s">
+      <c r="N288" s="15" t="s">
         <v>770</v>
       </c>
       <c r="O288" s="13" t="s">
@@ -15016,7 +15028,7 @@
       <c r="M293" s="15" t="s">
         <v>771</v>
       </c>
-      <c r="N293" s="13" t="s">
+      <c r="N293" s="15" t="s">
         <v>782</v>
       </c>
       <c r="O293" s="13" t="s">
@@ -15083,7 +15095,7 @@
       <c r="M294" s="15" t="s">
         <v>796</v>
       </c>
-      <c r="N294" s="13" t="s">
+      <c r="N294" s="15" t="s">
         <v>797</v>
       </c>
       <c r="O294" s="13" t="s">
@@ -15132,7 +15144,7 @@
       <c r="M295" s="15" t="s">
         <v>803</v>
       </c>
-      <c r="N295" s="13" t="s">
+      <c r="N295" s="15" t="s">
         <v>804</v>
       </c>
       <c r="O295" s="13" t="s">
@@ -15267,7 +15279,7 @@
       <c r="M298" s="15" t="s">
         <v>824</v>
       </c>
-      <c r="N298" s="13" t="s">
+      <c r="N298" s="15" t="s">
         <v>825</v>
       </c>
       <c r="O298" s="13" t="s">
@@ -15355,7 +15367,7 @@
       <c r="M300" s="41" t="s">
         <v>787</v>
       </c>
-      <c r="N300" s="13" t="s">
+      <c r="N300" s="15" t="s">
         <v>832</v>
       </c>
       <c r="O300" s="13" t="s">
@@ -15425,7 +15437,7 @@
       <c r="M301" s="11" t="s">
         <v>846</v>
       </c>
-      <c r="N301" s="13" t="s">
+      <c r="N301" s="15" t="s">
         <v>847</v>
       </c>
       <c r="O301" s="13" t="s">
@@ -15697,7 +15709,7 @@
       <c r="M308" s="15" t="s">
         <v>877</v>
       </c>
-      <c r="N308" s="13" t="s">
+      <c r="N308" s="15" t="s">
         <v>878</v>
       </c>
       <c r="O308" s="13" t="s">
@@ -15789,7 +15801,7 @@
       <c r="M310" s="15" t="s">
         <v>892</v>
       </c>
-      <c r="N310" s="13" t="s">
+      <c r="N310" s="15" t="s">
         <v>893</v>
       </c>
       <c r="P310" s="14" t="s">
@@ -15919,7 +15931,7 @@
       <c r="M312" s="15" t="s">
         <v>920</v>
       </c>
-      <c r="N312" s="13" t="s">
+      <c r="N312" s="46" t="s">
         <v>921</v>
       </c>
       <c r="O312" s="13"/>
@@ -15969,7 +15981,7 @@
       <c r="M313" s="15" t="s">
         <v>929</v>
       </c>
-      <c r="N313" s="13" t="s">
+      <c r="N313" s="15" t="s">
         <v>930</v>
       </c>
       <c r="AC313" s="13"/>
@@ -16007,10 +16019,10 @@
       <c r="L314" s="10" t="s">
         <v>935</v>
       </c>
-      <c r="M314" s="46" t="s">
+      <c r="M314" s="47" t="s">
         <v>936</v>
       </c>
-      <c r="N314" s="8" t="s">
+      <c r="N314" s="48" t="s">
         <v>937</v>
       </c>
       <c r="O314" s="13" t="s">
@@ -16102,7 +16114,7 @@
         <v>935</v>
       </c>
       <c r="M315" s="8"/>
-      <c r="N315" s="13" t="s">
+      <c r="N315" s="46" t="s">
         <v>937</v>
       </c>
       <c r="O315" s="13" t="s">
@@ -16190,10 +16202,10 @@
       <c r="L316" s="44" t="s">
         <v>964</v>
       </c>
-      <c r="M316" s="47" t="s">
+      <c r="M316" s="48" t="s">
         <v>965</v>
       </c>
-      <c r="N316" s="13" t="s">
+      <c r="N316" s="26" t="s">
         <v>966</v>
       </c>
       <c r="O316" s="13" t="s">
@@ -16319,7 +16331,7 @@
       <c r="L318" s="11" t="s">
         <v>812</v>
       </c>
-      <c r="M318" s="46" t="s">
+      <c r="M318" s="47" t="s">
         <v>986</v>
       </c>
       <c r="O318" s="13"/>
@@ -16342,10 +16354,10 @@
       <c r="F319" s="0" t="s">
         <v>511</v>
       </c>
-      <c r="G319" s="48" t="s">
+      <c r="G319" s="49" t="s">
         <v>987</v>
       </c>
-      <c r="H319" s="48" t="s">
+      <c r="H319" s="49" t="s">
         <v>988</v>
       </c>
       <c r="I319" s="0" t="str">
@@ -16437,7 +16449,7 @@
       <c r="M321" s="15" t="s">
         <v>997</v>
       </c>
-      <c r="N321" s="13" t="s">
+      <c r="N321" s="15" t="s">
         <v>998</v>
       </c>
       <c r="O321" s="13" t="s">
@@ -16521,7 +16533,7 @@
       <c r="L323" s="11" t="s">
         <v>812</v>
       </c>
-      <c r="M323" s="46" t="s">
+      <c r="M323" s="47" t="s">
         <v>1006</v>
       </c>
       <c r="N323" s="7"/>
@@ -16593,10 +16605,10 @@
       <c r="L325" s="11" t="s">
         <v>1018</v>
       </c>
-      <c r="M325" s="49" t="s">
+      <c r="M325" s="50" t="s">
         <v>1019</v>
       </c>
-      <c r="N325" s="13" t="s">
+      <c r="N325" s="15" t="s">
         <v>1020</v>
       </c>
       <c r="O325" s="13" t="s">
@@ -16687,7 +16699,7 @@
       <c r="M326" s="26" t="s">
         <v>1042</v>
       </c>
-      <c r="N326" s="13" t="s">
+      <c r="N326" s="46" t="s">
         <v>1043</v>
       </c>
       <c r="O326" s="13" t="s">
@@ -16729,16 +16741,16 @@
       <c r="AE326" s="45"/>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B327" s="50"/>
+      <c r="B327" s="51"/>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B328" s="50"/>
+      <c r="B328" s="51"/>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B329" s="50"/>
+      <c r="B329" s="51"/>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B330" s="50"/>
+      <c r="B330" s="51"/>
       <c r="D330" s="1"/>
       <c r="E330" s="0" t="s">
         <v>1056</v>
@@ -16749,13 +16761,13 @@
       <c r="E331" s="0" t="s">
         <v>1057</v>
       </c>
-      <c r="L331" s="51"/>
+      <c r="L331" s="52"/>
       <c r="M331" s="0" t="s">
         <v>1058</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D332" s="52"/>
+      <c r="D332" s="53"/>
       <c r="E332" s="0" t="s">
         <v>1059</v>
       </c>
@@ -16765,7 +16777,7 @@
       </c>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D333" s="53"/>
+      <c r="D333" s="54"/>
       <c r="E333" s="0" t="s">
         <v>1061</v>
       </c>
@@ -16775,31 +16787,31 @@
       </c>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L335" s="54"/>
+      <c r="L335" s="55"/>
       <c r="M335" s="0" t="s">
         <v>1063</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L336" s="55"/>
+      <c r="L336" s="56"/>
       <c r="M336" s="0" t="s">
         <v>1064</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L337" s="56"/>
+      <c r="L337" s="57"/>
       <c r="M337" s="0" t="s">
         <v>1065</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L338" s="57"/>
+      <c r="L338" s="58"/>
       <c r="M338" s="0" t="s">
         <v>1066</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L339" s="58"/>
+      <c r="L339" s="59"/>
       <c r="M339" s="0" t="s">
         <v>1067</v>
       </c>
@@ -17451,7 +17463,7 @@
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.11"/>
@@ -17479,7 +17491,7 @@
       <c r="F1" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="J1" s="59" t="str">
+      <c r="J1" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K1)),RIGHT(K1,LEN(K1)-FIND(" ",K1)))</f>
         <v>aalternata</v>
       </c>
@@ -17513,7 +17525,7 @@
       <c r="F2" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="J2" s="59" t="str">
+      <c r="J2" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K2)),RIGHT(K2,LEN(K2)-FIND(" ",K2)))</f>
         <v>aalternata</v>
       </c>
@@ -17540,7 +17552,7 @@
       <c r="F3" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="J3" s="59" t="str">
+      <c r="J3" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K3)),RIGHT(K3,LEN(K3)-FIND(" ",K3)))</f>
         <v>aalternata</v>
       </c>
@@ -17567,7 +17579,7 @@
       <c r="F4" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="J4" s="59" t="str">
+      <c r="J4" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K4)),RIGHT(K4,LEN(K4)-FIND(" ",K4)))</f>
         <v>aapis</v>
       </c>
@@ -17601,7 +17613,7 @@
       <c r="F5" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="J5" s="60" t="s">
+      <c r="J5" s="61" t="s">
         <v>1068</v>
       </c>
       <c r="K5" s="7" t="s">
@@ -17634,7 +17646,7 @@
       <c r="F6" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="J6" s="59" t="str">
+      <c r="J6" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K6)),RIGHT(K6,LEN(K6)-FIND(" ",K6)))</f>
         <v>acoronavirus</v>
       </c>
@@ -17668,7 +17680,7 @@
       <c r="F7" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="J7" s="59" t="str">
+      <c r="J7" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K7)),RIGHT(K7,LEN(K7)-FIND(" ",K7)))</f>
         <v>aflavus</v>
       </c>
@@ -17702,7 +17714,7 @@
       <c r="F8" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="J8" s="59" t="str">
+      <c r="J8" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K8)),RIGHT(K8,LEN(K8)-FIND(" ",K8)))</f>
         <v>afumigatus</v>
       </c>
@@ -17736,7 +17748,7 @@
       <c r="F9" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="J9" s="59" t="str">
+      <c r="J9" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K9)),RIGHT(K9,LEN(K9)-FIND(" ",K9)))</f>
         <v>aflavus</v>
       </c>
@@ -17763,7 +17775,7 @@
       <c r="F10" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="J10" s="60" t="s">
+      <c r="J10" s="61" t="s">
         <v>1069</v>
       </c>
       <c r="K10" s="6" t="s">
@@ -17796,7 +17808,7 @@
       <c r="F11" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="J11" s="59" t="str">
+      <c r="J11" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K11)),RIGHT(K11,LEN(K11)-FIND(" ",K11)))</f>
         <v>afumigatus</v>
       </c>
@@ -17823,7 +17835,7 @@
       <c r="F12" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="J12" s="59" t="str">
+      <c r="J12" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K12)),RIGHT(K12,LEN(K12)-FIND(" ",K12)))</f>
         <v>afumigatus</v>
       </c>
@@ -17844,7 +17856,7 @@
         <f aca="false">SUM(F1:F12)</f>
         <v>106</v>
       </c>
-      <c r="J13" s="59" t="str">
+      <c r="J13" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K13)),RIGHT(K13,LEN(K13)-FIND(" ",K13)))</f>
         <v>afumigatus</v>
       </c>
@@ -17853,7 +17865,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J14" s="59" t="str">
+      <c r="J14" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K14)),RIGHT(K14,LEN(K14)-FIND(" ",K14)))</f>
         <v>afumigatus</v>
       </c>
@@ -17862,7 +17874,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J15" s="59" t="str">
+      <c r="J15" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K15)),RIGHT(K15,LEN(K15)-FIND(" ",K15)))</f>
         <v>afumigatus</v>
       </c>
@@ -17871,7 +17883,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J16" s="59" t="str">
+      <c r="J16" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K16)),RIGHT(K16,LEN(K16)-FIND(" ",K16)))</f>
         <v>afumigatus</v>
       </c>
@@ -17880,7 +17892,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J17" s="59" t="str">
+      <c r="J17" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K17)),RIGHT(K17,LEN(K17)-FIND(" ",K17)))</f>
         <v>amarginale</v>
       </c>
@@ -17896,7 +17908,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J18" s="59" t="str">
+      <c r="J18" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K18)),RIGHT(K18,LEN(K18)-FIND(" ",K18)))</f>
         <v>aniger</v>
       </c>
@@ -17912,7 +17924,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J19" s="59" t="str">
+      <c r="J19" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K19)),RIGHT(K19,LEN(K19)-FIND(" ",K19)))</f>
         <v>aparasiticus</v>
       </c>
@@ -17928,7 +17940,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J20" s="60" t="s">
+      <c r="J20" s="61" t="s">
         <v>1070</v>
       </c>
       <c r="K20" s="6" t="s">
@@ -17943,7 +17955,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J21" s="59" t="str">
+      <c r="J21" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K21)),RIGHT(K21,LEN(K21)-FIND(" ",K21)))</f>
         <v>aterreus</v>
       </c>
@@ -17959,7 +17971,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J22" s="59" t="str">
+      <c r="J22" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K22)),RIGHT(K22,LEN(K22)-FIND(" ",K22)))</f>
         <v>aviscosus</v>
       </c>
@@ -17975,7 +17987,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J23" s="59" t="str">
+      <c r="J23" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K23)),RIGHT(K23,LEN(K23)-FIND(" ",K23)))</f>
         <v>babortus</v>
       </c>
@@ -17991,7 +18003,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J24" s="60" t="s">
+      <c r="J24" s="61" t="s">
         <v>1071</v>
       </c>
       <c r="K24" s="6" t="s">
@@ -18006,7 +18018,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J25" s="59" t="str">
+      <c r="J25" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K25)),RIGHT(K25,LEN(K25)-FIND(" ",K25)))</f>
         <v>babortus</v>
       </c>
@@ -18015,7 +18027,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J26" s="59" t="str">
+      <c r="J26" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K26)),RIGHT(K26,LEN(K26)-FIND(" ",K26)))</f>
         <v>babortus</v>
       </c>
@@ -18024,7 +18036,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J27" s="59" t="str">
+      <c r="J27" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K27)),RIGHT(K27,LEN(K27)-FIND(" ",K27)))</f>
         <v>banthracis</v>
       </c>
@@ -18040,7 +18052,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J28" s="59" t="str">
+      <c r="J28" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K28)),RIGHT(K28,LEN(K28)-FIND(" ",K28)))</f>
         <v>balphaherpesvirus 1</v>
       </c>
@@ -18049,7 +18061,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J29" s="59" t="str">
+      <c r="J29" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K29)),RIGHT(K29,LEN(K29)-FIND(" ",K29)))</f>
         <v>bbronchiseptica</v>
       </c>
@@ -18065,7 +18077,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J30" s="59" t="str">
+      <c r="J30" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K30)),RIGHT(K30,LEN(K30)-FIND(" ",K30)))</f>
         <v>banthracis</v>
       </c>
@@ -18074,7 +18086,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J31" s="59" t="str">
+      <c r="J31" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K31)),RIGHT(K31,LEN(K31)-FIND(" ",K31)))</f>
         <v>banthracis</v>
       </c>
@@ -18083,7 +18095,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J32" s="59" t="str">
+      <c r="J32" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K32)),RIGHT(K32,LEN(K32)-FIND(" ",K32)))</f>
         <v>bdermatitidis</v>
       </c>
@@ -18099,7 +18111,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J33" s="59" t="str">
+      <c r="J33" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K33)),RIGHT(K33,LEN(K33)-FIND(" ",K33)))</f>
         <v>bbronchiseptica</v>
       </c>
@@ -18108,7 +18120,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J34" s="59" t="str">
+      <c r="J34" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K34)),RIGHT(K34,LEN(K34)-FIND(" ",K34)))</f>
         <v>bbronchiseptica</v>
       </c>
@@ -18117,7 +18129,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J35" s="60" t="s">
+      <c r="J35" s="61" t="s">
         <v>1072</v>
       </c>
       <c r="K35" s="6" t="s">
@@ -18132,7 +18144,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J36" s="59" t="str">
+      <c r="J36" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K36)),RIGHT(K36,LEN(K36)-FIND(" ",K36)))</f>
         <v>bdermatitidis</v>
       </c>
@@ -18141,7 +18153,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J37" s="59" t="str">
+      <c r="J37" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K37)),RIGHT(K37,LEN(K37)-FIND(" ",K37)))</f>
         <v>bdermatitidis</v>
       </c>
@@ -18150,7 +18162,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J38" s="59" t="str">
+      <c r="J38" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K38)),RIGHT(K38,LEN(K38)-FIND(" ",K38)))</f>
         <v>bhyodysenteriae</v>
       </c>
@@ -18166,7 +18178,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J39" s="60" t="s">
+      <c r="J39" s="61" t="s">
         <v>1073</v>
       </c>
       <c r="K39" s="7" t="s">
@@ -18181,7 +18193,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J40" s="59" t="str">
+      <c r="J40" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K40)),RIGHT(K40,LEN(K40)-FIND(" ",K40)))</f>
         <v>bmelitensis</v>
       </c>
@@ -18197,7 +18209,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J41" s="60" t="s">
+      <c r="J41" s="61" t="s">
         <v>1074</v>
       </c>
       <c r="K41" s="6" t="s">
@@ -18212,7 +18224,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J42" s="59" t="str">
+      <c r="J42" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K42)),RIGHT(K42,LEN(K42)-FIND(" ",K42)))</f>
         <v>bmelitensis</v>
       </c>
@@ -18221,7 +18233,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J43" s="60" t="s">
+      <c r="J43" s="61" t="s">
         <v>1075</v>
       </c>
       <c r="K43" s="7" t="s">
@@ -18236,7 +18248,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J44" s="59" t="str">
+      <c r="J44" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K44)),RIGHT(K44,LEN(K44)-FIND(" ",K44)))</f>
         <v>branarum</v>
       </c>
@@ -18252,7 +18264,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J45" s="59" t="str">
+      <c r="J45" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K45)),RIGHT(K45,LEN(K45)-FIND(" ",K45)))</f>
         <v>bsuis</v>
       </c>
@@ -18268,7 +18280,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J46" s="60" t="s">
+      <c r="J46" s="61" t="s">
         <v>1076</v>
       </c>
       <c r="K46" s="7" t="s">
@@ -18283,7 +18295,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J47" s="60" t="s">
+      <c r="J47" s="61" t="s">
         <v>1077</v>
       </c>
       <c r="K47" s="6" t="s">
@@ -18298,7 +18310,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J48" s="59" t="str">
+      <c r="J48" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K48)),RIGHT(K48,LEN(K48)-FIND(" ",K48)))</f>
         <v>bviral diarrhea virus 1</v>
       </c>
@@ -18307,7 +18319,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J49" s="59" t="str">
+      <c r="J49" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K49)),RIGHT(K49,LEN(K49)-FIND(" ",K49)))</f>
         <v>bviral diarrhea virus 1</v>
       </c>
@@ -18316,7 +18328,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J50" s="59" t="str">
+      <c r="J50" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K50)),RIGHT(K50,LEN(K50)-FIND(" ",K50)))</f>
         <v>bvirus</v>
       </c>
@@ -18332,7 +18344,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J51" s="59" t="str">
+      <c r="J51" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K51)),RIGHT(K51,LEN(K51)-FIND(" ",K51)))</f>
         <v>bviral diarrhea virus 2</v>
       </c>
@@ -18341,7 +18353,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J52" s="59" t="str">
+      <c r="J52" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K52)),RIGHT(K52,LEN(K52)-FIND(" ",K52)))</f>
         <v>cabortus</v>
       </c>
@@ -18357,7 +18369,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J53" s="59" t="str">
+      <c r="J53" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K53)),RIGHT(K53,LEN(K53)-FIND(" ",K53)))</f>
         <v>bvirus</v>
       </c>
@@ -18366,7 +18378,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J54" s="60" t="s">
+      <c r="J54" s="61" t="s">
         <v>1078</v>
       </c>
       <c r="K54" s="7" t="s">
@@ -18381,7 +18393,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J55" s="59" t="str">
+      <c r="J55" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K55)),RIGHT(K55,LEN(K55)-FIND(" ",K55)))</f>
         <v>cabortus</v>
       </c>
@@ -18390,7 +18402,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J56" s="60" t="s">
+      <c r="J56" s="61" t="s">
         <v>1079</v>
       </c>
       <c r="K56" s="7" t="s">
@@ -18405,7 +18417,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J57" s="59" t="str">
+      <c r="J57" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K57)),RIGHT(K57,LEN(K57)-FIND(" ",K57)))</f>
         <v>calbicans</v>
       </c>
@@ -18421,7 +18433,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J58" s="59" t="str">
+      <c r="J58" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K58)),RIGHT(K58,LEN(K58)-FIND(" ",K58)))</f>
         <v>candersoni</v>
       </c>
@@ -18437,7 +18449,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J59" s="59" t="str">
+      <c r="J59" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K59)),RIGHT(K59,LEN(K59)-FIND(" ",K59)))</f>
         <v>calbicans</v>
       </c>
@@ -18446,7 +18458,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J60" s="59" t="str">
+      <c r="J60" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K60)),RIGHT(K60,LEN(K60)-FIND(" ",K60)))</f>
         <v>calbicans</v>
       </c>
@@ -18455,7 +18467,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J61" s="59" t="str">
+      <c r="J61" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K61)),RIGHT(K61,LEN(K61)-FIND(" ",K61)))</f>
         <v>calbicans</v>
       </c>
@@ -18464,7 +18476,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J62" s="59" t="str">
+      <c r="J62" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K62)),RIGHT(K62,LEN(K62)-FIND(" ",K62)))</f>
         <v>calbicans</v>
       </c>
@@ -18473,7 +18485,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J63" s="59" t="str">
+      <c r="J63" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K63)),RIGHT(K63,LEN(K63)-FIND(" ",K63)))</f>
         <v>calbicans</v>
       </c>
@@ -18482,7 +18494,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J64" s="59" t="str">
+      <c r="J64" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K64)),RIGHT(K64,LEN(K64)-FIND(" ",K64)))</f>
         <v>calbicans</v>
       </c>
@@ -18491,7 +18503,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J65" s="59" t="str">
+      <c r="J65" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K65)),RIGHT(K65,LEN(K65)-FIND(" ",K65)))</f>
         <v>calbicans</v>
       </c>
@@ -18500,7 +18512,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J66" s="60" t="s">
+      <c r="J66" s="61" t="s">
         <v>1080</v>
       </c>
       <c r="K66" s="7" t="s">
@@ -18515,7 +18527,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J67" s="59" t="str">
+      <c r="J67" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K67)),RIGHT(K67,LEN(K67)-FIND(" ",K67)))</f>
         <v>cauris</v>
       </c>
@@ -18531,7 +18543,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J68" s="59" t="str">
+      <c r="J68" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K68)),RIGHT(K68,LEN(K68)-FIND(" ",K68)))</f>
         <v>cbantiana</v>
       </c>
@@ -18547,7 +18559,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J69" s="60" t="s">
+      <c r="J69" s="61" t="s">
         <v>1081</v>
       </c>
       <c r="K69" s="7" t="s">
@@ -18562,7 +18574,7 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J70" s="59" t="str">
+      <c r="J70" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K70)),RIGHT(K70,LEN(K70)-FIND(" ",K70)))</f>
         <v>cbantiana</v>
       </c>
@@ -18571,7 +18583,7 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J71" s="59" t="str">
+      <c r="J71" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K71)),RIGHT(K71,LEN(K71)-FIND(" ",K71)))</f>
         <v>cbantiana</v>
       </c>
@@ -18580,7 +18592,7 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J72" s="59" t="str">
+      <c r="J72" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K72)),RIGHT(K72,LEN(K72)-FIND(" ",K72)))</f>
         <v>cbovis</v>
       </c>
@@ -18596,7 +18608,7 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J73" s="59" t="str">
+      <c r="J73" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K73)),RIGHT(K73,LEN(K73)-FIND(" ",K73)))</f>
         <v>cburnetii</v>
       </c>
@@ -18612,7 +18624,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J74" s="59" t="str">
+      <c r="J74" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K74)),RIGHT(K74,LEN(K74)-FIND(" ",K74)))</f>
         <v>ccoronatus</v>
       </c>
@@ -18628,7 +18640,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J75" s="59" t="str">
+      <c r="J75" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K75)),RIGHT(K75,LEN(K75)-FIND(" ",K75)))</f>
         <v>cburnetii</v>
       </c>
@@ -18637,7 +18649,7 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J76" s="59" t="str">
+      <c r="J76" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K76)),RIGHT(K76,LEN(K76)-FIND(" ",K76)))</f>
         <v>ccoronavirus</v>
       </c>
@@ -18653,7 +18665,7 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J77" s="59" t="str">
+      <c r="J77" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K77)),RIGHT(K77,LEN(K77)-FIND(" ",K77)))</f>
         <v>cdifficile</v>
       </c>
@@ -18669,7 +18681,7 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J78" s="59" t="str">
+      <c r="J78" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K78)),RIGHT(K78,LEN(K78)-FIND(" ",K78)))</f>
         <v>cfelis</v>
       </c>
@@ -18685,7 +18697,7 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J79" s="59" t="str">
+      <c r="J79" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K79)),RIGHT(K79,LEN(K79)-FIND(" ",K79)))</f>
         <v>cgattii</v>
       </c>
@@ -18701,7 +18713,7 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J80" s="60" t="s">
+      <c r="J80" s="61" t="s">
         <v>1082</v>
       </c>
       <c r="K80" s="7" t="s">
@@ -18716,7 +18728,7 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J81" s="59" t="str">
+      <c r="J81" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K81)),RIGHT(K81,LEN(K81)-FIND(" ",K81)))</f>
         <v>cgattii</v>
       </c>
@@ -18725,7 +18737,7 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J82" s="59" t="str">
+      <c r="J82" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K82)),RIGHT(K82,LEN(K82)-FIND(" ",K82)))</f>
         <v>cgattii</v>
       </c>
@@ -18734,7 +18746,7 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J83" s="59" t="str">
+      <c r="J83" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K83)),RIGHT(K83,LEN(K83)-FIND(" ",K83)))</f>
         <v>cgattii</v>
       </c>
@@ -18743,7 +18755,7 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J84" s="59" t="str">
+      <c r="J84" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K84)),RIGHT(K84,LEN(K84)-FIND(" ",K84)))</f>
         <v>cgattii</v>
       </c>
@@ -18752,7 +18764,7 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J85" s="59" t="str">
+      <c r="J85" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K85)),RIGHT(K85,LEN(K85)-FIND(" ",K85)))</f>
         <v>cimmitis</v>
       </c>
@@ -18768,7 +18780,7 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J86" s="59" t="str">
+      <c r="J86" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K86)),RIGHT(K86,LEN(K86)-FIND(" ",K86)))</f>
         <v>cjejuni</v>
       </c>
@@ -18784,7 +18796,7 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J87" s="59" t="str">
+      <c r="J87" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K87)),RIGHT(K87,LEN(K87)-FIND(" ",K87)))</f>
         <v>cimmitis</v>
       </c>
@@ -18793,7 +18805,7 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J88" s="59" t="str">
+      <c r="J88" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K88)),RIGHT(K88,LEN(K88)-FIND(" ",K88)))</f>
         <v>cneoformans</v>
       </c>
@@ -18809,7 +18821,7 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J89" s="59" t="str">
+      <c r="J89" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K89)),RIGHT(K89,LEN(K89)-FIND(" ",K89)))</f>
         <v>cjejuni</v>
       </c>
@@ -18818,7 +18830,7 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J90" s="60" t="s">
+      <c r="J90" s="61" t="s">
         <v>1084</v>
       </c>
       <c r="K90" s="7" t="s">
@@ -18833,7 +18845,7 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J91" s="59" t="str">
+      <c r="J91" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K91)),RIGHT(K91,LEN(K91)-FIND(" ",K91)))</f>
         <v>cneoformans</v>
       </c>
@@ -18842,7 +18854,7 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J92" s="59" t="str">
+      <c r="J92" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K92)),RIGHT(K92,LEN(K92)-FIND(" ",K92)))</f>
         <v>cneoformans</v>
       </c>
@@ -18851,7 +18863,7 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J93" s="59" t="str">
+      <c r="J93" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K93)),RIGHT(K93,LEN(K93)-FIND(" ",K93)))</f>
         <v>cneoformans</v>
       </c>
@@ -18860,7 +18872,7 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J94" s="59" t="str">
+      <c r="J94" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K94)),RIGHT(K94,LEN(K94)-FIND(" ",K94)))</f>
         <v>cparvovirus</v>
       </c>
@@ -18876,7 +18888,7 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J95" s="59" t="str">
+      <c r="J95" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K95)),RIGHT(K95,LEN(K95)-FIND(" ",K95)))</f>
         <v>cparvum</v>
       </c>
@@ -18892,7 +18904,7 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J96" s="60" t="s">
+      <c r="J96" s="61" t="s">
         <v>1085</v>
       </c>
       <c r="K96" s="7" t="s">
@@ -18907,7 +18919,7 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J97" s="60" t="s">
+      <c r="J97" s="61" t="s">
         <v>1086</v>
       </c>
       <c r="K97" s="7" t="s">
@@ -18922,7 +18934,7 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J98" s="60" t="s">
+      <c r="J98" s="61" t="s">
         <v>1087</v>
       </c>
       <c r="K98" s="7" t="s">
@@ -18937,7 +18949,7 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J99" s="60" t="s">
+      <c r="J99" s="61" t="s">
         <v>1088</v>
       </c>
       <c r="K99" s="7" t="s">
@@ -18952,7 +18964,7 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J100" s="60" t="s">
+      <c r="J100" s="61" t="s">
         <v>1089</v>
       </c>
       <c r="K100" s="7" t="s">
@@ -18967,7 +18979,7 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J101" s="59" t="str">
+      <c r="J101" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K101)),RIGHT(K101,LEN(K101)-FIND(" ",K101)))</f>
         <v>cperfringens C</v>
       </c>
@@ -18976,7 +18988,7 @@
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J102" s="59" t="str">
+      <c r="J102" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K102)),RIGHT(K102,LEN(K102)-FIND(" ",K102)))</f>
         <v>cpseudotuberculosis</v>
       </c>
@@ -18992,7 +19004,7 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J103" s="59" t="str">
+      <c r="J103" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K103)),RIGHT(K103,LEN(K103)-FIND(" ",K103)))</f>
         <v>cpsittaci</v>
       </c>
@@ -19008,7 +19020,7 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J104" s="59" t="str">
+      <c r="J104" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K104)),RIGHT(K104,LEN(K104)-FIND(" ",K104)))</f>
         <v>cpseudotuberculosis</v>
       </c>
@@ -19017,7 +19029,7 @@
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J105" s="59" t="str">
+      <c r="J105" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K105)),RIGHT(K105,LEN(K105)-FIND(" ",K105)))</f>
         <v>cpurpurea</v>
       </c>
@@ -19033,7 +19045,7 @@
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J106" s="59" t="str">
+      <c r="J106" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K106)),RIGHT(K106,LEN(K106)-FIND(" ",K106)))</f>
         <v>cryanae</v>
       </c>
@@ -19049,7 +19061,7 @@
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J107" s="60" t="s">
+      <c r="J107" s="61" t="s">
         <v>1090</v>
       </c>
       <c r="K107" s="6" t="s">
@@ -19064,7 +19076,7 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J108" s="59" t="str">
+      <c r="J108" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K108)),RIGHT(K108,LEN(K108)-FIND(" ",K108)))</f>
         <v>ctetani</v>
       </c>
@@ -19080,7 +19092,7 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J109" s="59" t="str">
+      <c r="J109" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K109)),RIGHT(K109,LEN(K109)-FIND(" ",K109)))</f>
         <v>ctrachomatis</v>
       </c>
@@ -19096,7 +19108,7 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J110" s="59" t="str">
+      <c r="J110" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K110)),RIGHT(K110,LEN(K110)-FIND(" ",K110)))</f>
         <v>ctetani</v>
       </c>
@@ -19105,7 +19117,7 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J111" s="59" t="str">
+      <c r="J111" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K111)),RIGHT(K111,LEN(K111)-FIND(" ",K111)))</f>
         <v>ctetani</v>
       </c>
@@ -19114,7 +19126,7 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J112" s="59" t="str">
+      <c r="J112" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K112)),RIGHT(K112,LEN(K112)-FIND(" ",K112)))</f>
         <v>ctetani</v>
       </c>
@@ -19123,7 +19135,7 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J113" s="60" t="s">
+      <c r="J113" s="61" t="s">
         <v>1091</v>
       </c>
       <c r="K113" s="7" t="s">
@@ -19138,7 +19150,7 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J114" s="59" t="str">
+      <c r="J114" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K114)),RIGHT(K114,LEN(K114)-FIND(" ",K114)))</f>
         <v>dcongolensis</v>
       </c>
@@ -19154,7 +19166,7 @@
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J115" s="59" t="str">
+      <c r="J115" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K115)),RIGHT(K115,LEN(K115)-FIND(" ",K115)))</f>
         <v>dnodosus</v>
       </c>
@@ -19170,7 +19182,7 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J116" s="60" t="s">
+      <c r="J116" s="61" t="s">
         <v>1095</v>
       </c>
       <c r="K116" s="7" t="s">
@@ -19185,7 +19197,7 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J117" s="59" t="str">
+      <c r="J117" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K117)),RIGHT(K117,LEN(K117)-FIND(" ",K117)))</f>
         <v>dnodosus</v>
       </c>
@@ -19194,7 +19206,7 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J118" s="60" t="s">
+      <c r="J118" s="61" t="s">
         <v>1096</v>
       </c>
       <c r="K118" s="7" t="s">
@@ -19209,7 +19221,7 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J119" s="60" t="s">
+      <c r="J119" s="61" t="s">
         <v>1097</v>
       </c>
       <c r="K119" s="7" t="s">
@@ -19224,7 +19236,7 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J120" s="60" t="s">
+      <c r="J120" s="61" t="s">
         <v>1098</v>
       </c>
       <c r="K120" s="7" t="s">
@@ -19239,7 +19251,7 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J121" s="59" t="str">
+      <c r="J121" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K121)),RIGHT(K121,LEN(K121)-FIND(" ",K121)))</f>
         <v>ecoli</v>
       </c>
@@ -19255,7 +19267,7 @@
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J122" s="60" t="s">
+      <c r="J122" s="61" t="s">
         <v>1099</v>
       </c>
       <c r="K122" s="0" t="s">
@@ -19270,7 +19282,7 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J123" s="59" t="str">
+      <c r="J123" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K123)),RIGHT(K123,LEN(K123)-FIND(" ",K123)))</f>
         <v>ecoli</v>
       </c>
@@ -19279,7 +19291,7 @@
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J124" s="59" t="str">
+      <c r="J124" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K124)),RIGHT(K124,LEN(K124)-FIND(" ",K124)))</f>
         <v>ecoli</v>
       </c>
@@ -19288,7 +19300,7 @@
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J125" s="59" t="str">
+      <c r="J125" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K125)),RIGHT(K125,LEN(K125)-FIND(" ",K125)))</f>
         <v>ecoli</v>
       </c>
@@ -19297,7 +19309,7 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J126" s="59" t="str">
+      <c r="J126" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K126)),RIGHT(K126,LEN(K126)-FIND(" ",K126)))</f>
         <v>ecoli</v>
       </c>
@@ -19306,7 +19318,7 @@
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J127" s="59" t="str">
+      <c r="J127" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K127)),RIGHT(K127,LEN(K127)-FIND(" ",K127)))</f>
         <v>ecoli</v>
       </c>
@@ -19315,7 +19327,7 @@
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J128" s="59" t="str">
+      <c r="J128" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K128)),RIGHT(K128,LEN(K128)-FIND(" ",K128)))</f>
         <v>ecoli</v>
       </c>
@@ -19324,7 +19336,7 @@
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J129" s="59" t="str">
+      <c r="J129" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K129)),RIGHT(K129,LEN(K129)-FIND(" ",K129)))</f>
         <v>edermatitidis</v>
       </c>
@@ -19340,7 +19352,7 @@
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J130" s="60" t="s">
+      <c r="J130" s="61" t="s">
         <v>1100</v>
       </c>
       <c r="K130" s="7" t="s">
@@ -19355,7 +19367,7 @@
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J131" s="59" t="str">
+      <c r="J131" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K131)),RIGHT(K131,LEN(K131)-FIND(" ",K131)))</f>
         <v>edermatitidis</v>
       </c>
@@ -19364,7 +19376,7 @@
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J132" s="59" t="str">
+      <c r="J132" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K132)),RIGHT(K132,LEN(K132)-FIND(" ",K132)))</f>
         <v>edermatitidis</v>
       </c>
@@ -19373,7 +19385,7 @@
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J133" s="60" t="s">
+      <c r="J133" s="61" t="s">
         <v>1101</v>
       </c>
       <c r="K133" s="6" t="s">
@@ -19388,7 +19400,7 @@
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J134" s="60" t="s">
+      <c r="J134" s="61" t="s">
         <v>1102</v>
       </c>
       <c r="K134" s="6" t="s">
@@ -19403,7 +19415,7 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J135" s="59" t="str">
+      <c r="J135" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K135)),RIGHT(K135,LEN(K135)-FIND(" ",K135)))</f>
         <v>ehemorrhagic disease virus</v>
       </c>
@@ -19412,7 +19424,7 @@
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J136" s="60" t="s">
+      <c r="J136" s="61" t="s">
         <v>1103</v>
       </c>
       <c r="K136" s="7" t="s">
@@ -19427,7 +19439,7 @@
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J137" s="60" t="s">
+      <c r="J137" s="61" t="s">
         <v>1104</v>
       </c>
       <c r="K137" s="7" t="s">
@@ -19442,7 +19454,7 @@
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J138" s="59" t="str">
+      <c r="J138" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K138)),RIGHT(K138,LEN(K138)-FIND(" ",K138)))</f>
         <v>erhusiopathiae</v>
       </c>
@@ -19458,7 +19470,7 @@
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J139" s="59" t="str">
+      <c r="J139" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K139)),RIGHT(K139,LEN(K139)-FIND(" ",K139)))</f>
         <v>erotavirus</v>
       </c>
@@ -19474,7 +19486,7 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J140" s="60" t="s">
+      <c r="J140" s="61" t="s">
         <v>1105</v>
       </c>
       <c r="K140" s="7" t="s">
@@ -19489,7 +19501,7 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J141" s="59" t="str">
+      <c r="J141" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K141)),RIGHT(K141,LEN(K141)-FIND(" ",K141)))</f>
         <v>fcalicivirus</v>
       </c>
@@ -19505,7 +19517,7 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J142" s="60" t="s">
+      <c r="J142" s="61" t="s">
         <v>1106</v>
       </c>
       <c r="K142" s="7" t="s">
@@ -19520,7 +19532,7 @@
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J143" s="59" t="str">
+      <c r="J143" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K143)),RIGHT(K143,LEN(K143)-FIND(" ",K143)))</f>
         <v>fgraminearum</v>
       </c>
@@ -19536,7 +19548,7 @@
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J144" s="59" t="str">
+      <c r="J144" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K144)),RIGHT(K144,LEN(K144)-FIND(" ",K144)))</f>
         <v>fdisease virus</v>
       </c>
@@ -19545,7 +19557,7 @@
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J145" s="59" t="str">
+      <c r="J145" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K145)),RIGHT(K145,LEN(K145)-FIND(" ",K145)))</f>
         <v>fdisease virus</v>
       </c>
@@ -19554,7 +19566,7 @@
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J146" s="59" t="str">
+      <c r="J146" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K146)),RIGHT(K146,LEN(K146)-FIND(" ",K146)))</f>
         <v>fdisease virus</v>
       </c>
@@ -19563,7 +19575,7 @@
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J147" s="59" t="str">
+      <c r="J147" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K147)),RIGHT(K147,LEN(K147)-FIND(" ",K147)))</f>
         <v>fdisease virus</v>
       </c>
@@ -19572,7 +19584,7 @@
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J148" s="59" t="str">
+      <c r="J148" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K148)),RIGHT(K148,LEN(K148)-FIND(" ",K148)))</f>
         <v>fdisease virus</v>
       </c>
@@ -19581,7 +19593,7 @@
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J149" s="60" t="s">
+      <c r="J149" s="61" t="s">
         <v>1107</v>
       </c>
       <c r="K149" s="7" t="s">
@@ -19596,7 +19608,7 @@
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J150" s="60" t="s">
+      <c r="J150" s="61" t="s">
         <v>1108</v>
       </c>
       <c r="K150" s="7" t="s">
@@ -19611,7 +19623,7 @@
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J151" s="60" t="s">
+      <c r="J151" s="61" t="s">
         <v>1109</v>
       </c>
       <c r="K151" s="7" t="s">
@@ -19626,7 +19638,7 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J152" s="59" t="str">
+      <c r="J152" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K152)),RIGHT(K152,LEN(K152)-FIND(" ",K152)))</f>
         <v>fnecrophorum</v>
       </c>
@@ -19642,7 +19654,7 @@
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J153" s="60" t="s">
+      <c r="J153" s="61" t="s">
         <v>1110</v>
       </c>
       <c r="K153" s="7" t="s">
@@ -19657,7 +19669,7 @@
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J154" s="59" t="str">
+      <c r="J154" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K154)),RIGHT(K154,LEN(K154)-FIND(" ",K154)))</f>
         <v>fnecrophorum</v>
       </c>
@@ -19666,7 +19678,7 @@
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J155" s="59" t="str">
+      <c r="J155" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K155)),RIGHT(K155,LEN(K155)-FIND(" ",K155)))</f>
         <v>fproliferatum</v>
       </c>
@@ -19682,7 +19694,7 @@
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J156" s="59" t="str">
+      <c r="J156" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K156)),RIGHT(K156,LEN(K156)-FIND(" ",K156)))</f>
         <v>fverticillioides</v>
       </c>
@@ -19698,7 +19710,7 @@
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J157" s="59" t="str">
+      <c r="J157" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K157)),RIGHT(K157,LEN(K157)-FIND(" ",K157)))</f>
         <v>fproliferatum</v>
       </c>
@@ -19707,7 +19719,7 @@
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J158" s="59" t="str">
+      <c r="J158" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K158)),RIGHT(K158,LEN(K158)-FIND(" ",K158)))</f>
         <v>fvirus</v>
       </c>
@@ -19723,7 +19735,7 @@
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J159" s="59" t="str">
+      <c r="J159" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K159)),RIGHT(K159,LEN(K159)-FIND(" ",K159)))</f>
         <v>fverticillioides (moniliforme)</v>
       </c>
@@ -19732,7 +19744,7 @@
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J160" s="60" t="s">
+      <c r="J160" s="61" t="s">
         <v>1113</v>
       </c>
       <c r="K160" s="7" t="s">
@@ -19747,7 +19759,7 @@
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J161" s="60" t="s">
+      <c r="J161" s="61" t="s">
         <v>1114</v>
       </c>
       <c r="K161" s="0" t="s">
@@ -19762,7 +19774,7 @@
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J162" s="60" t="s">
+      <c r="J162" s="61" t="s">
         <v>1115</v>
       </c>
       <c r="K162" s="0" t="s">
@@ -19777,7 +19789,7 @@
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J163" s="60" t="s">
+      <c r="J163" s="61" t="s">
         <v>1116</v>
       </c>
       <c r="K163" s="0" t="s">
@@ -19792,7 +19804,7 @@
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J164" s="59" t="str">
+      <c r="J164" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K164)),RIGHT(K164,LEN(K164)-FIND(" ",K164)))</f>
         <v>hcapsulatum</v>
       </c>
@@ -19808,7 +19820,7 @@
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J165" s="60" t="s">
+      <c r="J165" s="61" t="s">
         <v>1117</v>
       </c>
       <c r="K165" s="7" t="s">
@@ -19823,7 +19835,7 @@
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J166" s="59" t="str">
+      <c r="J166" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K166)),RIGHT(K166,LEN(K166)-FIND(" ",K166)))</f>
         <v>hcapsulatum</v>
       </c>
@@ -19832,7 +19844,7 @@
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J167" s="59" t="str">
+      <c r="J167" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K167)),RIGHT(K167,LEN(K167)-FIND(" ",K167)))</f>
         <v>hcapsulatum</v>
       </c>
@@ -19841,7 +19853,7 @@
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J168" s="60" t="s">
+      <c r="J168" s="61" t="s">
         <v>1120</v>
       </c>
       <c r="K168" s="0" t="s">
@@ -19856,7 +19868,7 @@
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J169" s="60" t="s">
+      <c r="J169" s="61" t="s">
         <v>1121</v>
       </c>
       <c r="K169" s="0" t="s">
@@ -19871,7 +19883,7 @@
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J170" s="60" t="s">
+      <c r="J170" s="61" t="s">
         <v>1122</v>
       </c>
       <c r="K170" s="0" t="s">
@@ -19886,7 +19898,7 @@
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J171" s="60" t="s">
+      <c r="J171" s="61" t="s">
         <v>1123</v>
       </c>
       <c r="K171" s="0" t="s">
@@ -19901,13 +19913,13 @@
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J172" s="60" t="s">
+      <c r="J172" s="61" t="s">
         <v>1124</v>
       </c>
-      <c r="K172" s="48" t="s">
+      <c r="K172" s="49" t="s">
         <v>987</v>
       </c>
-      <c r="L172" s="48" t="s">
+      <c r="L172" s="49" t="s">
         <v>988</v>
       </c>
       <c r="M172" s="0" t="str">
@@ -19916,7 +19928,7 @@
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J173" s="60" t="s">
+      <c r="J173" s="61" t="s">
         <v>1125</v>
       </c>
       <c r="K173" s="0" t="s">
@@ -19931,7 +19943,7 @@
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J174" s="60" t="s">
+      <c r="J174" s="61" t="s">
         <v>1126</v>
       </c>
       <c r="K174" s="0" t="s">
@@ -19946,7 +19958,7 @@
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J175" s="60" t="s">
+      <c r="J175" s="61" t="s">
         <v>1127</v>
       </c>
       <c r="K175" s="0" t="s">
@@ -19961,7 +19973,7 @@
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J176" s="60" t="s">
+      <c r="J176" s="61" t="s">
         <v>1128</v>
       </c>
       <c r="K176" s="7" t="s">
@@ -19976,7 +19988,7 @@
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J177" s="60" t="s">
+      <c r="J177" s="61" t="s">
         <v>1129</v>
       </c>
       <c r="K177" s="0" t="s">
@@ -19991,7 +20003,7 @@
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J178" s="60" t="s">
+      <c r="J178" s="61" t="s">
         <v>1130</v>
       </c>
       <c r="K178" s="7" t="s">
@@ -20006,7 +20018,7 @@
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J179" s="60" t="s">
+      <c r="J179" s="61" t="s">
         <v>1131</v>
       </c>
       <c r="K179" s="0" t="s">
@@ -20021,7 +20033,7 @@
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J180" s="59" t="str">
+      <c r="J180" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K180)),RIGHT(K180,LEN(K180)-FIND(" ",K180)))</f>
         <v>iA (H3N2)</v>
       </c>
@@ -20030,7 +20042,7 @@
       </c>
     </row>
     <row r="181" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J181" s="59" t="str">
+      <c r="J181" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K181)),RIGHT(K181,LEN(K181)-FIND(" ",K181)))</f>
         <v>lautumnalis</v>
       </c>
@@ -20046,7 +20058,7 @@
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J182" s="59" t="str">
+      <c r="J182" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K182)),RIGHT(K182,LEN(K182)-FIND(" ",K182)))</f>
         <v>lborgpetersenii</v>
       </c>
@@ -20062,7 +20074,7 @@
       </c>
     </row>
     <row r="183" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J183" s="59" t="str">
+      <c r="J183" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K183)),RIGHT(K183,LEN(K183)-FIND(" ",K183)))</f>
         <v>lgrippothyphosa</v>
       </c>
@@ -20078,7 +20090,7 @@
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J184" s="59" t="str">
+      <c r="J184" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K184)),RIGHT(K184,LEN(K184)-FIND(" ",K184)))</f>
         <v>lborgpetersenii</v>
       </c>
@@ -20087,7 +20099,7 @@
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J185" s="59" t="str">
+      <c r="J185" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K185)),RIGHT(K185,LEN(K185)-FIND(" ",K185)))</f>
         <v>lhyos</v>
       </c>
@@ -20103,7 +20115,7 @@
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J186" s="59" t="str">
+      <c r="J186" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K186)),RIGHT(K186,LEN(K186)-FIND(" ",K186)))</f>
         <v>linterrogans</v>
       </c>
@@ -20119,7 +20131,7 @@
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J187" s="59" t="str">
+      <c r="J187" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K187)),RIGHT(K187,LEN(K187)-FIND(" ",K187)))</f>
         <v>lintracellularis</v>
       </c>
@@ -20135,7 +20147,7 @@
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J188" s="59" t="str">
+      <c r="J188" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K188)),RIGHT(K188,LEN(K188)-FIND(" ",K188)))</f>
         <v>linterrogans</v>
       </c>
@@ -20144,7 +20156,7 @@
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J189" s="59" t="str">
+      <c r="J189" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K189)),RIGHT(K189,LEN(K189)-FIND(" ",K189)))</f>
         <v>linterrogans</v>
       </c>
@@ -20153,7 +20165,7 @@
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J190" s="59" t="str">
+      <c r="J190" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K190)),RIGHT(K190,LEN(K190)-FIND(" ",K190)))</f>
         <v>linterrogans</v>
       </c>
@@ -20162,7 +20174,7 @@
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J191" s="59" t="str">
+      <c r="J191" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K191)),RIGHT(K191,LEN(K191)-FIND(" ",K191)))</f>
         <v>lkirschneri</v>
       </c>
@@ -20178,7 +20190,7 @@
       </c>
     </row>
     <row r="192" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J192" s="59" t="str">
+      <c r="J192" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K192)),RIGHT(K192,LEN(K192)-FIND(" ",K192)))</f>
         <v>lmonocytogenes</v>
       </c>
@@ -20194,7 +20206,7 @@
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J193" s="59" t="str">
+      <c r="J193" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K193)),RIGHT(K193,LEN(K193)-FIND(" ",K193)))</f>
         <v>lkirschneri</v>
       </c>
@@ -20203,7 +20215,7 @@
       </c>
     </row>
     <row r="194" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J194" s="59" t="str">
+      <c r="J194" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K194)),RIGHT(K194,LEN(K194)-FIND(" ",K194)))</f>
         <v>lpomona</v>
       </c>
@@ -20219,7 +20231,7 @@
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J195" s="59" t="str">
+      <c r="J195" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K195)),RIGHT(K195,LEN(K195)-FIND(" ",K195)))</f>
         <v>lrabies</v>
       </c>
@@ -20235,7 +20247,7 @@
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J196" s="60" t="s">
+      <c r="J196" s="61" t="s">
         <v>1133</v>
       </c>
       <c r="K196" s="6" t="s">
@@ -20250,7 +20262,7 @@
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J197" s="59" t="str">
+      <c r="J197" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K197)),RIGHT(K197,LEN(K197)-FIND(" ",K197)))</f>
         <v>lrabies</v>
       </c>
@@ -20259,7 +20271,7 @@
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J198" s="59" t="str">
+      <c r="J198" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K198)),RIGHT(K198,LEN(K198)-FIND(" ",K198)))</f>
         <v>lrabies</v>
       </c>
@@ -20268,7 +20280,7 @@
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J199" s="60" t="s">
+      <c r="J199" s="61" t="s">
         <v>1134</v>
       </c>
       <c r="K199" s="7" t="s">
@@ -20283,7 +20295,7 @@
       </c>
     </row>
     <row r="200" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J200" s="59" t="str">
+      <c r="J200" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K200)),RIGHT(K200,LEN(K200)-FIND(" ",K200)))</f>
         <v>lskin disease virus</v>
       </c>
@@ -20292,7 +20304,7 @@
       </c>
     </row>
     <row r="201" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J201" s="59" t="str">
+      <c r="J201" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K201)),RIGHT(K201,LEN(K201)-FIND(" ",K201)))</f>
         <v>malcelaphinegamma1</v>
       </c>
@@ -20308,7 +20320,7 @@
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J202" s="60" t="s">
+      <c r="J202" s="61" t="s">
         <v>1135</v>
       </c>
       <c r="K202" s="7" t="s">
@@ -20323,7 +20335,7 @@
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J203" s="59" t="str">
+      <c r="J203" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K203)),RIGHT(K203,LEN(K203)-FIND(" ",K203)))</f>
         <v>mbovis</v>
       </c>
@@ -20339,7 +20351,7 @@
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J204" s="59" t="str">
+      <c r="J204" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K204)),RIGHT(K204,LEN(K204)-FIND(" ",K204)))</f>
         <v>mavium subsp. Paratuberculosis</v>
       </c>
@@ -20348,7 +20360,7 @@
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J205" s="59" t="str">
+      <c r="J205" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K205)),RIGHT(K205,LEN(K205)-FIND(" ",K205)))</f>
         <v>mavium subsp. Paratuberculosis</v>
       </c>
@@ -20357,7 +20369,7 @@
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J206" s="59" t="str">
+      <c r="J206" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K206)),RIGHT(K206,LEN(K206)-FIND(" ",K206)))</f>
         <v>mcanis</v>
       </c>
@@ -20373,7 +20385,7 @@
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J207" s="59" t="str">
+      <c r="J207" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K207)),RIGHT(K207,LEN(K207)-FIND(" ",K207)))</f>
         <v>mbovis</v>
       </c>
@@ -20382,7 +20394,7 @@
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J208" s="59" t="str">
+      <c r="J208" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K208)),RIGHT(K208,LEN(K208)-FIND(" ",K208)))</f>
         <v>mbovis</v>
       </c>
@@ -20391,7 +20403,7 @@
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J209" s="59" t="str">
+      <c r="J209" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K209)),RIGHT(K209,LEN(K209)-FIND(" ",K209)))</f>
         <v>mcanis</v>
       </c>
@@ -20407,7 +20419,7 @@
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J210" s="60" t="s">
+      <c r="J210" s="61" t="s">
         <v>1138</v>
       </c>
       <c r="K210" s="7" t="s">
@@ -20422,7 +20434,7 @@
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J211" s="59" t="str">
+      <c r="J211" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K211)),RIGHT(K211,LEN(K211)-FIND(" ",K211)))</f>
         <v>mcanis</v>
       </c>
@@ -20431,7 +20443,7 @@
       </c>
     </row>
     <row r="212" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J212" s="59" t="str">
+      <c r="J212" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K212)),RIGHT(K212,LEN(K212)-FIND(" ",K212)))</f>
         <v>mcaprinegamma2</v>
       </c>
@@ -20447,7 +20459,7 @@
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J213" s="59" t="str">
+      <c r="J213" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K213)),RIGHT(K213,LEN(K213)-FIND(" ",K213)))</f>
         <v>mconjunctivae</v>
       </c>
@@ -20463,7 +20475,7 @@
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J214" s="60" t="s">
+      <c r="J214" s="61" t="s">
         <v>1139</v>
       </c>
       <c r="K214" s="7" t="s">
@@ -20478,7 +20490,7 @@
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J215" s="59" t="str">
+      <c r="J215" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K215)),RIGHT(K215,LEN(K215)-FIND(" ",K215)))</f>
         <v>mgallisepticum</v>
       </c>
@@ -20494,7 +20506,7 @@
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J216" s="59" t="str">
+      <c r="J216" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K216)),RIGHT(K216,LEN(K216)-FIND(" ",K216)))</f>
         <v>mhaemolytica</v>
       </c>
@@ -20510,7 +20522,7 @@
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J217" s="59" t="str">
+      <c r="J217" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K217)),RIGHT(K217,LEN(K217)-FIND(" ",K217)))</f>
         <v>mmycoides</v>
       </c>
@@ -20526,7 +20538,7 @@
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J218" s="59" t="str">
+      <c r="J218" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K218)),RIGHT(K218,LEN(K218)-FIND(" ",K218)))</f>
         <v>mhaemolytica</v>
       </c>
@@ -20535,7 +20547,7 @@
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J219" s="59" t="str">
+      <c r="J219" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K219)),RIGHT(K219,LEN(K219)-FIND(" ",K219)))</f>
         <v>mnanum</v>
       </c>
@@ -20551,7 +20563,7 @@
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J220" s="59" t="str">
+      <c r="J220" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K220)),RIGHT(K220,LEN(K220)-FIND(" ",K220)))</f>
         <v>movinegamma2</v>
       </c>
@@ -20567,7 +20579,7 @@
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J221" s="59" t="str">
+      <c r="J221" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K221)),RIGHT(K221,LEN(K221)-FIND(" ",K221)))</f>
         <v>movis</v>
       </c>
@@ -20583,7 +20595,7 @@
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J222" s="59" t="str">
+      <c r="J222" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K222)),RIGHT(K222,LEN(K222)-FIND(" ",K222)))</f>
         <v>mpachydermatis</v>
       </c>
@@ -20599,7 +20611,7 @@
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J223" s="59" t="str">
+      <c r="J223" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K223)),RIGHT(K223,LEN(K223)-FIND(" ",K223)))</f>
         <v>movis</v>
       </c>
@@ -20608,7 +20620,7 @@
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J224" s="59" t="str">
+      <c r="J224" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K224)),RIGHT(K224,LEN(K224)-FIND(" ",K224)))</f>
         <v>mplutonius</v>
       </c>
@@ -20624,7 +20636,7 @@
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J225" s="59" t="str">
+      <c r="J225" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K225)),RIGHT(K225,LEN(K225)-FIND(" ",K225)))</f>
         <v>mpachydermatis</v>
       </c>
@@ -20633,7 +20645,7 @@
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J226" s="59" t="str">
+      <c r="J226" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K226)),RIGHT(K226,LEN(K226)-FIND(" ",K226)))</f>
         <v>mtuberculosis</v>
       </c>
@@ -20649,7 +20661,7 @@
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J227" s="59" t="str">
+      <c r="J227" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K227)),RIGHT(K227,LEN(K227)-FIND(" ",K227)))</f>
         <v>napis</v>
       </c>
@@ -20665,7 +20677,7 @@
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J228" s="59" t="str">
+      <c r="J228" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K228)),RIGHT(K228,LEN(K228)-FIND(" ",K228)))</f>
         <v>nasteroides</v>
       </c>
@@ -20681,7 +20693,7 @@
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J229" s="59" t="str">
+      <c r="J229" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K229)),RIGHT(K229,LEN(K229)-FIND(" ",K229)))</f>
         <v>nbrasiliensis</v>
       </c>
@@ -20697,7 +20709,7 @@
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J230" s="60" t="s">
+      <c r="J230" s="61" t="s">
         <v>1144</v>
       </c>
       <c r="K230" s="7" t="s">
@@ -20712,7 +20724,7 @@
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J231" s="60" t="s">
+      <c r="J231" s="61" t="s">
         <v>1145</v>
       </c>
       <c r="K231" s="0" t="s">
@@ -20727,7 +20739,7 @@
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J232" s="59" t="str">
+      <c r="J232" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K232)),RIGHT(K232,LEN(K232)-FIND(" ",K232)))</f>
         <v>ngonorrhoeae</v>
       </c>
@@ -20743,7 +20755,7 @@
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J233" s="60" t="s">
+      <c r="J233" s="61" t="s">
         <v>1146</v>
       </c>
       <c r="K233" s="0" t="s">
@@ -20758,7 +20770,7 @@
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J234" s="59" t="str">
+      <c r="J234" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K234)),RIGHT(K234,LEN(K234)-FIND(" ",K234)))</f>
         <v>nmeningitidis</v>
       </c>
@@ -20774,7 +20786,7 @@
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J235" s="59" t="str">
+      <c r="J235" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K235)),RIGHT(K235,LEN(K235)-FIND(" ",K235)))</f>
         <v>nristicii</v>
       </c>
@@ -20790,7 +20802,7 @@
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J236" s="59" t="str">
+      <c r="J236" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K236)),RIGHT(K236,LEN(K236)-FIND(" ",K236)))</f>
         <v>ovirus</v>
       </c>
@@ -20806,7 +20818,7 @@
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J237" s="59" t="str">
+      <c r="J237" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K237)),RIGHT(K237,LEN(K237)-FIND(" ",K237)))</f>
         <v>paeruginosa</v>
       </c>
@@ -20822,7 +20834,7 @@
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J238" s="59" t="str">
+      <c r="J238" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K238)),RIGHT(K238,LEN(K238)-FIND(" ",K238)))</f>
         <v>ovirus</v>
       </c>
@@ -20831,7 +20843,7 @@
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J239" s="59" t="str">
+      <c r="J239" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K239)),RIGHT(K239,LEN(K239)-FIND(" ",K239)))</f>
         <v>pchartarum</v>
       </c>
@@ -20847,7 +20859,7 @@
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J240" s="59" t="str">
+      <c r="J240" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K240)),RIGHT(K240,LEN(K240)-FIND(" ",K240)))</f>
         <v>paeruginosa</v>
       </c>
@@ -20856,7 +20868,7 @@
       </c>
     </row>
     <row r="241" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J241" s="60" t="s">
+      <c r="J241" s="61" t="s">
         <v>1147</v>
       </c>
       <c r="K241" s="6" t="s">
@@ -20871,7 +20883,7 @@
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J242" s="60" t="s">
+      <c r="J242" s="61" t="s">
         <v>1149</v>
       </c>
       <c r="K242" s="7" t="s">
@@ -20886,7 +20898,7 @@
       </c>
     </row>
     <row r="243" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J243" s="60" t="s">
+      <c r="J243" s="61" t="s">
         <v>1150</v>
       </c>
       <c r="K243" s="6" t="s">
@@ -20901,7 +20913,7 @@
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J244" s="59" t="str">
+      <c r="J244" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K244)),RIGHT(K244,LEN(K244)-FIND(" ",K244)))</f>
         <v>plarvae</v>
       </c>
@@ -20917,7 +20929,7 @@
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J245" s="59" t="str">
+      <c r="J245" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K245)),RIGHT(K245,LEN(K245)-FIND(" ",K245)))</f>
         <v>pmultocida</v>
       </c>
@@ -20933,7 +20945,7 @@
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J246" s="59" t="str">
+      <c r="J246" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K246)),RIGHT(K246,LEN(K246)-FIND(" ",K246)))</f>
         <v>ppuberulum</v>
       </c>
@@ -20949,7 +20961,7 @@
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J247" s="59" t="str">
+      <c r="J247" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K247)),RIGHT(K247,LEN(K247)-FIND(" ",K247)))</f>
         <v>pmultocida</v>
       </c>
@@ -20958,7 +20970,7 @@
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J248" s="59" t="str">
+      <c r="J248" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K248)),RIGHT(K248,LEN(K248)-FIND(" ",K248)))</f>
         <v>pmultocida</v>
       </c>
@@ -20967,7 +20979,7 @@
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J249" s="59" t="str">
+      <c r="J249" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K249)),RIGHT(K249,LEN(K249)-FIND(" ",K249)))</f>
         <v>pmultocida</v>
       </c>
@@ -20976,7 +20988,7 @@
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J250" s="59" t="str">
+      <c r="J250" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K250)),RIGHT(K250,LEN(K250)-FIND(" ",K250)))</f>
         <v>pmultocida</v>
       </c>
@@ -20985,7 +20997,7 @@
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J251" s="59" t="str">
+      <c r="J251" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K251)),RIGHT(K251,LEN(K251)-FIND(" ",K251)))</f>
         <v>pmultocida</v>
       </c>
@@ -20994,7 +21006,7 @@
       </c>
     </row>
     <row r="252" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J252" s="60" t="s">
+      <c r="J252" s="61" t="s">
         <v>1151</v>
       </c>
       <c r="K252" s="6" t="s">
@@ -21009,7 +21021,7 @@
       </c>
     </row>
     <row r="253" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J253" s="60" t="s">
+      <c r="J253" s="61" t="s">
         <v>1152</v>
       </c>
       <c r="K253" s="6" t="s">
@@ -21024,7 +21036,7 @@
       </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J254" s="60" t="s">
+      <c r="J254" s="61" t="s">
         <v>1153</v>
       </c>
       <c r="K254" s="7" t="s">
@@ -21039,7 +21051,7 @@
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J255" s="60" t="s">
+      <c r="J255" s="61" t="s">
         <v>1154</v>
       </c>
       <c r="K255" s="7" t="s">
@@ -21054,7 +21066,7 @@
       </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J256" s="60" t="s">
+      <c r="J256" s="61" t="s">
         <v>1155</v>
       </c>
       <c r="K256" s="7" t="s">
@@ -21069,7 +21081,7 @@
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J257" s="60" t="s">
+      <c r="J257" s="61" t="s">
         <v>1156</v>
       </c>
       <c r="K257" s="7" t="s">
@@ -21084,7 +21096,7 @@
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J258" s="60" t="s">
+      <c r="J258" s="61" t="s">
         <v>1157</v>
       </c>
       <c r="K258" s="7" t="s">
@@ -21099,7 +21111,7 @@
       </c>
     </row>
     <row r="259" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J259" s="59" t="str">
+      <c r="J259" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K259)),RIGHT(K259,LEN(K259)-FIND(" ",K259)))</f>
         <v>rvirus</v>
       </c>
@@ -21115,7 +21127,7 @@
       </c>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J260" s="59" t="str">
+      <c r="J260" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K260)),RIGHT(K260,LEN(K260)-FIND(" ",K260)))</f>
         <v>sagalactiae</v>
       </c>
@@ -21131,7 +21143,7 @@
       </c>
     </row>
     <row r="261" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J261" s="59" t="str">
+      <c r="J261" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K261)),RIGHT(K261,LEN(K261)-FIND(" ",K261)))</f>
         <v>rvirus</v>
       </c>
@@ -21140,7 +21152,7 @@
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J262" s="59" t="str">
+      <c r="J262" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K262)),RIGHT(K262,LEN(K262)-FIND(" ",K262)))</f>
         <v>sagona</v>
       </c>
@@ -21156,7 +21168,7 @@
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J263" s="60" t="s">
+      <c r="J263" s="61" t="s">
         <v>1158</v>
       </c>
       <c r="K263" s="7" t="s">
@@ -21171,7 +21183,7 @@
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J264" s="59" t="str">
+      <c r="J264" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K264)),RIGHT(K264,LEN(K264)-FIND(" ",K264)))</f>
         <v>saureus</v>
       </c>
@@ -21187,7 +21199,7 @@
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J265" s="59" t="str">
+      <c r="J265" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K265)),RIGHT(K265,LEN(K265)-FIND(" ",K265)))</f>
         <v>scanis</v>
       </c>
@@ -21203,7 +21215,7 @@
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J266" s="59" t="str">
+      <c r="J266" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K266)),RIGHT(K266,LEN(K266)-FIND(" ",K266)))</f>
         <v>saureus</v>
       </c>
@@ -21212,7 +21224,7 @@
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J267" s="59" t="str">
+      <c r="J267" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K267)),RIGHT(K267,LEN(K267)-FIND(" ",K267)))</f>
         <v>saureus</v>
       </c>
@@ -21221,7 +21233,7 @@
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J268" s="59" t="str">
+      <c r="J268" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K268)),RIGHT(K268,LEN(K268)-FIND(" ",K268)))</f>
         <v>saureus</v>
       </c>
@@ -21230,7 +21242,7 @@
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J269" s="59" t="str">
+      <c r="J269" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K269)),RIGHT(K269,LEN(K269)-FIND(" ",K269)))</f>
         <v>saureus</v>
       </c>
@@ -21239,7 +21251,7 @@
       </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J270" s="60" t="s">
+      <c r="J270" s="61" t="s">
         <v>1159</v>
       </c>
       <c r="K270" s="7" t="s">
@@ -21254,7 +21266,7 @@
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J271" s="59" t="str">
+      <c r="J271" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K271)),RIGHT(K271,LEN(K271)-FIND(" ",K271)))</f>
         <v>scanis</v>
       </c>
@@ -21263,7 +21275,7 @@
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J272" s="59" t="str">
+      <c r="J272" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K272)),RIGHT(K272,LEN(K272)-FIND(" ",K272)))</f>
         <v>scholeraesuis</v>
       </c>
@@ -21279,7 +21291,7 @@
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J273" s="59" t="str">
+      <c r="J273" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K273)),RIGHT(K273,LEN(K273)-FIND(" ",K273)))</f>
         <v>sdublin</v>
       </c>
@@ -21295,7 +21307,7 @@
       </c>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J274" s="59" t="str">
+      <c r="J274" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K274)),RIGHT(K274,LEN(K274)-FIND(" ",K274)))</f>
         <v>sdysenteriae</v>
       </c>
@@ -21311,7 +21323,7 @@
       </c>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J275" s="59" t="str">
+      <c r="J275" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K275)),RIGHT(K275,LEN(K275)-FIND(" ",K275)))</f>
         <v>senteritidis</v>
       </c>
@@ -21327,7 +21339,7 @@
       </c>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J276" s="60" t="s">
+      <c r="J276" s="61" t="s">
         <v>1161</v>
       </c>
       <c r="K276" s="7" t="s">
@@ -21342,7 +21354,7 @@
       </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J277" s="60" t="s">
+      <c r="J277" s="61" t="s">
         <v>1164</v>
       </c>
       <c r="K277" s="7" t="s">
@@ -21357,7 +21369,7 @@
       </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J278" s="59" t="str">
+      <c r="J278" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K278)),RIGHT(K278,LEN(K278)-FIND(" ",K278)))</f>
         <v>sfelis</v>
       </c>
@@ -21373,7 +21385,7 @@
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J279" s="59" t="str">
+      <c r="J279" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K279)),RIGHT(K279,LEN(K279)-FIND(" ",K279)))</f>
         <v>sequi subsp. Zooepidemicus</v>
       </c>
@@ -21382,7 +21394,7 @@
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J280" s="59" t="str">
+      <c r="J280" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K280)),RIGHT(K280,LEN(K280)-FIND(" ",K280)))</f>
         <v>sequi subsp. Zooepidemicus</v>
       </c>
@@ -21391,7 +21403,7 @@
       </c>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J281" s="59" t="str">
+      <c r="J281" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K281)),RIGHT(K281,LEN(K281)-FIND(" ",K281)))</f>
         <v>sflexneri</v>
       </c>
@@ -21407,7 +21419,7 @@
       </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J282" s="59" t="str">
+      <c r="J282" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K282)),RIGHT(K282,LEN(K282)-FIND(" ",K282)))</f>
         <v>sgallinarum</v>
       </c>
@@ -21423,7 +21435,7 @@
       </c>
     </row>
     <row r="283" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J283" s="59" t="str">
+      <c r="J283" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K283)),RIGHT(K283,LEN(K283)-FIND(" ",K283)))</f>
         <v>shyicus</v>
       </c>
@@ -21439,7 +21451,7 @@
       </c>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J284" s="60" t="s">
+      <c r="J284" s="61" t="s">
         <v>1169</v>
       </c>
       <c r="K284" s="7" t="s">
@@ -21454,7 +21466,7 @@
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J285" s="60" t="s">
+      <c r="J285" s="61" t="s">
         <v>1170</v>
       </c>
       <c r="K285" s="7" t="s">
@@ -21469,7 +21481,7 @@
       </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J286" s="59" t="str">
+      <c r="J286" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K286)),RIGHT(K286,LEN(K286)-FIND(" ",K286)))</f>
         <v>sintermedius</v>
       </c>
@@ -21485,7 +21497,7 @@
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J287" s="59" t="str">
+      <c r="J287" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K287)),RIGHT(K287,LEN(K287)-FIND(" ",K287)))</f>
         <v>snewport</v>
       </c>
@@ -21501,7 +21513,7 @@
       </c>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J288" s="59" t="str">
+      <c r="J288" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K288)),RIGHT(K288,LEN(K288)-FIND(" ",K288)))</f>
         <v>spneumoniae</v>
       </c>
@@ -21517,7 +21529,7 @@
       </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J289" s="59" t="str">
+      <c r="J289" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K289)),RIGHT(K289,LEN(K289)-FIND(" ",K289)))</f>
         <v>spseudintermedius</v>
       </c>
@@ -21533,7 +21545,7 @@
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J290" s="59" t="str">
+      <c r="J290" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K290)),RIGHT(K290,LEN(K290)-FIND(" ",K290)))</f>
         <v>spullorum</v>
       </c>
@@ -21549,7 +21561,7 @@
       </c>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J291" s="59" t="str">
+      <c r="J291" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K291)),RIGHT(K291,LEN(K291)-FIND(" ",K291)))</f>
         <v>spseudintermedius</v>
       </c>
@@ -21558,7 +21570,7 @@
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J292" s="59" t="str">
+      <c r="J292" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K292)),RIGHT(K292,LEN(K292)-FIND(" ",K292)))</f>
         <v>spseudintermedius</v>
       </c>
@@ -21567,7 +21579,7 @@
       </c>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J293" s="59" t="str">
+      <c r="J293" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K293)),RIGHT(K293,LEN(K293)-FIND(" ",K293)))</f>
         <v>sschenckii</v>
       </c>
@@ -21583,7 +21595,7 @@
       </c>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J294" s="59" t="str">
+      <c r="J294" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K294)),RIGHT(K294,LEN(K294)-FIND(" ",K294)))</f>
         <v>ssonnei</v>
       </c>
@@ -21599,7 +21611,7 @@
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J295" s="59" t="str">
+      <c r="J295" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K295)),RIGHT(K295,LEN(K295)-FIND(" ",K295)))</f>
         <v>sschenckii</v>
       </c>
@@ -21608,7 +21620,7 @@
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J296" s="59" t="str">
+      <c r="J296" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K296)),RIGHT(K296,LEN(K296)-FIND(" ",K296)))</f>
         <v>sschenckii</v>
       </c>
@@ -21617,7 +21629,7 @@
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J297" s="60" t="s">
+      <c r="J297" s="61" t="s">
         <v>1173</v>
       </c>
       <c r="K297" s="7" t="s">
@@ -21632,7 +21644,7 @@
       </c>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J298" s="59" t="str">
+      <c r="J298" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K298)),RIGHT(K298,LEN(K298)-FIND(" ",K298)))</f>
         <v>styphimurium</v>
       </c>
@@ -21648,7 +21660,7 @@
       </c>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J299" s="59" t="str">
+      <c r="J299" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K299)),RIGHT(K299,LEN(K299)-FIND(" ",K299)))</f>
         <v>styphimurium</v>
       </c>
@@ -21664,7 +21676,7 @@
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J300" s="59" t="str">
+      <c r="J300" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K300)),RIGHT(K300,LEN(K300)-FIND(" ",K300)))</f>
         <v>styphimurium</v>
       </c>
@@ -21673,7 +21685,7 @@
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J301" s="59" t="str">
+      <c r="J301" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K301)),RIGHT(K301,LEN(K301)-FIND(" ",K301)))</f>
         <v>styphimurium</v>
       </c>
@@ -21682,7 +21694,7 @@
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J302" s="59" t="str">
+      <c r="J302" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K302)),RIGHT(K302,LEN(K302)-FIND(" ",K302)))</f>
         <v>styphimurium</v>
       </c>
@@ -21691,7 +21703,7 @@
       </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J303" s="59" t="str">
+      <c r="J303" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K303)),RIGHT(K303,LEN(K303)-FIND(" ",K303)))</f>
         <v>styphimurium</v>
       </c>
@@ -21700,7 +21712,7 @@
       </c>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J304" s="60" t="s">
+      <c r="J304" s="61" t="s">
         <v>1175</v>
       </c>
       <c r="K304" s="7" t="s">
@@ -21715,7 +21727,7 @@
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J305" s="60" t="s">
+      <c r="J305" s="61" t="s">
         <v>1176</v>
       </c>
       <c r="K305" s="7" t="s">
@@ -21730,7 +21742,7 @@
       </c>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J306" s="60" t="s">
+      <c r="J306" s="61" t="s">
         <v>1177</v>
       </c>
       <c r="K306" s="7" t="s">
@@ -21745,7 +21757,7 @@
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J307" s="59" t="str">
+      <c r="J307" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K307)),RIGHT(K307,LEN(K307)-FIND(" ",K307)))</f>
         <v>svirus</v>
       </c>
@@ -21754,7 +21766,7 @@
       </c>
     </row>
     <row r="308" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J308" s="59" t="str">
+      <c r="J308" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K308)),RIGHT(K308,LEN(K308)-FIND(" ",K308)))</f>
         <v>svirus</v>
       </c>
@@ -21763,7 +21775,7 @@
       </c>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J309" s="60" t="s">
+      <c r="J309" s="61" t="s">
         <v>1178</v>
       </c>
       <c r="K309" s="7" t="s">
@@ -21778,7 +21790,7 @@
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J310" s="59" t="str">
+      <c r="J310" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K310)),RIGHT(K310,LEN(K310)-FIND(" ",K310)))</f>
         <v>tequinum</v>
       </c>
@@ -21794,7 +21806,7 @@
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J311" s="60" t="s">
+      <c r="J311" s="61" t="s">
         <v>1179</v>
       </c>
       <c r="K311" s="7" t="s">
@@ -21809,7 +21821,7 @@
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J312" s="59" t="str">
+      <c r="J312" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K312)),RIGHT(K312,LEN(K312)-FIND(" ",K312)))</f>
         <v>tmentagrophytes</v>
       </c>
@@ -21825,7 +21837,7 @@
       </c>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J313" s="59" t="str">
+      <c r="J313" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K313)),RIGHT(K313,LEN(K313)-FIND(" ",K313)))</f>
         <v>tpallidum</v>
       </c>
@@ -21841,7 +21853,7 @@
       </c>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J314" s="59" t="str">
+      <c r="J314" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K314)),RIGHT(K314,LEN(K314)-FIND(" ",K314)))</f>
         <v>tmentagrophytes</v>
       </c>
@@ -21850,7 +21862,7 @@
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J315" s="59" t="str">
+      <c r="J315" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K315)),RIGHT(K315,LEN(K315)-FIND(" ",K315)))</f>
         <v>trubrum</v>
       </c>
@@ -21866,7 +21878,7 @@
       </c>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J316" s="59" t="str">
+      <c r="J316" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K316)),RIGHT(K316,LEN(K316)-FIND(" ",K316)))</f>
         <v>tverrucosum</v>
       </c>
@@ -21882,7 +21894,7 @@
       </c>
     </row>
     <row r="317" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J317" s="60" t="s">
+      <c r="J317" s="61" t="s">
         <v>1180</v>
       </c>
       <c r="K317" s="6" t="s">
@@ -21897,7 +21909,7 @@
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J318" s="59" t="str">
+      <c r="J318" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K318)),RIGHT(K318,LEN(K318)-FIND(" ",K318)))</f>
         <v>tverrucosum</v>
       </c>
@@ -21906,7 +21918,7 @@
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J319" s="59" t="str">
+      <c r="J319" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K319)),RIGHT(K319,LEN(K319)-FIND(" ",K319)))</f>
         <v>tverrucosum</v>
       </c>
@@ -21915,7 +21927,7 @@
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J320" s="59" t="str">
+      <c r="J320" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K320)),RIGHT(K320,LEN(K320)-FIND(" ",K320)))</f>
         <v>tverrucosum</v>
       </c>
@@ -21924,7 +21936,7 @@
       </c>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J321" s="59" t="str">
+      <c r="J321" s="60" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K321)),RIGHT(K321,LEN(K321)-FIND(" ",K321)))</f>
         <v>tverrucosum</v>
       </c>
@@ -21933,7 +21945,7 @@
       </c>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J322" s="60" t="s">
+      <c r="J322" s="61" t="s">
         <v>1181</v>
       </c>
       <c r="K322" s="0" t="s">
@@ -21948,7 +21960,7 @@
       </c>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J323" s="60" t="s">
+      <c r="J323" s="61" t="s">
         <v>1182</v>
       </c>
       <c r="K323" s="7" t="s">
@@ -21963,7 +21975,7 @@
       </c>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J324" s="60" t="s">
+      <c r="J324" s="61" t="s">
         <v>1183</v>
       </c>
       <c r="K324" s="0" t="s">
@@ -21978,7 +21990,7 @@
       </c>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J325" s="60" t="s">
+      <c r="J325" s="61" t="s">
         <v>1184</v>
       </c>
       <c r="K325" s="0" t="s">
@@ -21993,7 +22005,7 @@
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J326" s="59"/>
+      <c r="J326" s="60"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -22017,7 +22029,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
@@ -23605,7 +23617,7 @@
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A318" s="48" t="s">
+      <c r="A318" s="49" t="s">
         <v>988</v>
       </c>
     </row>
@@ -23666,7 +23678,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.89"/>
@@ -25032,7 +25044,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.99"/>
@@ -25041,24 +25053,24 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>1189</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="62" t="s">
         <v>1190</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="63" t="s">
         <v>1191</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="49" t="s">
         <v>214</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="49" t="s">
         <v>238</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="49" t="s">
         <v>697</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -25067,112 +25079,112 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>665</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="64" t="s">
         <v>559</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="64" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="65" t="s">
         <v>185</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="64" t="s">
         <v>575</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="49" t="s">
         <v>419</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="49" t="s">
         <v>267</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="49" t="s">
         <v>724</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="64" t="s">
         <v>463</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="49" t="s">
         <v>688</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="49" t="s">
         <v>188</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="49" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="49" t="s">
         <v>422</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="64" t="s">
         <v>590</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="49" t="s">
         <v>182</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="49" t="s">
         <v>442</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="64" t="s">
         <v>598</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="49" t="s">
         <v>345</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="49" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="49" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="49" t="s">
         <v>200</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="49" t="s">
         <v>156</v>
       </c>
-      <c r="C11" s="63" t="s">
+      <c r="C11" s="64" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="49" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>843</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="49" t="s">
         <v>55</v>
       </c>
     </row>
@@ -25180,117 +25192,117 @@
       <c r="A13" s="0" t="s">
         <v>778</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="49" t="s">
         <v>309</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="C13" s="64" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="49" t="s">
         <v>211</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="49" t="s">
         <v>650</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="49" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="49" t="s">
         <v>428</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="49" t="s">
         <v>456</v>
       </c>
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="49" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="49" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="49" t="s">
         <v>450</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="49" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="49" t="s">
         <v>348</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="49" t="s">
         <v>617</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="49" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="49" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="49" t="s">
         <v>453</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="49" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="49" t="s">
         <v>706</v>
       </c>
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="49" t="s">
         <v>620</v>
       </c>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="49" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="48" t="s">
+      <c r="A21" s="49" t="s">
         <v>208</v>
       </c>
-      <c r="B21" s="48" t="s">
+      <c r="B21" s="49" t="s">
         <v>144</v>
       </c>
-      <c r="C21" s="48" t="s">
+      <c r="C21" s="49" t="s">
         <v>684</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="49" t="s">
         <v>431</v>
       </c>
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="C22" s="63" t="s">
+      <c r="C22" s="64" t="s">
         <v>502</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="48" t="s">
+      <c r="A23" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="49" t="s">
         <v>152</v>
       </c>
       <c r="C23" s="0" t="s">
@@ -25298,21 +25310,21 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="49" t="s">
         <v>358</v>
       </c>
-      <c r="B24" s="48" t="s">
+      <c r="B24" s="49" t="s">
         <v>636</v>
       </c>
-      <c r="C24" s="48" t="s">
+      <c r="C24" s="49" t="s">
         <v>692</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="49" t="s">
         <v>633</v>
       </c>
       <c r="C25" s="0" t="s">
@@ -25320,187 +25332,187 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="48" t="s">
+      <c r="A26" s="49" t="s">
         <v>341</v>
       </c>
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="49" t="s">
         <v>639</v>
       </c>
-      <c r="C26" s="63" t="s">
+      <c r="C26" s="64" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="49" t="s">
         <v>217</v>
       </c>
-      <c r="B27" s="48" t="s">
+      <c r="B27" s="49" t="s">
         <v>642</v>
       </c>
-      <c r="C27" s="63" t="s">
+      <c r="C27" s="64" t="s">
         <v>659</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="64" t="s">
+      <c r="A28" s="65" t="s">
         <v>703</v>
       </c>
-      <c r="B28" s="48" t="s">
+      <c r="B28" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="C28" s="48" t="s">
+      <c r="C28" s="49" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="64" t="s">
+      <c r="A29" s="65" t="s">
         <v>416</v>
       </c>
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="C29" s="48" t="s">
+      <c r="C29" s="49" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="48" t="s">
+      <c r="A30" s="49" t="s">
         <v>669</v>
       </c>
-      <c r="B30" s="63" t="s">
+      <c r="B30" s="64" t="s">
         <v>476</v>
       </c>
-      <c r="C30" s="48" t="s">
+      <c r="C30" s="49" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="64" t="s">
+      <c r="A31" s="65" t="s">
         <v>425</v>
       </c>
-      <c r="B31" s="48" t="s">
+      <c r="B31" s="49" t="s">
         <v>257</v>
       </c>
-      <c r="C31" s="48" t="s">
+      <c r="C31" s="49" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="48" t="s">
+      <c r="A32" s="49" t="s">
         <v>608</v>
       </c>
-      <c r="B32" s="48" t="s">
+      <c r="B32" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="48" t="s">
+      <c r="C32" s="49" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="48" t="s">
+      <c r="A33" s="49" t="s">
         <v>204</v>
       </c>
-      <c r="B33" s="63" t="s">
+      <c r="B33" s="64" t="s">
         <v>467</v>
       </c>
-      <c r="C33" s="48" t="s">
+      <c r="C33" s="49" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="48" t="s">
+      <c r="A34" s="49" t="s">
         <v>351</v>
       </c>
-      <c r="B34" s="65" t="s">
+      <c r="B34" s="66" t="s">
         <v>438</v>
       </c>
-      <c r="C34" s="48" t="s">
+      <c r="C34" s="49" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="48" t="s">
+      <c r="A35" s="49" t="s">
         <v>354</v>
       </c>
-      <c r="B35" s="48" t="s">
+      <c r="B35" s="49" t="s">
         <v>312</v>
       </c>
-      <c r="C35" s="48" t="s">
+      <c r="C35" s="49" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="49" t="s">
         <v>763</v>
       </c>
-      <c r="B36" s="65" t="s">
+      <c r="B36" s="66" t="s">
         <v>436</v>
       </c>
-      <c r="C36" s="48" t="s">
+      <c r="C36" s="49" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="48" t="s">
+      <c r="A37" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="64" t="s">
+      <c r="B37" s="65" t="s">
         <v>440</v>
       </c>
-      <c r="C37" s="48" t="s">
+      <c r="C37" s="49" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="48" t="s">
+      <c r="B38" s="49" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="48" t="s">
+      <c r="C38" s="49" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="48" t="s">
+      <c r="B39" s="49" t="s">
         <v>220</v>
       </c>
-      <c r="C39" s="48" t="s">
+      <c r="C39" s="49" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="65" t="s">
+      <c r="B40" s="66" t="s">
         <v>434</v>
       </c>
-      <c r="C40" s="48" t="s">
+      <c r="C40" s="49" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="63" t="s">
+      <c r="B41" s="64" t="s">
         <v>614</v>
       </c>
-      <c r="C41" s="48" t="s">
+      <c r="C41" s="49" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="48" t="s">
+      <c r="B42" s="49" t="s">
         <v>228</v>
       </c>
-      <c r="C42" s="48" t="s">
+      <c r="C42" s="49" t="s">
         <v>728</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="48" t="s">
+      <c r="B43" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="C43" s="48" t="s">
+      <c r="C43" s="49" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="48" t="s">
+      <c r="B44" s="49" t="s">
         <v>677</v>
       </c>
       <c r="C44" s="0" t="s">
@@ -25508,7 +25520,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="48" t="s">
+      <c r="B45" s="49" t="s">
         <v>64</v>
       </c>
       <c r="C45" s="0" t="s">
@@ -25516,7 +25528,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="48" t="s">
+      <c r="B46" s="49" t="s">
         <v>35</v>
       </c>
       <c r="C46" s="0" t="s">
@@ -25532,7 +25544,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="48" t="s">
+      <c r="B48" s="49" t="s">
         <v>117</v>
       </c>
       <c r="C48" s="0" t="s">
@@ -25540,7 +25552,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="48" t="s">
+      <c r="B49" s="49" t="s">
         <v>106</v>
       </c>
       <c r="C49" s="0" t="s">
@@ -25548,7 +25560,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="48" t="s">
+      <c r="B50" s="49" t="s">
         <v>715</v>
       </c>
       <c r="C50" s="0" t="s">
@@ -25564,7 +25576,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="48" t="s">
+      <c r="B52" s="49" t="s">
         <v>140</v>
       </c>
       <c r="C52" s="0" t="s">
@@ -25575,7 +25587,7 @@
       <c r="B53" s="0" t="s">
         <v>869</v>
       </c>
-      <c r="C53" s="48" t="s">
+      <c r="C53" s="49" t="s">
         <v>988</v>
       </c>
     </row>
@@ -25588,15 +25600,15 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="48" t="s">
+      <c r="B55" s="49" t="s">
         <v>373</v>
       </c>
-      <c r="C55" s="48" t="s">
+      <c r="C55" s="49" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="48" t="s">
+      <c r="B56" s="49" t="s">
         <v>242</v>
       </c>
       <c r="C56" s="0" t="s">
@@ -25604,15 +25616,15 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="48" t="s">
+      <c r="B57" s="49" t="s">
         <v>245</v>
       </c>
-      <c r="C57" s="48" t="s">
+      <c r="C57" s="49" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="48" t="s">
+      <c r="B58" s="49" t="s">
         <v>673</v>
       </c>
       <c r="C58" s="0" t="s">
@@ -25620,34 +25632,34 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="48" t="s">
+      <c r="B59" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="C59" s="63" t="s">
+      <c r="C59" s="64" t="s">
         <v>594</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="48" t="s">
+      <c r="B60" s="49" t="s">
         <v>231</v>
       </c>
-      <c r="C60" s="48" t="s">
+      <c r="C60" s="49" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="48" t="s">
+      <c r="B61" s="49" t="s">
         <v>368</v>
       </c>
-      <c r="C61" s="63" t="s">
+      <c r="C61" s="64" t="s">
         <v>572</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="48" t="s">
+      <c r="B62" s="49" t="s">
         <v>376</v>
       </c>
-      <c r="C62" s="63" t="s">
+      <c r="C62" s="64" t="s">
         <v>581</v>
       </c>
     </row>
@@ -25655,15 +25667,15 @@
       <c r="B63" s="0" t="s">
         <v>445</v>
       </c>
-      <c r="C63" s="63" t="s">
+      <c r="C63" s="64" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="48" t="s">
+      <c r="B64" s="49" t="s">
         <v>654</v>
       </c>
-      <c r="C64" s="48" t="s">
+      <c r="C64" s="49" t="s">
         <v>733</v>
       </c>
     </row>
@@ -25671,28 +25683,28 @@
       <c r="B65" s="0" t="s">
         <v>830</v>
       </c>
-      <c r="C65" s="48" t="s">
+      <c r="C65" s="49" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="48" t="s">
+      <c r="B66" s="49" t="s">
         <v>720</v>
       </c>
-      <c r="C66" s="48" t="s">
+      <c r="C66" s="49" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="48" t="s">
+      <c r="B67" s="49" t="s">
         <v>657</v>
       </c>
-      <c r="C67" s="48" t="s">
+      <c r="C67" s="49" t="s">
         <v>741</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="48" t="s">
+      <c r="B68" s="49" t="s">
         <v>718</v>
       </c>
       <c r="C68" s="0" t="s">
@@ -25700,7 +25712,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="48" t="s">
+      <c r="B69" s="49" t="s">
         <v>249</v>
       </c>
       <c r="C69" s="0" t="s">
@@ -25708,10 +25720,10 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="48" t="s">
+      <c r="B70" s="49" t="s">
         <v>235</v>
       </c>
-      <c r="C70" s="48" t="s">
+      <c r="C70" s="49" t="s">
         <v>164</v>
       </c>
     </row>
@@ -25719,7 +25731,7 @@
       <c r="B71" s="0" t="s">
         <v>858</v>
       </c>
-      <c r="C71" s="48" t="s">
+      <c r="C71" s="49" t="s">
         <v>175</v>
       </c>
     </row>
@@ -25727,7 +25739,7 @@
       <c r="B72" s="0" t="s">
         <v>861</v>
       </c>
-      <c r="C72" s="63" t="s">
+      <c r="C72" s="64" t="s">
         <v>535</v>
       </c>
     </row>
@@ -25735,76 +25747,76 @@
       <c r="B73" s="0" t="s">
         <v>855</v>
       </c>
-      <c r="C73" s="63" t="s">
+      <c r="C73" s="64" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="48" t="s">
+      <c r="B74" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="C74" s="63" t="s">
+      <c r="C74" s="64" t="s">
         <v>538</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="48" t="s">
+      <c r="B75" s="49" t="s">
         <v>305</v>
       </c>
-      <c r="C75" s="63" t="s">
+      <c r="C75" s="64" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="63" t="s">
+      <c r="B76" s="64" t="s">
         <v>472</v>
       </c>
-      <c r="C76" s="63" t="s">
+      <c r="C76" s="64" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="48" t="s">
+      <c r="B77" s="49" t="s">
         <v>364</v>
       </c>
-      <c r="C77" s="48" t="s">
+      <c r="C77" s="49" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="48" t="s">
+      <c r="B78" s="49" t="s">
         <v>224</v>
       </c>
-      <c r="C78" s="48" t="s">
+      <c r="C78" s="49" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="48" t="s">
+      <c r="B79" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="C79" s="48" t="s">
+      <c r="C79" s="49" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="48" t="s">
+      <c r="B80" s="49" t="s">
         <v>260</v>
       </c>
-      <c r="C80" s="64" t="s">
+      <c r="C80" s="65" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="48" t="s">
+      <c r="B81" s="49" t="s">
         <v>379</v>
       </c>
-      <c r="C81" s="48" t="s">
+      <c r="C81" s="49" t="s">
         <v>680</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="48" t="s">
+      <c r="B82" s="49" t="s">
         <v>263</v>
       </c>
       <c r="C82" s="0" t="s">
@@ -25815,15 +25827,15 @@
       <c r="B83" s="0" t="s">
         <v>793</v>
       </c>
-      <c r="C83" s="48" t="s">
+      <c r="C83" s="49" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="48" t="s">
+      <c r="B84" s="49" t="s">
         <v>459</v>
       </c>
-      <c r="C84" s="48" t="s">
+      <c r="C84" s="49" t="s">
         <v>168</v>
       </c>
     </row>
@@ -25831,27 +25843,27 @@
       <c r="B85" s="0" t="s">
         <v>865</v>
       </c>
-      <c r="C85" s="48" t="s">
+      <c r="C85" s="49" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C86" s="48" t="s">
+      <c r="C86" s="49" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C87" s="48" t="s">
+      <c r="C87" s="49" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C88" s="48" t="s">
+      <c r="C88" s="49" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C89" s="48" t="s">
+      <c r="C89" s="49" t="s">
         <v>757</v>
       </c>
     </row>
@@ -25861,12 +25873,12 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="63" t="s">
+      <c r="C91" s="64" t="s">
         <v>626</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C92" s="48" t="s">
+      <c r="C92" s="49" t="s">
         <v>386</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working with pesky excel files and ones with semicolons
</commit_message>
<xml_diff>
--- a/info/apinet_survey (2).xlsx
+++ b/info/apinet_survey (2).xlsx
@@ -3747,12 +3747,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC99C00"/>
         <bgColor rgb="FFFFC000"/>
       </patternFill>
@@ -3777,6 +3771,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF7F7F7F"/>
         <bgColor rgb="FF969696"/>
       </patternFill>
@@ -3789,14 +3789,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4B01A6"/>
-        <bgColor rgb="FF800080"/>
+        <fgColor rgb="FFF5BBFE"/>
+        <bgColor rgb="FFF8CFCE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF5BBFE"/>
-        <bgColor rgb="FFF8CFCE"/>
+        <fgColor rgb="FF4B01A6"/>
+        <bgColor rgb="FF800080"/>
       </patternFill>
     </fill>
     <fill>
@@ -3856,7 +3856,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="66">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3917,7 +3917,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3925,31 +3925,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3957,11 +3957,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3977,7 +3977,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4009,11 +4009,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4021,7 +4021,23 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4029,27 +4045,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="14" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4065,11 +4061,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4077,11 +4073,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4093,7 +4089,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4117,7 +4113,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4209,11 +4205,11 @@
   </sheetPr>
   <dimension ref="A1:AK339"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L303" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q323" activeCellId="0" sqref="Q323"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T184" activeCellId="0" sqref="T184"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.12"/>
@@ -4222,12 +4218,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="58"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="11" min="9" style="0" width="58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="19.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="25"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="26" min="26" style="3" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="31" min="31" style="4" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="3" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="4" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14888,7 +14884,7 @@
       <c r="L289" s="10" t="s">
         <v>780</v>
       </c>
-      <c r="M289" s="26" t="s">
+      <c r="M289" s="15" t="s">
         <v>781</v>
       </c>
       <c r="N289" s="7"/>
@@ -16022,7 +16018,7 @@
       <c r="M314" s="47" t="s">
         <v>936</v>
       </c>
-      <c r="N314" s="48" t="s">
+      <c r="N314" s="47" t="s">
         <v>937</v>
       </c>
       <c r="O314" s="13" t="s">
@@ -16202,10 +16198,10 @@
       <c r="L316" s="44" t="s">
         <v>964</v>
       </c>
-      <c r="M316" s="48" t="s">
+      <c r="M316" s="47" t="s">
         <v>965</v>
       </c>
-      <c r="N316" s="26" t="s">
+      <c r="N316" s="15" t="s">
         <v>966</v>
       </c>
       <c r="O316" s="13" t="s">
@@ -16354,10 +16350,10 @@
       <c r="F319" s="0" t="s">
         <v>511</v>
       </c>
-      <c r="G319" s="49" t="s">
+      <c r="G319" s="48" t="s">
         <v>987</v>
       </c>
-      <c r="H319" s="49" t="s">
+      <c r="H319" s="48" t="s">
         <v>988</v>
       </c>
       <c r="I319" s="0" t="str">
@@ -16495,7 +16491,7 @@
       <c r="L322" s="10" t="s">
         <v>812</v>
       </c>
-      <c r="M322" s="26" t="s">
+      <c r="M322" s="15" t="s">
         <v>1006</v>
       </c>
       <c r="N322" s="7"/>
@@ -16605,7 +16601,7 @@
       <c r="L325" s="11" t="s">
         <v>1018</v>
       </c>
-      <c r="M325" s="50" t="s">
+      <c r="M325" s="49" t="s">
         <v>1019</v>
       </c>
       <c r="N325" s="15" t="s">
@@ -16696,7 +16692,7 @@
       <c r="L326" s="11" t="s">
         <v>1018</v>
       </c>
-      <c r="M326" s="26" t="s">
+      <c r="M326" s="15" t="s">
         <v>1042</v>
       </c>
       <c r="N326" s="46" t="s">
@@ -16741,16 +16737,16 @@
       <c r="AE326" s="45"/>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B327" s="51"/>
+      <c r="B327" s="50"/>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B328" s="51"/>
+      <c r="B328" s="50"/>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B329" s="51"/>
+      <c r="B329" s="50"/>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B330" s="51"/>
+      <c r="B330" s="50"/>
       <c r="D330" s="1"/>
       <c r="E330" s="0" t="s">
         <v>1056</v>
@@ -16761,13 +16757,13 @@
       <c r="E331" s="0" t="s">
         <v>1057</v>
       </c>
-      <c r="L331" s="52"/>
+      <c r="L331" s="51"/>
       <c r="M331" s="0" t="s">
         <v>1058</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D332" s="53"/>
+      <c r="D332" s="52"/>
       <c r="E332" s="0" t="s">
         <v>1059</v>
       </c>
@@ -16777,7 +16773,7 @@
       </c>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D333" s="54"/>
+      <c r="D333" s="53"/>
       <c r="E333" s="0" t="s">
         <v>1061</v>
       </c>
@@ -16787,31 +16783,31 @@
       </c>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L335" s="55"/>
+      <c r="L335" s="54"/>
       <c r="M335" s="0" t="s">
         <v>1063</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L336" s="56"/>
+      <c r="L336" s="55"/>
       <c r="M336" s="0" t="s">
         <v>1064</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L337" s="57"/>
+      <c r="L337" s="56"/>
       <c r="M337" s="0" t="s">
         <v>1065</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L338" s="58"/>
+      <c r="L338" s="57"/>
       <c r="M338" s="0" t="s">
         <v>1066</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L339" s="59"/>
+      <c r="L339" s="58"/>
       <c r="M339" s="0" t="s">
         <v>1067</v>
       </c>
@@ -17463,7 +17459,7 @@
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.11"/>
@@ -17491,7 +17487,7 @@
       <c r="F1" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="J1" s="60" t="str">
+      <c r="J1" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K1)),RIGHT(K1,LEN(K1)-FIND(" ",K1)))</f>
         <v>aalternata</v>
       </c>
@@ -17525,7 +17521,7 @@
       <c r="F2" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="J2" s="60" t="str">
+      <c r="J2" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K2)),RIGHT(K2,LEN(K2)-FIND(" ",K2)))</f>
         <v>aalternata</v>
       </c>
@@ -17552,7 +17548,7 @@
       <c r="F3" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="J3" s="60" t="str">
+      <c r="J3" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K3)),RIGHT(K3,LEN(K3)-FIND(" ",K3)))</f>
         <v>aalternata</v>
       </c>
@@ -17579,7 +17575,7 @@
       <c r="F4" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="J4" s="60" t="str">
+      <c r="J4" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K4)),RIGHT(K4,LEN(K4)-FIND(" ",K4)))</f>
         <v>aapis</v>
       </c>
@@ -17613,7 +17609,7 @@
       <c r="F5" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="J5" s="61" t="s">
+      <c r="J5" s="60" t="s">
         <v>1068</v>
       </c>
       <c r="K5" s="7" t="s">
@@ -17646,7 +17642,7 @@
       <c r="F6" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="J6" s="60" t="str">
+      <c r="J6" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K6)),RIGHT(K6,LEN(K6)-FIND(" ",K6)))</f>
         <v>acoronavirus</v>
       </c>
@@ -17680,7 +17676,7 @@
       <c r="F7" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="J7" s="60" t="str">
+      <c r="J7" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K7)),RIGHT(K7,LEN(K7)-FIND(" ",K7)))</f>
         <v>aflavus</v>
       </c>
@@ -17714,7 +17710,7 @@
       <c r="F8" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="J8" s="60" t="str">
+      <c r="J8" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K8)),RIGHT(K8,LEN(K8)-FIND(" ",K8)))</f>
         <v>afumigatus</v>
       </c>
@@ -17748,7 +17744,7 @@
       <c r="F9" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="J9" s="60" t="str">
+      <c r="J9" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K9)),RIGHT(K9,LEN(K9)-FIND(" ",K9)))</f>
         <v>aflavus</v>
       </c>
@@ -17775,7 +17771,7 @@
       <c r="F10" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="J10" s="61" t="s">
+      <c r="J10" s="60" t="s">
         <v>1069</v>
       </c>
       <c r="K10" s="6" t="s">
@@ -17808,7 +17804,7 @@
       <c r="F11" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="J11" s="60" t="str">
+      <c r="J11" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K11)),RIGHT(K11,LEN(K11)-FIND(" ",K11)))</f>
         <v>afumigatus</v>
       </c>
@@ -17835,7 +17831,7 @@
       <c r="F12" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="J12" s="60" t="str">
+      <c r="J12" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K12)),RIGHT(K12,LEN(K12)-FIND(" ",K12)))</f>
         <v>afumigatus</v>
       </c>
@@ -17856,7 +17852,7 @@
         <f aca="false">SUM(F1:F12)</f>
         <v>106</v>
       </c>
-      <c r="J13" s="60" t="str">
+      <c r="J13" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K13)),RIGHT(K13,LEN(K13)-FIND(" ",K13)))</f>
         <v>afumigatus</v>
       </c>
@@ -17865,7 +17861,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J14" s="60" t="str">
+      <c r="J14" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K14)),RIGHT(K14,LEN(K14)-FIND(" ",K14)))</f>
         <v>afumigatus</v>
       </c>
@@ -17874,7 +17870,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J15" s="60" t="str">
+      <c r="J15" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K15)),RIGHT(K15,LEN(K15)-FIND(" ",K15)))</f>
         <v>afumigatus</v>
       </c>
@@ -17883,7 +17879,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J16" s="60" t="str">
+      <c r="J16" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K16)),RIGHT(K16,LEN(K16)-FIND(" ",K16)))</f>
         <v>afumigatus</v>
       </c>
@@ -17892,7 +17888,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J17" s="60" t="str">
+      <c r="J17" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K17)),RIGHT(K17,LEN(K17)-FIND(" ",K17)))</f>
         <v>amarginale</v>
       </c>
@@ -17908,7 +17904,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J18" s="60" t="str">
+      <c r="J18" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K18)),RIGHT(K18,LEN(K18)-FIND(" ",K18)))</f>
         <v>aniger</v>
       </c>
@@ -17924,7 +17920,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J19" s="60" t="str">
+      <c r="J19" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K19)),RIGHT(K19,LEN(K19)-FIND(" ",K19)))</f>
         <v>aparasiticus</v>
       </c>
@@ -17940,7 +17936,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J20" s="61" t="s">
+      <c r="J20" s="60" t="s">
         <v>1070</v>
       </c>
       <c r="K20" s="6" t="s">
@@ -17955,7 +17951,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J21" s="60" t="str">
+      <c r="J21" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K21)),RIGHT(K21,LEN(K21)-FIND(" ",K21)))</f>
         <v>aterreus</v>
       </c>
@@ -17971,7 +17967,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J22" s="60" t="str">
+      <c r="J22" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K22)),RIGHT(K22,LEN(K22)-FIND(" ",K22)))</f>
         <v>aviscosus</v>
       </c>
@@ -17987,7 +17983,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J23" s="60" t="str">
+      <c r="J23" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K23)),RIGHT(K23,LEN(K23)-FIND(" ",K23)))</f>
         <v>babortus</v>
       </c>
@@ -18003,7 +17999,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J24" s="61" t="s">
+      <c r="J24" s="60" t="s">
         <v>1071</v>
       </c>
       <c r="K24" s="6" t="s">
@@ -18018,7 +18014,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J25" s="60" t="str">
+      <c r="J25" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K25)),RIGHT(K25,LEN(K25)-FIND(" ",K25)))</f>
         <v>babortus</v>
       </c>
@@ -18027,7 +18023,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J26" s="60" t="str">
+      <c r="J26" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K26)),RIGHT(K26,LEN(K26)-FIND(" ",K26)))</f>
         <v>babortus</v>
       </c>
@@ -18036,7 +18032,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J27" s="60" t="str">
+      <c r="J27" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K27)),RIGHT(K27,LEN(K27)-FIND(" ",K27)))</f>
         <v>banthracis</v>
       </c>
@@ -18052,7 +18048,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J28" s="60" t="str">
+      <c r="J28" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K28)),RIGHT(K28,LEN(K28)-FIND(" ",K28)))</f>
         <v>balphaherpesvirus 1</v>
       </c>
@@ -18061,7 +18057,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J29" s="60" t="str">
+      <c r="J29" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K29)),RIGHT(K29,LEN(K29)-FIND(" ",K29)))</f>
         <v>bbronchiseptica</v>
       </c>
@@ -18077,7 +18073,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J30" s="60" t="str">
+      <c r="J30" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K30)),RIGHT(K30,LEN(K30)-FIND(" ",K30)))</f>
         <v>banthracis</v>
       </c>
@@ -18086,7 +18082,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J31" s="60" t="str">
+      <c r="J31" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K31)),RIGHT(K31,LEN(K31)-FIND(" ",K31)))</f>
         <v>banthracis</v>
       </c>
@@ -18095,7 +18091,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J32" s="60" t="str">
+      <c r="J32" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K32)),RIGHT(K32,LEN(K32)-FIND(" ",K32)))</f>
         <v>bdermatitidis</v>
       </c>
@@ -18111,7 +18107,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J33" s="60" t="str">
+      <c r="J33" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K33)),RIGHT(K33,LEN(K33)-FIND(" ",K33)))</f>
         <v>bbronchiseptica</v>
       </c>
@@ -18120,7 +18116,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J34" s="60" t="str">
+      <c r="J34" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K34)),RIGHT(K34,LEN(K34)-FIND(" ",K34)))</f>
         <v>bbronchiseptica</v>
       </c>
@@ -18129,7 +18125,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J35" s="61" t="s">
+      <c r="J35" s="60" t="s">
         <v>1072</v>
       </c>
       <c r="K35" s="6" t="s">
@@ -18144,7 +18140,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J36" s="60" t="str">
+      <c r="J36" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K36)),RIGHT(K36,LEN(K36)-FIND(" ",K36)))</f>
         <v>bdermatitidis</v>
       </c>
@@ -18153,7 +18149,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J37" s="60" t="str">
+      <c r="J37" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K37)),RIGHT(K37,LEN(K37)-FIND(" ",K37)))</f>
         <v>bdermatitidis</v>
       </c>
@@ -18162,7 +18158,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J38" s="60" t="str">
+      <c r="J38" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K38)),RIGHT(K38,LEN(K38)-FIND(" ",K38)))</f>
         <v>bhyodysenteriae</v>
       </c>
@@ -18178,7 +18174,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J39" s="61" t="s">
+      <c r="J39" s="60" t="s">
         <v>1073</v>
       </c>
       <c r="K39" s="7" t="s">
@@ -18193,7 +18189,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J40" s="60" t="str">
+      <c r="J40" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K40)),RIGHT(K40,LEN(K40)-FIND(" ",K40)))</f>
         <v>bmelitensis</v>
       </c>
@@ -18209,7 +18205,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J41" s="61" t="s">
+      <c r="J41" s="60" t="s">
         <v>1074</v>
       </c>
       <c r="K41" s="6" t="s">
@@ -18224,7 +18220,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J42" s="60" t="str">
+      <c r="J42" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K42)),RIGHT(K42,LEN(K42)-FIND(" ",K42)))</f>
         <v>bmelitensis</v>
       </c>
@@ -18233,7 +18229,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J43" s="61" t="s">
+      <c r="J43" s="60" t="s">
         <v>1075</v>
       </c>
       <c r="K43" s="7" t="s">
@@ -18248,7 +18244,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J44" s="60" t="str">
+      <c r="J44" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K44)),RIGHT(K44,LEN(K44)-FIND(" ",K44)))</f>
         <v>branarum</v>
       </c>
@@ -18264,7 +18260,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J45" s="60" t="str">
+      <c r="J45" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K45)),RIGHT(K45,LEN(K45)-FIND(" ",K45)))</f>
         <v>bsuis</v>
       </c>
@@ -18280,7 +18276,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J46" s="61" t="s">
+      <c r="J46" s="60" t="s">
         <v>1076</v>
       </c>
       <c r="K46" s="7" t="s">
@@ -18295,7 +18291,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J47" s="61" t="s">
+      <c r="J47" s="60" t="s">
         <v>1077</v>
       </c>
       <c r="K47" s="6" t="s">
@@ -18310,7 +18306,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J48" s="60" t="str">
+      <c r="J48" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K48)),RIGHT(K48,LEN(K48)-FIND(" ",K48)))</f>
         <v>bviral diarrhea virus 1</v>
       </c>
@@ -18319,7 +18315,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J49" s="60" t="str">
+      <c r="J49" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K49)),RIGHT(K49,LEN(K49)-FIND(" ",K49)))</f>
         <v>bviral diarrhea virus 1</v>
       </c>
@@ -18328,7 +18324,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J50" s="60" t="str">
+      <c r="J50" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K50)),RIGHT(K50,LEN(K50)-FIND(" ",K50)))</f>
         <v>bvirus</v>
       </c>
@@ -18344,7 +18340,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J51" s="60" t="str">
+      <c r="J51" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K51)),RIGHT(K51,LEN(K51)-FIND(" ",K51)))</f>
         <v>bviral diarrhea virus 2</v>
       </c>
@@ -18353,7 +18349,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J52" s="60" t="str">
+      <c r="J52" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K52)),RIGHT(K52,LEN(K52)-FIND(" ",K52)))</f>
         <v>cabortus</v>
       </c>
@@ -18369,7 +18365,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J53" s="60" t="str">
+      <c r="J53" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K53)),RIGHT(K53,LEN(K53)-FIND(" ",K53)))</f>
         <v>bvirus</v>
       </c>
@@ -18378,7 +18374,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J54" s="61" t="s">
+      <c r="J54" s="60" t="s">
         <v>1078</v>
       </c>
       <c r="K54" s="7" t="s">
@@ -18393,7 +18389,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J55" s="60" t="str">
+      <c r="J55" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K55)),RIGHT(K55,LEN(K55)-FIND(" ",K55)))</f>
         <v>cabortus</v>
       </c>
@@ -18402,7 +18398,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J56" s="61" t="s">
+      <c r="J56" s="60" t="s">
         <v>1079</v>
       </c>
       <c r="K56" s="7" t="s">
@@ -18417,7 +18413,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J57" s="60" t="str">
+      <c r="J57" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K57)),RIGHT(K57,LEN(K57)-FIND(" ",K57)))</f>
         <v>calbicans</v>
       </c>
@@ -18433,7 +18429,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J58" s="60" t="str">
+      <c r="J58" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K58)),RIGHT(K58,LEN(K58)-FIND(" ",K58)))</f>
         <v>candersoni</v>
       </c>
@@ -18449,7 +18445,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J59" s="60" t="str">
+      <c r="J59" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K59)),RIGHT(K59,LEN(K59)-FIND(" ",K59)))</f>
         <v>calbicans</v>
       </c>
@@ -18458,7 +18454,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J60" s="60" t="str">
+      <c r="J60" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K60)),RIGHT(K60,LEN(K60)-FIND(" ",K60)))</f>
         <v>calbicans</v>
       </c>
@@ -18467,7 +18463,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J61" s="60" t="str">
+      <c r="J61" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K61)),RIGHT(K61,LEN(K61)-FIND(" ",K61)))</f>
         <v>calbicans</v>
       </c>
@@ -18476,7 +18472,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J62" s="60" t="str">
+      <c r="J62" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K62)),RIGHT(K62,LEN(K62)-FIND(" ",K62)))</f>
         <v>calbicans</v>
       </c>
@@ -18485,7 +18481,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J63" s="60" t="str">
+      <c r="J63" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K63)),RIGHT(K63,LEN(K63)-FIND(" ",K63)))</f>
         <v>calbicans</v>
       </c>
@@ -18494,7 +18490,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J64" s="60" t="str">
+      <c r="J64" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K64)),RIGHT(K64,LEN(K64)-FIND(" ",K64)))</f>
         <v>calbicans</v>
       </c>
@@ -18503,7 +18499,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J65" s="60" t="str">
+      <c r="J65" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K65)),RIGHT(K65,LEN(K65)-FIND(" ",K65)))</f>
         <v>calbicans</v>
       </c>
@@ -18512,7 +18508,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J66" s="61" t="s">
+      <c r="J66" s="60" t="s">
         <v>1080</v>
       </c>
       <c r="K66" s="7" t="s">
@@ -18527,7 +18523,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J67" s="60" t="str">
+      <c r="J67" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K67)),RIGHT(K67,LEN(K67)-FIND(" ",K67)))</f>
         <v>cauris</v>
       </c>
@@ -18543,7 +18539,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J68" s="60" t="str">
+      <c r="J68" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K68)),RIGHT(K68,LEN(K68)-FIND(" ",K68)))</f>
         <v>cbantiana</v>
       </c>
@@ -18559,7 +18555,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J69" s="61" t="s">
+      <c r="J69" s="60" t="s">
         <v>1081</v>
       </c>
       <c r="K69" s="7" t="s">
@@ -18574,7 +18570,7 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J70" s="60" t="str">
+      <c r="J70" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K70)),RIGHT(K70,LEN(K70)-FIND(" ",K70)))</f>
         <v>cbantiana</v>
       </c>
@@ -18583,7 +18579,7 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J71" s="60" t="str">
+      <c r="J71" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K71)),RIGHT(K71,LEN(K71)-FIND(" ",K71)))</f>
         <v>cbantiana</v>
       </c>
@@ -18592,7 +18588,7 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J72" s="60" t="str">
+      <c r="J72" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K72)),RIGHT(K72,LEN(K72)-FIND(" ",K72)))</f>
         <v>cbovis</v>
       </c>
@@ -18608,7 +18604,7 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J73" s="60" t="str">
+      <c r="J73" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K73)),RIGHT(K73,LEN(K73)-FIND(" ",K73)))</f>
         <v>cburnetii</v>
       </c>
@@ -18624,7 +18620,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J74" s="60" t="str">
+      <c r="J74" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K74)),RIGHT(K74,LEN(K74)-FIND(" ",K74)))</f>
         <v>ccoronatus</v>
       </c>
@@ -18640,7 +18636,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J75" s="60" t="str">
+      <c r="J75" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K75)),RIGHT(K75,LEN(K75)-FIND(" ",K75)))</f>
         <v>cburnetii</v>
       </c>
@@ -18649,7 +18645,7 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J76" s="60" t="str">
+      <c r="J76" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K76)),RIGHT(K76,LEN(K76)-FIND(" ",K76)))</f>
         <v>ccoronavirus</v>
       </c>
@@ -18665,7 +18661,7 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J77" s="60" t="str">
+      <c r="J77" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K77)),RIGHT(K77,LEN(K77)-FIND(" ",K77)))</f>
         <v>cdifficile</v>
       </c>
@@ -18681,7 +18677,7 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J78" s="60" t="str">
+      <c r="J78" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K78)),RIGHT(K78,LEN(K78)-FIND(" ",K78)))</f>
         <v>cfelis</v>
       </c>
@@ -18697,7 +18693,7 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J79" s="60" t="str">
+      <c r="J79" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K79)),RIGHT(K79,LEN(K79)-FIND(" ",K79)))</f>
         <v>cgattii</v>
       </c>
@@ -18713,7 +18709,7 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J80" s="61" t="s">
+      <c r="J80" s="60" t="s">
         <v>1082</v>
       </c>
       <c r="K80" s="7" t="s">
@@ -18728,7 +18724,7 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J81" s="60" t="str">
+      <c r="J81" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K81)),RIGHT(K81,LEN(K81)-FIND(" ",K81)))</f>
         <v>cgattii</v>
       </c>
@@ -18737,7 +18733,7 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J82" s="60" t="str">
+      <c r="J82" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K82)),RIGHT(K82,LEN(K82)-FIND(" ",K82)))</f>
         <v>cgattii</v>
       </c>
@@ -18746,7 +18742,7 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J83" s="60" t="str">
+      <c r="J83" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K83)),RIGHT(K83,LEN(K83)-FIND(" ",K83)))</f>
         <v>cgattii</v>
       </c>
@@ -18755,7 +18751,7 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J84" s="60" t="str">
+      <c r="J84" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K84)),RIGHT(K84,LEN(K84)-FIND(" ",K84)))</f>
         <v>cgattii</v>
       </c>
@@ -18764,7 +18760,7 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J85" s="60" t="str">
+      <c r="J85" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K85)),RIGHT(K85,LEN(K85)-FIND(" ",K85)))</f>
         <v>cimmitis</v>
       </c>
@@ -18780,7 +18776,7 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J86" s="60" t="str">
+      <c r="J86" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K86)),RIGHT(K86,LEN(K86)-FIND(" ",K86)))</f>
         <v>cjejuni</v>
       </c>
@@ -18796,7 +18792,7 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J87" s="60" t="str">
+      <c r="J87" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K87)),RIGHT(K87,LEN(K87)-FIND(" ",K87)))</f>
         <v>cimmitis</v>
       </c>
@@ -18805,7 +18801,7 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J88" s="60" t="str">
+      <c r="J88" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K88)),RIGHT(K88,LEN(K88)-FIND(" ",K88)))</f>
         <v>cneoformans</v>
       </c>
@@ -18821,7 +18817,7 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J89" s="60" t="str">
+      <c r="J89" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K89)),RIGHT(K89,LEN(K89)-FIND(" ",K89)))</f>
         <v>cjejuni</v>
       </c>
@@ -18830,7 +18826,7 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J90" s="61" t="s">
+      <c r="J90" s="60" t="s">
         <v>1084</v>
       </c>
       <c r="K90" s="7" t="s">
@@ -18845,7 +18841,7 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J91" s="60" t="str">
+      <c r="J91" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K91)),RIGHT(K91,LEN(K91)-FIND(" ",K91)))</f>
         <v>cneoformans</v>
       </c>
@@ -18854,7 +18850,7 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J92" s="60" t="str">
+      <c r="J92" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K92)),RIGHT(K92,LEN(K92)-FIND(" ",K92)))</f>
         <v>cneoformans</v>
       </c>
@@ -18863,7 +18859,7 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J93" s="60" t="str">
+      <c r="J93" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K93)),RIGHT(K93,LEN(K93)-FIND(" ",K93)))</f>
         <v>cneoformans</v>
       </c>
@@ -18872,7 +18868,7 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J94" s="60" t="str">
+      <c r="J94" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K94)),RIGHT(K94,LEN(K94)-FIND(" ",K94)))</f>
         <v>cparvovirus</v>
       </c>
@@ -18888,7 +18884,7 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J95" s="60" t="str">
+      <c r="J95" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K95)),RIGHT(K95,LEN(K95)-FIND(" ",K95)))</f>
         <v>cparvum</v>
       </c>
@@ -18904,7 +18900,7 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J96" s="61" t="s">
+      <c r="J96" s="60" t="s">
         <v>1085</v>
       </c>
       <c r="K96" s="7" t="s">
@@ -18919,7 +18915,7 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J97" s="61" t="s">
+      <c r="J97" s="60" t="s">
         <v>1086</v>
       </c>
       <c r="K97" s="7" t="s">
@@ -18934,7 +18930,7 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J98" s="61" t="s">
+      <c r="J98" s="60" t="s">
         <v>1087</v>
       </c>
       <c r="K98" s="7" t="s">
@@ -18949,7 +18945,7 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J99" s="61" t="s">
+      <c r="J99" s="60" t="s">
         <v>1088</v>
       </c>
       <c r="K99" s="7" t="s">
@@ -18964,7 +18960,7 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J100" s="61" t="s">
+      <c r="J100" s="60" t="s">
         <v>1089</v>
       </c>
       <c r="K100" s="7" t="s">
@@ -18979,7 +18975,7 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J101" s="60" t="str">
+      <c r="J101" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K101)),RIGHT(K101,LEN(K101)-FIND(" ",K101)))</f>
         <v>cperfringens C</v>
       </c>
@@ -18988,7 +18984,7 @@
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J102" s="60" t="str">
+      <c r="J102" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K102)),RIGHT(K102,LEN(K102)-FIND(" ",K102)))</f>
         <v>cpseudotuberculosis</v>
       </c>
@@ -19004,7 +19000,7 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J103" s="60" t="str">
+      <c r="J103" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K103)),RIGHT(K103,LEN(K103)-FIND(" ",K103)))</f>
         <v>cpsittaci</v>
       </c>
@@ -19020,7 +19016,7 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J104" s="60" t="str">
+      <c r="J104" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K104)),RIGHT(K104,LEN(K104)-FIND(" ",K104)))</f>
         <v>cpseudotuberculosis</v>
       </c>
@@ -19029,7 +19025,7 @@
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J105" s="60" t="str">
+      <c r="J105" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K105)),RIGHT(K105,LEN(K105)-FIND(" ",K105)))</f>
         <v>cpurpurea</v>
       </c>
@@ -19045,7 +19041,7 @@
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J106" s="60" t="str">
+      <c r="J106" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K106)),RIGHT(K106,LEN(K106)-FIND(" ",K106)))</f>
         <v>cryanae</v>
       </c>
@@ -19061,7 +19057,7 @@
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J107" s="61" t="s">
+      <c r="J107" s="60" t="s">
         <v>1090</v>
       </c>
       <c r="K107" s="6" t="s">
@@ -19076,7 +19072,7 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J108" s="60" t="str">
+      <c r="J108" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K108)),RIGHT(K108,LEN(K108)-FIND(" ",K108)))</f>
         <v>ctetani</v>
       </c>
@@ -19092,7 +19088,7 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J109" s="60" t="str">
+      <c r="J109" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K109)),RIGHT(K109,LEN(K109)-FIND(" ",K109)))</f>
         <v>ctrachomatis</v>
       </c>
@@ -19108,7 +19104,7 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J110" s="60" t="str">
+      <c r="J110" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K110)),RIGHT(K110,LEN(K110)-FIND(" ",K110)))</f>
         <v>ctetani</v>
       </c>
@@ -19117,7 +19113,7 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J111" s="60" t="str">
+      <c r="J111" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K111)),RIGHT(K111,LEN(K111)-FIND(" ",K111)))</f>
         <v>ctetani</v>
       </c>
@@ -19126,7 +19122,7 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J112" s="60" t="str">
+      <c r="J112" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K112)),RIGHT(K112,LEN(K112)-FIND(" ",K112)))</f>
         <v>ctetani</v>
       </c>
@@ -19135,7 +19131,7 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J113" s="61" t="s">
+      <c r="J113" s="60" t="s">
         <v>1091</v>
       </c>
       <c r="K113" s="7" t="s">
@@ -19150,7 +19146,7 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J114" s="60" t="str">
+      <c r="J114" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K114)),RIGHT(K114,LEN(K114)-FIND(" ",K114)))</f>
         <v>dcongolensis</v>
       </c>
@@ -19166,7 +19162,7 @@
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J115" s="60" t="str">
+      <c r="J115" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K115)),RIGHT(K115,LEN(K115)-FIND(" ",K115)))</f>
         <v>dnodosus</v>
       </c>
@@ -19182,7 +19178,7 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J116" s="61" t="s">
+      <c r="J116" s="60" t="s">
         <v>1095</v>
       </c>
       <c r="K116" s="7" t="s">
@@ -19197,7 +19193,7 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J117" s="60" t="str">
+      <c r="J117" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K117)),RIGHT(K117,LEN(K117)-FIND(" ",K117)))</f>
         <v>dnodosus</v>
       </c>
@@ -19206,7 +19202,7 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J118" s="61" t="s">
+      <c r="J118" s="60" t="s">
         <v>1096</v>
       </c>
       <c r="K118" s="7" t="s">
@@ -19221,7 +19217,7 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J119" s="61" t="s">
+      <c r="J119" s="60" t="s">
         <v>1097</v>
       </c>
       <c r="K119" s="7" t="s">
@@ -19236,7 +19232,7 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J120" s="61" t="s">
+      <c r="J120" s="60" t="s">
         <v>1098</v>
       </c>
       <c r="K120" s="7" t="s">
@@ -19251,7 +19247,7 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J121" s="60" t="str">
+      <c r="J121" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K121)),RIGHT(K121,LEN(K121)-FIND(" ",K121)))</f>
         <v>ecoli</v>
       </c>
@@ -19267,7 +19263,7 @@
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J122" s="61" t="s">
+      <c r="J122" s="60" t="s">
         <v>1099</v>
       </c>
       <c r="K122" s="0" t="s">
@@ -19282,7 +19278,7 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J123" s="60" t="str">
+      <c r="J123" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K123)),RIGHT(K123,LEN(K123)-FIND(" ",K123)))</f>
         <v>ecoli</v>
       </c>
@@ -19291,7 +19287,7 @@
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J124" s="60" t="str">
+      <c r="J124" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K124)),RIGHT(K124,LEN(K124)-FIND(" ",K124)))</f>
         <v>ecoli</v>
       </c>
@@ -19300,7 +19296,7 @@
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J125" s="60" t="str">
+      <c r="J125" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K125)),RIGHT(K125,LEN(K125)-FIND(" ",K125)))</f>
         <v>ecoli</v>
       </c>
@@ -19309,7 +19305,7 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J126" s="60" t="str">
+      <c r="J126" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K126)),RIGHT(K126,LEN(K126)-FIND(" ",K126)))</f>
         <v>ecoli</v>
       </c>
@@ -19318,7 +19314,7 @@
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J127" s="60" t="str">
+      <c r="J127" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K127)),RIGHT(K127,LEN(K127)-FIND(" ",K127)))</f>
         <v>ecoli</v>
       </c>
@@ -19327,7 +19323,7 @@
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J128" s="60" t="str">
+      <c r="J128" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K128)),RIGHT(K128,LEN(K128)-FIND(" ",K128)))</f>
         <v>ecoli</v>
       </c>
@@ -19336,7 +19332,7 @@
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J129" s="60" t="str">
+      <c r="J129" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K129)),RIGHT(K129,LEN(K129)-FIND(" ",K129)))</f>
         <v>edermatitidis</v>
       </c>
@@ -19352,7 +19348,7 @@
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J130" s="61" t="s">
+      <c r="J130" s="60" t="s">
         <v>1100</v>
       </c>
       <c r="K130" s="7" t="s">
@@ -19367,7 +19363,7 @@
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J131" s="60" t="str">
+      <c r="J131" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K131)),RIGHT(K131,LEN(K131)-FIND(" ",K131)))</f>
         <v>edermatitidis</v>
       </c>
@@ -19376,7 +19372,7 @@
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J132" s="60" t="str">
+      <c r="J132" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K132)),RIGHT(K132,LEN(K132)-FIND(" ",K132)))</f>
         <v>edermatitidis</v>
       </c>
@@ -19385,7 +19381,7 @@
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J133" s="61" t="s">
+      <c r="J133" s="60" t="s">
         <v>1101</v>
       </c>
       <c r="K133" s="6" t="s">
@@ -19400,7 +19396,7 @@
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J134" s="61" t="s">
+      <c r="J134" s="60" t="s">
         <v>1102</v>
       </c>
       <c r="K134" s="6" t="s">
@@ -19415,7 +19411,7 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J135" s="60" t="str">
+      <c r="J135" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K135)),RIGHT(K135,LEN(K135)-FIND(" ",K135)))</f>
         <v>ehemorrhagic disease virus</v>
       </c>
@@ -19424,7 +19420,7 @@
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J136" s="61" t="s">
+      <c r="J136" s="60" t="s">
         <v>1103</v>
       </c>
       <c r="K136" s="7" t="s">
@@ -19439,7 +19435,7 @@
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J137" s="61" t="s">
+      <c r="J137" s="60" t="s">
         <v>1104</v>
       </c>
       <c r="K137" s="7" t="s">
@@ -19454,7 +19450,7 @@
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J138" s="60" t="str">
+      <c r="J138" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K138)),RIGHT(K138,LEN(K138)-FIND(" ",K138)))</f>
         <v>erhusiopathiae</v>
       </c>
@@ -19470,7 +19466,7 @@
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J139" s="60" t="str">
+      <c r="J139" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K139)),RIGHT(K139,LEN(K139)-FIND(" ",K139)))</f>
         <v>erotavirus</v>
       </c>
@@ -19486,7 +19482,7 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J140" s="61" t="s">
+      <c r="J140" s="60" t="s">
         <v>1105</v>
       </c>
       <c r="K140" s="7" t="s">
@@ -19501,7 +19497,7 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J141" s="60" t="str">
+      <c r="J141" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K141)),RIGHT(K141,LEN(K141)-FIND(" ",K141)))</f>
         <v>fcalicivirus</v>
       </c>
@@ -19517,7 +19513,7 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J142" s="61" t="s">
+      <c r="J142" s="60" t="s">
         <v>1106</v>
       </c>
       <c r="K142" s="7" t="s">
@@ -19532,7 +19528,7 @@
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J143" s="60" t="str">
+      <c r="J143" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K143)),RIGHT(K143,LEN(K143)-FIND(" ",K143)))</f>
         <v>fgraminearum</v>
       </c>
@@ -19548,7 +19544,7 @@
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J144" s="60" t="str">
+      <c r="J144" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K144)),RIGHT(K144,LEN(K144)-FIND(" ",K144)))</f>
         <v>fdisease virus</v>
       </c>
@@ -19557,7 +19553,7 @@
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J145" s="60" t="str">
+      <c r="J145" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K145)),RIGHT(K145,LEN(K145)-FIND(" ",K145)))</f>
         <v>fdisease virus</v>
       </c>
@@ -19566,7 +19562,7 @@
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J146" s="60" t="str">
+      <c r="J146" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K146)),RIGHT(K146,LEN(K146)-FIND(" ",K146)))</f>
         <v>fdisease virus</v>
       </c>
@@ -19575,7 +19571,7 @@
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J147" s="60" t="str">
+      <c r="J147" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K147)),RIGHT(K147,LEN(K147)-FIND(" ",K147)))</f>
         <v>fdisease virus</v>
       </c>
@@ -19584,7 +19580,7 @@
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J148" s="60" t="str">
+      <c r="J148" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K148)),RIGHT(K148,LEN(K148)-FIND(" ",K148)))</f>
         <v>fdisease virus</v>
       </c>
@@ -19593,7 +19589,7 @@
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J149" s="61" t="s">
+      <c r="J149" s="60" t="s">
         <v>1107</v>
       </c>
       <c r="K149" s="7" t="s">
@@ -19608,7 +19604,7 @@
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J150" s="61" t="s">
+      <c r="J150" s="60" t="s">
         <v>1108</v>
       </c>
       <c r="K150" s="7" t="s">
@@ -19623,7 +19619,7 @@
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J151" s="61" t="s">
+      <c r="J151" s="60" t="s">
         <v>1109</v>
       </c>
       <c r="K151" s="7" t="s">
@@ -19638,7 +19634,7 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J152" s="60" t="str">
+      <c r="J152" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K152)),RIGHT(K152,LEN(K152)-FIND(" ",K152)))</f>
         <v>fnecrophorum</v>
       </c>
@@ -19654,7 +19650,7 @@
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J153" s="61" t="s">
+      <c r="J153" s="60" t="s">
         <v>1110</v>
       </c>
       <c r="K153" s="7" t="s">
@@ -19669,7 +19665,7 @@
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J154" s="60" t="str">
+      <c r="J154" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K154)),RIGHT(K154,LEN(K154)-FIND(" ",K154)))</f>
         <v>fnecrophorum</v>
       </c>
@@ -19678,7 +19674,7 @@
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J155" s="60" t="str">
+      <c r="J155" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K155)),RIGHT(K155,LEN(K155)-FIND(" ",K155)))</f>
         <v>fproliferatum</v>
       </c>
@@ -19694,7 +19690,7 @@
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J156" s="60" t="str">
+      <c r="J156" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K156)),RIGHT(K156,LEN(K156)-FIND(" ",K156)))</f>
         <v>fverticillioides</v>
       </c>
@@ -19710,7 +19706,7 @@
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J157" s="60" t="str">
+      <c r="J157" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K157)),RIGHT(K157,LEN(K157)-FIND(" ",K157)))</f>
         <v>fproliferatum</v>
       </c>
@@ -19719,7 +19715,7 @@
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J158" s="60" t="str">
+      <c r="J158" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K158)),RIGHT(K158,LEN(K158)-FIND(" ",K158)))</f>
         <v>fvirus</v>
       </c>
@@ -19735,7 +19731,7 @@
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J159" s="60" t="str">
+      <c r="J159" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K159)),RIGHT(K159,LEN(K159)-FIND(" ",K159)))</f>
         <v>fverticillioides (moniliforme)</v>
       </c>
@@ -19744,7 +19740,7 @@
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J160" s="61" t="s">
+      <c r="J160" s="60" t="s">
         <v>1113</v>
       </c>
       <c r="K160" s="7" t="s">
@@ -19759,7 +19755,7 @@
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J161" s="61" t="s">
+      <c r="J161" s="60" t="s">
         <v>1114</v>
       </c>
       <c r="K161" s="0" t="s">
@@ -19774,7 +19770,7 @@
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J162" s="61" t="s">
+      <c r="J162" s="60" t="s">
         <v>1115</v>
       </c>
       <c r="K162" s="0" t="s">
@@ -19789,7 +19785,7 @@
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J163" s="61" t="s">
+      <c r="J163" s="60" t="s">
         <v>1116</v>
       </c>
       <c r="K163" s="0" t="s">
@@ -19804,7 +19800,7 @@
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J164" s="60" t="str">
+      <c r="J164" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K164)),RIGHT(K164,LEN(K164)-FIND(" ",K164)))</f>
         <v>hcapsulatum</v>
       </c>
@@ -19820,7 +19816,7 @@
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J165" s="61" t="s">
+      <c r="J165" s="60" t="s">
         <v>1117</v>
       </c>
       <c r="K165" s="7" t="s">
@@ -19835,7 +19831,7 @@
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J166" s="60" t="str">
+      <c r="J166" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K166)),RIGHT(K166,LEN(K166)-FIND(" ",K166)))</f>
         <v>hcapsulatum</v>
       </c>
@@ -19844,7 +19840,7 @@
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J167" s="60" t="str">
+      <c r="J167" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K167)),RIGHT(K167,LEN(K167)-FIND(" ",K167)))</f>
         <v>hcapsulatum</v>
       </c>
@@ -19853,7 +19849,7 @@
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J168" s="61" t="s">
+      <c r="J168" s="60" t="s">
         <v>1120</v>
       </c>
       <c r="K168" s="0" t="s">
@@ -19868,7 +19864,7 @@
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J169" s="61" t="s">
+      <c r="J169" s="60" t="s">
         <v>1121</v>
       </c>
       <c r="K169" s="0" t="s">
@@ -19883,7 +19879,7 @@
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J170" s="61" t="s">
+      <c r="J170" s="60" t="s">
         <v>1122</v>
       </c>
       <c r="K170" s="0" t="s">
@@ -19898,7 +19894,7 @@
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J171" s="61" t="s">
+      <c r="J171" s="60" t="s">
         <v>1123</v>
       </c>
       <c r="K171" s="0" t="s">
@@ -19913,13 +19909,13 @@
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J172" s="61" t="s">
+      <c r="J172" s="60" t="s">
         <v>1124</v>
       </c>
-      <c r="K172" s="49" t="s">
+      <c r="K172" s="48" t="s">
         <v>987</v>
       </c>
-      <c r="L172" s="49" t="s">
+      <c r="L172" s="48" t="s">
         <v>988</v>
       </c>
       <c r="M172" s="0" t="str">
@@ -19928,7 +19924,7 @@
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J173" s="61" t="s">
+      <c r="J173" s="60" t="s">
         <v>1125</v>
       </c>
       <c r="K173" s="0" t="s">
@@ -19943,7 +19939,7 @@
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J174" s="61" t="s">
+      <c r="J174" s="60" t="s">
         <v>1126</v>
       </c>
       <c r="K174" s="0" t="s">
@@ -19958,7 +19954,7 @@
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J175" s="61" t="s">
+      <c r="J175" s="60" t="s">
         <v>1127</v>
       </c>
       <c r="K175" s="0" t="s">
@@ -19973,7 +19969,7 @@
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J176" s="61" t="s">
+      <c r="J176" s="60" t="s">
         <v>1128</v>
       </c>
       <c r="K176" s="7" t="s">
@@ -19988,7 +19984,7 @@
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J177" s="61" t="s">
+      <c r="J177" s="60" t="s">
         <v>1129</v>
       </c>
       <c r="K177" s="0" t="s">
@@ -20003,7 +19999,7 @@
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J178" s="61" t="s">
+      <c r="J178" s="60" t="s">
         <v>1130</v>
       </c>
       <c r="K178" s="7" t="s">
@@ -20018,7 +20014,7 @@
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J179" s="61" t="s">
+      <c r="J179" s="60" t="s">
         <v>1131</v>
       </c>
       <c r="K179" s="0" t="s">
@@ -20033,7 +20029,7 @@
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J180" s="60" t="str">
+      <c r="J180" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K180)),RIGHT(K180,LEN(K180)-FIND(" ",K180)))</f>
         <v>iA (H3N2)</v>
       </c>
@@ -20042,7 +20038,7 @@
       </c>
     </row>
     <row r="181" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J181" s="60" t="str">
+      <c r="J181" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K181)),RIGHT(K181,LEN(K181)-FIND(" ",K181)))</f>
         <v>lautumnalis</v>
       </c>
@@ -20058,7 +20054,7 @@
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J182" s="60" t="str">
+      <c r="J182" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K182)),RIGHT(K182,LEN(K182)-FIND(" ",K182)))</f>
         <v>lborgpetersenii</v>
       </c>
@@ -20074,7 +20070,7 @@
       </c>
     </row>
     <row r="183" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J183" s="60" t="str">
+      <c r="J183" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K183)),RIGHT(K183,LEN(K183)-FIND(" ",K183)))</f>
         <v>lgrippothyphosa</v>
       </c>
@@ -20090,7 +20086,7 @@
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J184" s="60" t="str">
+      <c r="J184" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K184)),RIGHT(K184,LEN(K184)-FIND(" ",K184)))</f>
         <v>lborgpetersenii</v>
       </c>
@@ -20099,7 +20095,7 @@
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J185" s="60" t="str">
+      <c r="J185" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K185)),RIGHT(K185,LEN(K185)-FIND(" ",K185)))</f>
         <v>lhyos</v>
       </c>
@@ -20115,7 +20111,7 @@
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J186" s="60" t="str">
+      <c r="J186" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K186)),RIGHT(K186,LEN(K186)-FIND(" ",K186)))</f>
         <v>linterrogans</v>
       </c>
@@ -20131,7 +20127,7 @@
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J187" s="60" t="str">
+      <c r="J187" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K187)),RIGHT(K187,LEN(K187)-FIND(" ",K187)))</f>
         <v>lintracellularis</v>
       </c>
@@ -20147,7 +20143,7 @@
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J188" s="60" t="str">
+      <c r="J188" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K188)),RIGHT(K188,LEN(K188)-FIND(" ",K188)))</f>
         <v>linterrogans</v>
       </c>
@@ -20156,7 +20152,7 @@
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J189" s="60" t="str">
+      <c r="J189" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K189)),RIGHT(K189,LEN(K189)-FIND(" ",K189)))</f>
         <v>linterrogans</v>
       </c>
@@ -20165,7 +20161,7 @@
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J190" s="60" t="str">
+      <c r="J190" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K190)),RIGHT(K190,LEN(K190)-FIND(" ",K190)))</f>
         <v>linterrogans</v>
       </c>
@@ -20174,7 +20170,7 @@
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J191" s="60" t="str">
+      <c r="J191" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K191)),RIGHT(K191,LEN(K191)-FIND(" ",K191)))</f>
         <v>lkirschneri</v>
       </c>
@@ -20190,7 +20186,7 @@
       </c>
     </row>
     <row r="192" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J192" s="60" t="str">
+      <c r="J192" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K192)),RIGHT(K192,LEN(K192)-FIND(" ",K192)))</f>
         <v>lmonocytogenes</v>
       </c>
@@ -20206,7 +20202,7 @@
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J193" s="60" t="str">
+      <c r="J193" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K193)),RIGHT(K193,LEN(K193)-FIND(" ",K193)))</f>
         <v>lkirschneri</v>
       </c>
@@ -20215,7 +20211,7 @@
       </c>
     </row>
     <row r="194" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J194" s="60" t="str">
+      <c r="J194" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K194)),RIGHT(K194,LEN(K194)-FIND(" ",K194)))</f>
         <v>lpomona</v>
       </c>
@@ -20231,7 +20227,7 @@
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J195" s="60" t="str">
+      <c r="J195" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K195)),RIGHT(K195,LEN(K195)-FIND(" ",K195)))</f>
         <v>lrabies</v>
       </c>
@@ -20247,7 +20243,7 @@
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J196" s="61" t="s">
+      <c r="J196" s="60" t="s">
         <v>1133</v>
       </c>
       <c r="K196" s="6" t="s">
@@ -20262,7 +20258,7 @@
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J197" s="60" t="str">
+      <c r="J197" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K197)),RIGHT(K197,LEN(K197)-FIND(" ",K197)))</f>
         <v>lrabies</v>
       </c>
@@ -20271,7 +20267,7 @@
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J198" s="60" t="str">
+      <c r="J198" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K198)),RIGHT(K198,LEN(K198)-FIND(" ",K198)))</f>
         <v>lrabies</v>
       </c>
@@ -20280,7 +20276,7 @@
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J199" s="61" t="s">
+      <c r="J199" s="60" t="s">
         <v>1134</v>
       </c>
       <c r="K199" s="7" t="s">
@@ -20295,7 +20291,7 @@
       </c>
     </row>
     <row r="200" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J200" s="60" t="str">
+      <c r="J200" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K200)),RIGHT(K200,LEN(K200)-FIND(" ",K200)))</f>
         <v>lskin disease virus</v>
       </c>
@@ -20304,7 +20300,7 @@
       </c>
     </row>
     <row r="201" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J201" s="60" t="str">
+      <c r="J201" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K201)),RIGHT(K201,LEN(K201)-FIND(" ",K201)))</f>
         <v>malcelaphinegamma1</v>
       </c>
@@ -20320,7 +20316,7 @@
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J202" s="61" t="s">
+      <c r="J202" s="60" t="s">
         <v>1135</v>
       </c>
       <c r="K202" s="7" t="s">
@@ -20335,7 +20331,7 @@
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J203" s="60" t="str">
+      <c r="J203" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K203)),RIGHT(K203,LEN(K203)-FIND(" ",K203)))</f>
         <v>mbovis</v>
       </c>
@@ -20351,7 +20347,7 @@
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J204" s="60" t="str">
+      <c r="J204" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K204)),RIGHT(K204,LEN(K204)-FIND(" ",K204)))</f>
         <v>mavium subsp. Paratuberculosis</v>
       </c>
@@ -20360,7 +20356,7 @@
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J205" s="60" t="str">
+      <c r="J205" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K205)),RIGHT(K205,LEN(K205)-FIND(" ",K205)))</f>
         <v>mavium subsp. Paratuberculosis</v>
       </c>
@@ -20369,7 +20365,7 @@
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J206" s="60" t="str">
+      <c r="J206" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K206)),RIGHT(K206,LEN(K206)-FIND(" ",K206)))</f>
         <v>mcanis</v>
       </c>
@@ -20385,7 +20381,7 @@
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J207" s="60" t="str">
+      <c r="J207" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K207)),RIGHT(K207,LEN(K207)-FIND(" ",K207)))</f>
         <v>mbovis</v>
       </c>
@@ -20394,7 +20390,7 @@
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J208" s="60" t="str">
+      <c r="J208" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K208)),RIGHT(K208,LEN(K208)-FIND(" ",K208)))</f>
         <v>mbovis</v>
       </c>
@@ -20403,7 +20399,7 @@
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J209" s="60" t="str">
+      <c r="J209" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K209)),RIGHT(K209,LEN(K209)-FIND(" ",K209)))</f>
         <v>mcanis</v>
       </c>
@@ -20419,7 +20415,7 @@
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J210" s="61" t="s">
+      <c r="J210" s="60" t="s">
         <v>1138</v>
       </c>
       <c r="K210" s="7" t="s">
@@ -20434,7 +20430,7 @@
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J211" s="60" t="str">
+      <c r="J211" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K211)),RIGHT(K211,LEN(K211)-FIND(" ",K211)))</f>
         <v>mcanis</v>
       </c>
@@ -20443,7 +20439,7 @@
       </c>
     </row>
     <row r="212" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J212" s="60" t="str">
+      <c r="J212" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K212)),RIGHT(K212,LEN(K212)-FIND(" ",K212)))</f>
         <v>mcaprinegamma2</v>
       </c>
@@ -20459,7 +20455,7 @@
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J213" s="60" t="str">
+      <c r="J213" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K213)),RIGHT(K213,LEN(K213)-FIND(" ",K213)))</f>
         <v>mconjunctivae</v>
       </c>
@@ -20475,7 +20471,7 @@
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J214" s="61" t="s">
+      <c r="J214" s="60" t="s">
         <v>1139</v>
       </c>
       <c r="K214" s="7" t="s">
@@ -20490,7 +20486,7 @@
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J215" s="60" t="str">
+      <c r="J215" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K215)),RIGHT(K215,LEN(K215)-FIND(" ",K215)))</f>
         <v>mgallisepticum</v>
       </c>
@@ -20506,7 +20502,7 @@
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J216" s="60" t="str">
+      <c r="J216" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K216)),RIGHT(K216,LEN(K216)-FIND(" ",K216)))</f>
         <v>mhaemolytica</v>
       </c>
@@ -20522,7 +20518,7 @@
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J217" s="60" t="str">
+      <c r="J217" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K217)),RIGHT(K217,LEN(K217)-FIND(" ",K217)))</f>
         <v>mmycoides</v>
       </c>
@@ -20538,7 +20534,7 @@
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J218" s="60" t="str">
+      <c r="J218" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K218)),RIGHT(K218,LEN(K218)-FIND(" ",K218)))</f>
         <v>mhaemolytica</v>
       </c>
@@ -20547,7 +20543,7 @@
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J219" s="60" t="str">
+      <c r="J219" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K219)),RIGHT(K219,LEN(K219)-FIND(" ",K219)))</f>
         <v>mnanum</v>
       </c>
@@ -20563,7 +20559,7 @@
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J220" s="60" t="str">
+      <c r="J220" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K220)),RIGHT(K220,LEN(K220)-FIND(" ",K220)))</f>
         <v>movinegamma2</v>
       </c>
@@ -20579,7 +20575,7 @@
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J221" s="60" t="str">
+      <c r="J221" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K221)),RIGHT(K221,LEN(K221)-FIND(" ",K221)))</f>
         <v>movis</v>
       </c>
@@ -20595,7 +20591,7 @@
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J222" s="60" t="str">
+      <c r="J222" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K222)),RIGHT(K222,LEN(K222)-FIND(" ",K222)))</f>
         <v>mpachydermatis</v>
       </c>
@@ -20611,7 +20607,7 @@
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J223" s="60" t="str">
+      <c r="J223" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K223)),RIGHT(K223,LEN(K223)-FIND(" ",K223)))</f>
         <v>movis</v>
       </c>
@@ -20620,7 +20616,7 @@
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J224" s="60" t="str">
+      <c r="J224" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K224)),RIGHT(K224,LEN(K224)-FIND(" ",K224)))</f>
         <v>mplutonius</v>
       </c>
@@ -20636,7 +20632,7 @@
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J225" s="60" t="str">
+      <c r="J225" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K225)),RIGHT(K225,LEN(K225)-FIND(" ",K225)))</f>
         <v>mpachydermatis</v>
       </c>
@@ -20645,7 +20641,7 @@
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J226" s="60" t="str">
+      <c r="J226" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K226)),RIGHT(K226,LEN(K226)-FIND(" ",K226)))</f>
         <v>mtuberculosis</v>
       </c>
@@ -20661,7 +20657,7 @@
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J227" s="60" t="str">
+      <c r="J227" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K227)),RIGHT(K227,LEN(K227)-FIND(" ",K227)))</f>
         <v>napis</v>
       </c>
@@ -20677,7 +20673,7 @@
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J228" s="60" t="str">
+      <c r="J228" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K228)),RIGHT(K228,LEN(K228)-FIND(" ",K228)))</f>
         <v>nasteroides</v>
       </c>
@@ -20693,7 +20689,7 @@
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J229" s="60" t="str">
+      <c r="J229" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K229)),RIGHT(K229,LEN(K229)-FIND(" ",K229)))</f>
         <v>nbrasiliensis</v>
       </c>
@@ -20709,7 +20705,7 @@
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J230" s="61" t="s">
+      <c r="J230" s="60" t="s">
         <v>1144</v>
       </c>
       <c r="K230" s="7" t="s">
@@ -20724,7 +20720,7 @@
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J231" s="61" t="s">
+      <c r="J231" s="60" t="s">
         <v>1145</v>
       </c>
       <c r="K231" s="0" t="s">
@@ -20739,7 +20735,7 @@
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J232" s="60" t="str">
+      <c r="J232" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K232)),RIGHT(K232,LEN(K232)-FIND(" ",K232)))</f>
         <v>ngonorrhoeae</v>
       </c>
@@ -20755,7 +20751,7 @@
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J233" s="61" t="s">
+      <c r="J233" s="60" t="s">
         <v>1146</v>
       </c>
       <c r="K233" s="0" t="s">
@@ -20770,7 +20766,7 @@
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J234" s="60" t="str">
+      <c r="J234" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K234)),RIGHT(K234,LEN(K234)-FIND(" ",K234)))</f>
         <v>nmeningitidis</v>
       </c>
@@ -20786,7 +20782,7 @@
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J235" s="60" t="str">
+      <c r="J235" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K235)),RIGHT(K235,LEN(K235)-FIND(" ",K235)))</f>
         <v>nristicii</v>
       </c>
@@ -20802,7 +20798,7 @@
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J236" s="60" t="str">
+      <c r="J236" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K236)),RIGHT(K236,LEN(K236)-FIND(" ",K236)))</f>
         <v>ovirus</v>
       </c>
@@ -20818,7 +20814,7 @@
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J237" s="60" t="str">
+      <c r="J237" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K237)),RIGHT(K237,LEN(K237)-FIND(" ",K237)))</f>
         <v>paeruginosa</v>
       </c>
@@ -20834,7 +20830,7 @@
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J238" s="60" t="str">
+      <c r="J238" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K238)),RIGHT(K238,LEN(K238)-FIND(" ",K238)))</f>
         <v>ovirus</v>
       </c>
@@ -20843,7 +20839,7 @@
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J239" s="60" t="str">
+      <c r="J239" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K239)),RIGHT(K239,LEN(K239)-FIND(" ",K239)))</f>
         <v>pchartarum</v>
       </c>
@@ -20859,7 +20855,7 @@
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J240" s="60" t="str">
+      <c r="J240" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K240)),RIGHT(K240,LEN(K240)-FIND(" ",K240)))</f>
         <v>paeruginosa</v>
       </c>
@@ -20868,7 +20864,7 @@
       </c>
     </row>
     <row r="241" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J241" s="61" t="s">
+      <c r="J241" s="60" t="s">
         <v>1147</v>
       </c>
       <c r="K241" s="6" t="s">
@@ -20883,7 +20879,7 @@
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J242" s="61" t="s">
+      <c r="J242" s="60" t="s">
         <v>1149</v>
       </c>
       <c r="K242" s="7" t="s">
@@ -20898,7 +20894,7 @@
       </c>
     </row>
     <row r="243" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J243" s="61" t="s">
+      <c r="J243" s="60" t="s">
         <v>1150</v>
       </c>
       <c r="K243" s="6" t="s">
@@ -20913,7 +20909,7 @@
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J244" s="60" t="str">
+      <c r="J244" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K244)),RIGHT(K244,LEN(K244)-FIND(" ",K244)))</f>
         <v>plarvae</v>
       </c>
@@ -20929,7 +20925,7 @@
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J245" s="60" t="str">
+      <c r="J245" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K245)),RIGHT(K245,LEN(K245)-FIND(" ",K245)))</f>
         <v>pmultocida</v>
       </c>
@@ -20945,7 +20941,7 @@
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J246" s="60" t="str">
+      <c r="J246" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K246)),RIGHT(K246,LEN(K246)-FIND(" ",K246)))</f>
         <v>ppuberulum</v>
       </c>
@@ -20961,7 +20957,7 @@
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J247" s="60" t="str">
+      <c r="J247" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K247)),RIGHT(K247,LEN(K247)-FIND(" ",K247)))</f>
         <v>pmultocida</v>
       </c>
@@ -20970,7 +20966,7 @@
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J248" s="60" t="str">
+      <c r="J248" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K248)),RIGHT(K248,LEN(K248)-FIND(" ",K248)))</f>
         <v>pmultocida</v>
       </c>
@@ -20979,7 +20975,7 @@
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J249" s="60" t="str">
+      <c r="J249" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K249)),RIGHT(K249,LEN(K249)-FIND(" ",K249)))</f>
         <v>pmultocida</v>
       </c>
@@ -20988,7 +20984,7 @@
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J250" s="60" t="str">
+      <c r="J250" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K250)),RIGHT(K250,LEN(K250)-FIND(" ",K250)))</f>
         <v>pmultocida</v>
       </c>
@@ -20997,7 +20993,7 @@
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J251" s="60" t="str">
+      <c r="J251" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K251)),RIGHT(K251,LEN(K251)-FIND(" ",K251)))</f>
         <v>pmultocida</v>
       </c>
@@ -21006,7 +21002,7 @@
       </c>
     </row>
     <row r="252" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J252" s="61" t="s">
+      <c r="J252" s="60" t="s">
         <v>1151</v>
       </c>
       <c r="K252" s="6" t="s">
@@ -21021,7 +21017,7 @@
       </c>
     </row>
     <row r="253" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J253" s="61" t="s">
+      <c r="J253" s="60" t="s">
         <v>1152</v>
       </c>
       <c r="K253" s="6" t="s">
@@ -21036,7 +21032,7 @@
       </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J254" s="61" t="s">
+      <c r="J254" s="60" t="s">
         <v>1153</v>
       </c>
       <c r="K254" s="7" t="s">
@@ -21051,7 +21047,7 @@
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J255" s="61" t="s">
+      <c r="J255" s="60" t="s">
         <v>1154</v>
       </c>
       <c r="K255" s="7" t="s">
@@ -21066,7 +21062,7 @@
       </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J256" s="61" t="s">
+      <c r="J256" s="60" t="s">
         <v>1155</v>
       </c>
       <c r="K256" s="7" t="s">
@@ -21081,7 +21077,7 @@
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J257" s="61" t="s">
+      <c r="J257" s="60" t="s">
         <v>1156</v>
       </c>
       <c r="K257" s="7" t="s">
@@ -21096,7 +21092,7 @@
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J258" s="61" t="s">
+      <c r="J258" s="60" t="s">
         <v>1157</v>
       </c>
       <c r="K258" s="7" t="s">
@@ -21111,7 +21107,7 @@
       </c>
     </row>
     <row r="259" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J259" s="60" t="str">
+      <c r="J259" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K259)),RIGHT(K259,LEN(K259)-FIND(" ",K259)))</f>
         <v>rvirus</v>
       </c>
@@ -21127,7 +21123,7 @@
       </c>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J260" s="60" t="str">
+      <c r="J260" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K260)),RIGHT(K260,LEN(K260)-FIND(" ",K260)))</f>
         <v>sagalactiae</v>
       </c>
@@ -21143,7 +21139,7 @@
       </c>
     </row>
     <row r="261" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J261" s="60" t="str">
+      <c r="J261" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K261)),RIGHT(K261,LEN(K261)-FIND(" ",K261)))</f>
         <v>rvirus</v>
       </c>
@@ -21152,7 +21148,7 @@
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J262" s="60" t="str">
+      <c r="J262" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K262)),RIGHT(K262,LEN(K262)-FIND(" ",K262)))</f>
         <v>sagona</v>
       </c>
@@ -21168,7 +21164,7 @@
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J263" s="61" t="s">
+      <c r="J263" s="60" t="s">
         <v>1158</v>
       </c>
       <c r="K263" s="7" t="s">
@@ -21183,7 +21179,7 @@
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J264" s="60" t="str">
+      <c r="J264" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K264)),RIGHT(K264,LEN(K264)-FIND(" ",K264)))</f>
         <v>saureus</v>
       </c>
@@ -21199,7 +21195,7 @@
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J265" s="60" t="str">
+      <c r="J265" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K265)),RIGHT(K265,LEN(K265)-FIND(" ",K265)))</f>
         <v>scanis</v>
       </c>
@@ -21215,7 +21211,7 @@
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J266" s="60" t="str">
+      <c r="J266" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K266)),RIGHT(K266,LEN(K266)-FIND(" ",K266)))</f>
         <v>saureus</v>
       </c>
@@ -21224,7 +21220,7 @@
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J267" s="60" t="str">
+      <c r="J267" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K267)),RIGHT(K267,LEN(K267)-FIND(" ",K267)))</f>
         <v>saureus</v>
       </c>
@@ -21233,7 +21229,7 @@
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J268" s="60" t="str">
+      <c r="J268" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K268)),RIGHT(K268,LEN(K268)-FIND(" ",K268)))</f>
         <v>saureus</v>
       </c>
@@ -21242,7 +21238,7 @@
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J269" s="60" t="str">
+      <c r="J269" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K269)),RIGHT(K269,LEN(K269)-FIND(" ",K269)))</f>
         <v>saureus</v>
       </c>
@@ -21251,7 +21247,7 @@
       </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J270" s="61" t="s">
+      <c r="J270" s="60" t="s">
         <v>1159</v>
       </c>
       <c r="K270" s="7" t="s">
@@ -21266,7 +21262,7 @@
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J271" s="60" t="str">
+      <c r="J271" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K271)),RIGHT(K271,LEN(K271)-FIND(" ",K271)))</f>
         <v>scanis</v>
       </c>
@@ -21275,7 +21271,7 @@
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J272" s="60" t="str">
+      <c r="J272" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K272)),RIGHT(K272,LEN(K272)-FIND(" ",K272)))</f>
         <v>scholeraesuis</v>
       </c>
@@ -21291,7 +21287,7 @@
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J273" s="60" t="str">
+      <c r="J273" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K273)),RIGHT(K273,LEN(K273)-FIND(" ",K273)))</f>
         <v>sdublin</v>
       </c>
@@ -21307,7 +21303,7 @@
       </c>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J274" s="60" t="str">
+      <c r="J274" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K274)),RIGHT(K274,LEN(K274)-FIND(" ",K274)))</f>
         <v>sdysenteriae</v>
       </c>
@@ -21323,7 +21319,7 @@
       </c>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J275" s="60" t="str">
+      <c r="J275" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K275)),RIGHT(K275,LEN(K275)-FIND(" ",K275)))</f>
         <v>senteritidis</v>
       </c>
@@ -21339,7 +21335,7 @@
       </c>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J276" s="61" t="s">
+      <c r="J276" s="60" t="s">
         <v>1161</v>
       </c>
       <c r="K276" s="7" t="s">
@@ -21354,7 +21350,7 @@
       </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J277" s="61" t="s">
+      <c r="J277" s="60" t="s">
         <v>1164</v>
       </c>
       <c r="K277" s="7" t="s">
@@ -21369,7 +21365,7 @@
       </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J278" s="60" t="str">
+      <c r="J278" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K278)),RIGHT(K278,LEN(K278)-FIND(" ",K278)))</f>
         <v>sfelis</v>
       </c>
@@ -21385,7 +21381,7 @@
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J279" s="60" t="str">
+      <c r="J279" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K279)),RIGHT(K279,LEN(K279)-FIND(" ",K279)))</f>
         <v>sequi subsp. Zooepidemicus</v>
       </c>
@@ -21394,7 +21390,7 @@
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J280" s="60" t="str">
+      <c r="J280" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K280)),RIGHT(K280,LEN(K280)-FIND(" ",K280)))</f>
         <v>sequi subsp. Zooepidemicus</v>
       </c>
@@ -21403,7 +21399,7 @@
       </c>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J281" s="60" t="str">
+      <c r="J281" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K281)),RIGHT(K281,LEN(K281)-FIND(" ",K281)))</f>
         <v>sflexneri</v>
       </c>
@@ -21419,7 +21415,7 @@
       </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J282" s="60" t="str">
+      <c r="J282" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K282)),RIGHT(K282,LEN(K282)-FIND(" ",K282)))</f>
         <v>sgallinarum</v>
       </c>
@@ -21435,7 +21431,7 @@
       </c>
     </row>
     <row r="283" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J283" s="60" t="str">
+      <c r="J283" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K283)),RIGHT(K283,LEN(K283)-FIND(" ",K283)))</f>
         <v>shyicus</v>
       </c>
@@ -21451,7 +21447,7 @@
       </c>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J284" s="61" t="s">
+      <c r="J284" s="60" t="s">
         <v>1169</v>
       </c>
       <c r="K284" s="7" t="s">
@@ -21466,7 +21462,7 @@
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J285" s="61" t="s">
+      <c r="J285" s="60" t="s">
         <v>1170</v>
       </c>
       <c r="K285" s="7" t="s">
@@ -21481,7 +21477,7 @@
       </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J286" s="60" t="str">
+      <c r="J286" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K286)),RIGHT(K286,LEN(K286)-FIND(" ",K286)))</f>
         <v>sintermedius</v>
       </c>
@@ -21497,7 +21493,7 @@
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J287" s="60" t="str">
+      <c r="J287" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K287)),RIGHT(K287,LEN(K287)-FIND(" ",K287)))</f>
         <v>snewport</v>
       </c>
@@ -21513,7 +21509,7 @@
       </c>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J288" s="60" t="str">
+      <c r="J288" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K288)),RIGHT(K288,LEN(K288)-FIND(" ",K288)))</f>
         <v>spneumoniae</v>
       </c>
@@ -21529,7 +21525,7 @@
       </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J289" s="60" t="str">
+      <c r="J289" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K289)),RIGHT(K289,LEN(K289)-FIND(" ",K289)))</f>
         <v>spseudintermedius</v>
       </c>
@@ -21545,7 +21541,7 @@
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J290" s="60" t="str">
+      <c r="J290" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K290)),RIGHT(K290,LEN(K290)-FIND(" ",K290)))</f>
         <v>spullorum</v>
       </c>
@@ -21561,7 +21557,7 @@
       </c>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J291" s="60" t="str">
+      <c r="J291" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K291)),RIGHT(K291,LEN(K291)-FIND(" ",K291)))</f>
         <v>spseudintermedius</v>
       </c>
@@ -21570,7 +21566,7 @@
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J292" s="60" t="str">
+      <c r="J292" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K292)),RIGHT(K292,LEN(K292)-FIND(" ",K292)))</f>
         <v>spseudintermedius</v>
       </c>
@@ -21579,7 +21575,7 @@
       </c>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J293" s="60" t="str">
+      <c r="J293" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K293)),RIGHT(K293,LEN(K293)-FIND(" ",K293)))</f>
         <v>sschenckii</v>
       </c>
@@ -21595,7 +21591,7 @@
       </c>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J294" s="60" t="str">
+      <c r="J294" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K294)),RIGHT(K294,LEN(K294)-FIND(" ",K294)))</f>
         <v>ssonnei</v>
       </c>
@@ -21611,7 +21607,7 @@
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J295" s="60" t="str">
+      <c r="J295" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K295)),RIGHT(K295,LEN(K295)-FIND(" ",K295)))</f>
         <v>sschenckii</v>
       </c>
@@ -21620,7 +21616,7 @@
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J296" s="60" t="str">
+      <c r="J296" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K296)),RIGHT(K296,LEN(K296)-FIND(" ",K296)))</f>
         <v>sschenckii</v>
       </c>
@@ -21629,7 +21625,7 @@
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J297" s="61" t="s">
+      <c r="J297" s="60" t="s">
         <v>1173</v>
       </c>
       <c r="K297" s="7" t="s">
@@ -21644,7 +21640,7 @@
       </c>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J298" s="60" t="str">
+      <c r="J298" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K298)),RIGHT(K298,LEN(K298)-FIND(" ",K298)))</f>
         <v>styphimurium</v>
       </c>
@@ -21660,7 +21656,7 @@
       </c>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J299" s="60" t="str">
+      <c r="J299" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K299)),RIGHT(K299,LEN(K299)-FIND(" ",K299)))</f>
         <v>styphimurium</v>
       </c>
@@ -21676,7 +21672,7 @@
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J300" s="60" t="str">
+      <c r="J300" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K300)),RIGHT(K300,LEN(K300)-FIND(" ",K300)))</f>
         <v>styphimurium</v>
       </c>
@@ -21685,7 +21681,7 @@
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J301" s="60" t="str">
+      <c r="J301" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K301)),RIGHT(K301,LEN(K301)-FIND(" ",K301)))</f>
         <v>styphimurium</v>
       </c>
@@ -21694,7 +21690,7 @@
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J302" s="60" t="str">
+      <c r="J302" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K302)),RIGHT(K302,LEN(K302)-FIND(" ",K302)))</f>
         <v>styphimurium</v>
       </c>
@@ -21703,7 +21699,7 @@
       </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J303" s="60" t="str">
+      <c r="J303" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K303)),RIGHT(K303,LEN(K303)-FIND(" ",K303)))</f>
         <v>styphimurium</v>
       </c>
@@ -21712,7 +21708,7 @@
       </c>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J304" s="61" t="s">
+      <c r="J304" s="60" t="s">
         <v>1175</v>
       </c>
       <c r="K304" s="7" t="s">
@@ -21727,7 +21723,7 @@
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J305" s="61" t="s">
+      <c r="J305" s="60" t="s">
         <v>1176</v>
       </c>
       <c r="K305" s="7" t="s">
@@ -21742,7 +21738,7 @@
       </c>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J306" s="61" t="s">
+      <c r="J306" s="60" t="s">
         <v>1177</v>
       </c>
       <c r="K306" s="7" t="s">
@@ -21757,7 +21753,7 @@
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J307" s="60" t="str">
+      <c r="J307" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K307)),RIGHT(K307,LEN(K307)-FIND(" ",K307)))</f>
         <v>svirus</v>
       </c>
@@ -21766,7 +21762,7 @@
       </c>
     </row>
     <row r="308" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J308" s="60" t="str">
+      <c r="J308" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K308)),RIGHT(K308,LEN(K308)-FIND(" ",K308)))</f>
         <v>svirus</v>
       </c>
@@ -21775,7 +21771,7 @@
       </c>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J309" s="61" t="s">
+      <c r="J309" s="60" t="s">
         <v>1178</v>
       </c>
       <c r="K309" s="7" t="s">
@@ -21790,7 +21786,7 @@
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J310" s="60" t="str">
+      <c r="J310" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K310)),RIGHT(K310,LEN(K310)-FIND(" ",K310)))</f>
         <v>tequinum</v>
       </c>
@@ -21806,7 +21802,7 @@
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J311" s="61" t="s">
+      <c r="J311" s="60" t="s">
         <v>1179</v>
       </c>
       <c r="K311" s="7" t="s">
@@ -21821,7 +21817,7 @@
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J312" s="60" t="str">
+      <c r="J312" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K312)),RIGHT(K312,LEN(K312)-FIND(" ",K312)))</f>
         <v>tmentagrophytes</v>
       </c>
@@ -21837,7 +21833,7 @@
       </c>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J313" s="60" t="str">
+      <c r="J313" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K313)),RIGHT(K313,LEN(K313)-FIND(" ",K313)))</f>
         <v>tpallidum</v>
       </c>
@@ -21853,7 +21849,7 @@
       </c>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J314" s="60" t="str">
+      <c r="J314" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K314)),RIGHT(K314,LEN(K314)-FIND(" ",K314)))</f>
         <v>tmentagrophytes</v>
       </c>
@@ -21862,7 +21858,7 @@
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J315" s="60" t="str">
+      <c r="J315" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K315)),RIGHT(K315,LEN(K315)-FIND(" ",K315)))</f>
         <v>trubrum</v>
       </c>
@@ -21878,7 +21874,7 @@
       </c>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J316" s="60" t="str">
+      <c r="J316" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K316)),RIGHT(K316,LEN(K316)-FIND(" ",K316)))</f>
         <v>tverrucosum</v>
       </c>
@@ -21894,7 +21890,7 @@
       </c>
     </row>
     <row r="317" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J317" s="61" t="s">
+      <c r="J317" s="60" t="s">
         <v>1180</v>
       </c>
       <c r="K317" s="6" t="s">
@@ -21909,7 +21905,7 @@
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J318" s="60" t="str">
+      <c r="J318" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K318)),RIGHT(K318,LEN(K318)-FIND(" ",K318)))</f>
         <v>tverrucosum</v>
       </c>
@@ -21918,7 +21914,7 @@
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J319" s="60" t="str">
+      <c r="J319" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K319)),RIGHT(K319,LEN(K319)-FIND(" ",K319)))</f>
         <v>tverrucosum</v>
       </c>
@@ -21927,7 +21923,7 @@
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J320" s="60" t="str">
+      <c r="J320" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K320)),RIGHT(K320,LEN(K320)-FIND(" ",K320)))</f>
         <v>tverrucosum</v>
       </c>
@@ -21936,7 +21932,7 @@
       </c>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J321" s="60" t="str">
+      <c r="J321" s="59" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K321)),RIGHT(K321,LEN(K321)-FIND(" ",K321)))</f>
         <v>tverrucosum</v>
       </c>
@@ -21945,7 +21941,7 @@
       </c>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J322" s="61" t="s">
+      <c r="J322" s="60" t="s">
         <v>1181</v>
       </c>
       <c r="K322" s="0" t="s">
@@ -21960,7 +21956,7 @@
       </c>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J323" s="61" t="s">
+      <c r="J323" s="60" t="s">
         <v>1182</v>
       </c>
       <c r="K323" s="7" t="s">
@@ -21975,7 +21971,7 @@
       </c>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J324" s="61" t="s">
+      <c r="J324" s="60" t="s">
         <v>1183</v>
       </c>
       <c r="K324" s="0" t="s">
@@ -21990,7 +21986,7 @@
       </c>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J325" s="61" t="s">
+      <c r="J325" s="60" t="s">
         <v>1184</v>
       </c>
       <c r="K325" s="0" t="s">
@@ -22005,7 +22001,7 @@
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J326" s="60"/>
+      <c r="J326" s="59"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -22029,7 +22025,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
@@ -23617,7 +23613,7 @@
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A318" s="49" t="s">
+      <c r="A318" s="48" t="s">
         <v>988</v>
       </c>
     </row>
@@ -23678,7 +23674,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.89"/>
@@ -25044,7 +25040,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.99"/>
@@ -25053,24 +25049,24 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="61" t="s">
         <v>1189</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="61" t="s">
         <v>1190</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="62" t="s">
         <v>1191</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="48" t="s">
         <v>214</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="48" t="s">
         <v>238</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="48" t="s">
         <v>697</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -25079,112 +25075,112 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="48" t="s">
         <v>665</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="63" t="s">
         <v>559</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="63" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="64" t="s">
         <v>185</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="63" t="s">
         <v>575</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="48" t="s">
         <v>419</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="48" t="s">
         <v>267</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="48" t="s">
         <v>724</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="63" t="s">
         <v>463</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="48" t="s">
         <v>688</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="48" t="s">
         <v>188</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="48" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="48" t="s">
         <v>422</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="63" t="s">
         <v>590</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="48" t="s">
         <v>182</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="48" t="s">
         <v>442</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" s="63" t="s">
         <v>598</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="48" t="s">
         <v>345</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="48" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="48" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="48" t="s">
         <v>200</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="48" t="s">
         <v>156</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="63" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="48" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>843</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="48" t="s">
         <v>55</v>
       </c>
     </row>
@@ -25192,117 +25188,117 @@
       <c r="A13" s="0" t="s">
         <v>778</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="48" t="s">
         <v>309</v>
       </c>
-      <c r="C13" s="64" t="s">
+      <c r="C13" s="63" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="49" t="s">
+      <c r="A14" s="48" t="s">
         <v>211</v>
       </c>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="48" t="s">
         <v>650</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="48" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="48" t="s">
         <v>428</v>
       </c>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="48" t="s">
         <v>456</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="48" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="48" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="48" t="s">
         <v>450</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="48" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="48" t="s">
         <v>348</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="48" t="s">
         <v>617</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="48" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="48" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="49" t="s">
+      <c r="A19" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="48" t="s">
         <v>453</v>
       </c>
-      <c r="C19" s="49" t="s">
+      <c r="C19" s="48" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="48" t="s">
         <v>706</v>
       </c>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="48" t="s">
         <v>620</v>
       </c>
-      <c r="C20" s="49" t="s">
+      <c r="C20" s="48" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="48" t="s">
         <v>208</v>
       </c>
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="48" t="s">
         <v>144</v>
       </c>
-      <c r="C21" s="49" t="s">
+      <c r="C21" s="48" t="s">
         <v>684</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="48" t="s">
         <v>431</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="C22" s="64" t="s">
+      <c r="C22" s="63" t="s">
         <v>502</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="49" t="s">
+      <c r="A23" s="48" t="s">
         <v>361</v>
       </c>
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="48" t="s">
         <v>152</v>
       </c>
       <c r="C23" s="0" t="s">
@@ -25310,21 +25306,21 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="48" t="s">
         <v>358</v>
       </c>
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="48" t="s">
         <v>636</v>
       </c>
-      <c r="C24" s="49" t="s">
+      <c r="C24" s="48" t="s">
         <v>692</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="49" t="s">
+      <c r="A25" s="48" t="s">
         <v>196</v>
       </c>
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="48" t="s">
         <v>633</v>
       </c>
       <c r="C25" s="0" t="s">
@@ -25332,187 +25328,187 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="48" t="s">
         <v>341</v>
       </c>
-      <c r="B26" s="49" t="s">
+      <c r="B26" s="48" t="s">
         <v>639</v>
       </c>
-      <c r="C26" s="64" t="s">
+      <c r="C26" s="63" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="48" t="s">
         <v>217</v>
       </c>
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="48" t="s">
         <v>642</v>
       </c>
-      <c r="C27" s="64" t="s">
+      <c r="C27" s="63" t="s">
         <v>659</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="65" t="s">
+      <c r="A28" s="64" t="s">
         <v>703</v>
       </c>
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="C28" s="49" t="s">
+      <c r="C28" s="48" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="65" t="s">
+      <c r="A29" s="64" t="s">
         <v>416</v>
       </c>
-      <c r="B29" s="49" t="s">
+      <c r="B29" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="C29" s="49" t="s">
+      <c r="C29" s="48" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="49" t="s">
+      <c r="A30" s="48" t="s">
         <v>669</v>
       </c>
-      <c r="B30" s="64" t="s">
+      <c r="B30" s="63" t="s">
         <v>476</v>
       </c>
-      <c r="C30" s="49" t="s">
+      <c r="C30" s="48" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="65" t="s">
+      <c r="A31" s="64" t="s">
         <v>425</v>
       </c>
-      <c r="B31" s="49" t="s">
+      <c r="B31" s="48" t="s">
         <v>257</v>
       </c>
-      <c r="C31" s="49" t="s">
+      <c r="C31" s="48" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="49" t="s">
+      <c r="A32" s="48" t="s">
         <v>608</v>
       </c>
-      <c r="B32" s="49" t="s">
+      <c r="B32" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="49" t="s">
+      <c r="C32" s="48" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="49" t="s">
+      <c r="A33" s="48" t="s">
         <v>204</v>
       </c>
-      <c r="B33" s="64" t="s">
+      <c r="B33" s="63" t="s">
         <v>467</v>
       </c>
-      <c r="C33" s="49" t="s">
+      <c r="C33" s="48" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="49" t="s">
+      <c r="A34" s="48" t="s">
         <v>351</v>
       </c>
-      <c r="B34" s="66" t="s">
+      <c r="B34" s="65" t="s">
         <v>438</v>
       </c>
-      <c r="C34" s="49" t="s">
+      <c r="C34" s="48" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="49" t="s">
+      <c r="A35" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="48" t="s">
         <v>312</v>
       </c>
-      <c r="C35" s="49" t="s">
+      <c r="C35" s="48" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="48" t="s">
         <v>763</v>
       </c>
-      <c r="B36" s="66" t="s">
+      <c r="B36" s="65" t="s">
         <v>436</v>
       </c>
-      <c r="C36" s="49" t="s">
+      <c r="C36" s="48" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="49" t="s">
+      <c r="A37" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="65" t="s">
+      <c r="B37" s="64" t="s">
         <v>440</v>
       </c>
-      <c r="C37" s="49" t="s">
+      <c r="C37" s="48" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="49" t="s">
+      <c r="B38" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="49" t="s">
+      <c r="C38" s="48" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="49" t="s">
+      <c r="B39" s="48" t="s">
         <v>220</v>
       </c>
-      <c r="C39" s="49" t="s">
+      <c r="C39" s="48" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="66" t="s">
+      <c r="B40" s="65" t="s">
         <v>434</v>
       </c>
-      <c r="C40" s="49" t="s">
+      <c r="C40" s="48" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="64" t="s">
+      <c r="B41" s="63" t="s">
         <v>614</v>
       </c>
-      <c r="C41" s="49" t="s">
+      <c r="C41" s="48" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="49" t="s">
+      <c r="B42" s="48" t="s">
         <v>228</v>
       </c>
-      <c r="C42" s="49" t="s">
+      <c r="C42" s="48" t="s">
         <v>728</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="49" t="s">
+      <c r="B43" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="C43" s="49" t="s">
+      <c r="C43" s="48" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="49" t="s">
+      <c r="B44" s="48" t="s">
         <v>677</v>
       </c>
       <c r="C44" s="0" t="s">
@@ -25520,7 +25516,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="49" t="s">
+      <c r="B45" s="48" t="s">
         <v>64</v>
       </c>
       <c r="C45" s="0" t="s">
@@ -25528,7 +25524,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="49" t="s">
+      <c r="B46" s="48" t="s">
         <v>35</v>
       </c>
       <c r="C46" s="0" t="s">
@@ -25544,7 +25540,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="49" t="s">
+      <c r="B48" s="48" t="s">
         <v>117</v>
       </c>
       <c r="C48" s="0" t="s">
@@ -25552,7 +25548,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="49" t="s">
+      <c r="B49" s="48" t="s">
         <v>106</v>
       </c>
       <c r="C49" s="0" t="s">
@@ -25560,7 +25556,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="49" t="s">
+      <c r="B50" s="48" t="s">
         <v>715</v>
       </c>
       <c r="C50" s="0" t="s">
@@ -25576,7 +25572,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="49" t="s">
+      <c r="B52" s="48" t="s">
         <v>140</v>
       </c>
       <c r="C52" s="0" t="s">
@@ -25587,7 +25583,7 @@
       <c r="B53" s="0" t="s">
         <v>869</v>
       </c>
-      <c r="C53" s="49" t="s">
+      <c r="C53" s="48" t="s">
         <v>988</v>
       </c>
     </row>
@@ -25600,15 +25596,15 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="49" t="s">
+      <c r="B55" s="48" t="s">
         <v>373</v>
       </c>
-      <c r="C55" s="49" t="s">
+      <c r="C55" s="48" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="49" t="s">
+      <c r="B56" s="48" t="s">
         <v>242</v>
       </c>
       <c r="C56" s="0" t="s">
@@ -25616,15 +25612,15 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="49" t="s">
+      <c r="B57" s="48" t="s">
         <v>245</v>
       </c>
-      <c r="C57" s="49" t="s">
+      <c r="C57" s="48" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="49" t="s">
+      <c r="B58" s="48" t="s">
         <v>673</v>
       </c>
       <c r="C58" s="0" t="s">
@@ -25632,34 +25628,34 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="49" t="s">
+      <c r="B59" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="C59" s="64" t="s">
+      <c r="C59" s="63" t="s">
         <v>594</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="49" t="s">
+      <c r="B60" s="48" t="s">
         <v>231</v>
       </c>
-      <c r="C60" s="49" t="s">
+      <c r="C60" s="48" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="49" t="s">
+      <c r="B61" s="48" t="s">
         <v>368</v>
       </c>
-      <c r="C61" s="64" t="s">
+      <c r="C61" s="63" t="s">
         <v>572</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="49" t="s">
+      <c r="B62" s="48" t="s">
         <v>376</v>
       </c>
-      <c r="C62" s="64" t="s">
+      <c r="C62" s="63" t="s">
         <v>581</v>
       </c>
     </row>
@@ -25667,15 +25663,15 @@
       <c r="B63" s="0" t="s">
         <v>445</v>
       </c>
-      <c r="C63" s="64" t="s">
+      <c r="C63" s="63" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="49" t="s">
+      <c r="B64" s="48" t="s">
         <v>654</v>
       </c>
-      <c r="C64" s="49" t="s">
+      <c r="C64" s="48" t="s">
         <v>733</v>
       </c>
     </row>
@@ -25683,28 +25679,28 @@
       <c r="B65" s="0" t="s">
         <v>830</v>
       </c>
-      <c r="C65" s="49" t="s">
+      <c r="C65" s="48" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="49" t="s">
+      <c r="B66" s="48" t="s">
         <v>720</v>
       </c>
-      <c r="C66" s="49" t="s">
+      <c r="C66" s="48" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="49" t="s">
+      <c r="B67" s="48" t="s">
         <v>657</v>
       </c>
-      <c r="C67" s="49" t="s">
+      <c r="C67" s="48" t="s">
         <v>741</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="49" t="s">
+      <c r="B68" s="48" t="s">
         <v>718</v>
       </c>
       <c r="C68" s="0" t="s">
@@ -25712,7 +25708,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="49" t="s">
+      <c r="B69" s="48" t="s">
         <v>249</v>
       </c>
       <c r="C69" s="0" t="s">
@@ -25720,10 +25716,10 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="49" t="s">
+      <c r="B70" s="48" t="s">
         <v>235</v>
       </c>
-      <c r="C70" s="49" t="s">
+      <c r="C70" s="48" t="s">
         <v>164</v>
       </c>
     </row>
@@ -25731,7 +25727,7 @@
       <c r="B71" s="0" t="s">
         <v>858</v>
       </c>
-      <c r="C71" s="49" t="s">
+      <c r="C71" s="48" t="s">
         <v>175</v>
       </c>
     </row>
@@ -25739,7 +25735,7 @@
       <c r="B72" s="0" t="s">
         <v>861</v>
       </c>
-      <c r="C72" s="64" t="s">
+      <c r="C72" s="63" t="s">
         <v>535</v>
       </c>
     </row>
@@ -25747,76 +25743,76 @@
       <c r="B73" s="0" t="s">
         <v>855</v>
       </c>
-      <c r="C73" s="64" t="s">
+      <c r="C73" s="63" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="49" t="s">
+      <c r="B74" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="C74" s="64" t="s">
+      <c r="C74" s="63" t="s">
         <v>538</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="49" t="s">
+      <c r="B75" s="48" t="s">
         <v>305</v>
       </c>
-      <c r="C75" s="64" t="s">
+      <c r="C75" s="63" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="64" t="s">
+      <c r="B76" s="63" t="s">
         <v>472</v>
       </c>
-      <c r="C76" s="64" t="s">
+      <c r="C76" s="63" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="49" t="s">
+      <c r="B77" s="48" t="s">
         <v>364</v>
       </c>
-      <c r="C77" s="49" t="s">
+      <c r="C77" s="48" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="49" t="s">
+      <c r="B78" s="48" t="s">
         <v>224</v>
       </c>
-      <c r="C78" s="49" t="s">
+      <c r="C78" s="48" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="49" t="s">
+      <c r="B79" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="C79" s="49" t="s">
+      <c r="C79" s="48" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="49" t="s">
+      <c r="B80" s="48" t="s">
         <v>260</v>
       </c>
-      <c r="C80" s="65" t="s">
+      <c r="C80" s="64" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="49" t="s">
+      <c r="B81" s="48" t="s">
         <v>379</v>
       </c>
-      <c r="C81" s="49" t="s">
+      <c r="C81" s="48" t="s">
         <v>680</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="49" t="s">
+      <c r="B82" s="48" t="s">
         <v>263</v>
       </c>
       <c r="C82" s="0" t="s">
@@ -25827,15 +25823,15 @@
       <c r="B83" s="0" t="s">
         <v>793</v>
       </c>
-      <c r="C83" s="49" t="s">
+      <c r="C83" s="48" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="49" t="s">
+      <c r="B84" s="48" t="s">
         <v>459</v>
       </c>
-      <c r="C84" s="49" t="s">
+      <c r="C84" s="48" t="s">
         <v>168</v>
       </c>
     </row>
@@ -25843,27 +25839,27 @@
       <c r="B85" s="0" t="s">
         <v>865</v>
       </c>
-      <c r="C85" s="49" t="s">
+      <c r="C85" s="48" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C86" s="49" t="s">
+      <c r="C86" s="48" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C87" s="49" t="s">
+      <c r="C87" s="48" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C88" s="49" t="s">
+      <c r="C88" s="48" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C89" s="49" t="s">
+      <c r="C89" s="48" t="s">
         <v>757</v>
       </c>
     </row>
@@ -25873,12 +25869,12 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="64" t="s">
+      <c r="C91" s="63" t="s">
         <v>626</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C92" s="49" t="s">
+      <c r="C92" s="48" t="s">
         <v>386</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing bugs to do with column names
</commit_message>
<xml_diff>
--- a/info/apinet_survey (2).xlsx
+++ b/info/apinet_survey (2).xlsx
@@ -3615,7 +3615,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3677,6 +3677,14 @@
     <font>
       <sz val="9"/>
       <name val="Verdana"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -3771,14 +3779,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor rgb="FF800000"/>
+        <fgColor rgb="FF4B01A6"/>
+        <bgColor rgb="FF800080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7F7F7F"/>
         <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor rgb="FF800000"/>
       </patternFill>
     </fill>
     <fill>
@@ -3791,12 +3805,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF5BBFE"/>
         <bgColor rgb="FFF8CFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4B01A6"/>
-        <bgColor rgb="FF800080"/>
       </patternFill>
     </fill>
     <fill>
@@ -3909,7 +3917,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3917,7 +3925,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3945,10 +3953,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3973,6 +3977,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3981,15 +3989,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4002,6 +4010,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4021,11 +4033,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4033,7 +4045,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="13" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="14" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4041,15 +4053,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4057,11 +4065,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4073,7 +4081,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4089,35 +4097,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4205,11 +4213,11 @@
   </sheetPr>
   <dimension ref="A1:AK339"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T184" activeCellId="0" sqref="T184"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H184" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R282" activeCellId="0" sqref="R282"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.12"/>
@@ -4467,10 +4475,10 @@
       <c r="P6" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="Q6" s="13" t="s">
+      <c r="Q6" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="R6" s="13" t="s">
+      <c r="R6" s="15" t="s">
         <v>43</v>
       </c>
       <c r="S6" s="11" t="s">
@@ -4637,7 +4645,7 @@
       <c r="M10" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="N10" s="15" t="s">
+      <c r="N10" s="13" t="s">
         <v>68</v>
       </c>
       <c r="O10" s="13" t="s">
@@ -4646,7 +4654,7 @@
       <c r="P10" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q10" s="13" t="s">
+      <c r="Q10" s="15" t="s">
         <v>70</v>
       </c>
     </row>
@@ -9093,7 +9101,7 @@
         <v>370</v>
       </c>
       <c r="M133" s="7"/>
-      <c r="N133" s="22"/>
+      <c r="N133" s="7"/>
     </row>
     <row r="134" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="n">
@@ -9593,7 +9601,7 @@
       <c r="K147" s="8" t="s">
         <v>411</v>
       </c>
-      <c r="L147" s="23" t="s">
+      <c r="L147" s="22" t="s">
         <v>412</v>
       </c>
       <c r="M147" s="7"/>
@@ -9954,10 +9962,10 @@
       <c r="F157" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="G157" s="24" t="s">
+      <c r="G157" s="23" t="s">
         <v>433</v>
       </c>
-      <c r="H157" s="24" t="s">
+      <c r="H157" s="23" t="s">
         <v>434</v>
       </c>
       <c r="I157" s="0" t="str">
@@ -9990,10 +9998,10 @@
       <c r="F158" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="G158" s="24" t="s">
+      <c r="G158" s="23" t="s">
         <v>435</v>
       </c>
-      <c r="H158" s="24" t="s">
+      <c r="H158" s="23" t="s">
         <v>436</v>
       </c>
       <c r="I158" s="0" t="str">
@@ -10026,17 +10034,17 @@
       <c r="F159" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="G159" s="24" t="s">
+      <c r="G159" s="23" t="s">
         <v>437</v>
       </c>
-      <c r="H159" s="24" t="s">
+      <c r="H159" s="23" t="s">
         <v>438</v>
       </c>
       <c r="I159" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Pig_",H159,": '",F159,"',")</f>
         <v>Pig_Leptospira_autumnalis: 'Leptospirosis',</v>
       </c>
-      <c r="J159" s="25" t="str">
+      <c r="J159" s="24" t="str">
         <f aca="false">_xlfn.CONCAT("'",H159,"': ['Bacteria'],")</f>
         <v>'Leptospira_autumnalis': ['Bacteria'],</v>
       </c>
@@ -10582,7 +10590,7 @@
       <c r="M174" s="11" t="s">
         <v>484</v>
       </c>
-      <c r="N174" s="26" t="s">
+      <c r="N174" s="13" t="s">
         <v>485</v>
       </c>
       <c r="O174" s="11" t="s">
@@ -10666,10 +10674,10 @@
       <c r="M176" s="11" t="s">
         <v>495</v>
       </c>
-      <c r="N176" s="15" t="s">
+      <c r="N176" s="13" t="s">
         <v>496</v>
       </c>
-      <c r="O176" s="13" t="s">
+      <c r="O176" s="25" t="s">
         <v>497</v>
       </c>
       <c r="P176" s="14" t="s">
@@ -10747,10 +10755,10 @@
       <c r="K178" s="8" t="s">
         <v>508</v>
       </c>
-      <c r="L178" s="27" t="s">
+      <c r="L178" s="26" t="s">
         <v>509</v>
       </c>
-      <c r="M178" s="28" t="s">
+      <c r="M178" s="27" t="s">
         <v>510</v>
       </c>
     </row>
@@ -10937,7 +10945,7 @@
       <c r="L183" s="10" t="s">
         <v>527</v>
       </c>
-      <c r="M183" s="13"/>
+      <c r="M183" s="15"/>
     </row>
     <row r="184" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="n">
@@ -11017,7 +11025,7 @@
       <c r="M185" s="11" t="s">
         <v>484</v>
       </c>
-      <c r="N185" s="26" t="s">
+      <c r="N185" s="13" t="s">
         <v>485</v>
       </c>
       <c r="O185" s="11" t="s">
@@ -11062,37 +11070,37 @@
       <c r="M186" s="11" t="s">
         <v>541</v>
       </c>
-      <c r="N186" s="15" t="s">
+      <c r="N186" s="13" t="s">
         <v>542</v>
       </c>
-      <c r="O186" s="13" t="s">
+      <c r="O186" s="28" t="s">
         <v>543</v>
       </c>
       <c r="P186" s="14" t="s">
         <v>544</v>
       </c>
-      <c r="Q186" s="13" t="s">
+      <c r="Q186" s="15" t="s">
         <v>545</v>
       </c>
       <c r="R186" s="11" t="s">
         <v>486</v>
       </c>
-      <c r="S186" s="13" t="s">
+      <c r="S186" s="15" t="s">
         <v>546</v>
       </c>
-      <c r="T186" s="13" t="s">
+      <c r="T186" s="15" t="s">
         <v>547</v>
       </c>
       <c r="U186" s="11" t="s">
         <v>548</v>
       </c>
-      <c r="V186" s="13" t="s">
+      <c r="V186" s="15" t="s">
         <v>549</v>
       </c>
-      <c r="W186" s="13" t="s">
+      <c r="W186" s="15" t="s">
         <v>550</v>
       </c>
-      <c r="X186" s="13" t="s">
+      <c r="X186" s="15" t="s">
         <v>551</v>
       </c>
     </row>
@@ -11134,7 +11142,7 @@
       <c r="M187" s="11" t="s">
         <v>541</v>
       </c>
-      <c r="N187" s="15" t="s">
+      <c r="N187" s="13" t="s">
         <v>542</v>
       </c>
       <c r="O187" s="13" t="s">
@@ -11143,25 +11151,25 @@
       <c r="P187" s="14" t="s">
         <v>544</v>
       </c>
-      <c r="Q187" s="13" t="s">
+      <c r="Q187" s="15" t="s">
         <v>545</v>
       </c>
       <c r="R187" s="11" t="s">
         <v>486</v>
       </c>
-      <c r="S187" s="13" t="s">
+      <c r="S187" s="15" t="s">
         <v>546</v>
       </c>
-      <c r="T187" s="13" t="s">
+      <c r="T187" s="15" t="s">
         <v>547</v>
       </c>
       <c r="U187" s="11" t="s">
         <v>548</v>
       </c>
-      <c r="V187" s="13" t="s">
+      <c r="V187" s="15" t="s">
         <v>549</v>
       </c>
-      <c r="W187" s="13" t="s">
+      <c r="W187" s="15" t="s">
         <v>550</v>
       </c>
     </row>
@@ -14300,13 +14308,13 @@
       <c r="K275" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="L275" s="23" t="s">
+      <c r="L275" s="22" t="s">
         <v>709</v>
       </c>
       <c r="M275" s="11" t="s">
         <v>710</v>
       </c>
-      <c r="N275" s="15" t="s">
+      <c r="N275" s="13" t="s">
         <v>711</v>
       </c>
       <c r="O275" s="13" t="s">
@@ -14575,10 +14583,10 @@
       <c r="L282" s="11" t="s">
         <v>735</v>
       </c>
-      <c r="M282" s="15" t="s">
+      <c r="M282" s="13" t="s">
         <v>736</v>
       </c>
-      <c r="N282" s="15" t="s">
+      <c r="N282" s="13" t="s">
         <v>737</v>
       </c>
       <c r="O282" s="13" t="s">
@@ -14658,22 +14666,22 @@
       <c r="L284" s="10" t="s">
         <v>748</v>
       </c>
-      <c r="M284" s="15" t="s">
+      <c r="M284" s="13" t="s">
         <v>749</v>
       </c>
-      <c r="N284" s="15" t="s">
+      <c r="N284" s="13" t="s">
         <v>750</v>
       </c>
-      <c r="O284" s="13" t="s">
+      <c r="O284" s="37" t="s">
         <v>751</v>
       </c>
       <c r="P284" s="14" t="s">
         <v>752</v>
       </c>
-      <c r="Q284" s="13" t="s">
+      <c r="Q284" s="15" t="s">
         <v>753</v>
       </c>
-      <c r="R284" s="13" t="s">
+      <c r="R284" s="15" t="s">
         <v>754</v>
       </c>
     </row>
@@ -14715,7 +14723,7 @@
       <c r="A286" s="0" t="n">
         <v>290</v>
       </c>
-      <c r="B286" s="37" t="s">
+      <c r="B286" s="38" t="s">
         <v>759</v>
       </c>
       <c r="C286" s="7" t="s">
@@ -14750,10 +14758,10 @@
       <c r="L286" s="10" t="s">
         <v>765</v>
       </c>
-      <c r="M286" s="15" t="s">
+      <c r="M286" s="13" t="s">
         <v>766</v>
       </c>
-      <c r="N286" s="15" t="s">
+      <c r="N286" s="13" t="s">
         <v>767</v>
       </c>
     </row>
@@ -14761,7 +14769,7 @@
       <c r="A287" s="17" t="n">
         <v>291</v>
       </c>
-      <c r="B287" s="38" t="s">
+      <c r="B287" s="39" t="s">
         <v>759</v>
       </c>
       <c r="C287" s="19"/>
@@ -14769,7 +14777,7 @@
         <v>11</v>
       </c>
       <c r="E287" s="19"/>
-      <c r="F287" s="39"/>
+      <c r="F287" s="40"/>
       <c r="G287" s="19" t="s">
         <v>353</v>
       </c>
@@ -14797,13 +14805,13 @@
       <c r="A288" s="0" t="n">
         <v>292</v>
       </c>
-      <c r="B288" s="37" t="s">
+      <c r="B288" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D288" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F288" s="40" t="s">
+      <c r="F288" s="41" t="s">
         <v>22</v>
       </c>
       <c r="G288" s="0" t="s">
@@ -14826,10 +14834,10 @@
       <c r="L288" s="10" t="s">
         <v>768</v>
       </c>
-      <c r="M288" s="15" t="s">
+      <c r="M288" s="13" t="s">
         <v>769</v>
       </c>
-      <c r="N288" s="15" t="s">
+      <c r="N288" s="13" t="s">
         <v>770</v>
       </c>
       <c r="O288" s="13" t="s">
@@ -14838,16 +14846,16 @@
       <c r="P288" s="14" t="s">
         <v>772</v>
       </c>
-      <c r="Q288" s="13" t="s">
+      <c r="Q288" s="15" t="s">
         <v>773</v>
       </c>
-      <c r="R288" s="13" t="s">
+      <c r="R288" s="15" t="s">
         <v>774</v>
       </c>
-      <c r="S288" s="13" t="s">
+      <c r="S288" s="15" t="s">
         <v>775</v>
       </c>
-      <c r="T288" s="13" t="s">
+      <c r="T288" s="15" t="s">
         <v>776</v>
       </c>
     </row>
@@ -14855,13 +14863,13 @@
       <c r="A289" s="0" t="n">
         <v>293</v>
       </c>
-      <c r="B289" s="37" t="s">
+      <c r="B289" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D289" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F289" s="40" t="s">
+      <c r="F289" s="41" t="s">
         <v>22</v>
       </c>
       <c r="G289" s="0" t="s">
@@ -14884,7 +14892,7 @@
       <c r="L289" s="10" t="s">
         <v>780</v>
       </c>
-      <c r="M289" s="15" t="s">
+      <c r="M289" s="13" t="s">
         <v>781</v>
       </c>
       <c r="N289" s="7"/>
@@ -14893,7 +14901,7 @@
       <c r="A290" s="0" t="n">
         <v>294</v>
       </c>
-      <c r="B290" s="37" t="s">
+      <c r="B290" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D290" s="7" t="s">
@@ -14926,7 +14934,7 @@
       <c r="A291" s="0" t="n">
         <v>295</v>
       </c>
-      <c r="B291" s="37" t="s">
+      <c r="B291" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D291" s="7" t="s">
@@ -14959,7 +14967,7 @@
       <c r="A292" s="0" t="n">
         <v>296</v>
       </c>
-      <c r="B292" s="37" t="s">
+      <c r="B292" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D292" s="7" t="s">
@@ -14992,7 +15000,7 @@
       <c r="A293" s="0" t="n">
         <v>297</v>
       </c>
-      <c r="B293" s="37" t="s">
+      <c r="B293" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D293" s="7" t="s">
@@ -15021,34 +15029,34 @@
       <c r="L293" s="10" t="s">
         <v>768</v>
       </c>
-      <c r="M293" s="15" t="s">
+      <c r="M293" s="13" t="s">
         <v>771</v>
       </c>
-      <c r="N293" s="15" t="s">
+      <c r="N293" s="13" t="s">
         <v>782</v>
       </c>
-      <c r="O293" s="13" t="s">
+      <c r="O293" s="15" t="s">
         <v>783</v>
       </c>
       <c r="P293" s="14" t="s">
         <v>784</v>
       </c>
-      <c r="Q293" s="13" t="s">
+      <c r="Q293" s="15" t="s">
         <v>785</v>
       </c>
-      <c r="R293" s="13" t="s">
+      <c r="R293" s="15" t="s">
         <v>786</v>
       </c>
-      <c r="S293" s="13" t="s">
+      <c r="S293" s="15" t="s">
         <v>787</v>
       </c>
-      <c r="T293" s="13" t="s">
+      <c r="T293" s="15" t="s">
         <v>788</v>
       </c>
       <c r="U293" s="11" t="s">
         <v>789</v>
       </c>
-      <c r="V293" s="13" t="s">
+      <c r="V293" s="15" t="s">
         <v>790</v>
       </c>
     </row>
@@ -15056,7 +15064,7 @@
       <c r="A294" s="0" t="n">
         <v>298</v>
       </c>
-      <c r="B294" s="37" t="s">
+      <c r="B294" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D294" s="0" t="s">
@@ -15088,19 +15096,19 @@
       <c r="L294" s="10" t="s">
         <v>795</v>
       </c>
-      <c r="M294" s="15" t="s">
+      <c r="M294" s="13" t="s">
         <v>796</v>
       </c>
-      <c r="N294" s="15" t="s">
+      <c r="N294" s="13" t="s">
         <v>797</v>
       </c>
-      <c r="O294" s="13" t="s">
+      <c r="O294" s="15" t="s">
         <v>798</v>
       </c>
       <c r="P294" s="14" t="s">
         <v>799</v>
       </c>
-      <c r="Q294" s="13" t="s">
+      <c r="Q294" s="15" t="s">
         <v>800</v>
       </c>
     </row>
@@ -15108,7 +15116,7 @@
       <c r="A295" s="0" t="n">
         <v>299</v>
       </c>
-      <c r="B295" s="37" t="s">
+      <c r="B295" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D295" s="0" t="s">
@@ -15137,28 +15145,28 @@
       <c r="L295" s="10" t="s">
         <v>802</v>
       </c>
-      <c r="M295" s="15" t="s">
+      <c r="M295" s="13" t="s">
         <v>803</v>
       </c>
-      <c r="N295" s="15" t="s">
+      <c r="N295" s="13" t="s">
         <v>804</v>
       </c>
-      <c r="O295" s="13" t="s">
+      <c r="O295" s="15" t="s">
         <v>805</v>
       </c>
       <c r="P295" s="14" t="s">
         <v>806</v>
       </c>
-      <c r="Q295" s="13" t="s">
+      <c r="Q295" s="15" t="s">
         <v>807</v>
       </c>
-      <c r="R295" s="13" t="s">
+      <c r="R295" s="15" t="s">
         <v>808</v>
       </c>
-      <c r="S295" s="13" t="s">
+      <c r="S295" s="15" t="s">
         <v>809</v>
       </c>
-      <c r="T295" s="13" t="s">
+      <c r="T295" s="15" t="s">
         <v>810</v>
       </c>
       <c r="U295" s="11" t="s">
@@ -15167,7 +15175,7 @@
       <c r="V295" s="11" t="s">
         <v>812</v>
       </c>
-      <c r="W295" s="13" t="s">
+      <c r="W295" s="15" t="s">
         <v>813</v>
       </c>
     </row>
@@ -15175,7 +15183,7 @@
       <c r="A296" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="B296" s="37" t="s">
+      <c r="B296" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D296" s="0" t="s">
@@ -15207,7 +15215,7 @@
       <c r="A297" s="0" t="n">
         <v>301</v>
       </c>
-      <c r="B297" s="37" t="s">
+      <c r="B297" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D297" s="0" t="s">
@@ -15243,7 +15251,7 @@
       <c r="A298" s="0" t="n">
         <v>302</v>
       </c>
-      <c r="B298" s="37" t="s">
+      <c r="B298" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D298" s="0" t="s">
@@ -15272,22 +15280,22 @@
       <c r="L298" s="10" t="s">
         <v>823</v>
       </c>
-      <c r="M298" s="15" t="s">
+      <c r="M298" s="13" t="s">
         <v>824</v>
       </c>
-      <c r="N298" s="15" t="s">
+      <c r="N298" s="13" t="s">
         <v>825</v>
       </c>
-      <c r="O298" s="13" t="s">
+      <c r="O298" s="15" t="s">
         <v>826</v>
       </c>
       <c r="P298" s="11" t="s">
         <v>812</v>
       </c>
-      <c r="Q298" s="13" t="s">
+      <c r="Q298" s="15" t="s">
         <v>827</v>
       </c>
-      <c r="R298" s="13" t="s">
+      <c r="R298" s="15" t="s">
         <v>828</v>
       </c>
     </row>
@@ -15295,7 +15303,7 @@
       <c r="A299" s="0" t="n">
         <v>303</v>
       </c>
-      <c r="B299" s="37" t="s">
+      <c r="B299" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D299" s="0" t="s">
@@ -15331,7 +15339,7 @@
       <c r="A300" s="0" t="n">
         <v>304</v>
       </c>
-      <c r="B300" s="37" t="s">
+      <c r="B300" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D300" s="0" t="s">
@@ -15360,40 +15368,40 @@
       <c r="L300" s="10" t="s">
         <v>802</v>
       </c>
-      <c r="M300" s="41" t="s">
+      <c r="M300" s="42" t="s">
         <v>787</v>
       </c>
-      <c r="N300" s="15" t="s">
+      <c r="N300" s="13" t="s">
         <v>832</v>
       </c>
-      <c r="O300" s="13" t="s">
+      <c r="O300" s="15" t="s">
         <v>833</v>
       </c>
       <c r="P300" s="14" t="s">
         <v>834</v>
       </c>
-      <c r="Q300" s="13" t="s">
+      <c r="Q300" s="15" t="s">
         <v>813</v>
       </c>
-      <c r="R300" s="13" t="s">
+      <c r="R300" s="15" t="s">
         <v>835</v>
       </c>
-      <c r="S300" s="13" t="s">
+      <c r="S300" s="15" t="s">
         <v>836</v>
       </c>
-      <c r="T300" s="13" t="s">
+      <c r="T300" s="15" t="s">
         <v>837</v>
       </c>
       <c r="U300" s="11" t="s">
         <v>838</v>
       </c>
-      <c r="V300" s="13" t="s">
+      <c r="V300" s="15" t="s">
         <v>839</v>
       </c>
-      <c r="W300" s="13" t="s">
+      <c r="W300" s="15" t="s">
         <v>840</v>
       </c>
-      <c r="X300" s="13" t="s">
+      <c r="X300" s="15" t="s">
         <v>841</v>
       </c>
     </row>
@@ -15401,7 +15409,7 @@
       <c r="A301" s="0" t="n">
         <v>305</v>
       </c>
-      <c r="B301" s="37" t="s">
+      <c r="B301" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D301" s="0" t="s">
@@ -15433,22 +15441,22 @@
       <c r="M301" s="11" t="s">
         <v>846</v>
       </c>
-      <c r="N301" s="15" t="s">
+      <c r="N301" s="13" t="s">
         <v>847</v>
       </c>
-      <c r="O301" s="13" t="s">
+      <c r="O301" s="15" t="s">
         <v>848</v>
       </c>
       <c r="P301" s="14" t="s">
         <v>849</v>
       </c>
-      <c r="Q301" s="13" t="s">
+      <c r="Q301" s="15" t="s">
         <v>850</v>
       </c>
-      <c r="R301" s="13" t="s">
+      <c r="R301" s="15" t="s">
         <v>851</v>
       </c>
-      <c r="S301" s="13" t="s">
+      <c r="S301" s="15" t="s">
         <v>852</v>
       </c>
     </row>
@@ -15456,13 +15464,13 @@
       <c r="A302" s="0" t="n">
         <v>306</v>
       </c>
-      <c r="B302" s="37" t="s">
+      <c r="B302" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D302" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="F302" s="40" t="s">
+      <c r="F302" s="41" t="s">
         <v>853</v>
       </c>
       <c r="G302" s="0" t="s">
@@ -15492,13 +15500,13 @@
       <c r="A303" s="0" t="n">
         <v>307</v>
       </c>
-      <c r="B303" s="37" t="s">
+      <c r="B303" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D303" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="F303" s="40" t="s">
+      <c r="F303" s="41" t="s">
         <v>853</v>
       </c>
       <c r="G303" s="0" t="s">
@@ -15528,13 +15536,13 @@
       <c r="A304" s="0" t="n">
         <v>308</v>
       </c>
-      <c r="B304" s="37" t="s">
+      <c r="B304" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D304" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="F304" s="40" t="s">
+      <c r="F304" s="41" t="s">
         <v>853</v>
       </c>
       <c r="G304" s="0" t="s">
@@ -15564,7 +15572,7 @@
       <c r="A305" s="0" t="n">
         <v>309</v>
       </c>
-      <c r="B305" s="37" t="s">
+      <c r="B305" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D305" s="0" t="s">
@@ -15596,7 +15604,7 @@
       <c r="A306" s="0" t="n">
         <v>310</v>
       </c>
-      <c r="B306" s="37" t="s">
+      <c r="B306" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D306" s="0" t="s">
@@ -15632,7 +15640,7 @@
       <c r="A307" s="0" t="n">
         <v>311</v>
       </c>
-      <c r="B307" s="37" t="s">
+      <c r="B307" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D307" s="0" t="s">
@@ -15664,16 +15672,16 @@
       <c r="L307" s="10" t="s">
         <v>872</v>
       </c>
-      <c r="M307" s="15" t="s">
+      <c r="M307" s="13" t="s">
         <v>873</v>
       </c>
-      <c r="N307" s="13"/>
+      <c r="N307" s="15"/>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="0" t="n">
         <v>312</v>
       </c>
-      <c r="B308" s="37" t="s">
+      <c r="B308" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D308" s="0" t="s">
@@ -15702,28 +15710,28 @@
       <c r="L308" s="35" t="s">
         <v>876</v>
       </c>
-      <c r="M308" s="15" t="s">
+      <c r="M308" s="13" t="s">
         <v>877</v>
       </c>
-      <c r="N308" s="15" t="s">
+      <c r="N308" s="13" t="s">
         <v>878</v>
       </c>
-      <c r="O308" s="13" t="s">
+      <c r="O308" s="15" t="s">
         <v>879</v>
       </c>
       <c r="P308" s="14" t="s">
         <v>880</v>
       </c>
-      <c r="Q308" s="42" t="s">
+      <c r="Q308" s="43" t="s">
         <v>881</v>
       </c>
-      <c r="R308" s="13" t="s">
+      <c r="R308" s="15" t="s">
         <v>882</v>
       </c>
-      <c r="S308" s="13" t="s">
+      <c r="S308" s="15" t="s">
         <v>883</v>
       </c>
-      <c r="T308" s="13" t="s">
+      <c r="T308" s="15" t="s">
         <v>884</v>
       </c>
     </row>
@@ -15731,7 +15739,7 @@
       <c r="A309" s="0" t="n">
         <v>313</v>
       </c>
-      <c r="B309" s="37" t="s">
+      <c r="B309" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D309" s="0" t="s">
@@ -15765,7 +15773,7 @@
       <c r="A310" s="0" t="n">
         <v>314</v>
       </c>
-      <c r="B310" s="37" t="s">
+      <c r="B310" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D310" s="0" t="s">
@@ -15777,7 +15785,7 @@
       <c r="G310" s="0" t="s">
         <v>889</v>
       </c>
-      <c r="H310" s="43" t="s">
+      <c r="H310" s="44" t="s">
         <v>890</v>
       </c>
       <c r="I310" s="0" t="str">
@@ -15791,64 +15799,64 @@
       <c r="K310" s="8" t="s">
         <v>891</v>
       </c>
-      <c r="L310" s="44" t="s">
+      <c r="L310" s="45" t="s">
         <v>881</v>
       </c>
-      <c r="M310" s="15" t="s">
+      <c r="M310" s="13" t="s">
         <v>892</v>
       </c>
-      <c r="N310" s="15" t="s">
+      <c r="N310" s="13" t="s">
         <v>893</v>
       </c>
       <c r="P310" s="14" t="s">
         <v>894</v>
       </c>
-      <c r="Q310" s="13" t="s">
+      <c r="Q310" s="15" t="s">
         <v>895</v>
       </c>
-      <c r="R310" s="13" t="s">
+      <c r="R310" s="15" t="s">
         <v>896</v>
       </c>
-      <c r="S310" s="13" t="s">
+      <c r="S310" s="15" t="s">
         <v>897</v>
       </c>
-      <c r="T310" s="13" t="s">
+      <c r="T310" s="15" t="s">
         <v>898</v>
       </c>
       <c r="U310" s="11" t="s">
         <v>899</v>
       </c>
-      <c r="V310" s="13" t="s">
+      <c r="V310" s="15" t="s">
         <v>900</v>
       </c>
-      <c r="W310" s="13" t="s">
+      <c r="W310" s="15" t="s">
         <v>901</v>
       </c>
-      <c r="X310" s="13" t="s">
+      <c r="X310" s="15" t="s">
         <v>902</v>
       </c>
-      <c r="Y310" s="13" t="s">
+      <c r="Y310" s="15" t="s">
         <v>903</v>
       </c>
-      <c r="Z310" s="27" t="s">
+      <c r="Z310" s="26" t="s">
         <v>904</v>
       </c>
-      <c r="AA310" s="13" t="s">
+      <c r="AA310" s="15" t="s">
         <v>905</v>
       </c>
-      <c r="AB310" s="13" t="s">
+      <c r="AB310" s="15" t="s">
         <v>906</v>
       </c>
-      <c r="AC310" s="13" t="s">
+      <c r="AC310" s="15" t="s">
         <v>907</v>
       </c>
-      <c r="AD310" s="13" t="s">
+      <c r="AD310" s="15" t="s">
         <v>908</v>
       </c>
-      <c r="AE310" s="45" t="s">
+      <c r="AE310" s="46" t="s">
         <v>909</v>
       </c>
-      <c r="AF310" s="13" t="s">
+      <c r="AF310" s="15" t="s">
         <v>910</v>
       </c>
       <c r="AK310" s="0" t="n">
@@ -15859,7 +15867,7 @@
       <c r="A311" s="0" t="n">
         <v>315</v>
       </c>
-      <c r="B311" s="37" t="s">
+      <c r="B311" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D311" s="0" t="s">
@@ -15895,7 +15903,7 @@
       <c r="A312" s="0" t="n">
         <v>316</v>
       </c>
-      <c r="B312" s="37" t="s">
+      <c r="B312" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D312" s="0" t="s">
@@ -15921,23 +15929,23 @@
       <c r="K312" s="8" t="s">
         <v>918</v>
       </c>
-      <c r="L312" s="44" t="s">
+      <c r="L312" s="45" t="s">
         <v>919</v>
       </c>
-      <c r="M312" s="15" t="s">
+      <c r="M312" s="13" t="s">
         <v>920</v>
       </c>
-      <c r="N312" s="46" t="s">
+      <c r="N312" s="13" t="s">
         <v>921</v>
       </c>
-      <c r="O312" s="13"/>
+      <c r="O312" s="15"/>
       <c r="P312" s="14" t="s">
         <v>922</v>
       </c>
-      <c r="Q312" s="13" t="s">
+      <c r="Q312" s="15" t="s">
         <v>923</v>
       </c>
-      <c r="R312" s="13" t="s">
+      <c r="R312" s="15" t="s">
         <v>924</v>
       </c>
     </row>
@@ -15945,7 +15953,7 @@
       <c r="A313" s="0" t="n">
         <v>317</v>
       </c>
-      <c r="B313" s="37" t="s">
+      <c r="B313" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D313" s="0" t="s">
@@ -15974,19 +15982,19 @@
       <c r="L313" s="10" t="s">
         <v>928</v>
       </c>
-      <c r="M313" s="15" t="s">
+      <c r="M313" s="13" t="s">
         <v>929</v>
       </c>
-      <c r="N313" s="15" t="s">
+      <c r="N313" s="13" t="s">
         <v>930</v>
       </c>
-      <c r="AC313" s="13"/>
+      <c r="AC313" s="15"/>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="0" t="n">
         <v>318</v>
       </c>
-      <c r="B314" s="37" t="s">
+      <c r="B314" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D314" s="0" t="s">
@@ -16021,55 +16029,55 @@
       <c r="N314" s="47" t="s">
         <v>937</v>
       </c>
-      <c r="O314" s="13" t="s">
+      <c r="O314" s="15" t="s">
         <v>938</v>
       </c>
       <c r="P314" s="14" t="s">
         <v>939</v>
       </c>
-      <c r="Q314" s="13" t="s">
+      <c r="Q314" s="15" t="s">
         <v>940</v>
       </c>
-      <c r="R314" s="13" t="s">
+      <c r="R314" s="15" t="s">
         <v>941</v>
       </c>
-      <c r="S314" s="13" t="s">
+      <c r="S314" s="15" t="s">
         <v>942</v>
       </c>
-      <c r="T314" s="13" t="s">
+      <c r="T314" s="15" t="s">
         <v>943</v>
       </c>
       <c r="U314" s="11" t="s">
         <v>944</v>
       </c>
-      <c r="V314" s="13" t="s">
+      <c r="V314" s="15" t="s">
         <v>945</v>
       </c>
-      <c r="W314" s="13" t="s">
+      <c r="W314" s="15" t="s">
         <v>946</v>
       </c>
-      <c r="X314" s="13" t="s">
+      <c r="X314" s="15" t="s">
         <v>947</v>
       </c>
-      <c r="Y314" s="13" t="s">
+      <c r="Y314" s="15" t="s">
         <v>948</v>
       </c>
-      <c r="Z314" s="27" t="s">
+      <c r="Z314" s="26" t="s">
         <v>949</v>
       </c>
-      <c r="AA314" s="13" t="s">
+      <c r="AA314" s="15" t="s">
         <v>950</v>
       </c>
-      <c r="AB314" s="13" t="s">
+      <c r="AB314" s="15" t="s">
         <v>951</v>
       </c>
-      <c r="AC314" s="13" t="s">
+      <c r="AC314" s="15" t="s">
         <v>952</v>
       </c>
-      <c r="AD314" s="13" t="s">
+      <c r="AD314" s="15" t="s">
         <v>953</v>
       </c>
-      <c r="AE314" s="45" t="s">
+      <c r="AE314" s="46" t="s">
         <v>954</v>
       </c>
       <c r="AK314" s="0" t="n">
@@ -16080,7 +16088,7 @@
       <c r="A315" s="0" t="n">
         <v>319</v>
       </c>
-      <c r="B315" s="37" t="s">
+      <c r="B315" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D315" s="0" t="s">
@@ -16110,58 +16118,58 @@
         <v>935</v>
       </c>
       <c r="M315" s="8"/>
-      <c r="N315" s="46" t="s">
+      <c r="N315" s="13" t="s">
         <v>937</v>
       </c>
-      <c r="O315" s="13" t="s">
+      <c r="O315" s="15" t="s">
         <v>938</v>
       </c>
       <c r="P315" s="14" t="s">
         <v>939</v>
       </c>
-      <c r="Q315" s="13" t="s">
+      <c r="Q315" s="15" t="s">
         <v>940</v>
       </c>
-      <c r="R315" s="13" t="s">
+      <c r="R315" s="15" t="s">
         <v>941</v>
       </c>
-      <c r="S315" s="13" t="s">
+      <c r="S315" s="15" t="s">
         <v>942</v>
       </c>
-      <c r="T315" s="13" t="s">
+      <c r="T315" s="15" t="s">
         <v>943</v>
       </c>
       <c r="U315" s="11" t="s">
         <v>944</v>
       </c>
-      <c r="V315" s="13" t="s">
+      <c r="V315" s="15" t="s">
         <v>945</v>
       </c>
-      <c r="W315" s="13" t="s">
+      <c r="W315" s="15" t="s">
         <v>946</v>
       </c>
-      <c r="X315" s="13" t="s">
+      <c r="X315" s="15" t="s">
         <v>947</v>
       </c>
-      <c r="Y315" s="13" t="s">
+      <c r="Y315" s="15" t="s">
         <v>948</v>
       </c>
-      <c r="Z315" s="27" t="s">
+      <c r="Z315" s="26" t="s">
         <v>949</v>
       </c>
-      <c r="AA315" s="13" t="s">
+      <c r="AA315" s="15" t="s">
         <v>950</v>
       </c>
-      <c r="AB315" s="13" t="s">
+      <c r="AB315" s="15" t="s">
         <v>951</v>
       </c>
-      <c r="AC315" s="13" t="s">
+      <c r="AC315" s="15" t="s">
         <v>952</v>
       </c>
-      <c r="AD315" s="13" t="s">
+      <c r="AD315" s="15" t="s">
         <v>958</v>
       </c>
-      <c r="AE315" s="45" t="s">
+      <c r="AE315" s="46" t="s">
         <v>959</v>
       </c>
     </row>
@@ -16169,7 +16177,7 @@
       <c r="A316" s="0" t="n">
         <v>320</v>
       </c>
-      <c r="B316" s="37" t="s">
+      <c r="B316" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D316" s="0" t="s">
@@ -16195,52 +16203,52 @@
       <c r="K316" s="8" t="s">
         <v>963</v>
       </c>
-      <c r="L316" s="44" t="s">
+      <c r="L316" s="45" t="s">
         <v>964</v>
       </c>
       <c r="M316" s="47" t="s">
         <v>965</v>
       </c>
-      <c r="N316" s="15" t="s">
+      <c r="N316" s="13" t="s">
         <v>966</v>
       </c>
-      <c r="O316" s="13" t="s">
+      <c r="O316" s="15" t="s">
         <v>967</v>
       </c>
       <c r="P316" s="14" t="s">
         <v>968</v>
       </c>
-      <c r="Q316" s="13" t="s">
+      <c r="Q316" s="15" t="s">
         <v>969</v>
       </c>
-      <c r="R316" s="13" t="s">
+      <c r="R316" s="15" t="s">
         <v>509</v>
       </c>
-      <c r="S316" s="13" t="s">
+      <c r="S316" s="15" t="s">
         <v>970</v>
       </c>
-      <c r="T316" s="13" t="s">
+      <c r="T316" s="15" t="s">
         <v>971</v>
       </c>
       <c r="U316" s="11" t="s">
         <v>972</v>
       </c>
-      <c r="V316" s="13" t="s">
+      <c r="V316" s="15" t="s">
         <v>973</v>
       </c>
-      <c r="W316" s="13" t="s">
+      <c r="W316" s="15" t="s">
         <v>974</v>
       </c>
-      <c r="X316" s="13" t="s">
+      <c r="X316" s="15" t="s">
         <v>975</v>
       </c>
-      <c r="Y316" s="13" t="s">
+      <c r="Y316" s="15" t="s">
         <v>976</v>
       </c>
-      <c r="Z316" s="27" t="s">
+      <c r="Z316" s="26" t="s">
         <v>977</v>
       </c>
-      <c r="AA316" s="13" t="s">
+      <c r="AA316" s="15" t="s">
         <v>978</v>
       </c>
     </row>
@@ -16248,7 +16256,7 @@
       <c r="A317" s="0" t="n">
         <v>321</v>
       </c>
-      <c r="B317" s="37" t="s">
+      <c r="B317" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D317" s="0" t="s">
@@ -16274,31 +16282,31 @@
       <c r="K317" s="8" t="s">
         <v>981</v>
       </c>
-      <c r="L317" s="44" t="s">
+      <c r="L317" s="45" t="s">
         <v>964</v>
       </c>
-      <c r="M317" s="15" t="s">
+      <c r="M317" s="13" t="s">
         <v>982</v>
       </c>
-      <c r="N317" s="13"/>
+      <c r="N317" s="15"/>
       <c r="P317" s="14"/>
-      <c r="Q317" s="13"/>
-      <c r="R317" s="13"/>
-      <c r="S317" s="13"/>
-      <c r="T317" s="13"/>
+      <c r="Q317" s="15"/>
+      <c r="R317" s="15"/>
+      <c r="S317" s="15"/>
+      <c r="T317" s="15"/>
       <c r="U317" s="11"/>
-      <c r="V317" s="13"/>
-      <c r="W317" s="13"/>
-      <c r="X317" s="13"/>
-      <c r="Y317" s="13"/>
-      <c r="Z317" s="27"/>
-      <c r="AA317" s="13"/>
+      <c r="V317" s="15"/>
+      <c r="W317" s="15"/>
+      <c r="X317" s="15"/>
+      <c r="Y317" s="15"/>
+      <c r="Z317" s="26"/>
+      <c r="AA317" s="15"/>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="0" t="n">
         <v>322</v>
       </c>
-      <c r="B318" s="37" t="s">
+      <c r="B318" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D318" s="0" t="s">
@@ -16330,18 +16338,18 @@
       <c r="M318" s="47" t="s">
         <v>986</v>
       </c>
-      <c r="O318" s="13"/>
+      <c r="O318" s="15"/>
       <c r="P318" s="14"/>
-      <c r="T318" s="13"/>
+      <c r="T318" s="15"/>
       <c r="U318" s="11"/>
-      <c r="Y318" s="13"/>
-      <c r="Z318" s="27"/>
+      <c r="Y318" s="15"/>
+      <c r="Z318" s="26"/>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="0" t="n">
         <v>323</v>
       </c>
-      <c r="B319" s="37" t="s">
+      <c r="B319" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D319" s="0" t="s">
@@ -16377,7 +16385,7 @@
       <c r="A320" s="0" t="n">
         <v>324</v>
       </c>
-      <c r="B320" s="37" t="s">
+      <c r="B320" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D320" s="0" t="s">
@@ -16413,7 +16421,7 @@
       <c r="A321" s="0" t="n">
         <v>325</v>
       </c>
-      <c r="B321" s="37" t="s">
+      <c r="B321" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D321" s="0" t="s">
@@ -16442,19 +16450,19 @@
       <c r="L321" s="10" t="s">
         <v>996</v>
       </c>
-      <c r="M321" s="15" t="s">
+      <c r="M321" s="13" t="s">
         <v>997</v>
       </c>
-      <c r="N321" s="15" t="s">
+      <c r="N321" s="13" t="s">
         <v>998</v>
       </c>
-      <c r="O321" s="13" t="s">
+      <c r="O321" s="15" t="s">
         <v>999</v>
       </c>
       <c r="P321" s="14" t="s">
         <v>1000</v>
       </c>
-      <c r="Q321" s="13" t="s">
+      <c r="Q321" s="15" t="s">
         <v>1001</v>
       </c>
     </row>
@@ -16462,7 +16470,7 @@
       <c r="A322" s="0" t="n">
         <v>326</v>
       </c>
-      <c r="B322" s="37" t="s">
+      <c r="B322" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D322" s="0" t="s">
@@ -16491,7 +16499,7 @@
       <c r="L322" s="10" t="s">
         <v>812</v>
       </c>
-      <c r="M322" s="15" t="s">
+      <c r="M322" s="13" t="s">
         <v>1006</v>
       </c>
       <c r="N322" s="7"/>
@@ -16500,7 +16508,7 @@
       <c r="A323" s="0" t="n">
         <v>327</v>
       </c>
-      <c r="B323" s="37" t="s">
+      <c r="B323" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D323" s="0" t="s">
@@ -16538,7 +16546,7 @@
       <c r="A324" s="0" t="n">
         <v>328</v>
       </c>
-      <c r="B324" s="37" t="s">
+      <c r="B324" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D324" s="0" t="s">
@@ -16572,7 +16580,7 @@
       <c r="A325" s="0" t="n">
         <v>329</v>
       </c>
-      <c r="B325" s="37" t="s">
+      <c r="B325" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D325" s="0" t="s">
@@ -16604,58 +16612,58 @@
       <c r="M325" s="49" t="s">
         <v>1019</v>
       </c>
-      <c r="N325" s="15" t="s">
+      <c r="N325" s="13" t="s">
         <v>1020</v>
       </c>
-      <c r="O325" s="13" t="s">
+      <c r="O325" s="15" t="s">
         <v>1021</v>
       </c>
       <c r="P325" s="14" t="s">
         <v>1022</v>
       </c>
-      <c r="Q325" s="13" t="s">
+      <c r="Q325" s="15" t="s">
         <v>1023</v>
       </c>
-      <c r="R325" s="13" t="s">
+      <c r="R325" s="15" t="s">
         <v>1024</v>
       </c>
-      <c r="S325" s="13" t="s">
+      <c r="S325" s="15" t="s">
         <v>1025</v>
       </c>
-      <c r="T325" s="13" t="s">
+      <c r="T325" s="15" t="s">
         <v>1026</v>
       </c>
       <c r="U325" s="11" t="s">
         <v>1027</v>
       </c>
-      <c r="V325" s="13" t="s">
+      <c r="V325" s="15" t="s">
         <v>1028</v>
       </c>
-      <c r="W325" s="13" t="s">
+      <c r="W325" s="15" t="s">
         <v>1029</v>
       </c>
-      <c r="X325" s="13" t="s">
+      <c r="X325" s="15" t="s">
         <v>1030</v>
       </c>
-      <c r="Y325" s="13" t="s">
+      <c r="Y325" s="15" t="s">
         <v>1031</v>
       </c>
-      <c r="Z325" s="27" t="s">
+      <c r="Z325" s="26" t="s">
         <v>1032</v>
       </c>
-      <c r="AA325" s="13" t="s">
+      <c r="AA325" s="15" t="s">
         <v>1033</v>
       </c>
-      <c r="AB325" s="13" t="s">
+      <c r="AB325" s="15" t="s">
         <v>1034</v>
       </c>
-      <c r="AC325" s="13" t="s">
+      <c r="AC325" s="15" t="s">
         <v>1035</v>
       </c>
-      <c r="AD325" s="13" t="s">
+      <c r="AD325" s="15" t="s">
         <v>1036</v>
       </c>
-      <c r="AE325" s="45" t="s">
+      <c r="AE325" s="46" t="s">
         <v>1037</v>
       </c>
     </row>
@@ -16663,7 +16671,7 @@
       <c r="A326" s="0" t="n">
         <v>330</v>
       </c>
-      <c r="B326" s="37" t="s">
+      <c r="B326" s="38" t="s">
         <v>759</v>
       </c>
       <c r="D326" s="0" t="s">
@@ -16692,49 +16700,49 @@
       <c r="L326" s="11" t="s">
         <v>1018</v>
       </c>
-      <c r="M326" s="15" t="s">
+      <c r="M326" s="13" t="s">
         <v>1042</v>
       </c>
-      <c r="N326" s="46" t="s">
+      <c r="N326" s="13" t="s">
         <v>1043</v>
       </c>
-      <c r="O326" s="13" t="s">
+      <c r="O326" s="15" t="s">
         <v>1044</v>
       </c>
       <c r="P326" s="14" t="s">
         <v>1045</v>
       </c>
-      <c r="Q326" s="13" t="s">
+      <c r="Q326" s="15" t="s">
         <v>1046</v>
       </c>
-      <c r="R326" s="13" t="s">
+      <c r="R326" s="15" t="s">
         <v>1047</v>
       </c>
-      <c r="S326" s="13" t="s">
+      <c r="S326" s="15" t="s">
         <v>1048</v>
       </c>
-      <c r="T326" s="13" t="s">
+      <c r="T326" s="15" t="s">
         <v>1049</v>
       </c>
       <c r="U326" s="11" t="s">
         <v>1050</v>
       </c>
-      <c r="V326" s="13" t="s">
+      <c r="V326" s="15" t="s">
         <v>1051</v>
       </c>
-      <c r="W326" s="13" t="s">
+      <c r="W326" s="15" t="s">
         <v>1052</v>
       </c>
-      <c r="X326" s="13" t="s">
+      <c r="X326" s="15" t="s">
         <v>1053</v>
       </c>
-      <c r="Y326" s="13" t="s">
+      <c r="Y326" s="15" t="s">
         <v>1054</v>
       </c>
-      <c r="Z326" s="27" t="s">
+      <c r="Z326" s="26" t="s">
         <v>1055</v>
       </c>
-      <c r="AE326" s="45"/>
+      <c r="AE326" s="46"/>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B327" s="50"/>
@@ -17459,7 +17467,7 @@
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.11"/>
@@ -20042,10 +20050,10 @@
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K181)),RIGHT(K181,LEN(K181)-FIND(" ",K181)))</f>
         <v>lautumnalis</v>
       </c>
-      <c r="K181" s="24" t="s">
+      <c r="K181" s="23" t="s">
         <v>437</v>
       </c>
-      <c r="L181" s="24" t="s">
+      <c r="L181" s="23" t="s">
         <v>438</v>
       </c>
       <c r="M181" s="0" t="str">
@@ -20074,10 +20082,10 @@
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K183)),RIGHT(K183,LEN(K183)-FIND(" ",K183)))</f>
         <v>lgrippothyphosa</v>
       </c>
-      <c r="K183" s="24" t="s">
+      <c r="K183" s="23" t="s">
         <v>435</v>
       </c>
-      <c r="L183" s="24" t="s">
+      <c r="L183" s="23" t="s">
         <v>436</v>
       </c>
       <c r="M183" s="0" t="str">
@@ -20099,10 +20107,10 @@
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K185)),RIGHT(K185,LEN(K185)-FIND(" ",K185)))</f>
         <v>lhyos</v>
       </c>
-      <c r="K185" s="24" t="s">
+      <c r="K185" s="23" t="s">
         <v>1132</v>
       </c>
-      <c r="L185" s="24" t="s">
+      <c r="L185" s="23" t="s">
         <v>440</v>
       </c>
       <c r="M185" s="0" t="str">
@@ -20215,10 +20223,10 @@
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K194)),RIGHT(K194,LEN(K194)-FIND(" ",K194)))</f>
         <v>lpomona</v>
       </c>
-      <c r="K194" s="24" t="s">
+      <c r="K194" s="23" t="s">
         <v>433</v>
       </c>
-      <c r="L194" s="24" t="s">
+      <c r="L194" s="23" t="s">
         <v>434</v>
       </c>
       <c r="M194" s="0" t="str">
@@ -22025,7 +22033,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
@@ -22803,17 +22811,17 @@
       </c>
     </row>
     <row r="156" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="24" t="s">
+      <c r="A156" s="23" t="s">
         <v>434</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="24" t="s">
+      <c r="A157" s="23" t="s">
         <v>436</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="24" t="s">
+      <c r="A158" s="23" t="s">
         <v>438</v>
       </c>
     </row>
@@ -23674,7 +23682,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.89"/>
@@ -25040,7 +25048,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.99"/>

</xml_diff>

<commit_message>
Use col name only unless not provided, then use filename. Also added new tool
</commit_message>
<xml_diff>
--- a/info/apinet_survey (2).xlsx
+++ b/info/apinet_survey (2).xlsx
@@ -3621,12 +3621,13 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3648,11 +3649,13 @@
       <sz val="10"/>
       <name val="Cantarell"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Cantarell"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -3660,6 +3663,7 @@
       <color rgb="FF0000EE"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -3667,17 +3671,20 @@
       <color rgb="FF4B01A6"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Cantarell"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Verdana"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -3685,6 +3692,7 @@
       <color rgb="FFC00000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -3692,6 +3700,7 @@
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -3699,22 +3708,32 @@
       <color rgb="FFFFC000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Liberation Mono;Courier New"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="20">
@@ -4082,7 +4101,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4094,7 +4113,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4138,31 +4157,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4251,10 +4270,10 @@
   <dimension ref="A1:AK340"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L281" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S301" activeCellId="0" sqref="S301"/>
+      <selection pane="topLeft" activeCell="S316" activeCellId="0" sqref="S316"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.12"/>
@@ -15765,7 +15784,7 @@
       <c r="R308" s="13" t="s">
         <v>882</v>
       </c>
-      <c r="S308" s="26" t="s">
+      <c r="S308" s="13" t="s">
         <v>883</v>
       </c>
       <c r="T308" s="26" t="s">
@@ -15854,7 +15873,7 @@
       <c r="R310" s="13" t="s">
         <v>896</v>
       </c>
-      <c r="S310" s="26" t="s">
+      <c r="S310" s="13" t="s">
         <v>897</v>
       </c>
       <c r="T310" s="26" t="s">
@@ -16078,7 +16097,7 @@
       <c r="R314" s="13" t="s">
         <v>941</v>
       </c>
-      <c r="S314" s="26" t="s">
+      <c r="S314" s="23" t="s">
         <v>942</v>
       </c>
       <c r="T314" s="26" t="s">
@@ -16170,7 +16189,7 @@
       <c r="R315" s="13" t="s">
         <v>941</v>
       </c>
-      <c r="S315" s="26" t="s">
+      <c r="S315" s="23" t="s">
         <v>942</v>
       </c>
       <c r="T315" s="26" t="s">
@@ -16261,7 +16280,7 @@
       <c r="R316" s="13" t="s">
         <v>509</v>
       </c>
-      <c r="S316" s="26" t="s">
+      <c r="S316" s="13" t="s">
         <v>970</v>
       </c>
       <c r="T316" s="26" t="s">
@@ -17516,7 +17535,7 @@
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.11"/>
@@ -22082,7 +22101,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.72"/>
   </cols>
@@ -23734,7 +23753,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.89"/>
@@ -25102,7 +25121,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.99"/>

</xml_diff>

<commit_message>
Finally figured out the RCC stuff- it's just ascii formatted like HTML
</commit_message>
<xml_diff>
--- a/info/apinet_survey (2).xlsx
+++ b/info/apinet_survey (2).xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3574" uniqueCount="1199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3573" uniqueCount="1198">
   <si>
     <t xml:space="preserve">Host Species</t>
   </si>
@@ -2628,9 +2628,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE174036</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE158814</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE150039</t>
@@ -3688,7 +3685,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3782,13 +3779,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FFC9211E"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4243,11 +4233,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4315,19 +4305,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4427,11 +4417,11 @@
   </sheetPr>
   <dimension ref="A1:AK346"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M267" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P300" activeCellId="0" sqref="P300"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L307" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q313" activeCellId="0" sqref="Q313"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.12"/>
@@ -11293,7 +11283,7 @@
       <c r="P186" s="13" t="s">
         <v>544</v>
       </c>
-      <c r="Q186" s="27" t="s">
+      <c r="Q186" s="13" t="s">
         <v>545</v>
       </c>
       <c r="R186" s="11" t="s">
@@ -11365,7 +11355,7 @@
       <c r="P187" s="13" t="s">
         <v>544</v>
       </c>
-      <c r="Q187" s="27" t="s">
+      <c r="Q187" s="13" t="s">
         <v>545</v>
       </c>
       <c r="R187" s="11" t="s">
@@ -15374,13 +15364,13 @@
       <c r="Q295" s="46" t="s">
         <v>807</v>
       </c>
-      <c r="R295" s="27" t="s">
+      <c r="R295" s="13" t="s">
         <v>808</v>
       </c>
       <c r="S295" s="13" t="s">
         <v>809</v>
       </c>
-      <c r="T295" s="27" t="s">
+      <c r="T295" s="13" t="s">
         <v>810</v>
       </c>
       <c r="U295" s="11" t="s">
@@ -15594,7 +15584,7 @@
       <c r="P300" s="27" t="s">
         <v>834</v>
       </c>
-      <c r="Q300" s="27" t="s">
+      <c r="Q300" s="44" t="s">
         <v>813</v>
       </c>
       <c r="R300" s="13" t="s">
@@ -15661,17 +15651,17 @@
       <c r="O301" s="49" t="s">
         <v>848</v>
       </c>
-      <c r="P301" s="44" t="s">
+      <c r="P301" s="44" t="n">
+        <v>223804</v>
+      </c>
+      <c r="Q301" s="27" t="s">
         <v>849</v>
       </c>
-      <c r="Q301" s="27" t="s">
+      <c r="R301" s="13" t="s">
         <v>850</v>
       </c>
-      <c r="R301" s="13" t="s">
+      <c r="S301" s="13" t="s">
         <v>851</v>
-      </c>
-      <c r="S301" s="13" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15685,13 +15675,13 @@
         <v>27</v>
       </c>
       <c r="F302" s="42" t="s">
+        <v>852</v>
+      </c>
+      <c r="G302" s="0" t="s">
         <v>853</v>
       </c>
-      <c r="G302" s="0" t="s">
+      <c r="H302" s="0" t="s">
         <v>854</v>
-      </c>
-      <c r="H302" s="0" t="s">
-        <v>855</v>
       </c>
       <c r="I302" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H302,": '",F302,"',")</f>
@@ -15702,7 +15692,7 @@
         <v>'Shigella_sonnei': ['Fungi'],</v>
       </c>
       <c r="K302" s="8" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="L302" s="11" t="s">
         <v>812</v>
@@ -15721,13 +15711,13 @@
         <v>27</v>
       </c>
       <c r="F303" s="42" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="G303" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="H303" s="0" t="s">
         <v>857</v>
-      </c>
-      <c r="H303" s="0" t="s">
-        <v>858</v>
       </c>
       <c r="I303" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H303,": '",F303,"',")</f>
@@ -15738,7 +15728,7 @@
         <v>'Shigella_dysenteriae': ['Fungi'],</v>
       </c>
       <c r="K303" s="8" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="L303" s="11" t="s">
         <v>812</v>
@@ -15757,13 +15747,13 @@
         <v>27</v>
       </c>
       <c r="F304" s="42" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="G304" s="0" t="s">
+        <v>859</v>
+      </c>
+      <c r="H304" s="0" t="s">
         <v>860</v>
-      </c>
-      <c r="H304" s="0" t="s">
-        <v>861</v>
       </c>
       <c r="I304" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H304,": '",F304,"',")</f>
@@ -15774,7 +15764,7 @@
         <v>'Shigella_flexneri': ['Fungi'],</v>
       </c>
       <c r="K304" s="8" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="L304" s="10" t="s">
         <v>812</v>
@@ -15793,13 +15783,13 @@
         <v>27</v>
       </c>
       <c r="F305" s="0" t="s">
+        <v>862</v>
+      </c>
+      <c r="G305" s="0" t="s">
         <v>863</v>
       </c>
-      <c r="G305" s="0" t="s">
+      <c r="H305" s="0" t="s">
         <v>864</v>
-      </c>
-      <c r="H305" s="0" t="s">
-        <v>865</v>
       </c>
       <c r="I305" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H305,": '",F305,"',")</f>
@@ -15810,7 +15800,7 @@
         <v>'Treponema_pallidum': ['Fungi'],</v>
       </c>
       <c r="K305" s="8" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="L305" s="8"/>
     </row>
@@ -15825,13 +15815,13 @@
         <v>27</v>
       </c>
       <c r="F306" s="0" t="s">
+        <v>866</v>
+      </c>
+      <c r="G306" s="0" t="s">
         <v>867</v>
       </c>
-      <c r="G306" s="0" t="s">
+      <c r="H306" s="0" t="s">
         <v>868</v>
-      </c>
-      <c r="H306" s="0" t="s">
-        <v>869</v>
       </c>
       <c r="I306" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H306,": '",F306,"',")</f>
@@ -15842,7 +15832,7 @@
         <v>'Neisseria_gonorrhoeae': ['Fungi'],</v>
       </c>
       <c r="K306" s="8" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="L306" s="10" t="s">
         <v>846</v>
@@ -15864,7 +15854,7 @@
         <v>20</v>
       </c>
       <c r="F307" s="0" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="G307" s="0" t="s">
         <v>274</v>
@@ -15884,10 +15874,10 @@
         <v>276</v>
       </c>
       <c r="L307" s="10" t="s">
+        <v>871</v>
+      </c>
+      <c r="M307" s="13" t="s">
         <v>872</v>
-      </c>
-      <c r="M307" s="13" t="s">
-        <v>873</v>
       </c>
       <c r="N307" s="26"/>
     </row>
@@ -15902,13 +15892,13 @@
         <v>52</v>
       </c>
       <c r="F308" s="0" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="G308" s="0" t="s">
+        <v>873</v>
+      </c>
+      <c r="H308" s="0" t="s">
         <v>874</v>
-      </c>
-      <c r="H308" s="0" t="s">
-        <v>875</v>
       </c>
       <c r="I308" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H308,": '",F308,"',")</f>
@@ -15922,31 +15912,31 @@
         <v>482</v>
       </c>
       <c r="L308" s="35" t="s">
+        <v>875</v>
+      </c>
+      <c r="M308" s="13" t="s">
         <v>876</v>
       </c>
-      <c r="M308" s="13" t="s">
+      <c r="N308" s="13" t="s">
         <v>877</v>
       </c>
-      <c r="N308" s="13" t="s">
+      <c r="O308" s="13" t="s">
         <v>878</v>
       </c>
-      <c r="O308" s="13" t="s">
+      <c r="P308" s="13" t="s">
         <v>879</v>
       </c>
-      <c r="P308" s="13" t="s">
+      <c r="Q308" s="50" t="s">
         <v>880</v>
       </c>
-      <c r="Q308" s="50" t="s">
+      <c r="R308" s="13" t="s">
         <v>881</v>
       </c>
-      <c r="R308" s="13" t="s">
+      <c r="S308" s="13" t="s">
         <v>882</v>
       </c>
-      <c r="S308" s="13" t="s">
+      <c r="T308" s="13" t="s">
         <v>883</v>
-      </c>
-      <c r="T308" s="13" t="s">
-        <v>884</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15960,13 +15950,13 @@
         <v>52</v>
       </c>
       <c r="F309" s="0" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="G309" s="0" t="s">
+        <v>884</v>
+      </c>
+      <c r="H309" s="0" t="s">
         <v>885</v>
-      </c>
-      <c r="H309" s="0" t="s">
-        <v>886</v>
       </c>
       <c r="I309" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H309,": '",F309,"',")</f>
@@ -15977,7 +15967,7 @@
         <v>'Influenza_B': ['Fungi'],</v>
       </c>
       <c r="K309" s="8" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="L309" s="8"/>
       <c r="M309" s="7"/>
@@ -15994,13 +15984,13 @@
         <v>52</v>
       </c>
       <c r="F310" s="0" t="s">
+        <v>887</v>
+      </c>
+      <c r="G310" s="0" t="s">
         <v>888</v>
       </c>
-      <c r="G310" s="0" t="s">
+      <c r="H310" s="51" t="s">
         <v>889</v>
-      </c>
-      <c r="H310" s="51" t="s">
-        <v>890</v>
       </c>
       <c r="I310" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H310,": '",F310,"',")</f>
@@ -16011,67 +16001,67 @@
         <v>'SARS_CoV_2': ['Fungi'],</v>
       </c>
       <c r="K310" s="8" t="s">
+        <v>890</v>
+      </c>
+      <c r="L310" s="52" t="s">
+        <v>880</v>
+      </c>
+      <c r="M310" s="13" t="s">
         <v>891</v>
       </c>
-      <c r="L310" s="52" t="s">
-        <v>881</v>
-      </c>
-      <c r="M310" s="13" t="s">
+      <c r="N310" s="13" t="s">
         <v>892</v>
       </c>
-      <c r="N310" s="13" t="s">
+      <c r="P310" s="13" t="s">
         <v>893</v>
       </c>
-      <c r="P310" s="13" t="s">
+      <c r="Q310" s="13" t="s">
         <v>894</v>
       </c>
-      <c r="Q310" s="27" t="s">
+      <c r="R310" s="13" t="s">
         <v>895</v>
       </c>
-      <c r="R310" s="13" t="s">
+      <c r="S310" s="13" t="s">
         <v>896</v>
       </c>
-      <c r="S310" s="13" t="s">
+      <c r="T310" s="13" t="s">
         <v>897</v>
       </c>
-      <c r="T310" s="13" t="s">
+      <c r="U310" s="11" t="s">
         <v>898</v>
       </c>
-      <c r="U310" s="11" t="s">
+      <c r="V310" s="26" t="s">
         <v>899</v>
       </c>
-      <c r="V310" s="26" t="s">
+      <c r="W310" s="26" t="s">
         <v>900</v>
       </c>
-      <c r="W310" s="26" t="s">
+      <c r="X310" s="26" t="s">
         <v>901</v>
       </c>
-      <c r="X310" s="26" t="s">
+      <c r="Y310" s="26" t="s">
         <v>902</v>
       </c>
-      <c r="Y310" s="26" t="s">
+      <c r="Z310" s="24" t="s">
         <v>903</v>
       </c>
-      <c r="Z310" s="24" t="s">
+      <c r="AA310" s="26" t="s">
         <v>904</v>
       </c>
-      <c r="AA310" s="26" t="s">
+      <c r="AB310" s="26" t="s">
         <v>905</v>
       </c>
-      <c r="AB310" s="26" t="s">
+      <c r="AC310" s="26" t="s">
         <v>906</v>
       </c>
-      <c r="AC310" s="26" t="s">
+      <c r="AD310" s="26" t="s">
         <v>907</v>
       </c>
-      <c r="AD310" s="26" t="s">
+      <c r="AE310" s="53" t="s">
         <v>908</v>
       </c>
-      <c r="AE310" s="53" t="s">
+      <c r="AF310" s="26" t="s">
         <v>909</v>
-      </c>
-      <c r="AF310" s="26" t="s">
-        <v>910</v>
       </c>
       <c r="AK310" s="0" t="n">
         <v>80</v>
@@ -16088,13 +16078,13 @@
         <v>52</v>
       </c>
       <c r="F311" s="0" t="s">
+        <v>910</v>
+      </c>
+      <c r="G311" s="0" t="s">
         <v>911</v>
       </c>
-      <c r="G311" s="0" t="s">
+      <c r="H311" s="0" t="s">
         <v>912</v>
-      </c>
-      <c r="H311" s="0" t="s">
-        <v>913</v>
       </c>
       <c r="I311" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H311,": '",F311,"',")</f>
@@ -16105,10 +16095,10 @@
         <v>'Human_Immunodeficiency_Virus_1': ['Fungi'],</v>
       </c>
       <c r="K311" s="8" t="s">
+        <v>913</v>
+      </c>
+      <c r="L311" s="10" t="s">
         <v>914</v>
-      </c>
-      <c r="L311" s="10" t="s">
-        <v>915</v>
       </c>
       <c r="M311" s="7"/>
       <c r="N311" s="7"/>
@@ -16124,13 +16114,13 @@
         <v>52</v>
       </c>
       <c r="F312" s="0" t="s">
+        <v>915</v>
+      </c>
+      <c r="G312" s="0" t="s">
         <v>916</v>
       </c>
-      <c r="G312" s="0" t="s">
-        <v>917</v>
-      </c>
       <c r="H312" s="0" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="I312" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H312,": '",F312,"',")</f>
@@ -16141,26 +16131,26 @@
         <v>'Coxsackievirus': ['Fungi'],</v>
       </c>
       <c r="K312" s="8" t="s">
+        <v>917</v>
+      </c>
+      <c r="L312" s="52" t="s">
         <v>918</v>
       </c>
-      <c r="L312" s="52" t="s">
+      <c r="M312" s="13" t="s">
         <v>919</v>
       </c>
-      <c r="M312" s="13" t="s">
+      <c r="N312" s="13" t="s">
         <v>920</v>
-      </c>
-      <c r="N312" s="13" t="s">
-        <v>921</v>
       </c>
       <c r="O312" s="26"/>
       <c r="P312" s="13" t="s">
+        <v>921</v>
+      </c>
+      <c r="Q312" s="46" t="s">
         <v>922</v>
       </c>
-      <c r="Q312" s="46" t="s">
+      <c r="R312" s="13" t="s">
         <v>923</v>
-      </c>
-      <c r="R312" s="13" t="s">
-        <v>924</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16174,13 +16164,13 @@
         <v>52</v>
       </c>
       <c r="F313" s="0" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="G313" s="0" t="s">
+        <v>924</v>
+      </c>
+      <c r="H313" s="0" t="s">
         <v>925</v>
-      </c>
-      <c r="H313" s="0" t="s">
-        <v>926</v>
       </c>
       <c r="I313" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H313,": '",F313,"',")</f>
@@ -16191,16 +16181,16 @@
         <v>'Enterovirus_D68': ['Fungi'],</v>
       </c>
       <c r="K313" s="8" t="s">
+        <v>926</v>
+      </c>
+      <c r="L313" s="10" t="s">
         <v>927</v>
       </c>
-      <c r="L313" s="10" t="s">
+      <c r="M313" s="13" t="s">
         <v>928</v>
       </c>
-      <c r="M313" s="13" t="s">
+      <c r="N313" s="13" t="s">
         <v>929</v>
-      </c>
-      <c r="N313" s="13" t="s">
-        <v>930</v>
       </c>
       <c r="AC313" s="26"/>
     </row>
@@ -16215,13 +16205,13 @@
         <v>52</v>
       </c>
       <c r="F314" s="0" t="s">
+        <v>930</v>
+      </c>
+      <c r="G314" s="0" t="s">
         <v>931</v>
       </c>
-      <c r="G314" s="0" t="s">
+      <c r="H314" s="0" t="s">
         <v>932</v>
-      </c>
-      <c r="H314" s="0" t="s">
-        <v>933</v>
       </c>
       <c r="I314" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H314,": '",F314,"',")</f>
@@ -16232,67 +16222,67 @@
         <v>'Human_papillomavirus_16': ['Fungi'],</v>
       </c>
       <c r="K314" s="8" t="s">
+        <v>933</v>
+      </c>
+      <c r="L314" s="10" t="s">
         <v>934</v>
       </c>
-      <c r="L314" s="10" t="s">
+      <c r="M314" s="54" t="s">
         <v>935</v>
       </c>
-      <c r="M314" s="54" t="s">
+      <c r="N314" s="54" t="s">
         <v>936</v>
       </c>
-      <c r="N314" s="54" t="s">
+      <c r="O314" s="13" t="s">
         <v>937</v>
       </c>
-      <c r="O314" s="13" t="s">
+      <c r="P314" s="13" t="s">
         <v>938</v>
       </c>
-      <c r="P314" s="27" t="s">
+      <c r="Q314" s="27" t="s">
         <v>939</v>
       </c>
-      <c r="Q314" s="27" t="s">
+      <c r="R314" s="13" t="s">
         <v>940</v>
       </c>
-      <c r="R314" s="13" t="s">
+      <c r="S314" s="27" t="s">
         <v>941</v>
       </c>
-      <c r="S314" s="27" t="s">
+      <c r="T314" s="55" t="s">
         <v>942</v>
       </c>
-      <c r="T314" s="55" t="s">
+      <c r="U314" s="11" t="s">
         <v>943</v>
       </c>
-      <c r="U314" s="11" t="s">
+      <c r="V314" s="26" t="s">
         <v>944</v>
       </c>
-      <c r="V314" s="26" t="s">
+      <c r="W314" s="26" t="s">
         <v>945</v>
       </c>
-      <c r="W314" s="26" t="s">
+      <c r="X314" s="26" t="s">
         <v>946</v>
       </c>
-      <c r="X314" s="26" t="s">
+      <c r="Y314" s="26" t="s">
         <v>947</v>
       </c>
-      <c r="Y314" s="26" t="s">
+      <c r="Z314" s="24" t="s">
         <v>948</v>
       </c>
-      <c r="Z314" s="24" t="s">
+      <c r="AA314" s="26" t="s">
         <v>949</v>
       </c>
-      <c r="AA314" s="26" t="s">
+      <c r="AB314" s="26" t="s">
         <v>950</v>
       </c>
-      <c r="AB314" s="26" t="s">
+      <c r="AC314" s="26" t="s">
         <v>951</v>
       </c>
-      <c r="AC314" s="26" t="s">
+      <c r="AD314" s="26" t="s">
         <v>952</v>
       </c>
-      <c r="AD314" s="26" t="s">
+      <c r="AE314" s="53" t="s">
         <v>953</v>
-      </c>
-      <c r="AE314" s="53" t="s">
-        <v>954</v>
       </c>
       <c r="AK314" s="0" t="n">
         <v>120</v>
@@ -16309,13 +16299,13 @@
         <v>52</v>
       </c>
       <c r="F315" s="0" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="G315" s="0" t="s">
+        <v>954</v>
+      </c>
+      <c r="H315" s="0" t="s">
         <v>955</v>
-      </c>
-      <c r="H315" s="0" t="s">
-        <v>956</v>
       </c>
       <c r="I315" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H315,": '",F315,"',")</f>
@@ -16326,65 +16316,65 @@
         <v>'Human_papillomavirus_18': ['Fungi'],</v>
       </c>
       <c r="K315" s="8" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="L315" s="11" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="M315" s="8"/>
       <c r="N315" s="13" t="s">
+        <v>936</v>
+      </c>
+      <c r="O315" s="13" t="s">
         <v>937</v>
       </c>
-      <c r="O315" s="13" t="s">
+      <c r="P315" s="13" t="s">
         <v>938</v>
       </c>
-      <c r="P315" s="27" t="s">
+      <c r="Q315" s="27" t="s">
         <v>939</v>
       </c>
-      <c r="Q315" s="27" t="s">
+      <c r="R315" s="13" t="s">
         <v>940</v>
       </c>
-      <c r="R315" s="13" t="s">
+      <c r="S315" s="27" t="s">
         <v>941</v>
       </c>
-      <c r="S315" s="27" t="s">
+      <c r="T315" s="55" t="s">
         <v>942</v>
       </c>
-      <c r="T315" s="55" t="s">
+      <c r="U315" s="11" t="s">
         <v>943</v>
       </c>
-      <c r="U315" s="11" t="s">
+      <c r="V315" s="26" t="s">
         <v>944</v>
       </c>
-      <c r="V315" s="26" t="s">
+      <c r="W315" s="26" t="s">
         <v>945</v>
       </c>
-      <c r="W315" s="26" t="s">
+      <c r="X315" s="26" t="s">
         <v>946</v>
       </c>
-      <c r="X315" s="26" t="s">
+      <c r="Y315" s="26" t="s">
         <v>947</v>
       </c>
-      <c r="Y315" s="26" t="s">
+      <c r="Z315" s="24" t="s">
         <v>948</v>
       </c>
-      <c r="Z315" s="24" t="s">
+      <c r="AA315" s="26" t="s">
         <v>949</v>
       </c>
-      <c r="AA315" s="26" t="s">
+      <c r="AB315" s="26" t="s">
         <v>950</v>
       </c>
-      <c r="AB315" s="26" t="s">
+      <c r="AC315" s="26" t="s">
         <v>951</v>
       </c>
-      <c r="AC315" s="26" t="s">
-        <v>952</v>
-      </c>
       <c r="AD315" s="26" t="s">
+        <v>957</v>
+      </c>
+      <c r="AE315" s="53" t="s">
         <v>958</v>
-      </c>
-      <c r="AE315" s="53" t="s">
-        <v>959</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16398,13 +16388,13 @@
         <v>52</v>
       </c>
       <c r="F316" s="0" t="s">
+        <v>959</v>
+      </c>
+      <c r="G316" s="0" t="s">
         <v>960</v>
       </c>
-      <c r="G316" s="0" t="s">
+      <c r="H316" s="0" t="s">
         <v>961</v>
-      </c>
-      <c r="H316" s="0" t="s">
-        <v>962</v>
       </c>
       <c r="I316" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H316,": '",F316,"',")</f>
@@ -16415,55 +16405,55 @@
         <v>'Herpes_simplex_virus_1': ['Fungi'],</v>
       </c>
       <c r="K316" s="8" t="s">
+        <v>962</v>
+      </c>
+      <c r="L316" s="52" t="s">
         <v>963</v>
       </c>
-      <c r="L316" s="52" t="s">
+      <c r="M316" s="54" t="s">
         <v>964</v>
       </c>
-      <c r="M316" s="54" t="s">
+      <c r="N316" s="13" t="s">
         <v>965</v>
       </c>
-      <c r="N316" s="13" t="s">
+      <c r="O316" s="13" t="s">
         <v>966</v>
       </c>
-      <c r="O316" s="13" t="s">
+      <c r="P316" s="13" t="s">
         <v>967</v>
       </c>
-      <c r="P316" s="13" t="s">
+      <c r="Q316" s="13" t="s">
         <v>968</v>
-      </c>
-      <c r="Q316" s="13" t="s">
-        <v>969</v>
       </c>
       <c r="R316" s="13" t="s">
         <v>509</v>
       </c>
-      <c r="S316" s="27" t="s">
+      <c r="S316" s="13" t="s">
+        <v>969</v>
+      </c>
+      <c r="T316" s="13" t="s">
         <v>970</v>
       </c>
-      <c r="T316" s="13" t="s">
+      <c r="U316" s="11" t="s">
         <v>971</v>
       </c>
-      <c r="U316" s="11" t="s">
+      <c r="V316" s="26" t="s">
         <v>972</v>
       </c>
-      <c r="V316" s="26" t="s">
+      <c r="W316" s="26" t="s">
         <v>973</v>
       </c>
-      <c r="W316" s="26" t="s">
+      <c r="X316" s="26" t="s">
         <v>974</v>
       </c>
-      <c r="X316" s="26" t="s">
+      <c r="Y316" s="26" t="s">
         <v>975</v>
       </c>
-      <c r="Y316" s="26" t="s">
+      <c r="Z316" s="24" t="s">
         <v>976</v>
       </c>
-      <c r="Z316" s="24" t="s">
+      <c r="AA316" s="26" t="s">
         <v>977</v>
-      </c>
-      <c r="AA316" s="26" t="s">
-        <v>978</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16477,13 +16467,13 @@
         <v>52</v>
       </c>
       <c r="F317" s="0" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="G317" s="0" t="s">
+        <v>978</v>
+      </c>
+      <c r="H317" s="0" t="s">
         <v>979</v>
-      </c>
-      <c r="H317" s="0" t="s">
-        <v>980</v>
       </c>
       <c r="I317" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H317,": '",F317,"',")</f>
@@ -16494,13 +16484,13 @@
         <v>'Herpes_simplex_virus_2': ['Fungi'],</v>
       </c>
       <c r="K317" s="8" t="s">
+        <v>980</v>
+      </c>
+      <c r="L317" s="52" t="s">
+        <v>963</v>
+      </c>
+      <c r="M317" s="13" t="s">
         <v>981</v>
-      </c>
-      <c r="L317" s="52" t="s">
-        <v>964</v>
-      </c>
-      <c r="M317" s="13" t="s">
-        <v>982</v>
       </c>
       <c r="N317" s="26"/>
       <c r="P317" s="33"/>
@@ -16530,10 +16520,10 @@
         <v>511</v>
       </c>
       <c r="G318" s="0" t="s">
+        <v>982</v>
+      </c>
+      <c r="H318" s="0" t="s">
         <v>983</v>
-      </c>
-      <c r="H318" s="0" t="s">
-        <v>984</v>
       </c>
       <c r="I318" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H318,": '",F318,"',")</f>
@@ -16544,13 +16534,13 @@
         <v>'Human_rotavirus_A': ['Fungi'],</v>
       </c>
       <c r="K318" s="8" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="L318" s="11" t="s">
         <v>812</v>
       </c>
       <c r="M318" s="54" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="O318" s="26"/>
       <c r="P318" s="33"/>
@@ -16573,10 +16563,10 @@
         <v>511</v>
       </c>
       <c r="G319" s="56" t="s">
+        <v>986</v>
+      </c>
+      <c r="H319" s="56" t="s">
         <v>987</v>
-      </c>
-      <c r="H319" s="56" t="s">
-        <v>988</v>
       </c>
       <c r="I319" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H319,": '",F319,"',")</f>
@@ -16609,10 +16599,10 @@
         <v>511</v>
       </c>
       <c r="G320" s="0" t="s">
+        <v>988</v>
+      </c>
+      <c r="H320" s="0" t="s">
         <v>989</v>
-      </c>
-      <c r="H320" s="0" t="s">
-        <v>990</v>
       </c>
       <c r="I320" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H320,": '",F320,"',")</f>
@@ -16623,7 +16613,7 @@
         <v>'Human_rotavirus_C': ['Fungi'],</v>
       </c>
       <c r="K320" s="8" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="L320" s="11" t="s">
         <v>812</v>
@@ -16642,13 +16632,13 @@
         <v>52</v>
       </c>
       <c r="F321" s="0" t="s">
+        <v>991</v>
+      </c>
+      <c r="G321" s="0" t="s">
         <v>992</v>
       </c>
-      <c r="G321" s="0" t="s">
+      <c r="H321" s="0" t="s">
         <v>993</v>
-      </c>
-      <c r="H321" s="0" t="s">
-        <v>994</v>
       </c>
       <c r="I321" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H321,": '",F321,"',")</f>
@@ -16659,25 +16649,25 @@
         <v>'Varicella_zoster_virus_Human_alphaherpesvirus_3': ['Fungi'],</v>
       </c>
       <c r="K321" s="8" t="s">
+        <v>994</v>
+      </c>
+      <c r="L321" s="10" t="s">
         <v>995</v>
       </c>
-      <c r="L321" s="10" t="s">
+      <c r="M321" s="13" t="s">
         <v>996</v>
       </c>
-      <c r="M321" s="13" t="s">
+      <c r="N321" s="13" t="s">
         <v>997</v>
       </c>
-      <c r="N321" s="13" t="s">
+      <c r="O321" s="13" t="s">
         <v>998</v>
       </c>
-      <c r="O321" s="13" t="s">
+      <c r="P321" s="57" t="s">
         <v>999</v>
       </c>
-      <c r="P321" s="57" t="s">
+      <c r="Q321" s="13" t="s">
         <v>1000</v>
-      </c>
-      <c r="Q321" s="13" t="s">
-        <v>1001</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16691,13 +16681,13 @@
         <v>52</v>
       </c>
       <c r="F322" s="0" t="s">
+        <v>1001</v>
+      </c>
+      <c r="G322" s="0" t="s">
         <v>1002</v>
       </c>
-      <c r="G322" s="0" t="s">
+      <c r="H322" s="0" t="s">
         <v>1003</v>
-      </c>
-      <c r="H322" s="0" t="s">
-        <v>1004</v>
       </c>
       <c r="I322" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H322,": '",F322,"',")</f>
@@ -16708,13 +16698,13 @@
         <v>'Norovirus_GI': ['Fungi'],</v>
       </c>
       <c r="K322" s="8" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="L322" s="10" t="s">
         <v>812</v>
       </c>
       <c r="M322" s="13" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="N322" s="7"/>
     </row>
@@ -16729,13 +16719,13 @@
         <v>52</v>
       </c>
       <c r="F323" s="0" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="G323" s="0" t="s">
+        <v>1006</v>
+      </c>
+      <c r="H323" s="0" t="s">
         <v>1007</v>
-      </c>
-      <c r="H323" s="0" t="s">
-        <v>1008</v>
       </c>
       <c r="I323" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H323,": '",F323,"',")</f>
@@ -16746,13 +16736,13 @@
         <v>'Norovirus_GV': ['Fungi'],</v>
       </c>
       <c r="K323" s="8" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="L323" s="11" t="s">
         <v>812</v>
       </c>
       <c r="M323" s="54" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="N323" s="7"/>
     </row>
@@ -16767,13 +16757,13 @@
         <v>52</v>
       </c>
       <c r="F324" s="0" t="s">
+        <v>1009</v>
+      </c>
+      <c r="G324" s="0" t="s">
         <v>1010</v>
       </c>
-      <c r="G324" s="0" t="s">
+      <c r="H324" s="0" t="s">
         <v>1011</v>
-      </c>
-      <c r="H324" s="0" t="s">
-        <v>1012</v>
       </c>
       <c r="I324" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H324,": '",F324,"',")</f>
@@ -16784,7 +16774,7 @@
         <v>'Hepatovirus_A': ['Fungi'],</v>
       </c>
       <c r="K324" s="8" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="L324" s="8"/>
       <c r="M324" s="7"/>
@@ -16801,13 +16791,13 @@
         <v>52</v>
       </c>
       <c r="F325" s="0" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G325" s="0" t="s">
         <v>1014</v>
       </c>
-      <c r="G325" s="0" t="s">
+      <c r="H325" s="0" t="s">
         <v>1015</v>
-      </c>
-      <c r="H325" s="0" t="s">
-        <v>1016</v>
       </c>
       <c r="I325" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H325,": '",F325,"',")</f>
@@ -16818,67 +16808,67 @@
         <v>'Hepatovirus_B': ['Fungi'],</v>
       </c>
       <c r="K325" s="8" t="s">
+        <v>1016</v>
+      </c>
+      <c r="L325" s="11" t="s">
         <v>1017</v>
       </c>
-      <c r="L325" s="11" t="s">
+      <c r="M325" s="58" t="s">
         <v>1018</v>
       </c>
-      <c r="M325" s="58" t="s">
+      <c r="N325" s="13" t="s">
         <v>1019</v>
       </c>
-      <c r="N325" s="13" t="s">
+      <c r="O325" s="13" t="s">
         <v>1020</v>
       </c>
-      <c r="O325" s="13" t="s">
+      <c r="P325" s="13" t="s">
         <v>1021</v>
       </c>
-      <c r="P325" s="13" t="s">
+      <c r="Q325" s="13" t="s">
         <v>1022</v>
       </c>
-      <c r="Q325" s="27" t="s">
+      <c r="R325" s="13" t="s">
         <v>1023</v>
       </c>
-      <c r="R325" s="13" t="s">
+      <c r="S325" s="58" t="s">
         <v>1024</v>
       </c>
-      <c r="S325" s="58" t="s">
+      <c r="T325" s="13" t="s">
         <v>1025</v>
       </c>
-      <c r="T325" s="13" t="s">
+      <c r="U325" s="11" t="s">
         <v>1026</v>
       </c>
-      <c r="U325" s="11" t="s">
+      <c r="V325" s="26" t="s">
         <v>1027</v>
       </c>
-      <c r="V325" s="26" t="s">
+      <c r="W325" s="26" t="s">
         <v>1028</v>
       </c>
-      <c r="W325" s="26" t="s">
+      <c r="X325" s="26" t="s">
         <v>1029</v>
       </c>
-      <c r="X325" s="26" t="s">
+      <c r="Y325" s="26" t="s">
         <v>1030</v>
       </c>
-      <c r="Y325" s="26" t="s">
+      <c r="Z325" s="24" t="s">
         <v>1031</v>
       </c>
-      <c r="Z325" s="24" t="s">
+      <c r="AA325" s="26" t="s">
         <v>1032</v>
       </c>
-      <c r="AA325" s="26" t="s">
+      <c r="AB325" s="26" t="s">
         <v>1033</v>
       </c>
-      <c r="AB325" s="26" t="s">
+      <c r="AC325" s="26" t="s">
         <v>1034</v>
       </c>
-      <c r="AC325" s="26" t="s">
+      <c r="AD325" s="26" t="s">
         <v>1035</v>
       </c>
-      <c r="AD325" s="26" t="s">
+      <c r="AE325" s="53" t="s">
         <v>1036</v>
-      </c>
-      <c r="AE325" s="53" t="s">
-        <v>1037</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16892,13 +16882,13 @@
         <v>52</v>
       </c>
       <c r="F326" s="0" t="s">
+        <v>1037</v>
+      </c>
+      <c r="G326" s="0" t="s">
         <v>1038</v>
       </c>
-      <c r="G326" s="0" t="s">
+      <c r="H326" s="0" t="s">
         <v>1039</v>
-      </c>
-      <c r="H326" s="0" t="s">
-        <v>1040</v>
       </c>
       <c r="I326" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("Human_",H326,": '",F326,"',")</f>
@@ -16909,52 +16899,52 @@
         <v>'Hepatovirus_C': ['Fungi'],</v>
       </c>
       <c r="K326" s="8" t="s">
+        <v>1040</v>
+      </c>
+      <c r="L326" s="11" t="s">
+        <v>1017</v>
+      </c>
+      <c r="M326" s="13" t="s">
         <v>1041</v>
       </c>
-      <c r="L326" s="11" t="s">
-        <v>1018</v>
-      </c>
-      <c r="M326" s="13" t="s">
+      <c r="N326" s="44" t="s">
         <v>1042</v>
       </c>
-      <c r="N326" s="44" t="s">
+      <c r="O326" s="13" t="s">
         <v>1043</v>
       </c>
-      <c r="O326" s="13" t="s">
+      <c r="P326" s="43" t="s">
         <v>1044</v>
       </c>
-      <c r="P326" s="43" t="s">
+      <c r="Q326" s="13" t="s">
         <v>1045</v>
       </c>
-      <c r="Q326" s="13" t="s">
+      <c r="R326" s="55" t="s">
         <v>1046</v>
       </c>
-      <c r="R326" s="55" t="s">
+      <c r="S326" s="13" t="s">
         <v>1047</v>
       </c>
-      <c r="S326" s="13" t="s">
+      <c r="T326" s="59" t="s">
+        <v>1044</v>
+      </c>
+      <c r="U326" s="11" t="s">
         <v>1048</v>
       </c>
-      <c r="T326" s="59" t="s">
-        <v>1045</v>
-      </c>
-      <c r="U326" s="11" t="s">
+      <c r="V326" s="26" t="s">
         <v>1049</v>
       </c>
-      <c r="V326" s="26" t="s">
+      <c r="W326" s="26" t="s">
         <v>1050</v>
       </c>
-      <c r="W326" s="26" t="s">
+      <c r="X326" s="26" t="s">
         <v>1051</v>
       </c>
-      <c r="X326" s="26" t="s">
+      <c r="Y326" s="26" t="s">
         <v>1052</v>
       </c>
-      <c r="Y326" s="26" t="s">
+      <c r="Z326" s="24" t="s">
         <v>1053</v>
-      </c>
-      <c r="Z326" s="24" t="s">
-        <v>1054</v>
       </c>
       <c r="AE326" s="53"/>
     </row>
@@ -16971,115 +16961,115 @@
       <c r="B330" s="60"/>
       <c r="D330" s="1"/>
       <c r="E330" s="0" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D331" s="4"/>
       <c r="E331" s="0" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L331" s="61"/>
       <c r="M331" s="0" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D332" s="62"/>
       <c r="E332" s="0" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="L332" s="31"/>
       <c r="M332" s="0" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D333" s="63"/>
       <c r="E333" s="0" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="L333" s="2"/>
       <c r="M333" s="0" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L334" s="64"/>
       <c r="M334" s="0" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L335" s="65"/>
       <c r="M335" s="0" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L336" s="66"/>
       <c r="M336" s="0" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L337" s="67"/>
       <c r="M337" s="0" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L338" s="68"/>
       <c r="M338" s="0" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L339" s="69"/>
       <c r="M339" s="0" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L340" s="70"/>
       <c r="M340" s="0" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L341" s="71"/>
       <c r="M341" s="0" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L342" s="72"/>
       <c r="M342" s="0" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L343" s="73"/>
       <c r="M343" s="0" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L344" s="74"/>
       <c r="M344" s="0" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L345" s="75"/>
       <c r="M345" s="0" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L346" s="76"/>
       <c r="M346" s="0" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
   </sheetData>
@@ -17526,186 +17516,185 @@
     <hyperlink ref="M301" r:id="rId434" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE120192"/>
     <hyperlink ref="N301" r:id="rId435" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE180784"/>
     <hyperlink ref="O301" r:id="rId436" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE174036"/>
-    <hyperlink ref="P301" r:id="rId437" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE158814"/>
-    <hyperlink ref="Q301" r:id="rId438" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE150039"/>
-    <hyperlink ref="R301" r:id="rId439" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE133358"/>
-    <hyperlink ref="S301" r:id="rId440" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE132525"/>
-    <hyperlink ref="K302" r:id="rId441" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0133748151/"/>
-    <hyperlink ref="L302" r:id="rId442" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE69529"/>
-    <hyperlink ref="K303" r:id="rId443" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0223540851/"/>
-    <hyperlink ref="L303" r:id="rId444" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE69529"/>
-    <hyperlink ref="K304" r:id="rId445" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0000069252/"/>
-    <hyperlink ref="L304" r:id="rId446" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE69529"/>
-    <hyperlink ref="K305" r:id="rId447" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0002467551/"/>
-    <hyperlink ref="K306" r:id="rId448" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0130300751/"/>
-    <hyperlink ref="L306" r:id="rId449" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE120192"/>
-    <hyperlink ref="K307" r:id="rId450" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008650851/"/>
-    <hyperlink ref="L307" r:id="rId451" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE244959"/>
-    <hyperlink ref="M307" r:id="rId452" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE186299"/>
-    <hyperlink ref="K308" r:id="rId453" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0013437851/"/>
-    <hyperlink ref="L308" r:id="rId454" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE224094"/>
-    <hyperlink ref="M308" r:id="rId455" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE186908"/>
-    <hyperlink ref="N308" r:id="rId456" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE165340"/>
-    <hyperlink ref="O308" r:id="rId457" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE156152"/>
-    <hyperlink ref="P308" r:id="rId458" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE156060"/>
-    <hyperlink ref="Q308" r:id="rId459" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE147507"/>
-    <hyperlink ref="R308" r:id="rId460" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE103604"/>
-    <hyperlink ref="S308" r:id="rId461" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE99079"/>
-    <hyperlink ref="T308" r:id="rId462" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE101760"/>
-    <hyperlink ref="K309" r:id="rId463" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008204952/"/>
-    <hyperlink ref="K310" r:id="rId464" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0098588952/"/>
-    <hyperlink ref="L310" r:id="rId465" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE147507"/>
-    <hyperlink ref="M310" r:id="rId466" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE167410"/>
-    <hyperlink ref="N310" r:id="rId467" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE255647"/>
-    <hyperlink ref="P310" r:id="rId468" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE266907"/>
-    <hyperlink ref="Q310" r:id="rId469" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE240766"/>
-    <hyperlink ref="R310" r:id="rId470" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE212861"/>
-    <hyperlink ref="S310" r:id="rId471" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE274964"/>
-    <hyperlink ref="T310" r:id="rId472" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE207981"/>
-    <hyperlink ref="U310" r:id="rId473" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE208587"/>
-    <hyperlink ref="V310" r:id="rId474" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE243217"/>
-    <hyperlink ref="W310" r:id="rId475" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE239595"/>
-    <hyperlink ref="X310" r:id="rId476" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE272381"/>
-    <hyperlink ref="Y310" r:id="rId477" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE178333"/>
-    <hyperlink ref="Z310" r:id="rId478" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE233943"/>
-    <hyperlink ref="AA310" r:id="rId479" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE202553"/>
-    <hyperlink ref="AB310" r:id="rId480" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE243268"/>
-    <hyperlink ref="AC310" r:id="rId481" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE252508"/>
-    <hyperlink ref="AD310" r:id="rId482" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE261002"/>
-    <hyperlink ref="AE310" r:id="rId483" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE236841"/>
-    <hyperlink ref="AF310" r:id="rId484" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE233557"/>
-    <hyperlink ref="K311" r:id="rId485" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008647651/"/>
-    <hyperlink ref="L311" r:id="rId486" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE235038"/>
-    <hyperlink ref="K312" r:id="rId487" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0088006151/"/>
-    <hyperlink ref="L312" r:id="rId488" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE262649"/>
-    <hyperlink ref="M312" r:id="rId489" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE269413"/>
-    <hyperlink ref="N312" r:id="rId490" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE278756"/>
-    <hyperlink ref="P312" r:id="rId491" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE184831"/>
-    <hyperlink ref="Q312" r:id="rId492" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE145074"/>
-    <hyperlink ref="R312" r:id="rId493" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE136734"/>
-    <hyperlink ref="K313" r:id="rId494" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0028167251/"/>
-    <hyperlink ref="L313" r:id="rId495" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE184488"/>
-    <hyperlink ref="M313" r:id="rId496" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE155925"/>
-    <hyperlink ref="N313" r:id="rId497" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE133378"/>
-    <hyperlink ref="K314" r:id="rId498" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008639453/"/>
-    <hyperlink ref="L314" r:id="rId499" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE235223"/>
-    <hyperlink ref="M314" r:id="rId500" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE226754"/>
-    <hyperlink ref="N314" r:id="rId501" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE250305"/>
-    <hyperlink ref="O314" r:id="rId502" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE205308"/>
-    <hyperlink ref="P314" r:id="rId503" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE223804"/>
-    <hyperlink ref="Q314" r:id="rId504" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE174317"/>
-    <hyperlink ref="R314" r:id="rId505" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE198100"/>
-    <hyperlink ref="S314" r:id="rId506" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE199029"/>
-    <hyperlink ref="T314" r:id="rId507" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE183454"/>
-    <hyperlink ref="U314" r:id="rId508" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE190222"/>
-    <hyperlink ref="V314" r:id="rId509" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE168244"/>
-    <hyperlink ref="W314" r:id="rId510" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE165883"/>
-    <hyperlink ref="X314" r:id="rId511" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE142482"/>
-    <hyperlink ref="Y314" r:id="rId512" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE153966"/>
-    <hyperlink ref="Z314" r:id="rId513" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE113942"/>
-    <hyperlink ref="AA314" r:id="rId514" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE123029"/>
-    <hyperlink ref="AB314" r:id="rId515" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE122512"/>
-    <hyperlink ref="AC314" r:id="rId516" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE122018"/>
-    <hyperlink ref="AD314" r:id="rId517" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE161875"/>
-    <hyperlink ref="AE314" r:id="rId518" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE240750"/>
-    <hyperlink ref="K315" r:id="rId519" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008656651/"/>
-    <hyperlink ref="L315" r:id="rId520" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE235223"/>
-    <hyperlink ref="N315" r:id="rId521" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE250305"/>
-    <hyperlink ref="O315" r:id="rId522" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE205308"/>
-    <hyperlink ref="P315" r:id="rId523" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE223804"/>
-    <hyperlink ref="Q315" r:id="rId524" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE174317"/>
-    <hyperlink ref="R315" r:id="rId525" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE198100"/>
-    <hyperlink ref="S315" r:id="rId526" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE199029"/>
-    <hyperlink ref="T315" r:id="rId527" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE183454"/>
-    <hyperlink ref="U315" r:id="rId528" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE190222"/>
-    <hyperlink ref="V315" r:id="rId529" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE168244"/>
-    <hyperlink ref="W315" r:id="rId530" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE165883"/>
-    <hyperlink ref="X315" r:id="rId531" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE142482"/>
-    <hyperlink ref="Y315" r:id="rId532" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE153966"/>
-    <hyperlink ref="Z315" r:id="rId533" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE113942"/>
-    <hyperlink ref="AA315" r:id="rId534" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE123029"/>
-    <hyperlink ref="AB315" r:id="rId535" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE122512"/>
-    <hyperlink ref="AC315" r:id="rId536" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE122018"/>
-    <hyperlink ref="AD315" r:id="rId537" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE249929"/>
-    <hyperlink ref="AE315" r:id="rId538" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE261673"/>
-    <hyperlink ref="K316" r:id="rId539" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008599852/"/>
-    <hyperlink ref="L316" r:id="rId540" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE208078"/>
-    <hyperlink ref="M316" r:id="rId541" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE272361"/>
-    <hyperlink ref="N316" r:id="rId542" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE287622"/>
-    <hyperlink ref="O316" r:id="rId543" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE209632"/>
-    <hyperlink ref="P316" r:id="rId544" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE234489"/>
-    <hyperlink ref="Q316" r:id="rId545" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE185239"/>
-    <hyperlink ref="R316" r:id="rId546" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE201012"/>
-    <hyperlink ref="S316" r:id="rId547" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE196269"/>
-    <hyperlink ref="T316" r:id="rId548" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE124118"/>
-    <hyperlink ref="U316" r:id="rId549" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE145496"/>
-    <hyperlink ref="V316" r:id="rId550" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE140068"/>
-    <hyperlink ref="W316" r:id="rId551" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE129715"/>
-    <hyperlink ref="X316" r:id="rId552" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE151912"/>
-    <hyperlink ref="Y316" r:id="rId553" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE120891"/>
-    <hyperlink ref="Z316" r:id="rId554" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE101435"/>
-    <hyperlink ref="AA316" r:id="rId555" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE95623"/>
-    <hyperlink ref="K317" r:id="rId556" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008583852/"/>
-    <hyperlink ref="L317" r:id="rId557" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE208078"/>
-    <hyperlink ref="M317" r:id="rId558" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE241702"/>
-    <hyperlink ref="K318" r:id="rId559" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCA_0026413751/"/>
-    <hyperlink ref="L318" r:id="rId560" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE69529"/>
-    <hyperlink ref="M318" r:id="rId561" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE90796"/>
-    <hyperlink ref="K319" r:id="rId562" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0009078351/"/>
-    <hyperlink ref="L319" r:id="rId563" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE69529"/>
-    <hyperlink ref="K320" r:id="rId564" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCA_0030876351/"/>
-    <hyperlink ref="L320" r:id="rId565" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE69529"/>
-    <hyperlink ref="K321" r:id="rId566" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008582851/"/>
-    <hyperlink ref="L321" r:id="rId567" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE242252"/>
-    <hyperlink ref="M321" r:id="rId568" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE141932"/>
-    <hyperlink ref="N321" r:id="rId569" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE130633"/>
-    <hyperlink ref="O321" r:id="rId570" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE206641"/>
-    <hyperlink ref="P321" r:id="rId571" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE223957"/>
-    <hyperlink ref="Q321" r:id="rId572" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE174694"/>
-    <hyperlink ref="K322" r:id="rId573" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008640051/"/>
-    <hyperlink ref="L322" r:id="rId574" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE69529"/>
-    <hyperlink ref="M322" r:id="rId575" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE205007"/>
-    <hyperlink ref="K323" r:id="rId576" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008684251/"/>
-    <hyperlink ref="L323" r:id="rId577" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE69529"/>
-    <hyperlink ref="M323" r:id="rId578" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE205007"/>
-    <hyperlink ref="K324" r:id="rId579" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008605051/"/>
-    <hyperlink ref="K325" r:id="rId580" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0030330551/"/>
-    <hyperlink ref="L325" r:id="rId581" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE250153"/>
-    <hyperlink ref="M325" r:id="rId582" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE159644"/>
-    <hyperlink ref="N325" r:id="rId583" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE208535"/>
-    <hyperlink ref="O325" r:id="rId584" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE208637"/>
-    <hyperlink ref="P325" r:id="rId585" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE198946"/>
-    <hyperlink ref="Q325" r:id="rId586" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE233661"/>
-    <hyperlink ref="R325" r:id="rId587" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE186178"/>
-    <hyperlink ref="S325" r:id="rId588" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE65389"/>
-    <hyperlink ref="T325" r:id="rId589" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE112118"/>
-    <hyperlink ref="U325" r:id="rId590" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE153946"/>
-    <hyperlink ref="V325" r:id="rId591" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE110345"/>
-    <hyperlink ref="W325" r:id="rId592" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE165727"/>
-    <hyperlink ref="X325" r:id="rId593" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE183156"/>
-    <hyperlink ref="Y325" r:id="rId594" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE194179"/>
-    <hyperlink ref="Z325" r:id="rId595" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE169110"/>
-    <hyperlink ref="AA325" r:id="rId596" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE224901"/>
-    <hyperlink ref="AB325" r:id="rId597" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE217838"/>
-    <hyperlink ref="AC325" r:id="rId598" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE260966"/>
-    <hyperlink ref="AD325" r:id="rId599" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE274114"/>
-    <hyperlink ref="AE325" r:id="rId600" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE288077"/>
-    <hyperlink ref="K326" r:id="rId601" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008618451/"/>
-    <hyperlink ref="L326" r:id="rId602" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE250153"/>
-    <hyperlink ref="M326" r:id="rId603" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE82177"/>
-    <hyperlink ref="N326" r:id="rId604" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE136339"/>
-    <hyperlink ref="O326" r:id="rId605" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE149601"/>
-    <hyperlink ref="P326" r:id="rId606" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE132548"/>
-    <hyperlink ref="Q326" r:id="rId607" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE206397"/>
-    <hyperlink ref="R326" r:id="rId608" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE185700"/>
-    <hyperlink ref="S326" r:id="rId609" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE234572"/>
-    <hyperlink ref="T326" r:id="rId610" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE132548"/>
-    <hyperlink ref="U326" r:id="rId611" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE163239"/>
-    <hyperlink ref="V326" r:id="rId612" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE119117"/>
-    <hyperlink ref="W326" r:id="rId613" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE132606"/>
-    <hyperlink ref="X326" r:id="rId614" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE212871"/>
-    <hyperlink ref="Y326" r:id="rId615" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE267834"/>
-    <hyperlink ref="Z326" r:id="rId616" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE84346"/>
+    <hyperlink ref="Q301" r:id="rId437" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE150039"/>
+    <hyperlink ref="R301" r:id="rId438" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE133358"/>
+    <hyperlink ref="S301" r:id="rId439" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE132525"/>
+    <hyperlink ref="K302" r:id="rId440" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0133748151/"/>
+    <hyperlink ref="L302" r:id="rId441" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE69529"/>
+    <hyperlink ref="K303" r:id="rId442" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0223540851/"/>
+    <hyperlink ref="L303" r:id="rId443" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE69529"/>
+    <hyperlink ref="K304" r:id="rId444" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0000069252/"/>
+    <hyperlink ref="L304" r:id="rId445" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE69529"/>
+    <hyperlink ref="K305" r:id="rId446" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0002467551/"/>
+    <hyperlink ref="K306" r:id="rId447" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0130300751/"/>
+    <hyperlink ref="L306" r:id="rId448" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE120192"/>
+    <hyperlink ref="K307" r:id="rId449" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008650851/"/>
+    <hyperlink ref="L307" r:id="rId450" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE244959"/>
+    <hyperlink ref="M307" r:id="rId451" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE186299"/>
+    <hyperlink ref="K308" r:id="rId452" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0013437851/"/>
+    <hyperlink ref="L308" r:id="rId453" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE224094"/>
+    <hyperlink ref="M308" r:id="rId454" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE186908"/>
+    <hyperlink ref="N308" r:id="rId455" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE165340"/>
+    <hyperlink ref="O308" r:id="rId456" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE156152"/>
+    <hyperlink ref="P308" r:id="rId457" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE156060"/>
+    <hyperlink ref="Q308" r:id="rId458" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE147507"/>
+    <hyperlink ref="R308" r:id="rId459" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE103604"/>
+    <hyperlink ref="S308" r:id="rId460" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE99079"/>
+    <hyperlink ref="T308" r:id="rId461" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE101760"/>
+    <hyperlink ref="K309" r:id="rId462" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008204952/"/>
+    <hyperlink ref="K310" r:id="rId463" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0098588952/"/>
+    <hyperlink ref="L310" r:id="rId464" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE147507"/>
+    <hyperlink ref="M310" r:id="rId465" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE167410"/>
+    <hyperlink ref="N310" r:id="rId466" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE255647"/>
+    <hyperlink ref="P310" r:id="rId467" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE266907"/>
+    <hyperlink ref="Q310" r:id="rId468" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE240766"/>
+    <hyperlink ref="R310" r:id="rId469" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE212861"/>
+    <hyperlink ref="S310" r:id="rId470" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE274964"/>
+    <hyperlink ref="T310" r:id="rId471" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE207981"/>
+    <hyperlink ref="U310" r:id="rId472" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE208587"/>
+    <hyperlink ref="V310" r:id="rId473" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE243217"/>
+    <hyperlink ref="W310" r:id="rId474" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE239595"/>
+    <hyperlink ref="X310" r:id="rId475" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE272381"/>
+    <hyperlink ref="Y310" r:id="rId476" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE178333"/>
+    <hyperlink ref="Z310" r:id="rId477" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE233943"/>
+    <hyperlink ref="AA310" r:id="rId478" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE202553"/>
+    <hyperlink ref="AB310" r:id="rId479" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE243268"/>
+    <hyperlink ref="AC310" r:id="rId480" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE252508"/>
+    <hyperlink ref="AD310" r:id="rId481" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE261002"/>
+    <hyperlink ref="AE310" r:id="rId482" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE236841"/>
+    <hyperlink ref="AF310" r:id="rId483" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE233557"/>
+    <hyperlink ref="K311" r:id="rId484" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008647651/"/>
+    <hyperlink ref="L311" r:id="rId485" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE235038"/>
+    <hyperlink ref="K312" r:id="rId486" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0088006151/"/>
+    <hyperlink ref="L312" r:id="rId487" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE262649"/>
+    <hyperlink ref="M312" r:id="rId488" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE269413"/>
+    <hyperlink ref="N312" r:id="rId489" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE278756"/>
+    <hyperlink ref="P312" r:id="rId490" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE184831"/>
+    <hyperlink ref="Q312" r:id="rId491" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE145074"/>
+    <hyperlink ref="R312" r:id="rId492" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE136734"/>
+    <hyperlink ref="K313" r:id="rId493" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0028167251/"/>
+    <hyperlink ref="L313" r:id="rId494" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE184488"/>
+    <hyperlink ref="M313" r:id="rId495" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE155925"/>
+    <hyperlink ref="N313" r:id="rId496" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE133378"/>
+    <hyperlink ref="K314" r:id="rId497" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008639453/"/>
+    <hyperlink ref="L314" r:id="rId498" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE235223"/>
+    <hyperlink ref="M314" r:id="rId499" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE226754"/>
+    <hyperlink ref="N314" r:id="rId500" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE250305"/>
+    <hyperlink ref="O314" r:id="rId501" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE205308"/>
+    <hyperlink ref="P314" r:id="rId502" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE223804"/>
+    <hyperlink ref="Q314" r:id="rId503" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE174317"/>
+    <hyperlink ref="R314" r:id="rId504" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE198100"/>
+    <hyperlink ref="S314" r:id="rId505" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE199029"/>
+    <hyperlink ref="T314" r:id="rId506" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE183454"/>
+    <hyperlink ref="U314" r:id="rId507" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE190222"/>
+    <hyperlink ref="V314" r:id="rId508" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE168244"/>
+    <hyperlink ref="W314" r:id="rId509" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE165883"/>
+    <hyperlink ref="X314" r:id="rId510" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE142482"/>
+    <hyperlink ref="Y314" r:id="rId511" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE153966"/>
+    <hyperlink ref="Z314" r:id="rId512" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE113942"/>
+    <hyperlink ref="AA314" r:id="rId513" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE123029"/>
+    <hyperlink ref="AB314" r:id="rId514" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE122512"/>
+    <hyperlink ref="AC314" r:id="rId515" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE122018"/>
+    <hyperlink ref="AD314" r:id="rId516" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE161875"/>
+    <hyperlink ref="AE314" r:id="rId517" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE240750"/>
+    <hyperlink ref="K315" r:id="rId518" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008656651/"/>
+    <hyperlink ref="L315" r:id="rId519" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE235223"/>
+    <hyperlink ref="N315" r:id="rId520" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE250305"/>
+    <hyperlink ref="O315" r:id="rId521" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE205308"/>
+    <hyperlink ref="P315" r:id="rId522" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE223804"/>
+    <hyperlink ref="Q315" r:id="rId523" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE174317"/>
+    <hyperlink ref="R315" r:id="rId524" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE198100"/>
+    <hyperlink ref="S315" r:id="rId525" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE199029"/>
+    <hyperlink ref="T315" r:id="rId526" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE183454"/>
+    <hyperlink ref="U315" r:id="rId527" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE190222"/>
+    <hyperlink ref="V315" r:id="rId528" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE168244"/>
+    <hyperlink ref="W315" r:id="rId529" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE165883"/>
+    <hyperlink ref="X315" r:id="rId530" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE142482"/>
+    <hyperlink ref="Y315" r:id="rId531" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE153966"/>
+    <hyperlink ref="Z315" r:id="rId532" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE113942"/>
+    <hyperlink ref="AA315" r:id="rId533" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE123029"/>
+    <hyperlink ref="AB315" r:id="rId534" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE122512"/>
+    <hyperlink ref="AC315" r:id="rId535" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE122018"/>
+    <hyperlink ref="AD315" r:id="rId536" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE249929"/>
+    <hyperlink ref="AE315" r:id="rId537" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE261673"/>
+    <hyperlink ref="K316" r:id="rId538" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008599852/"/>
+    <hyperlink ref="L316" r:id="rId539" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE208078"/>
+    <hyperlink ref="M316" r:id="rId540" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE272361"/>
+    <hyperlink ref="N316" r:id="rId541" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE287622"/>
+    <hyperlink ref="O316" r:id="rId542" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE209632"/>
+    <hyperlink ref="P316" r:id="rId543" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE234489"/>
+    <hyperlink ref="Q316" r:id="rId544" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE185239"/>
+    <hyperlink ref="R316" r:id="rId545" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE201012"/>
+    <hyperlink ref="S316" r:id="rId546" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE196269"/>
+    <hyperlink ref="T316" r:id="rId547" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE124118"/>
+    <hyperlink ref="U316" r:id="rId548" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE145496"/>
+    <hyperlink ref="V316" r:id="rId549" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE140068"/>
+    <hyperlink ref="W316" r:id="rId550" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE129715"/>
+    <hyperlink ref="X316" r:id="rId551" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE151912"/>
+    <hyperlink ref="Y316" r:id="rId552" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE120891"/>
+    <hyperlink ref="Z316" r:id="rId553" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE101435"/>
+    <hyperlink ref="AA316" r:id="rId554" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE95623"/>
+    <hyperlink ref="K317" r:id="rId555" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008583852/"/>
+    <hyperlink ref="L317" r:id="rId556" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE208078"/>
+    <hyperlink ref="M317" r:id="rId557" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE241702"/>
+    <hyperlink ref="K318" r:id="rId558" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCA_0026413751/"/>
+    <hyperlink ref="L318" r:id="rId559" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE69529"/>
+    <hyperlink ref="M318" r:id="rId560" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE90796"/>
+    <hyperlink ref="K319" r:id="rId561" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0009078351/"/>
+    <hyperlink ref="L319" r:id="rId562" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE69529"/>
+    <hyperlink ref="K320" r:id="rId563" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCA_0030876351/"/>
+    <hyperlink ref="L320" r:id="rId564" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE69529"/>
+    <hyperlink ref="K321" r:id="rId565" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008582851/"/>
+    <hyperlink ref="L321" r:id="rId566" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE242252"/>
+    <hyperlink ref="M321" r:id="rId567" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE141932"/>
+    <hyperlink ref="N321" r:id="rId568" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE130633"/>
+    <hyperlink ref="O321" r:id="rId569" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE206641"/>
+    <hyperlink ref="P321" r:id="rId570" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE223957"/>
+    <hyperlink ref="Q321" r:id="rId571" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE174694"/>
+    <hyperlink ref="K322" r:id="rId572" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008640051/"/>
+    <hyperlink ref="L322" r:id="rId573" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE69529"/>
+    <hyperlink ref="M322" r:id="rId574" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE205007"/>
+    <hyperlink ref="K323" r:id="rId575" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008684251/"/>
+    <hyperlink ref="L323" r:id="rId576" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE69529"/>
+    <hyperlink ref="M323" r:id="rId577" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE205007"/>
+    <hyperlink ref="K324" r:id="rId578" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008605051/"/>
+    <hyperlink ref="K325" r:id="rId579" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0030330551/"/>
+    <hyperlink ref="L325" r:id="rId580" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE250153"/>
+    <hyperlink ref="M325" r:id="rId581" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE159644"/>
+    <hyperlink ref="N325" r:id="rId582" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE208535"/>
+    <hyperlink ref="O325" r:id="rId583" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE208637"/>
+    <hyperlink ref="P325" r:id="rId584" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE198946"/>
+    <hyperlink ref="Q325" r:id="rId585" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE233661"/>
+    <hyperlink ref="R325" r:id="rId586" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE186178"/>
+    <hyperlink ref="S325" r:id="rId587" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE65389"/>
+    <hyperlink ref="T325" r:id="rId588" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE112118"/>
+    <hyperlink ref="U325" r:id="rId589" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE153946"/>
+    <hyperlink ref="V325" r:id="rId590" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE110345"/>
+    <hyperlink ref="W325" r:id="rId591" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE165727"/>
+    <hyperlink ref="X325" r:id="rId592" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE183156"/>
+    <hyperlink ref="Y325" r:id="rId593" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE194179"/>
+    <hyperlink ref="Z325" r:id="rId594" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE169110"/>
+    <hyperlink ref="AA325" r:id="rId595" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE224901"/>
+    <hyperlink ref="AB325" r:id="rId596" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE217838"/>
+    <hyperlink ref="AC325" r:id="rId597" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE260966"/>
+    <hyperlink ref="AD325" r:id="rId598" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE274114"/>
+    <hyperlink ref="AE325" r:id="rId599" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE288077"/>
+    <hyperlink ref="K326" r:id="rId600" display="https://www.ncbi.nlm.nih.gov/datasets/genome/GCF_0008618451/"/>
+    <hyperlink ref="L326" r:id="rId601" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE250153"/>
+    <hyperlink ref="M326" r:id="rId602" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE82177"/>
+    <hyperlink ref="N326" r:id="rId603" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE136339"/>
+    <hyperlink ref="O326" r:id="rId604" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE149601"/>
+    <hyperlink ref="P326" r:id="rId605" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE132548"/>
+    <hyperlink ref="Q326" r:id="rId606" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE206397"/>
+    <hyperlink ref="R326" r:id="rId607" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE185700"/>
+    <hyperlink ref="S326" r:id="rId608" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE234572"/>
+    <hyperlink ref="T326" r:id="rId609" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE132548"/>
+    <hyperlink ref="U326" r:id="rId610" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE163239"/>
+    <hyperlink ref="V326" r:id="rId611" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE119117"/>
+    <hyperlink ref="W326" r:id="rId612" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE132606"/>
+    <hyperlink ref="X326" r:id="rId613" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE212871"/>
+    <hyperlink ref="Y326" r:id="rId614" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE267834"/>
+    <hyperlink ref="Z326" r:id="rId615" display="https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE84346"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -17714,8 +17703,8 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId617"/>
-  <legacyDrawing r:id="rId618"/>
+  <drawing r:id="rId616"/>
+  <legacyDrawing r:id="rId617"/>
 </worksheet>
 </file>
 
@@ -17730,7 +17719,7 @@
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.11"/>
@@ -17881,7 +17870,7 @@
         <v>9</v>
       </c>
       <c r="J5" s="78" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>696</v>
@@ -18043,7 +18032,7 @@
         <v>5</v>
       </c>
       <c r="J10" s="78" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>574</v>
@@ -18208,7 +18197,7 @@
     </row>
     <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J20" s="78" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="K20" s="6" t="s">
         <v>491</v>
@@ -18271,7 +18260,7 @@
     </row>
     <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J24" s="78" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="K24" s="6" t="s">
         <v>589</v>
@@ -18397,7 +18386,7 @@
     </row>
     <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J35" s="78" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="K35" s="6" t="s">
         <v>597</v>
@@ -18446,7 +18435,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J39" s="78" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="K39" s="7" t="s">
         <v>79</v>
@@ -18477,7 +18466,7 @@
     </row>
     <row r="41" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J41" s="78" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="K41" s="6" t="s">
         <v>601</v>
@@ -18501,7 +18490,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J43" s="78" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="K43" s="7" t="s">
         <v>687</v>
@@ -18548,7 +18537,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J46" s="78" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="K46" s="7" t="s">
         <v>54</v>
@@ -18563,7 +18552,7 @@
     </row>
     <row r="47" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J47" s="78" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="K47" s="6" t="s">
         <v>567</v>
@@ -18646,7 +18635,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J54" s="78" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="K54" s="7" t="s">
         <v>285</v>
@@ -18670,7 +18659,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J56" s="78" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="K56" s="7" t="s">
         <v>289</v>
@@ -18780,7 +18769,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J66" s="78" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="K66" s="7" t="s">
         <v>159</v>
@@ -18827,7 +18816,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J69" s="78" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="K69" s="7" t="s">
         <v>683</v>
@@ -18981,13 +18970,13 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J80" s="78" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="K80" s="7" t="s">
         <v>299</v>
       </c>
       <c r="L80" s="7" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="M80" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L80,": '",K80,"',")</f>
@@ -19098,7 +19087,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J90" s="78" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="K90" s="7" t="s">
         <v>293</v>
@@ -19172,7 +19161,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J96" s="78" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="K96" s="7" t="s">
         <v>101</v>
@@ -19187,7 +19176,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J97" s="78" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="K97" s="7" t="s">
         <v>449</v>
@@ -19202,7 +19191,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J98" s="78" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="K98" s="7" t="s">
         <v>616</v>
@@ -19217,7 +19206,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J99" s="78" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="K99" s="7" t="s">
         <v>452</v>
@@ -19232,7 +19221,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J100" s="78" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="K100" s="7" t="s">
         <v>619</v>
@@ -19329,7 +19318,7 @@
     </row>
     <row r="107" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J107" s="78" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="K107" s="6" t="s">
         <v>501</v>
@@ -19403,13 +19392,13 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J113" s="78" t="s">
+        <v>1097</v>
+      </c>
+      <c r="K113" s="7" t="s">
         <v>1098</v>
       </c>
-      <c r="K113" s="7" t="s">
+      <c r="L113" s="7" t="s">
         <v>1099</v>
-      </c>
-      <c r="L113" s="7" t="s">
-        <v>1100</v>
       </c>
       <c r="M113" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L113,": '",K113,"',")</f>
@@ -19425,7 +19414,7 @@
         <v>120</v>
       </c>
       <c r="L114" s="7" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="M114" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L114,": '",K114,"',")</f>
@@ -19450,7 +19439,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J116" s="78" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="K116" s="7" t="s">
         <v>691</v>
@@ -19474,7 +19463,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J118" s="78" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="K118" s="7" t="s">
         <v>405</v>
@@ -19489,7 +19478,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J119" s="78" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="K119" s="7" t="s">
         <v>409</v>
@@ -19504,7 +19493,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J120" s="78" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="K120" s="7" t="s">
         <v>401</v>
@@ -19535,13 +19524,13 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J122" s="78" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="K122" s="0" t="s">
+        <v>924</v>
+      </c>
+      <c r="L122" s="0" t="s">
         <v>925</v>
-      </c>
-      <c r="L122" s="0" t="s">
-        <v>926</v>
       </c>
       <c r="M122" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L122,": '",K122,"',")</f>
@@ -19620,7 +19609,7 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J130" s="78" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="K130" s="7" t="s">
         <v>389</v>
@@ -19653,7 +19642,7 @@
     </row>
     <row r="133" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J133" s="78" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="K133" s="6" t="s">
         <v>58</v>
@@ -19668,7 +19657,7 @@
     </row>
     <row r="134" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J134" s="78" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="K134" s="6" t="s">
         <v>658</v>
@@ -19692,7 +19681,7 @@
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J136" s="78" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="K136" s="7" t="s">
         <v>393</v>
@@ -19707,7 +19696,7 @@
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J137" s="78" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="K137" s="7" t="s">
         <v>382</v>
@@ -19754,7 +19743,7 @@
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J140" s="78" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="K140" s="7" t="s">
         <v>322</v>
@@ -19785,7 +19774,7 @@
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J142" s="78" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="K142" s="7" t="s">
         <v>72</v>
@@ -19861,7 +19850,7 @@
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J149" s="78" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="K149" s="7" t="s">
         <v>315</v>
@@ -19876,7 +19865,7 @@
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J150" s="78" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="K150" s="7" t="s">
         <v>330</v>
@@ -19891,7 +19880,7 @@
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J151" s="78" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="K151" s="7" t="s">
         <v>326</v>
@@ -19922,7 +19911,7 @@
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J153" s="78" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="K153" s="7" t="s">
         <v>334</v>
@@ -19966,10 +19955,10 @@
         <v>fverticillioides</v>
       </c>
       <c r="K156" s="7" t="s">
+        <v>1117</v>
+      </c>
+      <c r="L156" s="7" t="s">
         <v>1118</v>
-      </c>
-      <c r="L156" s="7" t="s">
-        <v>1119</v>
       </c>
       <c r="M156" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L156,": '",K156,"',")</f>
@@ -20012,7 +20001,7 @@
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J160" s="78" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="K160" s="7" t="s">
         <v>170</v>
@@ -20027,13 +20016,13 @@
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J161" s="78" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="K161" s="0" t="s">
+        <v>1010</v>
+      </c>
+      <c r="L161" s="0" t="s">
         <v>1011</v>
-      </c>
-      <c r="L161" s="0" t="s">
-        <v>1012</v>
       </c>
       <c r="M161" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L161,": '",K161,"',")</f>
@@ -20042,13 +20031,13 @@
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J162" s="78" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="K162" s="0" t="s">
+        <v>1014</v>
+      </c>
+      <c r="L162" s="0" t="s">
         <v>1015</v>
-      </c>
-      <c r="L162" s="0" t="s">
-        <v>1016</v>
       </c>
       <c r="M162" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L162,": '",K162,"',")</f>
@@ -20057,13 +20046,13 @@
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J163" s="78" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="K163" s="0" t="s">
+        <v>1038</v>
+      </c>
+      <c r="L163" s="0" t="s">
         <v>1039</v>
-      </c>
-      <c r="L163" s="0" t="s">
-        <v>1040</v>
       </c>
       <c r="M163" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L163,": '",K163,"',")</f>
@@ -20088,13 +20077,13 @@
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J165" s="78" t="s">
+        <v>1123</v>
+      </c>
+      <c r="K165" s="7" t="s">
         <v>1124</v>
       </c>
-      <c r="K165" s="7" t="s">
+      <c r="L165" s="7" t="s">
         <v>1125</v>
-      </c>
-      <c r="L165" s="7" t="s">
-        <v>1126</v>
       </c>
       <c r="M165" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L165,": '",K165,"',")</f>
@@ -20121,13 +20110,13 @@
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J168" s="78" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="K168" s="0" t="s">
+        <v>911</v>
+      </c>
+      <c r="L168" s="0" t="s">
         <v>912</v>
-      </c>
-      <c r="L168" s="0" t="s">
-        <v>913</v>
       </c>
       <c r="M168" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L168,": '",K168,"',")</f>
@@ -20136,13 +20125,13 @@
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J169" s="78" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="K169" s="0" t="s">
+        <v>931</v>
+      </c>
+      <c r="L169" s="0" t="s">
         <v>932</v>
-      </c>
-      <c r="L169" s="0" t="s">
-        <v>933</v>
       </c>
       <c r="M169" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L169,": '",K169,"',")</f>
@@ -20151,13 +20140,13 @@
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J170" s="78" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="K170" s="0" t="s">
+        <v>954</v>
+      </c>
+      <c r="L170" s="0" t="s">
         <v>955</v>
-      </c>
-      <c r="L170" s="0" t="s">
-        <v>956</v>
       </c>
       <c r="M170" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L170,": '",K170,"',")</f>
@@ -20166,13 +20155,13 @@
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J171" s="78" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="K171" s="0" t="s">
+        <v>982</v>
+      </c>
+      <c r="L171" s="0" t="s">
         <v>983</v>
-      </c>
-      <c r="L171" s="0" t="s">
-        <v>984</v>
       </c>
       <c r="M171" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L171,": '",K171,"',")</f>
@@ -20181,13 +20170,13 @@
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J172" s="78" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="K172" s="56" t="s">
+        <v>986</v>
+      </c>
+      <c r="L172" s="56" t="s">
         <v>987</v>
-      </c>
-      <c r="L172" s="56" t="s">
-        <v>988</v>
       </c>
       <c r="M172" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L172,": '",K172,"',")</f>
@@ -20196,13 +20185,13 @@
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J173" s="78" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="K173" s="0" t="s">
+        <v>988</v>
+      </c>
+      <c r="L173" s="0" t="s">
         <v>989</v>
-      </c>
-      <c r="L173" s="0" t="s">
-        <v>990</v>
       </c>
       <c r="M173" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L173,": '",K173,"',")</f>
@@ -20211,13 +20200,13 @@
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J174" s="78" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="K174" s="0" t="s">
+        <v>960</v>
+      </c>
+      <c r="L174" s="0" t="s">
         <v>961</v>
-      </c>
-      <c r="L174" s="0" t="s">
-        <v>962</v>
       </c>
       <c r="M174" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L174,": '",K174,"',")</f>
@@ -20226,13 +20215,13 @@
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J175" s="78" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="K175" s="0" t="s">
+        <v>978</v>
+      </c>
+      <c r="L175" s="0" t="s">
         <v>979</v>
-      </c>
-      <c r="L175" s="0" t="s">
-        <v>980</v>
       </c>
       <c r="M175" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L175,": '",K175,"',")</f>
@@ -20241,7 +20230,7 @@
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J176" s="78" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="K176" s="7" t="s">
         <v>745</v>
@@ -20256,13 +20245,13 @@
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J177" s="78" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="K177" s="0" t="s">
+        <v>873</v>
+      </c>
+      <c r="L177" s="0" t="s">
         <v>874</v>
-      </c>
-      <c r="L177" s="0" t="s">
-        <v>875</v>
       </c>
       <c r="M177" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L177,": '",K177,"',")</f>
@@ -20271,7 +20260,7 @@
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J178" s="78" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="K178" s="7" t="s">
         <v>274</v>
@@ -20286,13 +20275,13 @@
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J179" s="78" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="K179" s="0" t="s">
+        <v>884</v>
+      </c>
+      <c r="L179" s="0" t="s">
         <v>885</v>
-      </c>
-      <c r="L179" s="0" t="s">
-        <v>886</v>
       </c>
       <c r="M179" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L179,": '",K179,"',")</f>
@@ -20371,7 +20360,7 @@
         <v>lhyos</v>
       </c>
       <c r="K185" s="21" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="L185" s="21" t="s">
         <v>440</v>
@@ -20515,7 +20504,7 @@
     </row>
     <row r="196" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J196" s="78" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="K196" s="6" t="s">
         <v>593</v>
@@ -20548,7 +20537,7 @@
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J199" s="78" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="K199" s="7" t="s">
         <v>702</v>
@@ -20588,13 +20577,13 @@
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J202" s="78" t="s">
+        <v>1141</v>
+      </c>
+      <c r="K202" s="7" t="s">
         <v>1142</v>
       </c>
-      <c r="K202" s="7" t="s">
+      <c r="L202" s="7" t="s">
         <v>1143</v>
-      </c>
-      <c r="L202" s="7" t="s">
-        <v>1144</v>
       </c>
       <c r="M202" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L202,": '",K202,"',")</f>
@@ -20623,7 +20612,7 @@
         <v>mavium subsp. Paratuberculosis</v>
       </c>
       <c r="K204" s="7" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20632,7 +20621,7 @@
         <v>mavium subsp. Paratuberculosis</v>
       </c>
       <c r="K205" s="7" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20687,7 +20676,7 @@
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J210" s="78" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="K210" s="7" t="s">
         <v>116</v>
@@ -20743,13 +20732,13 @@
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J214" s="78" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="K214" s="7" t="s">
         <v>732</v>
       </c>
       <c r="L214" s="7" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="M214" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L214,": '",K214,"',")</f>
@@ -20781,7 +20770,7 @@
         <v>135</v>
       </c>
       <c r="L216" s="7" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="M216" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L216,": '",K216,"',")</f>
@@ -20854,7 +20843,7 @@
         <v>139</v>
       </c>
       <c r="L221" s="7" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="M221" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L221,": '",K221,"',")</f>
@@ -20895,7 +20884,7 @@
         <v>676</v>
       </c>
       <c r="L224" s="7" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="M224" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L224,": '",K224,"',")</f>
@@ -20977,7 +20966,7 @@
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J230" s="78" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="K230" s="7" t="s">
         <v>740</v>
@@ -20992,13 +20981,13 @@
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J231" s="78" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="K231" s="0" t="s">
+        <v>1002</v>
+      </c>
+      <c r="L231" s="0" t="s">
         <v>1003</v>
-      </c>
-      <c r="L231" s="0" t="s">
-        <v>1004</v>
       </c>
       <c r="M231" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L231,": '",K231,"',")</f>
@@ -21011,10 +21000,10 @@
         <v>ngonorrhoeae</v>
       </c>
       <c r="K232" s="0" t="s">
+        <v>867</v>
+      </c>
+      <c r="L232" s="0" t="s">
         <v>868</v>
-      </c>
-      <c r="L232" s="0" t="s">
-        <v>869</v>
       </c>
       <c r="M232" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L232,": '",K232,"',")</f>
@@ -21023,13 +21012,13 @@
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J233" s="78" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="K233" s="0" t="s">
+        <v>1006</v>
+      </c>
+      <c r="L233" s="0" t="s">
         <v>1007</v>
-      </c>
-      <c r="L233" s="0" t="s">
-        <v>1008</v>
       </c>
       <c r="M233" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L233,": '",K233,"',")</f>
@@ -21136,13 +21125,13 @@
     </row>
     <row r="241" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J241" s="78" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="K241" s="6" t="s">
         <v>534</v>
       </c>
       <c r="L241" s="6" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="M241" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L241,": '",K241,"',")</f>
@@ -21151,7 +21140,7 @@
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J242" s="78" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="K242" s="7" t="s">
         <v>174</v>
@@ -21166,7 +21155,7 @@
     </row>
     <row r="243" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J243" s="78" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="K243" s="6" t="s">
         <v>529</v>
@@ -21274,7 +21263,7 @@
     </row>
     <row r="252" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J252" s="78" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="K252" s="6" t="s">
         <v>537</v>
@@ -21289,7 +21278,7 @@
     </row>
     <row r="253" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J253" s="78" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="K253" s="6" t="s">
         <v>552</v>
@@ -21304,7 +21293,7 @@
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J254" s="78" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="K254" s="7" t="s">
         <v>367</v>
@@ -21319,7 +21308,7 @@
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J255" s="78" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="K255" s="7" t="s">
         <v>512</v>
@@ -21334,7 +21323,7 @@
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J256" s="78" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K256" s="7" t="s">
         <v>515</v>
@@ -21349,7 +21338,7 @@
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J257" s="78" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="K257" s="7" t="s">
         <v>518</v>
@@ -21364,7 +21353,7 @@
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J258" s="78" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="K258" s="7" t="s">
         <v>521</v>
@@ -21436,7 +21425,7 @@
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J263" s="78" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="K263" s="7" t="s">
         <v>506</v>
@@ -21519,7 +21508,7 @@
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J270" s="78" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="K270" s="7" t="s">
         <v>234</v>
@@ -21563,7 +21552,7 @@
         <v>sdublin</v>
       </c>
       <c r="K273" s="7" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="L273" s="7" t="s">
         <v>654</v>
@@ -21579,10 +21568,10 @@
         <v>sdysenteriae</v>
       </c>
       <c r="K274" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="L274" s="0" t="s">
         <v>857</v>
-      </c>
-      <c r="L274" s="0" t="s">
-        <v>858</v>
       </c>
       <c r="M274" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L274,": '",K274,"',")</f>
@@ -21607,13 +21596,13 @@
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J276" s="78" t="s">
+        <v>1167</v>
+      </c>
+      <c r="K276" s="7" t="s">
         <v>1168</v>
       </c>
-      <c r="K276" s="7" t="s">
+      <c r="L276" s="7" t="s">
         <v>1169</v>
-      </c>
-      <c r="L276" s="7" t="s">
-        <v>1170</v>
       </c>
       <c r="M276" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L276,": '",K276,"',")</f>
@@ -21622,13 +21611,13 @@
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J277" s="78" t="s">
+        <v>1170</v>
+      </c>
+      <c r="K277" s="7" t="s">
         <v>1171</v>
       </c>
-      <c r="K277" s="7" t="s">
+      <c r="L277" s="7" t="s">
         <v>1172</v>
-      </c>
-      <c r="L277" s="7" t="s">
-        <v>1173</v>
       </c>
       <c r="M277" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L277,": '",K277,"',")</f>
@@ -21644,7 +21633,7 @@
         <v>304</v>
       </c>
       <c r="L278" s="7" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="M278" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L278,": '",K278,"',")</f>
@@ -21657,7 +21646,7 @@
         <v>sequi subsp. Zooepidemicus</v>
       </c>
       <c r="K279" s="7" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21666,7 +21655,7 @@
         <v>sequi subsp. Zooepidemicus</v>
       </c>
       <c r="K280" s="7" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21675,10 +21664,10 @@
         <v>sflexneri</v>
       </c>
       <c r="K281" s="0" t="s">
+        <v>859</v>
+      </c>
+      <c r="L281" s="0" t="s">
         <v>860</v>
-      </c>
-      <c r="L281" s="0" t="s">
-        <v>861</v>
       </c>
       <c r="M281" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L281,": '",K281,"',")</f>
@@ -21691,7 +21680,7 @@
         <v>sgallinarum</v>
       </c>
       <c r="K282" s="7" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="L282" s="7" t="s">
         <v>720</v>
@@ -21719,7 +21708,7 @@
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J284" s="78" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="K284" s="7" t="s">
         <v>480</v>
@@ -21734,7 +21723,7 @@
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J285" s="78" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="K285" s="7" t="s">
         <v>488</v>
@@ -21769,7 +21758,7 @@
         <v>snewport</v>
       </c>
       <c r="K287" s="7" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="L287" s="7" t="s">
         <v>657</v>
@@ -21817,7 +21806,7 @@
         <v>spullorum</v>
       </c>
       <c r="K290" s="34" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="L290" s="34" t="s">
         <v>718</v>
@@ -21867,10 +21856,10 @@
         <v>ssonnei</v>
       </c>
       <c r="K294" s="0" t="s">
+        <v>853</v>
+      </c>
+      <c r="L294" s="0" t="s">
         <v>854</v>
-      </c>
-      <c r="L294" s="0" t="s">
-        <v>855</v>
       </c>
       <c r="M294" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L294,": '",K294,"',")</f>
@@ -21897,7 +21886,7 @@
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J297" s="78" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="K297" s="7" t="s">
         <v>458</v>
@@ -21935,7 +21924,7 @@
         <v>822</v>
       </c>
       <c r="L299" s="0" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="M299" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L299,": '",K299,"',")</f>
@@ -21980,7 +21969,7 @@
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J304" s="78" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="K304" s="7" t="s">
         <v>76</v>
@@ -21995,7 +21984,7 @@
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J305" s="78" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="K305" s="7" t="s">
         <v>167</v>
@@ -22010,7 +21999,7 @@
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J306" s="78" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="K306" s="7" t="s">
         <v>679</v>
@@ -22043,7 +22032,7 @@
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J309" s="78" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="K309" s="7" t="s">
         <v>756</v>
@@ -22074,7 +22063,7 @@
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J311" s="78" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="K311" s="7" t="s">
         <v>524</v>
@@ -22109,10 +22098,10 @@
         <v>tpallidum</v>
       </c>
       <c r="K313" s="0" t="s">
+        <v>863</v>
+      </c>
+      <c r="L313" s="0" t="s">
         <v>864</v>
-      </c>
-      <c r="L313" s="0" t="s">
-        <v>865</v>
       </c>
       <c r="M313" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L313,": '",K313,"',")</f>
@@ -22162,7 +22151,7 @@
     </row>
     <row r="317" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J317" s="78" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="K317" s="6" t="s">
         <v>625</v>
@@ -22213,13 +22202,13 @@
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J322" s="78" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="K322" s="0" t="s">
+        <v>992</v>
+      </c>
+      <c r="L322" s="0" t="s">
         <v>993</v>
-      </c>
-      <c r="L322" s="0" t="s">
-        <v>994</v>
       </c>
       <c r="M322" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L322,": '",K322,"',")</f>
@@ -22228,7 +22217,7 @@
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J323" s="78" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="K323" s="7" t="s">
         <v>385</v>
@@ -22243,13 +22232,13 @@
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J324" s="78" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="K324" s="0" t="s">
+        <v>888</v>
+      </c>
+      <c r="L324" s="0" t="s">
         <v>889</v>
-      </c>
-      <c r="L324" s="0" t="s">
-        <v>890</v>
       </c>
       <c r="M324" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L324,": '",K324,"',")</f>
@@ -22258,13 +22247,13 @@
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J325" s="78" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="K325" s="0" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="L325" s="0" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="M325" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L325,": '",K325,"',")</f>
@@ -22296,7 +22285,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.72"/>
   </cols>
@@ -23803,27 +23792,27 @@
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="0" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="0" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="0" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="0" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="0" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23833,97 +23822,97 @@
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="0" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="0" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="0" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="0" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="0" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="0" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="0" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="0" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="0" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="0" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="0" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="56" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="0" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="0" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="0" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="0" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="0" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="0" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="0" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
   </sheetData>
@@ -23948,7 +23937,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.89"/>
@@ -24053,7 +24042,7 @@
         <v>11</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24071,7 +24060,7 @@
         <v>629</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24081,7 +24070,7 @@
         <v>354</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24091,7 +24080,7 @@
         <v>428</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25316,7 +25305,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.99"/>
@@ -25326,13 +25315,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="79" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B1" s="79" t="s">
         <v>1196</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="C1" s="80" t="s">
         <v>1197</v>
-      </c>
-      <c r="C1" s="80" t="s">
-        <v>1198</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25578,7 +25567,7 @@
         <v>152</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25600,7 +25589,7 @@
         <v>633</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25788,7 +25777,7 @@
         <v>677</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25796,7 +25785,7 @@
         <v>64</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25804,7 +25793,7 @@
         <v>35</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25812,7 +25801,7 @@
         <v>819</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25820,7 +25809,7 @@
         <v>117</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25828,7 +25817,7 @@
         <v>106</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25836,7 +25825,7 @@
         <v>715</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25844,7 +25833,7 @@
         <v>647</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25852,15 +25841,15 @@
         <v>140</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C53" s="56" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25868,7 +25857,7 @@
         <v>816</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25884,7 +25873,7 @@
         <v>242</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25900,7 +25889,7 @@
         <v>673</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25980,7 +25969,7 @@
         <v>718</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25988,7 +25977,7 @@
         <v>249</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26001,7 +25990,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="0" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C71" s="56" t="s">
         <v>175</v>
@@ -26009,7 +25998,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C72" s="81" t="s">
         <v>535</v>
@@ -26017,7 +26006,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C73" s="81" t="s">
         <v>530</v>
@@ -26092,7 +26081,7 @@
         <v>263</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26113,7 +26102,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C85" s="56" t="s">
         <v>507</v>
@@ -26141,7 +26130,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="0" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
RCC fix and remove NEG and POS ids
</commit_message>
<xml_diff>
--- a/info/apinet_survey (2).xlsx
+++ b/info/apinet_survey (2).xlsx
@@ -71,6 +71,35 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Output looks off</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V300" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">HUVEC only
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W326" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Which columns?</t>
         </r>
       </text>
     </comment>
@@ -3923,6 +3952,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF1300FF"/>
+        <bgColor rgb="FF0000EE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF860069"/>
         <bgColor rgb="FF800080"/>
       </patternFill>
@@ -3935,20 +3970,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF1300FF"/>
-        <bgColor rgb="FF0000EE"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0C5201"/>
         <bgColor rgb="FF30300B"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -3996,7 +4025,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="83">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4201,11 +4230,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="23" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="22" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="23" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4217,19 +4250,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="23" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="24" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4241,7 +4266,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="23" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4265,11 +4290,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="25" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="24" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="24" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="25" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4289,7 +4314,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4297,7 +4322,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="23" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4417,8 +4442,8 @@
   </sheetPr>
   <dimension ref="A1:AK346"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L307" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q313" activeCellId="0" sqref="Q313"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U310" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V318" activeCellId="0" sqref="V318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11295,16 +11320,16 @@
       <c r="T186" s="13" t="s">
         <v>547</v>
       </c>
-      <c r="U186" s="11" t="s">
+      <c r="U186" s="13" t="s">
         <v>548</v>
       </c>
-      <c r="V186" s="26" t="s">
+      <c r="V186" s="13" t="s">
         <v>549</v>
       </c>
-      <c r="W186" s="26" t="s">
+      <c r="W186" s="13" t="s">
         <v>550</v>
       </c>
-      <c r="X186" s="26" t="s">
+      <c r="X186" s="13" t="s">
         <v>551</v>
       </c>
     </row>
@@ -11367,13 +11392,13 @@
       <c r="T187" s="13" t="s">
         <v>547</v>
       </c>
-      <c r="U187" s="11" t="s">
+      <c r="U187" s="13" t="s">
         <v>548</v>
       </c>
-      <c r="V187" s="26" t="s">
+      <c r="V187" s="13" t="s">
         <v>549</v>
       </c>
-      <c r="W187" s="26" t="s">
+      <c r="W187" s="13" t="s">
         <v>550</v>
       </c>
     </row>
@@ -15257,10 +15282,10 @@
       <c r="T293" s="13" t="s">
         <v>788</v>
       </c>
-      <c r="U293" s="11" t="s">
+      <c r="U293" s="13" t="s">
         <v>789</v>
       </c>
-      <c r="V293" s="26" t="s">
+      <c r="V293" s="13" t="s">
         <v>790</v>
       </c>
     </row>
@@ -15373,13 +15398,13 @@
       <c r="T295" s="13" t="s">
         <v>810</v>
       </c>
-      <c r="U295" s="11" t="s">
+      <c r="U295" s="13" t="s">
         <v>811</v>
       </c>
       <c r="V295" s="11" t="s">
         <v>812</v>
       </c>
-      <c r="W295" s="26" t="s">
+      <c r="W295" s="44" t="s">
         <v>813</v>
       </c>
     </row>
@@ -15596,16 +15621,16 @@
       <c r="T300" s="13" t="s">
         <v>837</v>
       </c>
-      <c r="U300" s="11" t="s">
+      <c r="U300" s="13" t="s">
         <v>838</v>
       </c>
-      <c r="V300" s="26" t="s">
+      <c r="V300" s="49" t="s">
         <v>839</v>
       </c>
-      <c r="W300" s="26" t="s">
+      <c r="W300" s="13" t="s">
         <v>840</v>
       </c>
-      <c r="X300" s="26" t="s">
+      <c r="X300" s="13" t="s">
         <v>841</v>
       </c>
     </row>
@@ -15648,7 +15673,7 @@
       <c r="N301" s="13" t="s">
         <v>847</v>
       </c>
-      <c r="O301" s="49" t="s">
+      <c r="O301" s="50" t="s">
         <v>848</v>
       </c>
       <c r="P301" s="44" t="n">
@@ -15926,7 +15951,7 @@
       <c r="P308" s="13" t="s">
         <v>879</v>
       </c>
-      <c r="Q308" s="50" t="s">
+      <c r="Q308" s="51" t="s">
         <v>880</v>
       </c>
       <c r="R308" s="13" t="s">
@@ -15989,7 +16014,7 @@
       <c r="G310" s="0" t="s">
         <v>888</v>
       </c>
-      <c r="H310" s="51" t="s">
+      <c r="H310" s="52" t="s">
         <v>889</v>
       </c>
       <c r="I310" s="0" t="str">
@@ -16003,7 +16028,7 @@
       <c r="K310" s="8" t="s">
         <v>890</v>
       </c>
-      <c r="L310" s="52" t="s">
+      <c r="L310" s="53" t="s">
         <v>880</v>
       </c>
       <c r="M310" s="13" t="s">
@@ -16027,16 +16052,16 @@
       <c r="T310" s="13" t="s">
         <v>897</v>
       </c>
-      <c r="U310" s="11" t="s">
+      <c r="U310" s="13" t="s">
         <v>898</v>
       </c>
-      <c r="V310" s="26" t="s">
+      <c r="V310" s="44" t="s">
         <v>899</v>
       </c>
-      <c r="W310" s="26" t="s">
+      <c r="W310" s="13" t="s">
         <v>900</v>
       </c>
-      <c r="X310" s="26" t="s">
+      <c r="X310" s="13" t="s">
         <v>901</v>
       </c>
       <c r="Y310" s="26" t="s">
@@ -16057,7 +16082,7 @@
       <c r="AD310" s="26" t="s">
         <v>907</v>
       </c>
-      <c r="AE310" s="53" t="s">
+      <c r="AE310" s="54" t="s">
         <v>908</v>
       </c>
       <c r="AF310" s="26" t="s">
@@ -16133,7 +16158,7 @@
       <c r="K312" s="8" t="s">
         <v>917</v>
       </c>
-      <c r="L312" s="52" t="s">
+      <c r="L312" s="53" t="s">
         <v>918</v>
       </c>
       <c r="M312" s="13" t="s">
@@ -16227,10 +16252,10 @@
       <c r="L314" s="10" t="s">
         <v>934</v>
       </c>
-      <c r="M314" s="54" t="s">
+      <c r="M314" s="55" t="s">
         <v>935</v>
       </c>
-      <c r="N314" s="54" t="s">
+      <c r="N314" s="55" t="s">
         <v>936</v>
       </c>
       <c r="O314" s="13" t="s">
@@ -16248,19 +16273,19 @@
       <c r="S314" s="27" t="s">
         <v>941</v>
       </c>
-      <c r="T314" s="55" t="s">
+      <c r="T314" s="49" t="s">
         <v>942</v>
       </c>
-      <c r="U314" s="11" t="s">
+      <c r="U314" s="27" t="s">
         <v>943</v>
       </c>
-      <c r="V314" s="26" t="s">
+      <c r="V314" s="27" t="s">
         <v>944</v>
       </c>
-      <c r="W314" s="26" t="s">
+      <c r="W314" s="13" t="s">
         <v>945</v>
       </c>
-      <c r="X314" s="26" t="s">
+      <c r="X314" s="13" t="s">
         <v>946</v>
       </c>
       <c r="Y314" s="26" t="s">
@@ -16281,7 +16306,7 @@
       <c r="AD314" s="26" t="s">
         <v>952</v>
       </c>
-      <c r="AE314" s="53" t="s">
+      <c r="AE314" s="54" t="s">
         <v>953</v>
       </c>
       <c r="AK314" s="0" t="n">
@@ -16340,19 +16365,19 @@
       <c r="S315" s="27" t="s">
         <v>941</v>
       </c>
-      <c r="T315" s="55" t="s">
+      <c r="T315" s="49" t="s">
         <v>942</v>
       </c>
-      <c r="U315" s="11" t="s">
+      <c r="U315" s="27" t="s">
         <v>943</v>
       </c>
-      <c r="V315" s="26" t="s">
+      <c r="V315" s="27" t="s">
         <v>944</v>
       </c>
-      <c r="W315" s="26" t="s">
+      <c r="W315" s="13" t="s">
         <v>945</v>
       </c>
-      <c r="X315" s="26" t="s">
+      <c r="X315" s="13" t="s">
         <v>946</v>
       </c>
       <c r="Y315" s="26" t="s">
@@ -16373,7 +16398,7 @@
       <c r="AD315" s="26" t="s">
         <v>957</v>
       </c>
-      <c r="AE315" s="53" t="s">
+      <c r="AE315" s="54" t="s">
         <v>958</v>
       </c>
     </row>
@@ -16407,10 +16432,10 @@
       <c r="K316" s="8" t="s">
         <v>962</v>
       </c>
-      <c r="L316" s="52" t="s">
+      <c r="L316" s="53" t="s">
         <v>963</v>
       </c>
-      <c r="M316" s="54" t="s">
+      <c r="M316" s="55" t="s">
         <v>964</v>
       </c>
       <c r="N316" s="13" t="s">
@@ -16434,16 +16459,16 @@
       <c r="T316" s="13" t="s">
         <v>970</v>
       </c>
-      <c r="U316" s="11" t="s">
+      <c r="U316" s="13" t="s">
         <v>971</v>
       </c>
-      <c r="V316" s="26" t="s">
+      <c r="V316" s="13" t="s">
         <v>972</v>
       </c>
-      <c r="W316" s="26" t="s">
+      <c r="W316" s="13" t="s">
         <v>973</v>
       </c>
-      <c r="X316" s="26" t="s">
+      <c r="X316" s="13" t="s">
         <v>974</v>
       </c>
       <c r="Y316" s="26" t="s">
@@ -16486,7 +16511,7 @@
       <c r="K317" s="8" t="s">
         <v>980</v>
       </c>
-      <c r="L317" s="52" t="s">
+      <c r="L317" s="53" t="s">
         <v>963</v>
       </c>
       <c r="M317" s="13" t="s">
@@ -16539,7 +16564,7 @@
       <c r="L318" s="11" t="s">
         <v>812</v>
       </c>
-      <c r="M318" s="54" t="s">
+      <c r="M318" s="55" t="s">
         <v>985</v>
       </c>
       <c r="O318" s="26"/>
@@ -16741,7 +16766,7 @@
       <c r="L323" s="11" t="s">
         <v>812</v>
       </c>
-      <c r="M323" s="54" t="s">
+      <c r="M323" s="55" t="s">
         <v>1005</v>
       </c>
       <c r="N323" s="7"/>
@@ -16813,7 +16838,7 @@
       <c r="L325" s="11" t="s">
         <v>1017</v>
       </c>
-      <c r="M325" s="58" t="s">
+      <c r="M325" s="13" t="s">
         <v>1018</v>
       </c>
       <c r="N325" s="13" t="s">
@@ -16831,19 +16856,19 @@
       <c r="R325" s="13" t="s">
         <v>1023</v>
       </c>
-      <c r="S325" s="58" t="s">
+      <c r="S325" s="13" t="s">
         <v>1024</v>
       </c>
       <c r="T325" s="13" t="s">
         <v>1025</v>
       </c>
-      <c r="U325" s="11" t="s">
+      <c r="U325" s="13" t="s">
         <v>1026</v>
       </c>
-      <c r="V325" s="26" t="s">
+      <c r="V325" s="13" t="s">
         <v>1027</v>
       </c>
-      <c r="W325" s="26" t="s">
+      <c r="W325" s="49" t="s">
         <v>1028</v>
       </c>
       <c r="X325" s="26" t="s">
@@ -16867,7 +16892,7 @@
       <c r="AD325" s="26" t="s">
         <v>1035</v>
       </c>
-      <c r="AE325" s="53" t="s">
+      <c r="AE325" s="54" t="s">
         <v>1036</v>
       </c>
     </row>
@@ -16919,22 +16944,22 @@
       <c r="Q326" s="13" t="s">
         <v>1045</v>
       </c>
-      <c r="R326" s="55" t="s">
+      <c r="R326" s="49" t="s">
         <v>1046</v>
       </c>
       <c r="S326" s="13" t="s">
         <v>1047</v>
       </c>
-      <c r="T326" s="59" t="s">
+      <c r="T326" s="58" t="s">
         <v>1044</v>
       </c>
-      <c r="U326" s="11" t="s">
+      <c r="U326" s="13" t="s">
         <v>1048</v>
       </c>
-      <c r="V326" s="26" t="s">
+      <c r="V326" s="13" t="s">
         <v>1049</v>
       </c>
-      <c r="W326" s="26" t="s">
+      <c r="W326" s="27" t="s">
         <v>1050</v>
       </c>
       <c r="X326" s="26" t="s">
@@ -16946,19 +16971,19 @@
       <c r="Z326" s="24" t="s">
         <v>1053</v>
       </c>
-      <c r="AE326" s="53"/>
+      <c r="AE326" s="54"/>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B327" s="60"/>
+      <c r="B327" s="59"/>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B328" s="60"/>
+      <c r="B328" s="59"/>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B329" s="60"/>
+      <c r="B329" s="59"/>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B330" s="60"/>
+      <c r="B330" s="59"/>
       <c r="D330" s="1"/>
       <c r="E330" s="0" t="s">
         <v>1054</v>
@@ -16969,13 +16994,13 @@
       <c r="E331" s="0" t="s">
         <v>1055</v>
       </c>
-      <c r="L331" s="61"/>
+      <c r="L331" s="60"/>
       <c r="M331" s="0" t="s">
         <v>1056</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D332" s="62"/>
+      <c r="D332" s="61"/>
       <c r="E332" s="0" t="s">
         <v>1057</v>
       </c>
@@ -16985,7 +17010,7 @@
       </c>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D333" s="63"/>
+      <c r="D333" s="62"/>
       <c r="E333" s="0" t="s">
         <v>1059</v>
       </c>
@@ -16995,79 +17020,79 @@
       </c>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L334" s="64"/>
+      <c r="L334" s="63"/>
       <c r="M334" s="0" t="s">
         <v>1061</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L335" s="65"/>
+      <c r="L335" s="64"/>
       <c r="M335" s="0" t="s">
         <v>1062</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L336" s="66"/>
+      <c r="L336" s="65"/>
       <c r="M336" s="0" t="s">
         <v>1063</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L337" s="67"/>
+      <c r="L337" s="66"/>
       <c r="M337" s="0" t="s">
         <v>1064</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L338" s="68"/>
+      <c r="L338" s="67"/>
       <c r="M338" s="0" t="s">
         <v>1065</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L339" s="69"/>
+      <c r="L339" s="68"/>
       <c r="M339" s="0" t="s">
         <v>1066</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L340" s="70"/>
+      <c r="L340" s="69"/>
       <c r="M340" s="0" t="s">
         <v>1067</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L341" s="71"/>
+      <c r="L341" s="70"/>
       <c r="M341" s="0" t="s">
         <v>1068</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L342" s="72"/>
+      <c r="L342" s="71"/>
       <c r="M342" s="0" t="s">
         <v>1069</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L343" s="73"/>
+      <c r="L343" s="72"/>
       <c r="M343" s="0" t="s">
         <v>1070</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L344" s="74"/>
+      <c r="L344" s="73"/>
       <c r="M344" s="0" t="s">
         <v>1071</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L345" s="75"/>
+      <c r="L345" s="74"/>
       <c r="M345" s="0" t="s">
         <v>1072</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L346" s="76"/>
+      <c r="L346" s="75"/>
       <c r="M346" s="0" t="s">
         <v>1073</v>
       </c>
@@ -17747,7 +17772,7 @@
       <c r="F1" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="J1" s="77" t="str">
+      <c r="J1" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K1)),RIGHT(K1,LEN(K1)-FIND(" ",K1)))</f>
         <v>aalternata</v>
       </c>
@@ -17781,7 +17806,7 @@
       <c r="F2" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="J2" s="77" t="str">
+      <c r="J2" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K2)),RIGHT(K2,LEN(K2)-FIND(" ",K2)))</f>
         <v>aalternata</v>
       </c>
@@ -17808,7 +17833,7 @@
       <c r="F3" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="J3" s="77" t="str">
+      <c r="J3" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K3)),RIGHT(K3,LEN(K3)-FIND(" ",K3)))</f>
         <v>aalternata</v>
       </c>
@@ -17835,7 +17860,7 @@
       <c r="F4" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="J4" s="77" t="str">
+      <c r="J4" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K4)),RIGHT(K4,LEN(K4)-FIND(" ",K4)))</f>
         <v>aapis</v>
       </c>
@@ -17869,7 +17894,7 @@
       <c r="F5" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="J5" s="78" t="s">
+      <c r="J5" s="77" t="s">
         <v>1074</v>
       </c>
       <c r="K5" s="7" t="s">
@@ -17902,7 +17927,7 @@
       <c r="F6" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="J6" s="77" t="str">
+      <c r="J6" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K6)),RIGHT(K6,LEN(K6)-FIND(" ",K6)))</f>
         <v>acoronavirus</v>
       </c>
@@ -17936,7 +17961,7 @@
       <c r="F7" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="J7" s="77" t="str">
+      <c r="J7" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K7)),RIGHT(K7,LEN(K7)-FIND(" ",K7)))</f>
         <v>aflavus</v>
       </c>
@@ -17970,7 +17995,7 @@
       <c r="F8" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="J8" s="77" t="str">
+      <c r="J8" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K8)),RIGHT(K8,LEN(K8)-FIND(" ",K8)))</f>
         <v>afumigatus</v>
       </c>
@@ -18004,7 +18029,7 @@
       <c r="F9" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="J9" s="77" t="str">
+      <c r="J9" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K9)),RIGHT(K9,LEN(K9)-FIND(" ",K9)))</f>
         <v>aflavus</v>
       </c>
@@ -18031,7 +18056,7 @@
       <c r="F10" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="J10" s="78" t="s">
+      <c r="J10" s="77" t="s">
         <v>1075</v>
       </c>
       <c r="K10" s="6" t="s">
@@ -18064,7 +18089,7 @@
       <c r="F11" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="J11" s="77" t="str">
+      <c r="J11" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K11)),RIGHT(K11,LEN(K11)-FIND(" ",K11)))</f>
         <v>afumigatus</v>
       </c>
@@ -18091,7 +18116,7 @@
       <c r="F12" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="J12" s="77" t="str">
+      <c r="J12" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K12)),RIGHT(K12,LEN(K12)-FIND(" ",K12)))</f>
         <v>afumigatus</v>
       </c>
@@ -18112,7 +18137,7 @@
         <f aca="false">SUM(F1:F12)</f>
         <v>106</v>
       </c>
-      <c r="J13" s="77" t="str">
+      <c r="J13" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K13)),RIGHT(K13,LEN(K13)-FIND(" ",K13)))</f>
         <v>afumigatus</v>
       </c>
@@ -18121,7 +18146,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J14" s="77" t="str">
+      <c r="J14" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K14)),RIGHT(K14,LEN(K14)-FIND(" ",K14)))</f>
         <v>afumigatus</v>
       </c>
@@ -18130,7 +18155,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J15" s="77" t="str">
+      <c r="J15" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K15)),RIGHT(K15,LEN(K15)-FIND(" ",K15)))</f>
         <v>afumigatus</v>
       </c>
@@ -18139,7 +18164,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J16" s="77" t="str">
+      <c r="J16" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K16)),RIGHT(K16,LEN(K16)-FIND(" ",K16)))</f>
         <v>afumigatus</v>
       </c>
@@ -18148,7 +18173,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J17" s="77" t="str">
+      <c r="J17" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K17)),RIGHT(K17,LEN(K17)-FIND(" ",K17)))</f>
         <v>amarginale</v>
       </c>
@@ -18164,7 +18189,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J18" s="77" t="str">
+      <c r="J18" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K18)),RIGHT(K18,LEN(K18)-FIND(" ",K18)))</f>
         <v>aniger</v>
       </c>
@@ -18180,7 +18205,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J19" s="77" t="str">
+      <c r="J19" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K19)),RIGHT(K19,LEN(K19)-FIND(" ",K19)))</f>
         <v>aparasiticus</v>
       </c>
@@ -18196,7 +18221,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J20" s="78" t="s">
+      <c r="J20" s="77" t="s">
         <v>1076</v>
       </c>
       <c r="K20" s="6" t="s">
@@ -18211,7 +18236,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J21" s="77" t="str">
+      <c r="J21" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K21)),RIGHT(K21,LEN(K21)-FIND(" ",K21)))</f>
         <v>aterreus</v>
       </c>
@@ -18227,7 +18252,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J22" s="77" t="str">
+      <c r="J22" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K22)),RIGHT(K22,LEN(K22)-FIND(" ",K22)))</f>
         <v>aviscosus</v>
       </c>
@@ -18243,7 +18268,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J23" s="77" t="str">
+      <c r="J23" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K23)),RIGHT(K23,LEN(K23)-FIND(" ",K23)))</f>
         <v>babortus</v>
       </c>
@@ -18259,7 +18284,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J24" s="78" t="s">
+      <c r="J24" s="77" t="s">
         <v>1077</v>
       </c>
       <c r="K24" s="6" t="s">
@@ -18274,7 +18299,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J25" s="77" t="str">
+      <c r="J25" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K25)),RIGHT(K25,LEN(K25)-FIND(" ",K25)))</f>
         <v>babortus</v>
       </c>
@@ -18283,7 +18308,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J26" s="77" t="str">
+      <c r="J26" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K26)),RIGHT(K26,LEN(K26)-FIND(" ",K26)))</f>
         <v>babortus</v>
       </c>
@@ -18292,7 +18317,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J27" s="77" t="str">
+      <c r="J27" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K27)),RIGHT(K27,LEN(K27)-FIND(" ",K27)))</f>
         <v>banthracis</v>
       </c>
@@ -18308,7 +18333,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J28" s="77" t="str">
+      <c r="J28" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K28)),RIGHT(K28,LEN(K28)-FIND(" ",K28)))</f>
         <v>balphaherpesvirus 1</v>
       </c>
@@ -18317,7 +18342,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J29" s="77" t="str">
+      <c r="J29" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K29)),RIGHT(K29,LEN(K29)-FIND(" ",K29)))</f>
         <v>bbronchiseptica</v>
       </c>
@@ -18333,7 +18358,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J30" s="77" t="str">
+      <c r="J30" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K30)),RIGHT(K30,LEN(K30)-FIND(" ",K30)))</f>
         <v>banthracis</v>
       </c>
@@ -18342,7 +18367,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J31" s="77" t="str">
+      <c r="J31" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K31)),RIGHT(K31,LEN(K31)-FIND(" ",K31)))</f>
         <v>banthracis</v>
       </c>
@@ -18351,7 +18376,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J32" s="77" t="str">
+      <c r="J32" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K32)),RIGHT(K32,LEN(K32)-FIND(" ",K32)))</f>
         <v>bdermatitidis</v>
       </c>
@@ -18367,7 +18392,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J33" s="77" t="str">
+      <c r="J33" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K33)),RIGHT(K33,LEN(K33)-FIND(" ",K33)))</f>
         <v>bbronchiseptica</v>
       </c>
@@ -18376,7 +18401,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J34" s="77" t="str">
+      <c r="J34" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K34)),RIGHT(K34,LEN(K34)-FIND(" ",K34)))</f>
         <v>bbronchiseptica</v>
       </c>
@@ -18385,7 +18410,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J35" s="78" t="s">
+      <c r="J35" s="77" t="s">
         <v>1078</v>
       </c>
       <c r="K35" s="6" t="s">
@@ -18400,7 +18425,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J36" s="77" t="str">
+      <c r="J36" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K36)),RIGHT(K36,LEN(K36)-FIND(" ",K36)))</f>
         <v>bdermatitidis</v>
       </c>
@@ -18409,7 +18434,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J37" s="77" t="str">
+      <c r="J37" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K37)),RIGHT(K37,LEN(K37)-FIND(" ",K37)))</f>
         <v>bdermatitidis</v>
       </c>
@@ -18418,7 +18443,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J38" s="77" t="str">
+      <c r="J38" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K38)),RIGHT(K38,LEN(K38)-FIND(" ",K38)))</f>
         <v>bhyodysenteriae</v>
       </c>
@@ -18434,7 +18459,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J39" s="78" t="s">
+      <c r="J39" s="77" t="s">
         <v>1079</v>
       </c>
       <c r="K39" s="7" t="s">
@@ -18449,7 +18474,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J40" s="77" t="str">
+      <c r="J40" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K40)),RIGHT(K40,LEN(K40)-FIND(" ",K40)))</f>
         <v>bmelitensis</v>
       </c>
@@ -18465,7 +18490,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J41" s="78" t="s">
+      <c r="J41" s="77" t="s">
         <v>1080</v>
       </c>
       <c r="K41" s="6" t="s">
@@ -18480,7 +18505,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J42" s="77" t="str">
+      <c r="J42" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K42)),RIGHT(K42,LEN(K42)-FIND(" ",K42)))</f>
         <v>bmelitensis</v>
       </c>
@@ -18489,7 +18514,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J43" s="78" t="s">
+      <c r="J43" s="77" t="s">
         <v>1081</v>
       </c>
       <c r="K43" s="7" t="s">
@@ -18504,7 +18529,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J44" s="77" t="str">
+      <c r="J44" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K44)),RIGHT(K44,LEN(K44)-FIND(" ",K44)))</f>
         <v>branarum</v>
       </c>
@@ -18520,7 +18545,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J45" s="77" t="str">
+      <c r="J45" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K45)),RIGHT(K45,LEN(K45)-FIND(" ",K45)))</f>
         <v>bsuis</v>
       </c>
@@ -18536,7 +18561,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J46" s="78" t="s">
+      <c r="J46" s="77" t="s">
         <v>1082</v>
       </c>
       <c r="K46" s="7" t="s">
@@ -18551,7 +18576,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J47" s="78" t="s">
+      <c r="J47" s="77" t="s">
         <v>1083</v>
       </c>
       <c r="K47" s="6" t="s">
@@ -18566,7 +18591,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J48" s="77" t="str">
+      <c r="J48" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K48)),RIGHT(K48,LEN(K48)-FIND(" ",K48)))</f>
         <v>bviral diarrhea virus 1</v>
       </c>
@@ -18575,7 +18600,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J49" s="77" t="str">
+      <c r="J49" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K49)),RIGHT(K49,LEN(K49)-FIND(" ",K49)))</f>
         <v>bviral diarrhea virus 1</v>
       </c>
@@ -18584,7 +18609,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J50" s="77" t="str">
+      <c r="J50" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K50)),RIGHT(K50,LEN(K50)-FIND(" ",K50)))</f>
         <v>bvirus</v>
       </c>
@@ -18600,7 +18625,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J51" s="77" t="str">
+      <c r="J51" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K51)),RIGHT(K51,LEN(K51)-FIND(" ",K51)))</f>
         <v>bviral diarrhea virus 2</v>
       </c>
@@ -18609,7 +18634,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J52" s="77" t="str">
+      <c r="J52" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K52)),RIGHT(K52,LEN(K52)-FIND(" ",K52)))</f>
         <v>cabortus</v>
       </c>
@@ -18625,7 +18650,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J53" s="77" t="str">
+      <c r="J53" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K53)),RIGHT(K53,LEN(K53)-FIND(" ",K53)))</f>
         <v>bvirus</v>
       </c>
@@ -18634,7 +18659,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J54" s="78" t="s">
+      <c r="J54" s="77" t="s">
         <v>1084</v>
       </c>
       <c r="K54" s="7" t="s">
@@ -18649,7 +18674,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J55" s="77" t="str">
+      <c r="J55" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K55)),RIGHT(K55,LEN(K55)-FIND(" ",K55)))</f>
         <v>cabortus</v>
       </c>
@@ -18658,7 +18683,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J56" s="78" t="s">
+      <c r="J56" s="77" t="s">
         <v>1085</v>
       </c>
       <c r="K56" s="7" t="s">
@@ -18673,7 +18698,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J57" s="77" t="str">
+      <c r="J57" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K57)),RIGHT(K57,LEN(K57)-FIND(" ",K57)))</f>
         <v>calbicans</v>
       </c>
@@ -18689,7 +18714,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J58" s="77" t="str">
+      <c r="J58" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K58)),RIGHT(K58,LEN(K58)-FIND(" ",K58)))</f>
         <v>candersoni</v>
       </c>
@@ -18705,7 +18730,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J59" s="77" t="str">
+      <c r="J59" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K59)),RIGHT(K59,LEN(K59)-FIND(" ",K59)))</f>
         <v>calbicans</v>
       </c>
@@ -18714,7 +18739,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J60" s="77" t="str">
+      <c r="J60" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K60)),RIGHT(K60,LEN(K60)-FIND(" ",K60)))</f>
         <v>calbicans</v>
       </c>
@@ -18723,7 +18748,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J61" s="77" t="str">
+      <c r="J61" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K61)),RIGHT(K61,LEN(K61)-FIND(" ",K61)))</f>
         <v>calbicans</v>
       </c>
@@ -18732,7 +18757,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J62" s="77" t="str">
+      <c r="J62" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K62)),RIGHT(K62,LEN(K62)-FIND(" ",K62)))</f>
         <v>calbicans</v>
       </c>
@@ -18741,7 +18766,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J63" s="77" t="str">
+      <c r="J63" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K63)),RIGHT(K63,LEN(K63)-FIND(" ",K63)))</f>
         <v>calbicans</v>
       </c>
@@ -18750,7 +18775,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J64" s="77" t="str">
+      <c r="J64" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K64)),RIGHT(K64,LEN(K64)-FIND(" ",K64)))</f>
         <v>calbicans</v>
       </c>
@@ -18759,7 +18784,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J65" s="77" t="str">
+      <c r="J65" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K65)),RIGHT(K65,LEN(K65)-FIND(" ",K65)))</f>
         <v>calbicans</v>
       </c>
@@ -18768,7 +18793,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J66" s="78" t="s">
+      <c r="J66" s="77" t="s">
         <v>1086</v>
       </c>
       <c r="K66" s="7" t="s">
@@ -18783,7 +18808,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J67" s="77" t="str">
+      <c r="J67" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K67)),RIGHT(K67,LEN(K67)-FIND(" ",K67)))</f>
         <v>cauris</v>
       </c>
@@ -18799,7 +18824,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J68" s="77" t="str">
+      <c r="J68" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K68)),RIGHT(K68,LEN(K68)-FIND(" ",K68)))</f>
         <v>cbantiana</v>
       </c>
@@ -18815,7 +18840,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J69" s="78" t="s">
+      <c r="J69" s="77" t="s">
         <v>1087</v>
       </c>
       <c r="K69" s="7" t="s">
@@ -18830,7 +18855,7 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J70" s="77" t="str">
+      <c r="J70" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K70)),RIGHT(K70,LEN(K70)-FIND(" ",K70)))</f>
         <v>cbantiana</v>
       </c>
@@ -18839,7 +18864,7 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J71" s="77" t="str">
+      <c r="J71" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K71)),RIGHT(K71,LEN(K71)-FIND(" ",K71)))</f>
         <v>cbantiana</v>
       </c>
@@ -18848,7 +18873,7 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J72" s="77" t="str">
+      <c r="J72" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K72)),RIGHT(K72,LEN(K72)-FIND(" ",K72)))</f>
         <v>cbovis</v>
       </c>
@@ -18864,7 +18889,7 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J73" s="77" t="str">
+      <c r="J73" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K73)),RIGHT(K73,LEN(K73)-FIND(" ",K73)))</f>
         <v>cburnetii</v>
       </c>
@@ -18880,7 +18905,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J74" s="77" t="str">
+      <c r="J74" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K74)),RIGHT(K74,LEN(K74)-FIND(" ",K74)))</f>
         <v>ccoronatus</v>
       </c>
@@ -18896,7 +18921,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J75" s="77" t="str">
+      <c r="J75" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K75)),RIGHT(K75,LEN(K75)-FIND(" ",K75)))</f>
         <v>cburnetii</v>
       </c>
@@ -18905,7 +18930,7 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J76" s="77" t="str">
+      <c r="J76" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K76)),RIGHT(K76,LEN(K76)-FIND(" ",K76)))</f>
         <v>ccoronavirus</v>
       </c>
@@ -18921,7 +18946,7 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J77" s="77" t="str">
+      <c r="J77" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K77)),RIGHT(K77,LEN(K77)-FIND(" ",K77)))</f>
         <v>cdifficile</v>
       </c>
@@ -18937,7 +18962,7 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J78" s="77" t="str">
+      <c r="J78" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K78)),RIGHT(K78,LEN(K78)-FIND(" ",K78)))</f>
         <v>cfelis</v>
       </c>
@@ -18953,7 +18978,7 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J79" s="77" t="str">
+      <c r="J79" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K79)),RIGHT(K79,LEN(K79)-FIND(" ",K79)))</f>
         <v>cgattii</v>
       </c>
@@ -18969,7 +18994,7 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J80" s="78" t="s">
+      <c r="J80" s="77" t="s">
         <v>1088</v>
       </c>
       <c r="K80" s="7" t="s">
@@ -18984,7 +19009,7 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J81" s="77" t="str">
+      <c r="J81" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K81)),RIGHT(K81,LEN(K81)-FIND(" ",K81)))</f>
         <v>cgattii</v>
       </c>
@@ -18993,7 +19018,7 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J82" s="77" t="str">
+      <c r="J82" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K82)),RIGHT(K82,LEN(K82)-FIND(" ",K82)))</f>
         <v>cgattii</v>
       </c>
@@ -19002,7 +19027,7 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J83" s="77" t="str">
+      <c r="J83" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K83)),RIGHT(K83,LEN(K83)-FIND(" ",K83)))</f>
         <v>cgattii</v>
       </c>
@@ -19011,7 +19036,7 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J84" s="77" t="str">
+      <c r="J84" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K84)),RIGHT(K84,LEN(K84)-FIND(" ",K84)))</f>
         <v>cgattii</v>
       </c>
@@ -19020,7 +19045,7 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J85" s="77" t="str">
+      <c r="J85" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K85)),RIGHT(K85,LEN(K85)-FIND(" ",K85)))</f>
         <v>cimmitis</v>
       </c>
@@ -19036,7 +19061,7 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J86" s="77" t="str">
+      <c r="J86" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K86)),RIGHT(K86,LEN(K86)-FIND(" ",K86)))</f>
         <v>cjejuni</v>
       </c>
@@ -19052,7 +19077,7 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J87" s="77" t="str">
+      <c r="J87" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K87)),RIGHT(K87,LEN(K87)-FIND(" ",K87)))</f>
         <v>cimmitis</v>
       </c>
@@ -19061,7 +19086,7 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J88" s="77" t="str">
+      <c r="J88" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K88)),RIGHT(K88,LEN(K88)-FIND(" ",K88)))</f>
         <v>cneoformans</v>
       </c>
@@ -19077,7 +19102,7 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J89" s="77" t="str">
+      <c r="J89" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K89)),RIGHT(K89,LEN(K89)-FIND(" ",K89)))</f>
         <v>cjejuni</v>
       </c>
@@ -19086,7 +19111,7 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J90" s="78" t="s">
+      <c r="J90" s="77" t="s">
         <v>1090</v>
       </c>
       <c r="K90" s="7" t="s">
@@ -19101,7 +19126,7 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J91" s="77" t="str">
+      <c r="J91" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K91)),RIGHT(K91,LEN(K91)-FIND(" ",K91)))</f>
         <v>cneoformans</v>
       </c>
@@ -19110,7 +19135,7 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J92" s="77" t="str">
+      <c r="J92" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K92)),RIGHT(K92,LEN(K92)-FIND(" ",K92)))</f>
         <v>cneoformans</v>
       </c>
@@ -19119,7 +19144,7 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J93" s="77" t="str">
+      <c r="J93" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K93)),RIGHT(K93,LEN(K93)-FIND(" ",K93)))</f>
         <v>cneoformans</v>
       </c>
@@ -19128,7 +19153,7 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J94" s="77" t="str">
+      <c r="J94" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K94)),RIGHT(K94,LEN(K94)-FIND(" ",K94)))</f>
         <v>cparvovirus</v>
       </c>
@@ -19144,7 +19169,7 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J95" s="77" t="str">
+      <c r="J95" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K95)),RIGHT(K95,LEN(K95)-FIND(" ",K95)))</f>
         <v>cparvum</v>
       </c>
@@ -19160,7 +19185,7 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J96" s="78" t="s">
+      <c r="J96" s="77" t="s">
         <v>1091</v>
       </c>
       <c r="K96" s="7" t="s">
@@ -19175,7 +19200,7 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J97" s="78" t="s">
+      <c r="J97" s="77" t="s">
         <v>1092</v>
       </c>
       <c r="K97" s="7" t="s">
@@ -19190,7 +19215,7 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J98" s="78" t="s">
+      <c r="J98" s="77" t="s">
         <v>1093</v>
       </c>
       <c r="K98" s="7" t="s">
@@ -19205,7 +19230,7 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J99" s="78" t="s">
+      <c r="J99" s="77" t="s">
         <v>1094</v>
       </c>
       <c r="K99" s="7" t="s">
@@ -19220,7 +19245,7 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J100" s="78" t="s">
+      <c r="J100" s="77" t="s">
         <v>1095</v>
       </c>
       <c r="K100" s="7" t="s">
@@ -19235,7 +19260,7 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J101" s="77" t="str">
+      <c r="J101" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K101)),RIGHT(K101,LEN(K101)-FIND(" ",K101)))</f>
         <v>cperfringens C</v>
       </c>
@@ -19244,7 +19269,7 @@
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J102" s="77" t="str">
+      <c r="J102" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K102)),RIGHT(K102,LEN(K102)-FIND(" ",K102)))</f>
         <v>cpseudotuberculosis</v>
       </c>
@@ -19260,7 +19285,7 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J103" s="77" t="str">
+      <c r="J103" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K103)),RIGHT(K103,LEN(K103)-FIND(" ",K103)))</f>
         <v>cpsittaci</v>
       </c>
@@ -19276,7 +19301,7 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J104" s="77" t="str">
+      <c r="J104" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K104)),RIGHT(K104,LEN(K104)-FIND(" ",K104)))</f>
         <v>cpseudotuberculosis</v>
       </c>
@@ -19285,7 +19310,7 @@
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J105" s="77" t="str">
+      <c r="J105" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K105)),RIGHT(K105,LEN(K105)-FIND(" ",K105)))</f>
         <v>cpurpurea</v>
       </c>
@@ -19301,7 +19326,7 @@
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J106" s="77" t="str">
+      <c r="J106" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K106)),RIGHT(K106,LEN(K106)-FIND(" ",K106)))</f>
         <v>cryanae</v>
       </c>
@@ -19317,7 +19342,7 @@
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J107" s="78" t="s">
+      <c r="J107" s="77" t="s">
         <v>1096</v>
       </c>
       <c r="K107" s="6" t="s">
@@ -19332,7 +19357,7 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J108" s="77" t="str">
+      <c r="J108" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K108)),RIGHT(K108,LEN(K108)-FIND(" ",K108)))</f>
         <v>ctetani</v>
       </c>
@@ -19348,7 +19373,7 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J109" s="77" t="str">
+      <c r="J109" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K109)),RIGHT(K109,LEN(K109)-FIND(" ",K109)))</f>
         <v>ctrachomatis</v>
       </c>
@@ -19364,7 +19389,7 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J110" s="77" t="str">
+      <c r="J110" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K110)),RIGHT(K110,LEN(K110)-FIND(" ",K110)))</f>
         <v>ctetani</v>
       </c>
@@ -19373,7 +19398,7 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J111" s="77" t="str">
+      <c r="J111" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K111)),RIGHT(K111,LEN(K111)-FIND(" ",K111)))</f>
         <v>ctetani</v>
       </c>
@@ -19382,7 +19407,7 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J112" s="77" t="str">
+      <c r="J112" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K112)),RIGHT(K112,LEN(K112)-FIND(" ",K112)))</f>
         <v>ctetani</v>
       </c>
@@ -19391,7 +19416,7 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J113" s="78" t="s">
+      <c r="J113" s="77" t="s">
         <v>1097</v>
       </c>
       <c r="K113" s="7" t="s">
@@ -19406,7 +19431,7 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J114" s="77" t="str">
+      <c r="J114" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K114)),RIGHT(K114,LEN(K114)-FIND(" ",K114)))</f>
         <v>dcongolensis</v>
       </c>
@@ -19422,7 +19447,7 @@
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J115" s="77" t="str">
+      <c r="J115" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K115)),RIGHT(K115,LEN(K115)-FIND(" ",K115)))</f>
         <v>dnodosus</v>
       </c>
@@ -19438,7 +19463,7 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J116" s="78" t="s">
+      <c r="J116" s="77" t="s">
         <v>1101</v>
       </c>
       <c r="K116" s="7" t="s">
@@ -19453,7 +19478,7 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J117" s="77" t="str">
+      <c r="J117" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K117)),RIGHT(K117,LEN(K117)-FIND(" ",K117)))</f>
         <v>dnodosus</v>
       </c>
@@ -19462,7 +19487,7 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J118" s="78" t="s">
+      <c r="J118" s="77" t="s">
         <v>1102</v>
       </c>
       <c r="K118" s="7" t="s">
@@ -19477,7 +19502,7 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J119" s="78" t="s">
+      <c r="J119" s="77" t="s">
         <v>1103</v>
       </c>
       <c r="K119" s="7" t="s">
@@ -19492,7 +19517,7 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J120" s="78" t="s">
+      <c r="J120" s="77" t="s">
         <v>1104</v>
       </c>
       <c r="K120" s="7" t="s">
@@ -19507,7 +19532,7 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J121" s="77" t="str">
+      <c r="J121" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K121)),RIGHT(K121,LEN(K121)-FIND(" ",K121)))</f>
         <v>ecoli</v>
       </c>
@@ -19523,7 +19548,7 @@
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J122" s="78" t="s">
+      <c r="J122" s="77" t="s">
         <v>1105</v>
       </c>
       <c r="K122" s="0" t="s">
@@ -19538,7 +19563,7 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J123" s="77" t="str">
+      <c r="J123" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K123)),RIGHT(K123,LEN(K123)-FIND(" ",K123)))</f>
         <v>ecoli</v>
       </c>
@@ -19547,7 +19572,7 @@
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J124" s="77" t="str">
+      <c r="J124" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K124)),RIGHT(K124,LEN(K124)-FIND(" ",K124)))</f>
         <v>ecoli</v>
       </c>
@@ -19556,7 +19581,7 @@
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J125" s="77" t="str">
+      <c r="J125" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K125)),RIGHT(K125,LEN(K125)-FIND(" ",K125)))</f>
         <v>ecoli</v>
       </c>
@@ -19565,7 +19590,7 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J126" s="77" t="str">
+      <c r="J126" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K126)),RIGHT(K126,LEN(K126)-FIND(" ",K126)))</f>
         <v>ecoli</v>
       </c>
@@ -19574,7 +19599,7 @@
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J127" s="77" t="str">
+      <c r="J127" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K127)),RIGHT(K127,LEN(K127)-FIND(" ",K127)))</f>
         <v>ecoli</v>
       </c>
@@ -19583,7 +19608,7 @@
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J128" s="77" t="str">
+      <c r="J128" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K128)),RIGHT(K128,LEN(K128)-FIND(" ",K128)))</f>
         <v>ecoli</v>
       </c>
@@ -19592,7 +19617,7 @@
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J129" s="77" t="str">
+      <c r="J129" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K129)),RIGHT(K129,LEN(K129)-FIND(" ",K129)))</f>
         <v>edermatitidis</v>
       </c>
@@ -19608,7 +19633,7 @@
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J130" s="78" t="s">
+      <c r="J130" s="77" t="s">
         <v>1106</v>
       </c>
       <c r="K130" s="7" t="s">
@@ -19623,7 +19648,7 @@
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J131" s="77" t="str">
+      <c r="J131" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K131)),RIGHT(K131,LEN(K131)-FIND(" ",K131)))</f>
         <v>edermatitidis</v>
       </c>
@@ -19632,7 +19657,7 @@
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J132" s="77" t="str">
+      <c r="J132" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K132)),RIGHT(K132,LEN(K132)-FIND(" ",K132)))</f>
         <v>edermatitidis</v>
       </c>
@@ -19641,7 +19666,7 @@
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J133" s="78" t="s">
+      <c r="J133" s="77" t="s">
         <v>1107</v>
       </c>
       <c r="K133" s="6" t="s">
@@ -19656,7 +19681,7 @@
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J134" s="78" t="s">
+      <c r="J134" s="77" t="s">
         <v>1108</v>
       </c>
       <c r="K134" s="6" t="s">
@@ -19671,7 +19696,7 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J135" s="77" t="str">
+      <c r="J135" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K135)),RIGHT(K135,LEN(K135)-FIND(" ",K135)))</f>
         <v>ehemorrhagic disease virus</v>
       </c>
@@ -19680,7 +19705,7 @@
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J136" s="78" t="s">
+      <c r="J136" s="77" t="s">
         <v>1109</v>
       </c>
       <c r="K136" s="7" t="s">
@@ -19695,7 +19720,7 @@
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J137" s="78" t="s">
+      <c r="J137" s="77" t="s">
         <v>1110</v>
       </c>
       <c r="K137" s="7" t="s">
@@ -19710,7 +19735,7 @@
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J138" s="77" t="str">
+      <c r="J138" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K138)),RIGHT(K138,LEN(K138)-FIND(" ",K138)))</f>
         <v>erhusiopathiae</v>
       </c>
@@ -19726,7 +19751,7 @@
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J139" s="77" t="str">
+      <c r="J139" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K139)),RIGHT(K139,LEN(K139)-FIND(" ",K139)))</f>
         <v>erotavirus</v>
       </c>
@@ -19742,7 +19767,7 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J140" s="78" t="s">
+      <c r="J140" s="77" t="s">
         <v>1111</v>
       </c>
       <c r="K140" s="7" t="s">
@@ -19757,7 +19782,7 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J141" s="77" t="str">
+      <c r="J141" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K141)),RIGHT(K141,LEN(K141)-FIND(" ",K141)))</f>
         <v>fcalicivirus</v>
       </c>
@@ -19773,7 +19798,7 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J142" s="78" t="s">
+      <c r="J142" s="77" t="s">
         <v>1112</v>
       </c>
       <c r="K142" s="7" t="s">
@@ -19788,7 +19813,7 @@
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J143" s="77" t="str">
+      <c r="J143" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K143)),RIGHT(K143,LEN(K143)-FIND(" ",K143)))</f>
         <v>fgraminearum</v>
       </c>
@@ -19804,7 +19829,7 @@
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J144" s="77" t="str">
+      <c r="J144" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K144)),RIGHT(K144,LEN(K144)-FIND(" ",K144)))</f>
         <v>fdisease virus</v>
       </c>
@@ -19813,7 +19838,7 @@
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J145" s="77" t="str">
+      <c r="J145" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K145)),RIGHT(K145,LEN(K145)-FIND(" ",K145)))</f>
         <v>fdisease virus</v>
       </c>
@@ -19822,7 +19847,7 @@
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J146" s="77" t="str">
+      <c r="J146" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K146)),RIGHT(K146,LEN(K146)-FIND(" ",K146)))</f>
         <v>fdisease virus</v>
       </c>
@@ -19831,7 +19856,7 @@
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J147" s="77" t="str">
+      <c r="J147" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K147)),RIGHT(K147,LEN(K147)-FIND(" ",K147)))</f>
         <v>fdisease virus</v>
       </c>
@@ -19840,7 +19865,7 @@
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J148" s="77" t="str">
+      <c r="J148" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K148)),RIGHT(K148,LEN(K148)-FIND(" ",K148)))</f>
         <v>fdisease virus</v>
       </c>
@@ -19849,7 +19874,7 @@
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J149" s="78" t="s">
+      <c r="J149" s="77" t="s">
         <v>1113</v>
       </c>
       <c r="K149" s="7" t="s">
@@ -19864,7 +19889,7 @@
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J150" s="78" t="s">
+      <c r="J150" s="77" t="s">
         <v>1114</v>
       </c>
       <c r="K150" s="7" t="s">
@@ -19879,7 +19904,7 @@
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J151" s="78" t="s">
+      <c r="J151" s="77" t="s">
         <v>1115</v>
       </c>
       <c r="K151" s="7" t="s">
@@ -19894,7 +19919,7 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J152" s="77" t="str">
+      <c r="J152" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K152)),RIGHT(K152,LEN(K152)-FIND(" ",K152)))</f>
         <v>fnecrophorum</v>
       </c>
@@ -19910,7 +19935,7 @@
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J153" s="78" t="s">
+      <c r="J153" s="77" t="s">
         <v>1116</v>
       </c>
       <c r="K153" s="7" t="s">
@@ -19925,7 +19950,7 @@
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J154" s="77" t="str">
+      <c r="J154" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K154)),RIGHT(K154,LEN(K154)-FIND(" ",K154)))</f>
         <v>fnecrophorum</v>
       </c>
@@ -19934,7 +19959,7 @@
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J155" s="77" t="str">
+      <c r="J155" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K155)),RIGHT(K155,LEN(K155)-FIND(" ",K155)))</f>
         <v>fproliferatum</v>
       </c>
@@ -19950,7 +19975,7 @@
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J156" s="77" t="str">
+      <c r="J156" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K156)),RIGHT(K156,LEN(K156)-FIND(" ",K156)))</f>
         <v>fverticillioides</v>
       </c>
@@ -19966,7 +19991,7 @@
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J157" s="77" t="str">
+      <c r="J157" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K157)),RIGHT(K157,LEN(K157)-FIND(" ",K157)))</f>
         <v>fproliferatum</v>
       </c>
@@ -19975,7 +20000,7 @@
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J158" s="77" t="str">
+      <c r="J158" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K158)),RIGHT(K158,LEN(K158)-FIND(" ",K158)))</f>
         <v>fvirus</v>
       </c>
@@ -19991,7 +20016,7 @@
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J159" s="77" t="str">
+      <c r="J159" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K159)),RIGHT(K159,LEN(K159)-FIND(" ",K159)))</f>
         <v>fverticillioides (moniliforme)</v>
       </c>
@@ -20000,7 +20025,7 @@
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J160" s="78" t="s">
+      <c r="J160" s="77" t="s">
         <v>1119</v>
       </c>
       <c r="K160" s="7" t="s">
@@ -20015,7 +20040,7 @@
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J161" s="78" t="s">
+      <c r="J161" s="77" t="s">
         <v>1120</v>
       </c>
       <c r="K161" s="0" t="s">
@@ -20030,7 +20055,7 @@
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J162" s="78" t="s">
+      <c r="J162" s="77" t="s">
         <v>1121</v>
       </c>
       <c r="K162" s="0" t="s">
@@ -20045,7 +20070,7 @@
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J163" s="78" t="s">
+      <c r="J163" s="77" t="s">
         <v>1122</v>
       </c>
       <c r="K163" s="0" t="s">
@@ -20060,7 +20085,7 @@
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J164" s="77" t="str">
+      <c r="J164" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K164)),RIGHT(K164,LEN(K164)-FIND(" ",K164)))</f>
         <v>hcapsulatum</v>
       </c>
@@ -20076,7 +20101,7 @@
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J165" s="78" t="s">
+      <c r="J165" s="77" t="s">
         <v>1123</v>
       </c>
       <c r="K165" s="7" t="s">
@@ -20091,7 +20116,7 @@
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J166" s="77" t="str">
+      <c r="J166" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K166)),RIGHT(K166,LEN(K166)-FIND(" ",K166)))</f>
         <v>hcapsulatum</v>
       </c>
@@ -20100,7 +20125,7 @@
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J167" s="77" t="str">
+      <c r="J167" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K167)),RIGHT(K167,LEN(K167)-FIND(" ",K167)))</f>
         <v>hcapsulatum</v>
       </c>
@@ -20109,7 +20134,7 @@
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J168" s="78" t="s">
+      <c r="J168" s="77" t="s">
         <v>1126</v>
       </c>
       <c r="K168" s="0" t="s">
@@ -20124,7 +20149,7 @@
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J169" s="78" t="s">
+      <c r="J169" s="77" t="s">
         <v>1127</v>
       </c>
       <c r="K169" s="0" t="s">
@@ -20139,7 +20164,7 @@
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J170" s="78" t="s">
+      <c r="J170" s="77" t="s">
         <v>1128</v>
       </c>
       <c r="K170" s="0" t="s">
@@ -20154,7 +20179,7 @@
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J171" s="78" t="s">
+      <c r="J171" s="77" t="s">
         <v>1129</v>
       </c>
       <c r="K171" s="0" t="s">
@@ -20169,7 +20194,7 @@
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J172" s="78" t="s">
+      <c r="J172" s="77" t="s">
         <v>1130</v>
       </c>
       <c r="K172" s="56" t="s">
@@ -20184,7 +20209,7 @@
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J173" s="78" t="s">
+      <c r="J173" s="77" t="s">
         <v>1131</v>
       </c>
       <c r="K173" s="0" t="s">
@@ -20199,7 +20224,7 @@
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J174" s="78" t="s">
+      <c r="J174" s="77" t="s">
         <v>1132</v>
       </c>
       <c r="K174" s="0" t="s">
@@ -20214,7 +20239,7 @@
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J175" s="78" t="s">
+      <c r="J175" s="77" t="s">
         <v>1133</v>
       </c>
       <c r="K175" s="0" t="s">
@@ -20229,7 +20254,7 @@
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J176" s="78" t="s">
+      <c r="J176" s="77" t="s">
         <v>1134</v>
       </c>
       <c r="K176" s="7" t="s">
@@ -20244,7 +20269,7 @@
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J177" s="78" t="s">
+      <c r="J177" s="77" t="s">
         <v>1135</v>
       </c>
       <c r="K177" s="0" t="s">
@@ -20259,7 +20284,7 @@
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J178" s="78" t="s">
+      <c r="J178" s="77" t="s">
         <v>1136</v>
       </c>
       <c r="K178" s="7" t="s">
@@ -20274,7 +20299,7 @@
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J179" s="78" t="s">
+      <c r="J179" s="77" t="s">
         <v>1137</v>
       </c>
       <c r="K179" s="0" t="s">
@@ -20289,7 +20314,7 @@
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J180" s="77" t="str">
+      <c r="J180" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K180)),RIGHT(K180,LEN(K180)-FIND(" ",K180)))</f>
         <v>iA (H3N2)</v>
       </c>
@@ -20298,7 +20323,7 @@
       </c>
     </row>
     <row r="181" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J181" s="77" t="str">
+      <c r="J181" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K181)),RIGHT(K181,LEN(K181)-FIND(" ",K181)))</f>
         <v>lautumnalis</v>
       </c>
@@ -20314,7 +20339,7 @@
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J182" s="77" t="str">
+      <c r="J182" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K182)),RIGHT(K182,LEN(K182)-FIND(" ",K182)))</f>
         <v>lborgpetersenii</v>
       </c>
@@ -20330,7 +20355,7 @@
       </c>
     </row>
     <row r="183" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J183" s="77" t="str">
+      <c r="J183" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K183)),RIGHT(K183,LEN(K183)-FIND(" ",K183)))</f>
         <v>lgrippothyphosa</v>
       </c>
@@ -20346,7 +20371,7 @@
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J184" s="77" t="str">
+      <c r="J184" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K184)),RIGHT(K184,LEN(K184)-FIND(" ",K184)))</f>
         <v>lborgpetersenii</v>
       </c>
@@ -20355,7 +20380,7 @@
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J185" s="77" t="str">
+      <c r="J185" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K185)),RIGHT(K185,LEN(K185)-FIND(" ",K185)))</f>
         <v>lhyos</v>
       </c>
@@ -20371,7 +20396,7 @@
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J186" s="77" t="str">
+      <c r="J186" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K186)),RIGHT(K186,LEN(K186)-FIND(" ",K186)))</f>
         <v>linterrogans</v>
       </c>
@@ -20387,7 +20412,7 @@
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J187" s="77" t="str">
+      <c r="J187" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K187)),RIGHT(K187,LEN(K187)-FIND(" ",K187)))</f>
         <v>lintracellularis</v>
       </c>
@@ -20403,7 +20428,7 @@
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J188" s="77" t="str">
+      <c r="J188" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K188)),RIGHT(K188,LEN(K188)-FIND(" ",K188)))</f>
         <v>linterrogans</v>
       </c>
@@ -20412,7 +20437,7 @@
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J189" s="77" t="str">
+      <c r="J189" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K189)),RIGHT(K189,LEN(K189)-FIND(" ",K189)))</f>
         <v>linterrogans</v>
       </c>
@@ -20421,7 +20446,7 @@
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J190" s="77" t="str">
+      <c r="J190" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K190)),RIGHT(K190,LEN(K190)-FIND(" ",K190)))</f>
         <v>linterrogans</v>
       </c>
@@ -20430,7 +20455,7 @@
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J191" s="77" t="str">
+      <c r="J191" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K191)),RIGHT(K191,LEN(K191)-FIND(" ",K191)))</f>
         <v>lkirschneri</v>
       </c>
@@ -20446,7 +20471,7 @@
       </c>
     </row>
     <row r="192" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J192" s="77" t="str">
+      <c r="J192" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K192)),RIGHT(K192,LEN(K192)-FIND(" ",K192)))</f>
         <v>lmonocytogenes</v>
       </c>
@@ -20462,7 +20487,7 @@
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J193" s="77" t="str">
+      <c r="J193" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K193)),RIGHT(K193,LEN(K193)-FIND(" ",K193)))</f>
         <v>lkirschneri</v>
       </c>
@@ -20471,7 +20496,7 @@
       </c>
     </row>
     <row r="194" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J194" s="77" t="str">
+      <c r="J194" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K194)),RIGHT(K194,LEN(K194)-FIND(" ",K194)))</f>
         <v>lpomona</v>
       </c>
@@ -20487,7 +20512,7 @@
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J195" s="77" t="str">
+      <c r="J195" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K195)),RIGHT(K195,LEN(K195)-FIND(" ",K195)))</f>
         <v>lrabies</v>
       </c>
@@ -20503,7 +20528,7 @@
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J196" s="78" t="s">
+      <c r="J196" s="77" t="s">
         <v>1139</v>
       </c>
       <c r="K196" s="6" t="s">
@@ -20518,7 +20543,7 @@
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J197" s="77" t="str">
+      <c r="J197" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K197)),RIGHT(K197,LEN(K197)-FIND(" ",K197)))</f>
         <v>lrabies</v>
       </c>
@@ -20527,7 +20552,7 @@
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J198" s="77" t="str">
+      <c r="J198" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K198)),RIGHT(K198,LEN(K198)-FIND(" ",K198)))</f>
         <v>lrabies</v>
       </c>
@@ -20536,7 +20561,7 @@
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J199" s="78" t="s">
+      <c r="J199" s="77" t="s">
         <v>1140</v>
       </c>
       <c r="K199" s="7" t="s">
@@ -20551,7 +20576,7 @@
       </c>
     </row>
     <row r="200" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J200" s="77" t="str">
+      <c r="J200" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K200)),RIGHT(K200,LEN(K200)-FIND(" ",K200)))</f>
         <v>lskin disease virus</v>
       </c>
@@ -20560,7 +20585,7 @@
       </c>
     </row>
     <row r="201" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J201" s="77" t="str">
+      <c r="J201" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K201)),RIGHT(K201,LEN(K201)-FIND(" ",K201)))</f>
         <v>malcelaphinegamma1</v>
       </c>
@@ -20576,7 +20601,7 @@
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J202" s="78" t="s">
+      <c r="J202" s="77" t="s">
         <v>1141</v>
       </c>
       <c r="K202" s="7" t="s">
@@ -20591,7 +20616,7 @@
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J203" s="77" t="str">
+      <c r="J203" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K203)),RIGHT(K203,LEN(K203)-FIND(" ",K203)))</f>
         <v>mbovis</v>
       </c>
@@ -20607,7 +20632,7 @@
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J204" s="77" t="str">
+      <c r="J204" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K204)),RIGHT(K204,LEN(K204)-FIND(" ",K204)))</f>
         <v>mavium subsp. Paratuberculosis</v>
       </c>
@@ -20616,7 +20641,7 @@
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J205" s="77" t="str">
+      <c r="J205" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K205)),RIGHT(K205,LEN(K205)-FIND(" ",K205)))</f>
         <v>mavium subsp. Paratuberculosis</v>
       </c>
@@ -20625,7 +20650,7 @@
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J206" s="77" t="str">
+      <c r="J206" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K206)),RIGHT(K206,LEN(K206)-FIND(" ",K206)))</f>
         <v>mcanis</v>
       </c>
@@ -20641,7 +20666,7 @@
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J207" s="77" t="str">
+      <c r="J207" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K207)),RIGHT(K207,LEN(K207)-FIND(" ",K207)))</f>
         <v>mbovis</v>
       </c>
@@ -20650,7 +20675,7 @@
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J208" s="77" t="str">
+      <c r="J208" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K208)),RIGHT(K208,LEN(K208)-FIND(" ",K208)))</f>
         <v>mbovis</v>
       </c>
@@ -20659,7 +20684,7 @@
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J209" s="77" t="str">
+      <c r="J209" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K209)),RIGHT(K209,LEN(K209)-FIND(" ",K209)))</f>
         <v>mcanis</v>
       </c>
@@ -20675,7 +20700,7 @@
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J210" s="78" t="s">
+      <c r="J210" s="77" t="s">
         <v>1144</v>
       </c>
       <c r="K210" s="7" t="s">
@@ -20690,7 +20715,7 @@
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J211" s="77" t="str">
+      <c r="J211" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K211)),RIGHT(K211,LEN(K211)-FIND(" ",K211)))</f>
         <v>mcanis</v>
       </c>
@@ -20699,7 +20724,7 @@
       </c>
     </row>
     <row r="212" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J212" s="77" t="str">
+      <c r="J212" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K212)),RIGHT(K212,LEN(K212)-FIND(" ",K212)))</f>
         <v>mcaprinegamma2</v>
       </c>
@@ -20715,7 +20740,7 @@
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J213" s="77" t="str">
+      <c r="J213" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K213)),RIGHT(K213,LEN(K213)-FIND(" ",K213)))</f>
         <v>mconjunctivae</v>
       </c>
@@ -20731,7 +20756,7 @@
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J214" s="78" t="s">
+      <c r="J214" s="77" t="s">
         <v>1145</v>
       </c>
       <c r="K214" s="7" t="s">
@@ -20746,7 +20771,7 @@
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J215" s="77" t="str">
+      <c r="J215" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K215)),RIGHT(K215,LEN(K215)-FIND(" ",K215)))</f>
         <v>mgallisepticum</v>
       </c>
@@ -20762,7 +20787,7 @@
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J216" s="77" t="str">
+      <c r="J216" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K216)),RIGHT(K216,LEN(K216)-FIND(" ",K216)))</f>
         <v>mhaemolytica</v>
       </c>
@@ -20778,7 +20803,7 @@
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J217" s="77" t="str">
+      <c r="J217" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K217)),RIGHT(K217,LEN(K217)-FIND(" ",K217)))</f>
         <v>mmycoides</v>
       </c>
@@ -20794,7 +20819,7 @@
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J218" s="77" t="str">
+      <c r="J218" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K218)),RIGHT(K218,LEN(K218)-FIND(" ",K218)))</f>
         <v>mhaemolytica</v>
       </c>
@@ -20803,7 +20828,7 @@
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J219" s="77" t="str">
+      <c r="J219" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K219)),RIGHT(K219,LEN(K219)-FIND(" ",K219)))</f>
         <v>mnanum</v>
       </c>
@@ -20819,7 +20844,7 @@
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J220" s="77" t="str">
+      <c r="J220" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K220)),RIGHT(K220,LEN(K220)-FIND(" ",K220)))</f>
         <v>movinegamma2</v>
       </c>
@@ -20835,7 +20860,7 @@
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J221" s="77" t="str">
+      <c r="J221" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K221)),RIGHT(K221,LEN(K221)-FIND(" ",K221)))</f>
         <v>movis</v>
       </c>
@@ -20851,7 +20876,7 @@
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J222" s="77" t="str">
+      <c r="J222" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K222)),RIGHT(K222,LEN(K222)-FIND(" ",K222)))</f>
         <v>mpachydermatis</v>
       </c>
@@ -20867,7 +20892,7 @@
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J223" s="77" t="str">
+      <c r="J223" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K223)),RIGHT(K223,LEN(K223)-FIND(" ",K223)))</f>
         <v>movis</v>
       </c>
@@ -20876,7 +20901,7 @@
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J224" s="77" t="str">
+      <c r="J224" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K224)),RIGHT(K224,LEN(K224)-FIND(" ",K224)))</f>
         <v>mplutonius</v>
       </c>
@@ -20892,7 +20917,7 @@
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J225" s="77" t="str">
+      <c r="J225" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K225)),RIGHT(K225,LEN(K225)-FIND(" ",K225)))</f>
         <v>mpachydermatis</v>
       </c>
@@ -20901,7 +20926,7 @@
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J226" s="77" t="str">
+      <c r="J226" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K226)),RIGHT(K226,LEN(K226)-FIND(" ",K226)))</f>
         <v>mtuberculosis</v>
       </c>
@@ -20917,7 +20942,7 @@
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J227" s="77" t="str">
+      <c r="J227" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K227)),RIGHT(K227,LEN(K227)-FIND(" ",K227)))</f>
         <v>napis</v>
       </c>
@@ -20933,7 +20958,7 @@
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J228" s="77" t="str">
+      <c r="J228" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K228)),RIGHT(K228,LEN(K228)-FIND(" ",K228)))</f>
         <v>nasteroides</v>
       </c>
@@ -20949,7 +20974,7 @@
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J229" s="77" t="str">
+      <c r="J229" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K229)),RIGHT(K229,LEN(K229)-FIND(" ",K229)))</f>
         <v>nbrasiliensis</v>
       </c>
@@ -20965,7 +20990,7 @@
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J230" s="78" t="s">
+      <c r="J230" s="77" t="s">
         <v>1150</v>
       </c>
       <c r="K230" s="7" t="s">
@@ -20980,7 +21005,7 @@
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J231" s="78" t="s">
+      <c r="J231" s="77" t="s">
         <v>1151</v>
       </c>
       <c r="K231" s="0" t="s">
@@ -20995,7 +21020,7 @@
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J232" s="77" t="str">
+      <c r="J232" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K232)),RIGHT(K232,LEN(K232)-FIND(" ",K232)))</f>
         <v>ngonorrhoeae</v>
       </c>
@@ -21011,7 +21036,7 @@
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J233" s="78" t="s">
+      <c r="J233" s="77" t="s">
         <v>1152</v>
       </c>
       <c r="K233" s="0" t="s">
@@ -21026,7 +21051,7 @@
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J234" s="77" t="str">
+      <c r="J234" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K234)),RIGHT(K234,LEN(K234)-FIND(" ",K234)))</f>
         <v>nmeningitidis</v>
       </c>
@@ -21042,7 +21067,7 @@
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J235" s="77" t="str">
+      <c r="J235" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K235)),RIGHT(K235,LEN(K235)-FIND(" ",K235)))</f>
         <v>nristicii</v>
       </c>
@@ -21058,7 +21083,7 @@
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J236" s="77" t="str">
+      <c r="J236" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K236)),RIGHT(K236,LEN(K236)-FIND(" ",K236)))</f>
         <v>ovirus</v>
       </c>
@@ -21074,7 +21099,7 @@
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J237" s="77" t="str">
+      <c r="J237" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K237)),RIGHT(K237,LEN(K237)-FIND(" ",K237)))</f>
         <v>paeruginosa</v>
       </c>
@@ -21090,7 +21115,7 @@
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J238" s="77" t="str">
+      <c r="J238" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K238)),RIGHT(K238,LEN(K238)-FIND(" ",K238)))</f>
         <v>ovirus</v>
       </c>
@@ -21099,7 +21124,7 @@
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J239" s="77" t="str">
+      <c r="J239" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K239)),RIGHT(K239,LEN(K239)-FIND(" ",K239)))</f>
         <v>pchartarum</v>
       </c>
@@ -21115,7 +21140,7 @@
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J240" s="77" t="str">
+      <c r="J240" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K240)),RIGHT(K240,LEN(K240)-FIND(" ",K240)))</f>
         <v>paeruginosa</v>
       </c>
@@ -21124,7 +21149,7 @@
       </c>
     </row>
     <row r="241" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J241" s="78" t="s">
+      <c r="J241" s="77" t="s">
         <v>1153</v>
       </c>
       <c r="K241" s="6" t="s">
@@ -21139,7 +21164,7 @@
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J242" s="78" t="s">
+      <c r="J242" s="77" t="s">
         <v>1155</v>
       </c>
       <c r="K242" s="7" t="s">
@@ -21154,7 +21179,7 @@
       </c>
     </row>
     <row r="243" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J243" s="78" t="s">
+      <c r="J243" s="77" t="s">
         <v>1156</v>
       </c>
       <c r="K243" s="6" t="s">
@@ -21169,7 +21194,7 @@
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J244" s="77" t="str">
+      <c r="J244" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K244)),RIGHT(K244,LEN(K244)-FIND(" ",K244)))</f>
         <v>plarvae</v>
       </c>
@@ -21185,7 +21210,7 @@
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J245" s="77" t="str">
+      <c r="J245" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K245)),RIGHT(K245,LEN(K245)-FIND(" ",K245)))</f>
         <v>pmultocida</v>
       </c>
@@ -21201,7 +21226,7 @@
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J246" s="77" t="str">
+      <c r="J246" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K246)),RIGHT(K246,LEN(K246)-FIND(" ",K246)))</f>
         <v>ppuberulum</v>
       </c>
@@ -21217,7 +21242,7 @@
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J247" s="77" t="str">
+      <c r="J247" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K247)),RIGHT(K247,LEN(K247)-FIND(" ",K247)))</f>
         <v>pmultocida</v>
       </c>
@@ -21226,7 +21251,7 @@
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J248" s="77" t="str">
+      <c r="J248" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K248)),RIGHT(K248,LEN(K248)-FIND(" ",K248)))</f>
         <v>pmultocida</v>
       </c>
@@ -21235,7 +21260,7 @@
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J249" s="77" t="str">
+      <c r="J249" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K249)),RIGHT(K249,LEN(K249)-FIND(" ",K249)))</f>
         <v>pmultocida</v>
       </c>
@@ -21244,7 +21269,7 @@
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J250" s="77" t="str">
+      <c r="J250" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K250)),RIGHT(K250,LEN(K250)-FIND(" ",K250)))</f>
         <v>pmultocida</v>
       </c>
@@ -21253,7 +21278,7 @@
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J251" s="77" t="str">
+      <c r="J251" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K251)),RIGHT(K251,LEN(K251)-FIND(" ",K251)))</f>
         <v>pmultocida</v>
       </c>
@@ -21262,7 +21287,7 @@
       </c>
     </row>
     <row r="252" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J252" s="78" t="s">
+      <c r="J252" s="77" t="s">
         <v>1157</v>
       </c>
       <c r="K252" s="6" t="s">
@@ -21277,7 +21302,7 @@
       </c>
     </row>
     <row r="253" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J253" s="78" t="s">
+      <c r="J253" s="77" t="s">
         <v>1158</v>
       </c>
       <c r="K253" s="6" t="s">
@@ -21292,7 +21317,7 @@
       </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J254" s="78" t="s">
+      <c r="J254" s="77" t="s">
         <v>1159</v>
       </c>
       <c r="K254" s="7" t="s">
@@ -21307,7 +21332,7 @@
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J255" s="78" t="s">
+      <c r="J255" s="77" t="s">
         <v>1160</v>
       </c>
       <c r="K255" s="7" t="s">
@@ -21322,7 +21347,7 @@
       </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J256" s="78" t="s">
+      <c r="J256" s="77" t="s">
         <v>1161</v>
       </c>
       <c r="K256" s="7" t="s">
@@ -21337,7 +21362,7 @@
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J257" s="78" t="s">
+      <c r="J257" s="77" t="s">
         <v>1162</v>
       </c>
       <c r="K257" s="7" t="s">
@@ -21352,7 +21377,7 @@
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J258" s="78" t="s">
+      <c r="J258" s="77" t="s">
         <v>1163</v>
       </c>
       <c r="K258" s="7" t="s">
@@ -21367,7 +21392,7 @@
       </c>
     </row>
     <row r="259" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J259" s="77" t="str">
+      <c r="J259" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K259)),RIGHT(K259,LEN(K259)-FIND(" ",K259)))</f>
         <v>rvirus</v>
       </c>
@@ -21383,7 +21408,7 @@
       </c>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J260" s="77" t="str">
+      <c r="J260" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K260)),RIGHT(K260,LEN(K260)-FIND(" ",K260)))</f>
         <v>sagalactiae</v>
       </c>
@@ -21399,7 +21424,7 @@
       </c>
     </row>
     <row r="261" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J261" s="77" t="str">
+      <c r="J261" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K261)),RIGHT(K261,LEN(K261)-FIND(" ",K261)))</f>
         <v>rvirus</v>
       </c>
@@ -21408,7 +21433,7 @@
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J262" s="77" t="str">
+      <c r="J262" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K262)),RIGHT(K262,LEN(K262)-FIND(" ",K262)))</f>
         <v>sagona</v>
       </c>
@@ -21424,7 +21449,7 @@
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J263" s="78" t="s">
+      <c r="J263" s="77" t="s">
         <v>1164</v>
       </c>
       <c r="K263" s="7" t="s">
@@ -21439,7 +21464,7 @@
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J264" s="77" t="str">
+      <c r="J264" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K264)),RIGHT(K264,LEN(K264)-FIND(" ",K264)))</f>
         <v>saureus</v>
       </c>
@@ -21455,7 +21480,7 @@
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J265" s="77" t="str">
+      <c r="J265" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K265)),RIGHT(K265,LEN(K265)-FIND(" ",K265)))</f>
         <v>scanis</v>
       </c>
@@ -21471,7 +21496,7 @@
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J266" s="77" t="str">
+      <c r="J266" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K266)),RIGHT(K266,LEN(K266)-FIND(" ",K266)))</f>
         <v>saureus</v>
       </c>
@@ -21480,7 +21505,7 @@
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J267" s="77" t="str">
+      <c r="J267" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K267)),RIGHT(K267,LEN(K267)-FIND(" ",K267)))</f>
         <v>saureus</v>
       </c>
@@ -21489,7 +21514,7 @@
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J268" s="77" t="str">
+      <c r="J268" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K268)),RIGHT(K268,LEN(K268)-FIND(" ",K268)))</f>
         <v>saureus</v>
       </c>
@@ -21498,7 +21523,7 @@
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J269" s="77" t="str">
+      <c r="J269" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K269)),RIGHT(K269,LEN(K269)-FIND(" ",K269)))</f>
         <v>saureus</v>
       </c>
@@ -21507,7 +21532,7 @@
       </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J270" s="78" t="s">
+      <c r="J270" s="77" t="s">
         <v>1165</v>
       </c>
       <c r="K270" s="7" t="s">
@@ -21522,7 +21547,7 @@
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J271" s="77" t="str">
+      <c r="J271" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K271)),RIGHT(K271,LEN(K271)-FIND(" ",K271)))</f>
         <v>scanis</v>
       </c>
@@ -21531,7 +21556,7 @@
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J272" s="77" t="str">
+      <c r="J272" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K272)),RIGHT(K272,LEN(K272)-FIND(" ",K272)))</f>
         <v>scholeraesuis</v>
       </c>
@@ -21547,7 +21572,7 @@
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J273" s="77" t="str">
+      <c r="J273" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K273)),RIGHT(K273,LEN(K273)-FIND(" ",K273)))</f>
         <v>sdublin</v>
       </c>
@@ -21563,7 +21588,7 @@
       </c>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J274" s="77" t="str">
+      <c r="J274" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K274)),RIGHT(K274,LEN(K274)-FIND(" ",K274)))</f>
         <v>sdysenteriae</v>
       </c>
@@ -21579,7 +21604,7 @@
       </c>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J275" s="77" t="str">
+      <c r="J275" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K275)),RIGHT(K275,LEN(K275)-FIND(" ",K275)))</f>
         <v>senteritidis</v>
       </c>
@@ -21595,7 +21620,7 @@
       </c>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J276" s="78" t="s">
+      <c r="J276" s="77" t="s">
         <v>1167</v>
       </c>
       <c r="K276" s="7" t="s">
@@ -21610,7 +21635,7 @@
       </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J277" s="78" t="s">
+      <c r="J277" s="77" t="s">
         <v>1170</v>
       </c>
       <c r="K277" s="7" t="s">
@@ -21625,7 +21650,7 @@
       </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J278" s="77" t="str">
+      <c r="J278" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K278)),RIGHT(K278,LEN(K278)-FIND(" ",K278)))</f>
         <v>sfelis</v>
       </c>
@@ -21641,7 +21666,7 @@
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J279" s="77" t="str">
+      <c r="J279" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K279)),RIGHT(K279,LEN(K279)-FIND(" ",K279)))</f>
         <v>sequi subsp. Zooepidemicus</v>
       </c>
@@ -21650,7 +21675,7 @@
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J280" s="77" t="str">
+      <c r="J280" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K280)),RIGHT(K280,LEN(K280)-FIND(" ",K280)))</f>
         <v>sequi subsp. Zooepidemicus</v>
       </c>
@@ -21659,7 +21684,7 @@
       </c>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J281" s="77" t="str">
+      <c r="J281" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K281)),RIGHT(K281,LEN(K281)-FIND(" ",K281)))</f>
         <v>sflexneri</v>
       </c>
@@ -21675,7 +21700,7 @@
       </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J282" s="77" t="str">
+      <c r="J282" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K282)),RIGHT(K282,LEN(K282)-FIND(" ",K282)))</f>
         <v>sgallinarum</v>
       </c>
@@ -21691,7 +21716,7 @@
       </c>
     </row>
     <row r="283" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J283" s="77" t="str">
+      <c r="J283" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K283)),RIGHT(K283,LEN(K283)-FIND(" ",K283)))</f>
         <v>shyicus</v>
       </c>
@@ -21707,7 +21732,7 @@
       </c>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J284" s="78" t="s">
+      <c r="J284" s="77" t="s">
         <v>1175</v>
       </c>
       <c r="K284" s="7" t="s">
@@ -21722,7 +21747,7 @@
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J285" s="78" t="s">
+      <c r="J285" s="77" t="s">
         <v>1176</v>
       </c>
       <c r="K285" s="7" t="s">
@@ -21737,7 +21762,7 @@
       </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J286" s="77" t="str">
+      <c r="J286" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K286)),RIGHT(K286,LEN(K286)-FIND(" ",K286)))</f>
         <v>sintermedius</v>
       </c>
@@ -21753,7 +21778,7 @@
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J287" s="77" t="str">
+      <c r="J287" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K287)),RIGHT(K287,LEN(K287)-FIND(" ",K287)))</f>
         <v>snewport</v>
       </c>
@@ -21769,7 +21794,7 @@
       </c>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J288" s="77" t="str">
+      <c r="J288" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K288)),RIGHT(K288,LEN(K288)-FIND(" ",K288)))</f>
         <v>spneumoniae</v>
       </c>
@@ -21785,7 +21810,7 @@
       </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J289" s="77" t="str">
+      <c r="J289" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K289)),RIGHT(K289,LEN(K289)-FIND(" ",K289)))</f>
         <v>spseudintermedius</v>
       </c>
@@ -21801,7 +21826,7 @@
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J290" s="77" t="str">
+      <c r="J290" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K290)),RIGHT(K290,LEN(K290)-FIND(" ",K290)))</f>
         <v>spullorum</v>
       </c>
@@ -21817,7 +21842,7 @@
       </c>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J291" s="77" t="str">
+      <c r="J291" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K291)),RIGHT(K291,LEN(K291)-FIND(" ",K291)))</f>
         <v>spseudintermedius</v>
       </c>
@@ -21826,7 +21851,7 @@
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J292" s="77" t="str">
+      <c r="J292" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K292)),RIGHT(K292,LEN(K292)-FIND(" ",K292)))</f>
         <v>spseudintermedius</v>
       </c>
@@ -21835,7 +21860,7 @@
       </c>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J293" s="77" t="str">
+      <c r="J293" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K293)),RIGHT(K293,LEN(K293)-FIND(" ",K293)))</f>
         <v>sschenckii</v>
       </c>
@@ -21851,7 +21876,7 @@
       </c>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J294" s="77" t="str">
+      <c r="J294" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K294)),RIGHT(K294,LEN(K294)-FIND(" ",K294)))</f>
         <v>ssonnei</v>
       </c>
@@ -21867,7 +21892,7 @@
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J295" s="77" t="str">
+      <c r="J295" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K295)),RIGHT(K295,LEN(K295)-FIND(" ",K295)))</f>
         <v>sschenckii</v>
       </c>
@@ -21876,7 +21901,7 @@
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J296" s="77" t="str">
+      <c r="J296" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K296)),RIGHT(K296,LEN(K296)-FIND(" ",K296)))</f>
         <v>sschenckii</v>
       </c>
@@ -21885,7 +21910,7 @@
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J297" s="78" t="s">
+      <c r="J297" s="77" t="s">
         <v>1179</v>
       </c>
       <c r="K297" s="7" t="s">
@@ -21900,7 +21925,7 @@
       </c>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J298" s="77" t="str">
+      <c r="J298" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K298)),RIGHT(K298,LEN(K298)-FIND(" ",K298)))</f>
         <v>styphimurium</v>
       </c>
@@ -21916,7 +21941,7 @@
       </c>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J299" s="77" t="str">
+      <c r="J299" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K299)),RIGHT(K299,LEN(K299)-FIND(" ",K299)))</f>
         <v>styphimurium</v>
       </c>
@@ -21932,7 +21957,7 @@
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J300" s="77" t="str">
+      <c r="J300" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K300)),RIGHT(K300,LEN(K300)-FIND(" ",K300)))</f>
         <v>styphimurium</v>
       </c>
@@ -21941,7 +21966,7 @@
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J301" s="77" t="str">
+      <c r="J301" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K301)),RIGHT(K301,LEN(K301)-FIND(" ",K301)))</f>
         <v>styphimurium</v>
       </c>
@@ -21950,7 +21975,7 @@
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J302" s="77" t="str">
+      <c r="J302" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K302)),RIGHT(K302,LEN(K302)-FIND(" ",K302)))</f>
         <v>styphimurium</v>
       </c>
@@ -21959,7 +21984,7 @@
       </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J303" s="77" t="str">
+      <c r="J303" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K303)),RIGHT(K303,LEN(K303)-FIND(" ",K303)))</f>
         <v>styphimurium</v>
       </c>
@@ -21968,7 +21993,7 @@
       </c>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J304" s="78" t="s">
+      <c r="J304" s="77" t="s">
         <v>1181</v>
       </c>
       <c r="K304" s="7" t="s">
@@ -21983,7 +22008,7 @@
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J305" s="78" t="s">
+      <c r="J305" s="77" t="s">
         <v>1182</v>
       </c>
       <c r="K305" s="7" t="s">
@@ -21998,7 +22023,7 @@
       </c>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J306" s="78" t="s">
+      <c r="J306" s="77" t="s">
         <v>1183</v>
       </c>
       <c r="K306" s="7" t="s">
@@ -22013,7 +22038,7 @@
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J307" s="77" t="str">
+      <c r="J307" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K307)),RIGHT(K307,LEN(K307)-FIND(" ",K307)))</f>
         <v>svirus</v>
       </c>
@@ -22022,7 +22047,7 @@
       </c>
     </row>
     <row r="308" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J308" s="77" t="str">
+      <c r="J308" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K308)),RIGHT(K308,LEN(K308)-FIND(" ",K308)))</f>
         <v>svirus</v>
       </c>
@@ -22031,7 +22056,7 @@
       </c>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J309" s="78" t="s">
+      <c r="J309" s="77" t="s">
         <v>1184</v>
       </c>
       <c r="K309" s="7" t="s">
@@ -22046,7 +22071,7 @@
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J310" s="77" t="str">
+      <c r="J310" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K310)),RIGHT(K310,LEN(K310)-FIND(" ",K310)))</f>
         <v>tequinum</v>
       </c>
@@ -22062,7 +22087,7 @@
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J311" s="78" t="s">
+      <c r="J311" s="77" t="s">
         <v>1185</v>
       </c>
       <c r="K311" s="7" t="s">
@@ -22077,7 +22102,7 @@
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J312" s="77" t="str">
+      <c r="J312" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K312)),RIGHT(K312,LEN(K312)-FIND(" ",K312)))</f>
         <v>tmentagrophytes</v>
       </c>
@@ -22093,7 +22118,7 @@
       </c>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J313" s="77" t="str">
+      <c r="J313" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K313)),RIGHT(K313,LEN(K313)-FIND(" ",K313)))</f>
         <v>tpallidum</v>
       </c>
@@ -22109,7 +22134,7 @@
       </c>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J314" s="77" t="str">
+      <c r="J314" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K314)),RIGHT(K314,LEN(K314)-FIND(" ",K314)))</f>
         <v>tmentagrophytes</v>
       </c>
@@ -22118,7 +22143,7 @@
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J315" s="77" t="str">
+      <c r="J315" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K315)),RIGHT(K315,LEN(K315)-FIND(" ",K315)))</f>
         <v>trubrum</v>
       </c>
@@ -22134,7 +22159,7 @@
       </c>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J316" s="77" t="str">
+      <c r="J316" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K316)),RIGHT(K316,LEN(K316)-FIND(" ",K316)))</f>
         <v>tverrucosum</v>
       </c>
@@ -22150,7 +22175,7 @@
       </c>
     </row>
     <row r="317" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J317" s="78" t="s">
+      <c r="J317" s="77" t="s">
         <v>1186</v>
       </c>
       <c r="K317" s="6" t="s">
@@ -22165,7 +22190,7 @@
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J318" s="77" t="str">
+      <c r="J318" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K318)),RIGHT(K318,LEN(K318)-FIND(" ",K318)))</f>
         <v>tverrucosum</v>
       </c>
@@ -22174,7 +22199,7 @@
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J319" s="77" t="str">
+      <c r="J319" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K319)),RIGHT(K319,LEN(K319)-FIND(" ",K319)))</f>
         <v>tverrucosum</v>
       </c>
@@ -22183,7 +22208,7 @@
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J320" s="77" t="str">
+      <c r="J320" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K320)),RIGHT(K320,LEN(K320)-FIND(" ",K320)))</f>
         <v>tverrucosum</v>
       </c>
@@ -22192,7 +22217,7 @@
       </c>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J321" s="77" t="str">
+      <c r="J321" s="76" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K321)),RIGHT(K321,LEN(K321)-FIND(" ",K321)))</f>
         <v>tverrucosum</v>
       </c>
@@ -22201,7 +22226,7 @@
       </c>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J322" s="78" t="s">
+      <c r="J322" s="77" t="s">
         <v>1187</v>
       </c>
       <c r="K322" s="0" t="s">
@@ -22216,7 +22241,7 @@
       </c>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J323" s="78" t="s">
+      <c r="J323" s="77" t="s">
         <v>1188</v>
       </c>
       <c r="K323" s="7" t="s">
@@ -22231,7 +22256,7 @@
       </c>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J324" s="78" t="s">
+      <c r="J324" s="77" t="s">
         <v>1189</v>
       </c>
       <c r="K324" s="0" t="s">
@@ -22246,7 +22271,7 @@
       </c>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J325" s="78" t="s">
+      <c r="J325" s="77" t="s">
         <v>1190</v>
       </c>
       <c r="K325" s="0" t="s">
@@ -22261,7 +22286,7 @@
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J326" s="77"/>
+      <c r="J326" s="76"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -25314,13 +25339,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="78" t="s">
         <v>1195</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="78" t="s">
         <v>1196</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="79" t="s">
         <v>1197</v>
       </c>
     </row>
@@ -25343,21 +25368,21 @@
       <c r="A3" s="56" t="s">
         <v>665</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="80" t="s">
         <v>559</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="80" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="81" t="s">
         <v>185</v>
       </c>
       <c r="B4" s="56" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="80" t="s">
         <v>575</v>
       </c>
     </row>
@@ -25376,7 +25401,7 @@
       <c r="A6" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="81" t="s">
+      <c r="B6" s="80" t="s">
         <v>463</v>
       </c>
       <c r="C6" s="56" t="s">
@@ -25401,7 +25426,7 @@
       <c r="B8" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="81" t="s">
+      <c r="C8" s="80" t="s">
         <v>590</v>
       </c>
     </row>
@@ -25412,7 +25437,7 @@
       <c r="B9" s="56" t="s">
         <v>442</v>
       </c>
-      <c r="C9" s="81" t="s">
+      <c r="C9" s="80" t="s">
         <v>598</v>
       </c>
     </row>
@@ -25434,7 +25459,7 @@
       <c r="B11" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="C11" s="81" t="s">
+      <c r="C11" s="80" t="s">
         <v>602</v>
       </c>
     </row>
@@ -25456,7 +25481,7 @@
       <c r="B13" s="56" t="s">
         <v>309</v>
       </c>
-      <c r="C13" s="81" t="s">
+      <c r="C13" s="80" t="s">
         <v>568</v>
       </c>
     </row>
@@ -25555,7 +25580,7 @@
       <c r="B22" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="C22" s="81" t="s">
+      <c r="C22" s="80" t="s">
         <v>502</v>
       </c>
     </row>
@@ -25599,7 +25624,7 @@
       <c r="B26" s="56" t="s">
         <v>639</v>
       </c>
-      <c r="C26" s="81" t="s">
+      <c r="C26" s="80" t="s">
         <v>59</v>
       </c>
     </row>
@@ -25610,12 +25635,12 @@
       <c r="B27" s="56" t="s">
         <v>642</v>
       </c>
-      <c r="C27" s="81" t="s">
+      <c r="C27" s="80" t="s">
         <v>659</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="82" t="s">
+      <c r="A28" s="81" t="s">
         <v>703</v>
       </c>
       <c r="B28" s="56" t="s">
@@ -25626,7 +25651,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="82" t="s">
+      <c r="A29" s="81" t="s">
         <v>416</v>
       </c>
       <c r="B29" s="56" t="s">
@@ -25640,7 +25665,7 @@
       <c r="A30" s="56" t="s">
         <v>669</v>
       </c>
-      <c r="B30" s="81" t="s">
+      <c r="B30" s="80" t="s">
         <v>476</v>
       </c>
       <c r="C30" s="56" t="s">
@@ -25648,7 +25673,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="82" t="s">
+      <c r="A31" s="81" t="s">
         <v>425</v>
       </c>
       <c r="B31" s="56" t="s">
@@ -25673,7 +25698,7 @@
       <c r="A33" s="56" t="s">
         <v>204</v>
       </c>
-      <c r="B33" s="81" t="s">
+      <c r="B33" s="80" t="s">
         <v>467</v>
       </c>
       <c r="C33" s="56" t="s">
@@ -25684,7 +25709,7 @@
       <c r="A34" s="56" t="s">
         <v>351</v>
       </c>
-      <c r="B34" s="83" t="s">
+      <c r="B34" s="82" t="s">
         <v>438</v>
       </c>
       <c r="C34" s="56" t="s">
@@ -25706,7 +25731,7 @@
       <c r="A36" s="56" t="s">
         <v>763</v>
       </c>
-      <c r="B36" s="83" t="s">
+      <c r="B36" s="82" t="s">
         <v>436</v>
       </c>
       <c r="C36" s="56" t="s">
@@ -25717,7 +25742,7 @@
       <c r="A37" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="82" t="s">
+      <c r="B37" s="81" t="s">
         <v>440</v>
       </c>
       <c r="C37" s="56" t="s">
@@ -25741,7 +25766,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="83" t="s">
+      <c r="B40" s="82" t="s">
         <v>434</v>
       </c>
       <c r="C40" s="56" t="s">
@@ -25749,7 +25774,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="81" t="s">
+      <c r="B41" s="80" t="s">
         <v>614</v>
       </c>
       <c r="C41" s="56" t="s">
@@ -25896,7 +25921,7 @@
       <c r="B59" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="C59" s="81" t="s">
+      <c r="C59" s="80" t="s">
         <v>594</v>
       </c>
     </row>
@@ -25912,7 +25937,7 @@
       <c r="B61" s="56" t="s">
         <v>368</v>
       </c>
-      <c r="C61" s="81" t="s">
+      <c r="C61" s="80" t="s">
         <v>572</v>
       </c>
     </row>
@@ -25920,7 +25945,7 @@
       <c r="B62" s="56" t="s">
         <v>376</v>
       </c>
-      <c r="C62" s="81" t="s">
+      <c r="C62" s="80" t="s">
         <v>581</v>
       </c>
     </row>
@@ -25928,7 +25953,7 @@
       <c r="B63" s="0" t="s">
         <v>445</v>
       </c>
-      <c r="C63" s="81" t="s">
+      <c r="C63" s="80" t="s">
         <v>578</v>
       </c>
     </row>
@@ -26000,7 +26025,7 @@
       <c r="B72" s="0" t="s">
         <v>860</v>
       </c>
-      <c r="C72" s="81" t="s">
+      <c r="C72" s="80" t="s">
         <v>535</v>
       </c>
     </row>
@@ -26008,7 +26033,7 @@
       <c r="B73" s="0" t="s">
         <v>854</v>
       </c>
-      <c r="C73" s="81" t="s">
+      <c r="C73" s="80" t="s">
         <v>530</v>
       </c>
     </row>
@@ -26016,7 +26041,7 @@
       <c r="B74" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="C74" s="81" t="s">
+      <c r="C74" s="80" t="s">
         <v>538</v>
       </c>
     </row>
@@ -26024,15 +26049,15 @@
       <c r="B75" s="56" t="s">
         <v>305</v>
       </c>
-      <c r="C75" s="81" t="s">
+      <c r="C75" s="80" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="81" t="s">
+      <c r="B76" s="80" t="s">
         <v>472</v>
       </c>
-      <c r="C76" s="81" t="s">
+      <c r="C76" s="80" t="s">
         <v>586</v>
       </c>
     </row>
@@ -26064,7 +26089,7 @@
       <c r="B80" s="56" t="s">
         <v>260</v>
       </c>
-      <c r="C80" s="82" t="s">
+      <c r="C80" s="81" t="s">
         <v>522</v>
       </c>
     </row>
@@ -26134,7 +26159,7 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="81" t="s">
+      <c r="C91" s="80" t="s">
         <v>626</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished all easy files, need to go back through for those with various issues
</commit_message>
<xml_diff>
--- a/info/apinet_survey (2).xlsx
+++ b/info/apinet_survey (2).xlsx
@@ -40,7 +40,6 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="0"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Pooled only</t>
         </r>
@@ -54,7 +53,6 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="0"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Use col. 4</t>
         </r>
@@ -68,7 +66,6 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="0"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Output looks off</t>
         </r>
@@ -82,7 +79,6 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="0"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">HUVEC only
 </t>
@@ -97,7 +93,6 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="0"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Which columns?</t>
         </r>
@@ -3714,13 +3709,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3742,13 +3736,11 @@
       <sz val="10"/>
       <name val="Cantarell"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Cantarell"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -3756,7 +3748,6 @@
       <color rgb="FF0000EE"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -3764,20 +3755,17 @@
       <color rgb="FF4B01A6"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Cantarell"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Verdana"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -3785,7 +3773,6 @@
       <color rgb="FFC00000"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -3793,7 +3780,6 @@
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -3801,32 +3787,22 @@
       <color rgb="FFFFC000"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Liberation Mono;Courier New"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="26">
@@ -4242,15 +4218,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4262,7 +4234,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4330,31 +4306,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4442,11 +4418,11 @@
   </sheetPr>
   <dimension ref="A1:AK346"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U310" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V318" activeCellId="0" sqref="V318"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z303" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE318" activeCellId="0" sqref="AE318"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.12"/>
@@ -16064,28 +16040,28 @@
       <c r="X310" s="13" t="s">
         <v>901</v>
       </c>
-      <c r="Y310" s="26" t="s">
+      <c r="Y310" s="13" t="s">
         <v>902</v>
       </c>
-      <c r="Z310" s="24" t="s">
+      <c r="Z310" s="27" t="s">
         <v>903</v>
       </c>
-      <c r="AA310" s="26" t="s">
+      <c r="AA310" s="13" t="s">
         <v>904</v>
       </c>
-      <c r="AB310" s="26" t="s">
+      <c r="AB310" s="27" t="s">
         <v>905</v>
       </c>
-      <c r="AC310" s="26" t="s">
+      <c r="AC310" s="13" t="s">
         <v>906</v>
       </c>
-      <c r="AD310" s="26" t="s">
+      <c r="AD310" s="27" t="s">
         <v>907</v>
       </c>
-      <c r="AE310" s="54" t="s">
+      <c r="AE310" s="13" t="s">
         <v>908</v>
       </c>
-      <c r="AF310" s="26" t="s">
+      <c r="AF310" s="44" t="s">
         <v>909</v>
       </c>
       <c r="AK310" s="0" t="n">
@@ -16252,10 +16228,10 @@
       <c r="L314" s="10" t="s">
         <v>934</v>
       </c>
-      <c r="M314" s="55" t="s">
+      <c r="M314" s="54" t="s">
         <v>935</v>
       </c>
-      <c r="N314" s="55" t="s">
+      <c r="N314" s="54" t="s">
         <v>936</v>
       </c>
       <c r="O314" s="13" t="s">
@@ -16288,25 +16264,25 @@
       <c r="X314" s="13" t="s">
         <v>946</v>
       </c>
-      <c r="Y314" s="26" t="s">
+      <c r="Y314" s="13" t="s">
         <v>947</v>
       </c>
-      <c r="Z314" s="24" t="s">
+      <c r="Z314" s="27" t="s">
         <v>948</v>
       </c>
-      <c r="AA314" s="26" t="s">
+      <c r="AA314" s="27" t="s">
         <v>949</v>
       </c>
-      <c r="AB314" s="26" t="s">
+      <c r="AB314" s="27" t="s">
         <v>950</v>
       </c>
-      <c r="AC314" s="26" t="s">
+      <c r="AC314" s="13" t="s">
         <v>951</v>
       </c>
-      <c r="AD314" s="26" t="s">
+      <c r="AD314" s="13" t="s">
         <v>952</v>
       </c>
-      <c r="AE314" s="54" t="s">
+      <c r="AE314" s="13" t="s">
         <v>953</v>
       </c>
       <c r="AK314" s="0" t="n">
@@ -16380,25 +16356,25 @@
       <c r="X315" s="13" t="s">
         <v>946</v>
       </c>
-      <c r="Y315" s="26" t="s">
+      <c r="Y315" s="13" t="s">
         <v>947</v>
       </c>
-      <c r="Z315" s="24" t="s">
+      <c r="Z315" s="27" t="s">
         <v>948</v>
       </c>
-      <c r="AA315" s="26" t="s">
+      <c r="AA315" s="27" t="s">
         <v>949</v>
       </c>
-      <c r="AB315" s="26" t="s">
+      <c r="AB315" s="27" t="s">
         <v>950</v>
       </c>
-      <c r="AC315" s="26" t="s">
+      <c r="AC315" s="13" t="s">
         <v>951</v>
       </c>
-      <c r="AD315" s="26" t="s">
+      <c r="AD315" s="27" t="s">
         <v>957</v>
       </c>
-      <c r="AE315" s="54" t="s">
+      <c r="AE315" s="13" t="s">
         <v>958</v>
       </c>
     </row>
@@ -16435,7 +16411,7 @@
       <c r="L316" s="53" t="s">
         <v>963</v>
       </c>
-      <c r="M316" s="55" t="s">
+      <c r="M316" s="54" t="s">
         <v>964</v>
       </c>
       <c r="N316" s="13" t="s">
@@ -16471,10 +16447,10 @@
       <c r="X316" s="13" t="s">
         <v>974</v>
       </c>
-      <c r="Y316" s="26" t="s">
+      <c r="Y316" s="13" t="s">
         <v>975</v>
       </c>
-      <c r="Z316" s="24" t="s">
+      <c r="Z316" s="13" t="s">
         <v>976</v>
       </c>
       <c r="AA316" s="26" t="s">
@@ -16564,7 +16540,7 @@
       <c r="L318" s="11" t="s">
         <v>812</v>
       </c>
-      <c r="M318" s="55" t="s">
+      <c r="M318" s="54" t="s">
         <v>985</v>
       </c>
       <c r="O318" s="26"/>
@@ -16587,10 +16563,10 @@
       <c r="F319" s="0" t="s">
         <v>511</v>
       </c>
-      <c r="G319" s="56" t="s">
+      <c r="G319" s="55" t="s">
         <v>986</v>
       </c>
-      <c r="H319" s="56" t="s">
+      <c r="H319" s="55" t="s">
         <v>987</v>
       </c>
       <c r="I319" s="0" t="str">
@@ -16688,7 +16664,7 @@
       <c r="O321" s="13" t="s">
         <v>998</v>
       </c>
-      <c r="P321" s="57" t="s">
+      <c r="P321" s="56" t="s">
         <v>999</v>
       </c>
       <c r="Q321" s="13" t="s">
@@ -16766,7 +16742,7 @@
       <c r="L323" s="11" t="s">
         <v>812</v>
       </c>
-      <c r="M323" s="55" t="s">
+      <c r="M323" s="54" t="s">
         <v>1005</v>
       </c>
       <c r="N323" s="7"/>
@@ -16871,28 +16847,28 @@
       <c r="W325" s="49" t="s">
         <v>1028</v>
       </c>
-      <c r="X325" s="26" t="s">
+      <c r="X325" s="13" t="s">
         <v>1029</v>
       </c>
-      <c r="Y325" s="26" t="s">
+      <c r="Y325" s="13" t="s">
         <v>1030</v>
       </c>
-      <c r="Z325" s="24" t="s">
+      <c r="Z325" s="27" t="s">
         <v>1031</v>
       </c>
       <c r="AA325" s="26" t="s">
         <v>1032</v>
       </c>
-      <c r="AB325" s="26" t="s">
+      <c r="AB325" s="13" t="s">
         <v>1033</v>
       </c>
-      <c r="AC325" s="26" t="s">
+      <c r="AC325" s="13" t="s">
         <v>1034</v>
       </c>
-      <c r="AD325" s="26" t="s">
+      <c r="AD325" s="44" t="s">
         <v>1035</v>
       </c>
-      <c r="AE325" s="54" t="s">
+      <c r="AE325" s="13" t="s">
         <v>1036</v>
       </c>
     </row>
@@ -16950,7 +16926,7 @@
       <c r="S326" s="13" t="s">
         <v>1047</v>
       </c>
-      <c r="T326" s="58" t="s">
+      <c r="T326" s="57" t="s">
         <v>1044</v>
       </c>
       <c r="U326" s="13" t="s">
@@ -16962,16 +16938,16 @@
       <c r="W326" s="27" t="s">
         <v>1050</v>
       </c>
-      <c r="X326" s="26" t="s">
+      <c r="X326" s="27" t="s">
         <v>1051</v>
       </c>
-      <c r="Y326" s="26" t="s">
+      <c r="Y326" s="13" t="s">
         <v>1052</v>
       </c>
-      <c r="Z326" s="24" t="s">
+      <c r="Z326" s="27" t="s">
         <v>1053</v>
       </c>
-      <c r="AE326" s="54"/>
+      <c r="AE326" s="58"/>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B327" s="59"/>
@@ -17744,7 +17720,7 @@
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.11"/>
@@ -20197,10 +20173,10 @@
       <c r="J172" s="77" t="s">
         <v>1130</v>
       </c>
-      <c r="K172" s="56" t="s">
+      <c r="K172" s="55" t="s">
         <v>986</v>
       </c>
-      <c r="L172" s="56" t="s">
+      <c r="L172" s="55" t="s">
         <v>987</v>
       </c>
       <c r="M172" s="0" t="str">
@@ -22306,11 +22282,11 @@
   </sheetPr>
   <dimension ref="A1:A325"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.72"/>
   </cols>
@@ -23901,7 +23877,7 @@
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A318" s="56" t="s">
+      <c r="A318" s="55" t="s">
         <v>987</v>
       </c>
     </row>
@@ -23962,7 +23938,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.89"/>
@@ -25326,11 +25302,11 @@
   </sheetPr>
   <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.99"/>
@@ -25350,13 +25326,13 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="55" t="s">
         <v>214</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="55" t="s">
         <v>238</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="55" t="s">
         <v>697</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -25365,7 +25341,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="55" t="s">
         <v>665</v>
       </c>
       <c r="B3" s="80" t="s">
@@ -25379,7 +25355,7 @@
       <c r="A4" s="81" t="s">
         <v>185</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="55" t="s">
         <v>129</v>
       </c>
       <c r="C4" s="80" t="s">
@@ -25387,43 +25363,43 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="55" t="s">
         <v>419</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="55" t="s">
         <v>267</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="55" t="s">
         <v>724</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="55" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="80" t="s">
         <v>463</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="55" t="s">
         <v>688</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="55" t="s">
         <v>188</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="55" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="55" t="s">
         <v>422</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="55" t="s">
         <v>109</v>
       </c>
       <c r="C8" s="80" t="s">
@@ -25431,10 +25407,10 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="55" t="s">
         <v>182</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="55" t="s">
         <v>442</v>
       </c>
       <c r="C9" s="80" t="s">
@@ -25442,21 +25418,21 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="55" t="s">
         <v>345</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="55" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="55" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="55" t="s">
         <v>200</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="55" t="s">
         <v>156</v>
       </c>
       <c r="C11" s="80" t="s">
@@ -25464,13 +25440,13 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="56" t="s">
+      <c r="A12" s="55" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>843</v>
       </c>
-      <c r="C12" s="56" t="s">
+      <c r="C12" s="55" t="s">
         <v>55</v>
       </c>
     </row>
@@ -25478,7 +25454,7 @@
       <c r="A13" s="0" t="s">
         <v>778</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="55" t="s">
         <v>309</v>
       </c>
       <c r="C13" s="80" t="s">
@@ -25486,98 +25462,98 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="55" t="s">
         <v>211</v>
       </c>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="55" t="s">
         <v>650</v>
       </c>
-      <c r="C14" s="56" t="s">
+      <c r="C14" s="55" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="55" t="s">
         <v>428</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="55" t="s">
         <v>456</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" s="55" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="56" t="s">
+      <c r="A16" s="55" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="55" t="s">
         <v>450</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="55" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="55" t="s">
         <v>348</v>
       </c>
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="55" t="s">
         <v>617</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="55" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="55" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="55" t="s">
         <v>453</v>
       </c>
-      <c r="C19" s="56" t="s">
+      <c r="C19" s="55" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="55" t="s">
         <v>706</v>
       </c>
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="55" t="s">
         <v>620</v>
       </c>
-      <c r="C20" s="56" t="s">
+      <c r="C20" s="55" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="56" t="s">
+      <c r="A21" s="55" t="s">
         <v>208</v>
       </c>
-      <c r="B21" s="56" t="s">
+      <c r="B21" s="55" t="s">
         <v>144</v>
       </c>
-      <c r="C21" s="56" t="s">
+      <c r="C21" s="55" t="s">
         <v>684</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="56" t="s">
+      <c r="A22" s="55" t="s">
         <v>431</v>
       </c>
-      <c r="B22" s="56" t="s">
+      <c r="B22" s="55" t="s">
         <v>113</v>
       </c>
       <c r="C22" s="80" t="s">
@@ -25585,10 +25561,10 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="56" t="s">
+      <c r="A23" s="55" t="s">
         <v>361</v>
       </c>
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="55" t="s">
         <v>152</v>
       </c>
       <c r="C23" s="0" t="s">
@@ -25596,21 +25572,21 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="56" t="s">
+      <c r="A24" s="55" t="s">
         <v>358</v>
       </c>
-      <c r="B24" s="56" t="s">
+      <c r="B24" s="55" t="s">
         <v>636</v>
       </c>
-      <c r="C24" s="56" t="s">
+      <c r="C24" s="55" t="s">
         <v>692</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="56" t="s">
+      <c r="A25" s="55" t="s">
         <v>196</v>
       </c>
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="55" t="s">
         <v>633</v>
       </c>
       <c r="C25" s="0" t="s">
@@ -25618,10 +25594,10 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="56" t="s">
+      <c r="A26" s="55" t="s">
         <v>341</v>
       </c>
-      <c r="B26" s="56" t="s">
+      <c r="B26" s="55" t="s">
         <v>639</v>
       </c>
       <c r="C26" s="80" t="s">
@@ -25629,10 +25605,10 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="56" t="s">
+      <c r="A27" s="55" t="s">
         <v>217</v>
       </c>
-      <c r="B27" s="56" t="s">
+      <c r="B27" s="55" t="s">
         <v>642</v>
       </c>
       <c r="C27" s="80" t="s">
@@ -25643,10 +25619,10 @@
       <c r="A28" s="81" t="s">
         <v>703</v>
       </c>
-      <c r="B28" s="56" t="s">
+      <c r="B28" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="C28" s="56" t="s">
+      <c r="C28" s="55" t="s">
         <v>406</v>
       </c>
     </row>
@@ -25654,21 +25630,21 @@
       <c r="A29" s="81" t="s">
         <v>416</v>
       </c>
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="55" t="s">
         <v>125</v>
       </c>
-      <c r="C29" s="56" t="s">
+      <c r="C29" s="55" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="55" t="s">
         <v>669</v>
       </c>
       <c r="B30" s="80" t="s">
         <v>476</v>
       </c>
-      <c r="C30" s="56" t="s">
+      <c r="C30" s="55" t="s">
         <v>402</v>
       </c>
     </row>
@@ -25676,92 +25652,92 @@
       <c r="A31" s="81" t="s">
         <v>425</v>
       </c>
-      <c r="B31" s="56" t="s">
+      <c r="B31" s="55" t="s">
         <v>257</v>
       </c>
-      <c r="C31" s="56" t="s">
+      <c r="C31" s="55" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="56" t="s">
+      <c r="A32" s="55" t="s">
         <v>608</v>
       </c>
-      <c r="B32" s="56" t="s">
+      <c r="B32" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="56" t="s">
+      <c r="C32" s="55" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="56" t="s">
+      <c r="A33" s="55" t="s">
         <v>204</v>
       </c>
       <c r="B33" s="80" t="s">
         <v>467</v>
       </c>
-      <c r="C33" s="56" t="s">
+      <c r="C33" s="55" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="56" t="s">
+      <c r="A34" s="55" t="s">
         <v>351</v>
       </c>
       <c r="B34" s="82" t="s">
         <v>438</v>
       </c>
-      <c r="C34" s="56" t="s">
+      <c r="C34" s="55" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="56" t="s">
+      <c r="A35" s="55" t="s">
         <v>354</v>
       </c>
-      <c r="B35" s="56" t="s">
+      <c r="B35" s="55" t="s">
         <v>312</v>
       </c>
-      <c r="C35" s="56" t="s">
+      <c r="C35" s="55" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="56" t="s">
+      <c r="A36" s="55" t="s">
         <v>763</v>
       </c>
       <c r="B36" s="82" t="s">
         <v>436</v>
       </c>
-      <c r="C36" s="56" t="s">
+      <c r="C36" s="55" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="56" t="s">
+      <c r="A37" s="55" t="s">
         <v>14</v>
       </c>
       <c r="B37" s="81" t="s">
         <v>440</v>
       </c>
-      <c r="C37" s="56" t="s">
+      <c r="C37" s="55" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="56" t="s">
+      <c r="B38" s="55" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="56" t="s">
+      <c r="C38" s="55" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="56" t="s">
+      <c r="B39" s="55" t="s">
         <v>220</v>
       </c>
-      <c r="C39" s="56" t="s">
+      <c r="C39" s="55" t="s">
         <v>327</v>
       </c>
     </row>
@@ -25769,7 +25745,7 @@
       <c r="B40" s="82" t="s">
         <v>434</v>
       </c>
-      <c r="C40" s="56" t="s">
+      <c r="C40" s="55" t="s">
         <v>335</v>
       </c>
     </row>
@@ -25777,28 +25753,28 @@
       <c r="B41" s="80" t="s">
         <v>614</v>
       </c>
-      <c r="C41" s="56" t="s">
+      <c r="C41" s="55" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="56" t="s">
+      <c r="B42" s="55" t="s">
         <v>228</v>
       </c>
-      <c r="C42" s="56" t="s">
+      <c r="C42" s="55" t="s">
         <v>728</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="56" t="s">
+      <c r="B43" s="55" t="s">
         <v>136</v>
       </c>
-      <c r="C43" s="56" t="s">
+      <c r="C43" s="55" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="56" t="s">
+      <c r="B44" s="55" t="s">
         <v>677</v>
       </c>
       <c r="C44" s="0" t="s">
@@ -25806,7 +25782,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="56" t="s">
+      <c r="B45" s="55" t="s">
         <v>64</v>
       </c>
       <c r="C45" s="0" t="s">
@@ -25814,7 +25790,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="56" t="s">
+      <c r="B46" s="55" t="s">
         <v>35</v>
       </c>
       <c r="C46" s="0" t="s">
@@ -25830,7 +25806,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="56" t="s">
+      <c r="B48" s="55" t="s">
         <v>117</v>
       </c>
       <c r="C48" s="0" t="s">
@@ -25838,7 +25814,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="56" t="s">
+      <c r="B49" s="55" t="s">
         <v>106</v>
       </c>
       <c r="C49" s="0" t="s">
@@ -25846,7 +25822,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="56" t="s">
+      <c r="B50" s="55" t="s">
         <v>715</v>
       </c>
       <c r="C50" s="0" t="s">
@@ -25862,7 +25838,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="56" t="s">
+      <c r="B52" s="55" t="s">
         <v>140</v>
       </c>
       <c r="C52" s="0" t="s">
@@ -25873,7 +25849,7 @@
       <c r="B53" s="0" t="s">
         <v>868</v>
       </c>
-      <c r="C53" s="56" t="s">
+      <c r="C53" s="55" t="s">
         <v>987</v>
       </c>
     </row>
@@ -25886,15 +25862,15 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="56" t="s">
+      <c r="B55" s="55" t="s">
         <v>373</v>
       </c>
-      <c r="C55" s="56" t="s">
+      <c r="C55" s="55" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="56" t="s">
+      <c r="B56" s="55" t="s">
         <v>242</v>
       </c>
       <c r="C56" s="0" t="s">
@@ -25902,15 +25878,15 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="56" t="s">
+      <c r="B57" s="55" t="s">
         <v>245</v>
       </c>
-      <c r="C57" s="56" t="s">
+      <c r="C57" s="55" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="56" t="s">
+      <c r="B58" s="55" t="s">
         <v>673</v>
       </c>
       <c r="C58" s="0" t="s">
@@ -25918,7 +25894,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="56" t="s">
+      <c r="B59" s="55" t="s">
         <v>133</v>
       </c>
       <c r="C59" s="80" t="s">
@@ -25926,15 +25902,15 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="56" t="s">
+      <c r="B60" s="55" t="s">
         <v>231</v>
       </c>
-      <c r="C60" s="56" t="s">
+      <c r="C60" s="55" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="56" t="s">
+      <c r="B61" s="55" t="s">
         <v>368</v>
       </c>
       <c r="C61" s="80" t="s">
@@ -25942,7 +25918,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="56" t="s">
+      <c r="B62" s="55" t="s">
         <v>376</v>
       </c>
       <c r="C62" s="80" t="s">
@@ -25958,10 +25934,10 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="56" t="s">
+      <c r="B64" s="55" t="s">
         <v>654</v>
       </c>
-      <c r="C64" s="56" t="s">
+      <c r="C64" s="55" t="s">
         <v>733</v>
       </c>
     </row>
@@ -25969,28 +25945,28 @@
       <c r="B65" s="0" t="s">
         <v>830</v>
       </c>
-      <c r="C65" s="56" t="s">
+      <c r="C65" s="55" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="56" t="s">
+      <c r="B66" s="55" t="s">
         <v>720</v>
       </c>
-      <c r="C66" s="56" t="s">
+      <c r="C66" s="55" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="56" t="s">
+      <c r="B67" s="55" t="s">
         <v>657</v>
       </c>
-      <c r="C67" s="56" t="s">
+      <c r="C67" s="55" t="s">
         <v>741</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="56" t="s">
+      <c r="B68" s="55" t="s">
         <v>718</v>
       </c>
       <c r="C68" s="0" t="s">
@@ -25998,7 +25974,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="56" t="s">
+      <c r="B69" s="55" t="s">
         <v>249</v>
       </c>
       <c r="C69" s="0" t="s">
@@ -26006,10 +25982,10 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="56" t="s">
+      <c r="B70" s="55" t="s">
         <v>235</v>
       </c>
-      <c r="C70" s="56" t="s">
+      <c r="C70" s="55" t="s">
         <v>164</v>
       </c>
     </row>
@@ -26017,7 +25993,7 @@
       <c r="B71" s="0" t="s">
         <v>857</v>
       </c>
-      <c r="C71" s="56" t="s">
+      <c r="C71" s="55" t="s">
         <v>175</v>
       </c>
     </row>
@@ -26038,7 +26014,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="56" t="s">
+      <c r="B74" s="55" t="s">
         <v>95</v>
       </c>
       <c r="C74" s="80" t="s">
@@ -26046,7 +26022,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="56" t="s">
+      <c r="B75" s="55" t="s">
         <v>305</v>
       </c>
       <c r="C75" s="80" t="s">
@@ -26062,31 +26038,31 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="56" t="s">
+      <c r="B77" s="55" t="s">
         <v>364</v>
       </c>
-      <c r="C77" s="56" t="s">
+      <c r="C77" s="55" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="56" t="s">
+      <c r="B78" s="55" t="s">
         <v>224</v>
       </c>
-      <c r="C78" s="56" t="s">
+      <c r="C78" s="55" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="56" t="s">
+      <c r="B79" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="C79" s="56" t="s">
+      <c r="C79" s="55" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="56" t="s">
+      <c r="B80" s="55" t="s">
         <v>260</v>
       </c>
       <c r="C80" s="81" t="s">
@@ -26094,15 +26070,15 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="56" t="s">
+      <c r="B81" s="55" t="s">
         <v>379</v>
       </c>
-      <c r="C81" s="56" t="s">
+      <c r="C81" s="55" t="s">
         <v>680</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="56" t="s">
+      <c r="B82" s="55" t="s">
         <v>263</v>
       </c>
       <c r="C82" s="0" t="s">
@@ -26113,15 +26089,15 @@
       <c r="B83" s="0" t="s">
         <v>793</v>
       </c>
-      <c r="C83" s="56" t="s">
+      <c r="C83" s="55" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="56" t="s">
+      <c r="B84" s="55" t="s">
         <v>459</v>
       </c>
-      <c r="C84" s="56" t="s">
+      <c r="C84" s="55" t="s">
         <v>168</v>
       </c>
     </row>
@@ -26129,27 +26105,27 @@
       <c r="B85" s="0" t="s">
         <v>864</v>
       </c>
-      <c r="C85" s="56" t="s">
+      <c r="C85" s="55" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C86" s="56" t="s">
+      <c r="C86" s="55" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C87" s="56" t="s">
+      <c r="C87" s="55" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C88" s="56" t="s">
+      <c r="C88" s="55" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C89" s="56" t="s">
+      <c r="C89" s="55" t="s">
         <v>757</v>
       </c>
     </row>
@@ -26164,7 +26140,7 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C92" s="56" t="s">
+      <c r="C92" s="55" t="s">
         <v>386</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Trying to figure out bw files
</commit_message>
<xml_diff>
--- a/info/apinet_survey (2).xlsx
+++ b/info/apinet_survey (2).xlsx
@@ -40,6 +40,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Pooled only</t>
         </r>
@@ -53,8 +54,23 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Use col. 4</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q301" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Way more samples than page says</t>
         </r>
       </text>
     </comment>
@@ -66,8 +82,23 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Output looks off</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S314" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">How to format column names? Make sure to skiprows=[1]</t>
         </r>
       </text>
     </comment>
@@ -79,9 +110,24 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">HUVEC only
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V315" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Doesn’t line up</t>
         </r>
       </text>
     </comment>
@@ -93,8 +139,23 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Which columns?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AD310" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">3 columns but no headers. Which to use?</t>
         </r>
       </text>
     </comment>
@@ -3302,7 +3363,7 @@
     <t xml:space="preserve">Needs input</t>
   </si>
   <si>
-    <t xml:space="preserve">RCC file? Not sure how to read</t>
+    <t xml:space="preserve">bw file? Not sure how to read</t>
   </si>
   <si>
     <t xml:space="preserve">Other error – check back later</t>
@@ -3709,12 +3770,13 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3736,11 +3798,13 @@
       <sz val="10"/>
       <name val="Cantarell"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Cantarell"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -3748,6 +3812,7 @@
       <color rgb="FF0000EE"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -3755,17 +3820,20 @@
       <color rgb="FF4B01A6"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Cantarell"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Verdana"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -3773,6 +3841,7 @@
       <color rgb="FFC00000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -3780,6 +3849,7 @@
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -3787,22 +3857,32 @@
       <color rgb="FFFFC000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Liberation Mono;Courier New"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="26">
@@ -3874,8 +3954,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4B01A6"/>
-        <bgColor rgb="FF800080"/>
+        <fgColor rgb="FFC9211E"/>
+        <bgColor rgb="FFC00000"/>
       </patternFill>
     </fill>
     <fill>
@@ -3894,12 +3974,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF0BFF19"/>
         <bgColor rgb="FF33CCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC9211E"/>
-        <bgColor rgb="FFC00000"/>
       </patternFill>
     </fill>
     <fill>
@@ -3924,6 +3998,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF30300B"/>
         <bgColor rgb="FF333333"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4B01A6"/>
+        <bgColor rgb="FF800080"/>
       </patternFill>
     </fill>
     <fill>
@@ -4174,7 +4254,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4222,11 +4306,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4238,7 +4318,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4254,7 +4334,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="19" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4274,15 +4354,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="20" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4302,35 +4382,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="20" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="19" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4418,11 +4498,11 @@
   </sheetPr>
   <dimension ref="A1:AK346"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z303" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE318" activeCellId="0" sqref="AE318"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y304" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE329" activeCellId="0" sqref="AE329"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.12"/>
@@ -15500,7 +15580,7 @@
       <c r="Q298" s="46" t="s">
         <v>827</v>
       </c>
-      <c r="R298" s="27" t="s">
+      <c r="R298" s="48" t="s">
         <v>828</v>
       </c>
     </row>
@@ -15573,7 +15653,7 @@
       <c r="L300" s="10" t="s">
         <v>802</v>
       </c>
-      <c r="M300" s="48" t="s">
+      <c r="M300" s="49" t="s">
         <v>787</v>
       </c>
       <c r="N300" s="13" t="s">
@@ -15582,7 +15662,7 @@
       <c r="O300" s="13" t="s">
         <v>833</v>
       </c>
-      <c r="P300" s="27" t="s">
+      <c r="P300" s="13" t="s">
         <v>834</v>
       </c>
       <c r="Q300" s="44" t="s">
@@ -15600,7 +15680,7 @@
       <c r="U300" s="13" t="s">
         <v>838</v>
       </c>
-      <c r="V300" s="49" t="s">
+      <c r="V300" s="50" t="s">
         <v>839</v>
       </c>
       <c r="W300" s="13" t="s">
@@ -15649,13 +15729,13 @@
       <c r="N301" s="13" t="s">
         <v>847</v>
       </c>
-      <c r="O301" s="50" t="s">
+      <c r="O301" s="51" t="s">
         <v>848</v>
       </c>
       <c r="P301" s="44" t="n">
         <v>223804</v>
       </c>
-      <c r="Q301" s="27" t="s">
+      <c r="Q301" s="48" t="s">
         <v>849</v>
       </c>
       <c r="R301" s="13" t="s">
@@ -15927,7 +16007,7 @@
       <c r="P308" s="13" t="s">
         <v>879</v>
       </c>
-      <c r="Q308" s="51" t="s">
+      <c r="Q308" s="52" t="s">
         <v>880</v>
       </c>
       <c r="R308" s="13" t="s">
@@ -15990,7 +16070,7 @@
       <c r="G310" s="0" t="s">
         <v>888</v>
       </c>
-      <c r="H310" s="52" t="s">
+      <c r="H310" s="53" t="s">
         <v>889</v>
       </c>
       <c r="I310" s="0" t="str">
@@ -16004,7 +16084,7 @@
       <c r="K310" s="8" t="s">
         <v>890</v>
       </c>
-      <c r="L310" s="53" t="s">
+      <c r="L310" s="54" t="s">
         <v>880</v>
       </c>
       <c r="M310" s="13" t="s">
@@ -16043,19 +16123,19 @@
       <c r="Y310" s="13" t="s">
         <v>902</v>
       </c>
-      <c r="Z310" s="27" t="s">
+      <c r="Z310" s="48" t="s">
         <v>903</v>
       </c>
       <c r="AA310" s="13" t="s">
         <v>904</v>
       </c>
-      <c r="AB310" s="27" t="s">
+      <c r="AB310" s="48" t="s">
         <v>905</v>
       </c>
       <c r="AC310" s="13" t="s">
         <v>906</v>
       </c>
-      <c r="AD310" s="27" t="s">
+      <c r="AD310" s="48" t="s">
         <v>907</v>
       </c>
       <c r="AE310" s="13" t="s">
@@ -16134,7 +16214,7 @@
       <c r="K312" s="8" t="s">
         <v>917</v>
       </c>
-      <c r="L312" s="53" t="s">
+      <c r="L312" s="54" t="s">
         <v>918</v>
       </c>
       <c r="M312" s="13" t="s">
@@ -16228,10 +16308,10 @@
       <c r="L314" s="10" t="s">
         <v>934</v>
       </c>
-      <c r="M314" s="54" t="s">
+      <c r="M314" s="55" t="s">
         <v>935</v>
       </c>
-      <c r="N314" s="54" t="s">
+      <c r="N314" s="55" t="s">
         <v>936</v>
       </c>
       <c r="O314" s="13" t="s">
@@ -16240,22 +16320,22 @@
       <c r="P314" s="13" t="s">
         <v>938</v>
       </c>
-      <c r="Q314" s="27" t="s">
+      <c r="Q314" s="48" t="s">
         <v>939</v>
       </c>
       <c r="R314" s="13" t="s">
         <v>940</v>
       </c>
-      <c r="S314" s="27" t="s">
+      <c r="S314" s="48" t="s">
         <v>941</v>
       </c>
-      <c r="T314" s="49" t="s">
+      <c r="T314" s="50" t="s">
         <v>942</v>
       </c>
-      <c r="U314" s="27" t="s">
+      <c r="U314" s="13" t="s">
         <v>943</v>
       </c>
-      <c r="V314" s="27" t="s">
+      <c r="V314" s="48" t="s">
         <v>944</v>
       </c>
       <c r="W314" s="13" t="s">
@@ -16267,13 +16347,13 @@
       <c r="Y314" s="13" t="s">
         <v>947</v>
       </c>
-      <c r="Z314" s="27" t="s">
+      <c r="Z314" s="13" t="s">
         <v>948</v>
       </c>
-      <c r="AA314" s="27" t="s">
+      <c r="AA314" s="48" t="s">
         <v>949</v>
       </c>
-      <c r="AB314" s="27" t="s">
+      <c r="AB314" s="48" t="s">
         <v>950</v>
       </c>
       <c r="AC314" s="13" t="s">
@@ -16332,22 +16412,22 @@
       <c r="P315" s="13" t="s">
         <v>938</v>
       </c>
-      <c r="Q315" s="27" t="s">
+      <c r="Q315" s="48" t="s">
         <v>939</v>
       </c>
       <c r="R315" s="13" t="s">
         <v>940</v>
       </c>
-      <c r="S315" s="27" t="s">
+      <c r="S315" s="48" t="s">
         <v>941</v>
       </c>
-      <c r="T315" s="49" t="s">
+      <c r="T315" s="50" t="s">
         <v>942</v>
       </c>
-      <c r="U315" s="27" t="s">
+      <c r="U315" s="13" t="s">
         <v>943</v>
       </c>
-      <c r="V315" s="27" t="s">
+      <c r="V315" s="48" t="s">
         <v>944</v>
       </c>
       <c r="W315" s="13" t="s">
@@ -16359,19 +16439,19 @@
       <c r="Y315" s="13" t="s">
         <v>947</v>
       </c>
-      <c r="Z315" s="27" t="s">
+      <c r="Z315" s="13" t="s">
         <v>948</v>
       </c>
-      <c r="AA315" s="27" t="s">
+      <c r="AA315" s="48" t="s">
         <v>949</v>
       </c>
-      <c r="AB315" s="27" t="s">
+      <c r="AB315" s="48" t="s">
         <v>950</v>
       </c>
       <c r="AC315" s="13" t="s">
         <v>951</v>
       </c>
-      <c r="AD315" s="27" t="s">
+      <c r="AD315" s="48" t="s">
         <v>957</v>
       </c>
       <c r="AE315" s="13" t="s">
@@ -16408,10 +16488,10 @@
       <c r="K316" s="8" t="s">
         <v>962</v>
       </c>
-      <c r="L316" s="53" t="s">
+      <c r="L316" s="54" t="s">
         <v>963</v>
       </c>
-      <c r="M316" s="54" t="s">
+      <c r="M316" s="55" t="s">
         <v>964</v>
       </c>
       <c r="N316" s="13" t="s">
@@ -16453,7 +16533,7 @@
       <c r="Z316" s="13" t="s">
         <v>976</v>
       </c>
-      <c r="AA316" s="26" t="s">
+      <c r="AA316" s="13" t="s">
         <v>977</v>
       </c>
     </row>
@@ -16487,7 +16567,7 @@
       <c r="K317" s="8" t="s">
         <v>980</v>
       </c>
-      <c r="L317" s="53" t="s">
+      <c r="L317" s="54" t="s">
         <v>963</v>
       </c>
       <c r="M317" s="13" t="s">
@@ -16540,7 +16620,7 @@
       <c r="L318" s="11" t="s">
         <v>812</v>
       </c>
-      <c r="M318" s="54" t="s">
+      <c r="M318" s="55" t="s">
         <v>985</v>
       </c>
       <c r="O318" s="26"/>
@@ -16563,10 +16643,10 @@
       <c r="F319" s="0" t="s">
         <v>511</v>
       </c>
-      <c r="G319" s="55" t="s">
+      <c r="G319" s="56" t="s">
         <v>986</v>
       </c>
-      <c r="H319" s="55" t="s">
+      <c r="H319" s="56" t="s">
         <v>987</v>
       </c>
       <c r="I319" s="0" t="str">
@@ -16664,7 +16744,7 @@
       <c r="O321" s="13" t="s">
         <v>998</v>
       </c>
-      <c r="P321" s="56" t="s">
+      <c r="P321" s="27" t="s">
         <v>999</v>
       </c>
       <c r="Q321" s="13" t="s">
@@ -16742,7 +16822,7 @@
       <c r="L323" s="11" t="s">
         <v>812</v>
       </c>
-      <c r="M323" s="54" t="s">
+      <c r="M323" s="55" t="s">
         <v>1005</v>
       </c>
       <c r="N323" s="7"/>
@@ -16844,7 +16924,7 @@
       <c r="V325" s="13" t="s">
         <v>1027</v>
       </c>
-      <c r="W325" s="49" t="s">
+      <c r="W325" s="50" t="s">
         <v>1028</v>
       </c>
       <c r="X325" s="13" t="s">
@@ -16853,7 +16933,7 @@
       <c r="Y325" s="13" t="s">
         <v>1030</v>
       </c>
-      <c r="Z325" s="27" t="s">
+      <c r="Z325" s="48" t="s">
         <v>1031</v>
       </c>
       <c r="AA325" s="26" t="s">
@@ -16920,7 +17000,7 @@
       <c r="Q326" s="13" t="s">
         <v>1045</v>
       </c>
-      <c r="R326" s="49" t="s">
+      <c r="R326" s="50" t="s">
         <v>1046</v>
       </c>
       <c r="S326" s="13" t="s">
@@ -16935,16 +17015,16 @@
       <c r="V326" s="13" t="s">
         <v>1049</v>
       </c>
-      <c r="W326" s="27" t="s">
+      <c r="W326" s="48" t="s">
         <v>1050</v>
       </c>
-      <c r="X326" s="27" t="s">
+      <c r="X326" s="48" t="s">
         <v>1051</v>
       </c>
       <c r="Y326" s="13" t="s">
         <v>1052</v>
       </c>
-      <c r="Z326" s="27" t="s">
+      <c r="Z326" s="48" t="s">
         <v>1053</v>
       </c>
       <c r="AE326" s="58"/>
@@ -17720,7 +17800,7 @@
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.11"/>
@@ -20173,10 +20253,10 @@
       <c r="J172" s="77" t="s">
         <v>1130</v>
       </c>
-      <c r="K172" s="55" t="s">
+      <c r="K172" s="56" t="s">
         <v>986</v>
       </c>
-      <c r="L172" s="55" t="s">
+      <c r="L172" s="56" t="s">
         <v>987</v>
       </c>
       <c r="M172" s="0" t="str">
@@ -22286,7 +22366,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.72"/>
   </cols>
@@ -23877,7 +23957,7 @@
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A318" s="55" t="s">
+      <c r="A318" s="56" t="s">
         <v>987</v>
       </c>
     </row>
@@ -23938,7 +24018,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.89"/>
@@ -25306,7 +25386,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.99"/>
@@ -25326,13 +25406,13 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="56" t="s">
         <v>214</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="56" t="s">
         <v>238</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="56" t="s">
         <v>697</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -25341,7 +25421,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="56" t="s">
         <v>665</v>
       </c>
       <c r="B3" s="80" t="s">
@@ -25355,7 +25435,7 @@
       <c r="A4" s="81" t="s">
         <v>185</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="56" t="s">
         <v>129</v>
       </c>
       <c r="C4" s="80" t="s">
@@ -25363,43 +25443,43 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="56" t="s">
         <v>419</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>724</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="56" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="80" t="s">
         <v>463</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="56" t="s">
         <v>688</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="56" t="s">
         <v>188</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="56" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="56" t="s">
         <v>422</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="56" t="s">
         <v>109</v>
       </c>
       <c r="C8" s="80" t="s">
@@ -25407,10 +25487,10 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="56" t="s">
         <v>182</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="56" t="s">
         <v>442</v>
       </c>
       <c r="C9" s="80" t="s">
@@ -25418,21 +25498,21 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="55" t="s">
+      <c r="A10" s="56" t="s">
         <v>345</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="56" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="56" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="55" t="s">
+      <c r="A11" s="56" t="s">
         <v>200</v>
       </c>
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="56" t="s">
         <v>156</v>
       </c>
       <c r="C11" s="80" t="s">
@@ -25440,13 +25520,13 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="55" t="s">
+      <c r="A12" s="56" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>843</v>
       </c>
-      <c r="C12" s="55" t="s">
+      <c r="C12" s="56" t="s">
         <v>55</v>
       </c>
     </row>
@@ -25454,7 +25534,7 @@
       <c r="A13" s="0" t="s">
         <v>778</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="56" t="s">
         <v>309</v>
       </c>
       <c r="C13" s="80" t="s">
@@ -25462,98 +25542,98 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="56" t="s">
         <v>211</v>
       </c>
-      <c r="B14" s="55" t="s">
+      <c r="B14" s="56" t="s">
         <v>650</v>
       </c>
-      <c r="C14" s="55" t="s">
+      <c r="C14" s="56" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="56" t="s">
         <v>428</v>
       </c>
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="56" t="s">
         <v>456</v>
       </c>
-      <c r="C15" s="55" t="s">
+      <c r="C15" s="56" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="55" t="s">
+      <c r="A16" s="56" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="56" t="s">
         <v>450</v>
       </c>
-      <c r="C16" s="55" t="s">
+      <c r="C16" s="56" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="55" t="s">
+      <c r="A17" s="56" t="s">
         <v>348</v>
       </c>
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="56" t="s">
         <v>617</v>
       </c>
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="56" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="B18" s="55" t="s">
+      <c r="B18" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="55" t="s">
+      <c r="C18" s="56" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="56" t="s">
         <v>453</v>
       </c>
-      <c r="C19" s="55" t="s">
+      <c r="C19" s="56" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="55" t="s">
+      <c r="A20" s="56" t="s">
         <v>706</v>
       </c>
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="56" t="s">
         <v>620</v>
       </c>
-      <c r="C20" s="55" t="s">
+      <c r="C20" s="56" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="55" t="s">
+      <c r="A21" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="B21" s="55" t="s">
+      <c r="B21" s="56" t="s">
         <v>144</v>
       </c>
-      <c r="C21" s="55" t="s">
+      <c r="C21" s="56" t="s">
         <v>684</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="55" t="s">
+      <c r="A22" s="56" t="s">
         <v>431</v>
       </c>
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="56" t="s">
         <v>113</v>
       </c>
       <c r="C22" s="80" t="s">
@@ -25561,10 +25641,10 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="55" t="s">
+      <c r="A23" s="56" t="s">
         <v>361</v>
       </c>
-      <c r="B23" s="55" t="s">
+      <c r="B23" s="56" t="s">
         <v>152</v>
       </c>
       <c r="C23" s="0" t="s">
@@ -25572,21 +25652,21 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="55" t="s">
+      <c r="A24" s="56" t="s">
         <v>358</v>
       </c>
-      <c r="B24" s="55" t="s">
+      <c r="B24" s="56" t="s">
         <v>636</v>
       </c>
-      <c r="C24" s="55" t="s">
+      <c r="C24" s="56" t="s">
         <v>692</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="55" t="s">
+      <c r="A25" s="56" t="s">
         <v>196</v>
       </c>
-      <c r="B25" s="55" t="s">
+      <c r="B25" s="56" t="s">
         <v>633</v>
       </c>
       <c r="C25" s="0" t="s">
@@ -25594,10 +25674,10 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="55" t="s">
+      <c r="A26" s="56" t="s">
         <v>341</v>
       </c>
-      <c r="B26" s="55" t="s">
+      <c r="B26" s="56" t="s">
         <v>639</v>
       </c>
       <c r="C26" s="80" t="s">
@@ -25605,10 +25685,10 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="55" t="s">
+      <c r="A27" s="56" t="s">
         <v>217</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="56" t="s">
         <v>642</v>
       </c>
       <c r="C27" s="80" t="s">
@@ -25619,10 +25699,10 @@
       <c r="A28" s="81" t="s">
         <v>703</v>
       </c>
-      <c r="B28" s="55" t="s">
+      <c r="B28" s="56" t="s">
         <v>121</v>
       </c>
-      <c r="C28" s="55" t="s">
+      <c r="C28" s="56" t="s">
         <v>406</v>
       </c>
     </row>
@@ -25630,21 +25710,21 @@
       <c r="A29" s="81" t="s">
         <v>416</v>
       </c>
-      <c r="B29" s="55" t="s">
+      <c r="B29" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="C29" s="55" t="s">
+      <c r="C29" s="56" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="55" t="s">
+      <c r="A30" s="56" t="s">
         <v>669</v>
       </c>
       <c r="B30" s="80" t="s">
         <v>476</v>
       </c>
-      <c r="C30" s="55" t="s">
+      <c r="C30" s="56" t="s">
         <v>402</v>
       </c>
     </row>
@@ -25652,92 +25732,92 @@
       <c r="A31" s="81" t="s">
         <v>425</v>
       </c>
-      <c r="B31" s="55" t="s">
+      <c r="B31" s="56" t="s">
         <v>257</v>
       </c>
-      <c r="C31" s="55" t="s">
+      <c r="C31" s="56" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="55" t="s">
+      <c r="A32" s="56" t="s">
         <v>608</v>
       </c>
-      <c r="B32" s="55" t="s">
+      <c r="B32" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="55" t="s">
+      <c r="C32" s="56" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="55" t="s">
+      <c r="A33" s="56" t="s">
         <v>204</v>
       </c>
       <c r="B33" s="80" t="s">
         <v>467</v>
       </c>
-      <c r="C33" s="55" t="s">
+      <c r="C33" s="56" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="55" t="s">
+      <c r="A34" s="56" t="s">
         <v>351</v>
       </c>
       <c r="B34" s="82" t="s">
         <v>438</v>
       </c>
-      <c r="C34" s="55" t="s">
+      <c r="C34" s="56" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="55" t="s">
+      <c r="A35" s="56" t="s">
         <v>354</v>
       </c>
-      <c r="B35" s="55" t="s">
+      <c r="B35" s="56" t="s">
         <v>312</v>
       </c>
-      <c r="C35" s="55" t="s">
+      <c r="C35" s="56" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="55" t="s">
+      <c r="A36" s="56" t="s">
         <v>763</v>
       </c>
       <c r="B36" s="82" t="s">
         <v>436</v>
       </c>
-      <c r="C36" s="55" t="s">
+      <c r="C36" s="56" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="55" t="s">
+      <c r="A37" s="56" t="s">
         <v>14</v>
       </c>
       <c r="B37" s="81" t="s">
         <v>440</v>
       </c>
-      <c r="C37" s="55" t="s">
+      <c r="C37" s="56" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="55" t="s">
+      <c r="B38" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="55" t="s">
+      <c r="C38" s="56" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="55" t="s">
+      <c r="B39" s="56" t="s">
         <v>220</v>
       </c>
-      <c r="C39" s="55" t="s">
+      <c r="C39" s="56" t="s">
         <v>327</v>
       </c>
     </row>
@@ -25745,7 +25825,7 @@
       <c r="B40" s="82" t="s">
         <v>434</v>
       </c>
-      <c r="C40" s="55" t="s">
+      <c r="C40" s="56" t="s">
         <v>335</v>
       </c>
     </row>
@@ -25753,28 +25833,28 @@
       <c r="B41" s="80" t="s">
         <v>614</v>
       </c>
-      <c r="C41" s="55" t="s">
+      <c r="C41" s="56" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="55" t="s">
+      <c r="B42" s="56" t="s">
         <v>228</v>
       </c>
-      <c r="C42" s="55" t="s">
+      <c r="C42" s="56" t="s">
         <v>728</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="55" t="s">
+      <c r="B43" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="C43" s="55" t="s">
+      <c r="C43" s="56" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="55" t="s">
+      <c r="B44" s="56" t="s">
         <v>677</v>
       </c>
       <c r="C44" s="0" t="s">
@@ -25782,7 +25862,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="55" t="s">
+      <c r="B45" s="56" t="s">
         <v>64</v>
       </c>
       <c r="C45" s="0" t="s">
@@ -25790,7 +25870,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="55" t="s">
+      <c r="B46" s="56" t="s">
         <v>35</v>
       </c>
       <c r="C46" s="0" t="s">
@@ -25806,7 +25886,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="55" t="s">
+      <c r="B48" s="56" t="s">
         <v>117</v>
       </c>
       <c r="C48" s="0" t="s">
@@ -25814,7 +25894,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="55" t="s">
+      <c r="B49" s="56" t="s">
         <v>106</v>
       </c>
       <c r="C49" s="0" t="s">
@@ -25822,7 +25902,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="55" t="s">
+      <c r="B50" s="56" t="s">
         <v>715</v>
       </c>
       <c r="C50" s="0" t="s">
@@ -25838,7 +25918,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="55" t="s">
+      <c r="B52" s="56" t="s">
         <v>140</v>
       </c>
       <c r="C52" s="0" t="s">
@@ -25849,7 +25929,7 @@
       <c r="B53" s="0" t="s">
         <v>868</v>
       </c>
-      <c r="C53" s="55" t="s">
+      <c r="C53" s="56" t="s">
         <v>987</v>
       </c>
     </row>
@@ -25862,15 +25942,15 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="55" t="s">
+      <c r="B55" s="56" t="s">
         <v>373</v>
       </c>
-      <c r="C55" s="55" t="s">
+      <c r="C55" s="56" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="55" t="s">
+      <c r="B56" s="56" t="s">
         <v>242</v>
       </c>
       <c r="C56" s="0" t="s">
@@ -25878,15 +25958,15 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="55" t="s">
+      <c r="B57" s="56" t="s">
         <v>245</v>
       </c>
-      <c r="C57" s="55" t="s">
+      <c r="C57" s="56" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="55" t="s">
+      <c r="B58" s="56" t="s">
         <v>673</v>
       </c>
       <c r="C58" s="0" t="s">
@@ -25894,7 +25974,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="55" t="s">
+      <c r="B59" s="56" t="s">
         <v>133</v>
       </c>
       <c r="C59" s="80" t="s">
@@ -25902,15 +25982,15 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="55" t="s">
+      <c r="B60" s="56" t="s">
         <v>231</v>
       </c>
-      <c r="C60" s="55" t="s">
+      <c r="C60" s="56" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="55" t="s">
+      <c r="B61" s="56" t="s">
         <v>368</v>
       </c>
       <c r="C61" s="80" t="s">
@@ -25918,7 +25998,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="55" t="s">
+      <c r="B62" s="56" t="s">
         <v>376</v>
       </c>
       <c r="C62" s="80" t="s">
@@ -25934,10 +26014,10 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="55" t="s">
+      <c r="B64" s="56" t="s">
         <v>654</v>
       </c>
-      <c r="C64" s="55" t="s">
+      <c r="C64" s="56" t="s">
         <v>733</v>
       </c>
     </row>
@@ -25945,28 +26025,28 @@
       <c r="B65" s="0" t="s">
         <v>830</v>
       </c>
-      <c r="C65" s="55" t="s">
+      <c r="C65" s="56" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="55" t="s">
+      <c r="B66" s="56" t="s">
         <v>720</v>
       </c>
-      <c r="C66" s="55" t="s">
+      <c r="C66" s="56" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="55" t="s">
+      <c r="B67" s="56" t="s">
         <v>657</v>
       </c>
-      <c r="C67" s="55" t="s">
+      <c r="C67" s="56" t="s">
         <v>741</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="55" t="s">
+      <c r="B68" s="56" t="s">
         <v>718</v>
       </c>
       <c r="C68" s="0" t="s">
@@ -25974,7 +26054,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="55" t="s">
+      <c r="B69" s="56" t="s">
         <v>249</v>
       </c>
       <c r="C69" s="0" t="s">
@@ -25982,10 +26062,10 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="55" t="s">
+      <c r="B70" s="56" t="s">
         <v>235</v>
       </c>
-      <c r="C70" s="55" t="s">
+      <c r="C70" s="56" t="s">
         <v>164</v>
       </c>
     </row>
@@ -25993,7 +26073,7 @@
       <c r="B71" s="0" t="s">
         <v>857</v>
       </c>
-      <c r="C71" s="55" t="s">
+      <c r="C71" s="56" t="s">
         <v>175</v>
       </c>
     </row>
@@ -26014,7 +26094,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="55" t="s">
+      <c r="B74" s="56" t="s">
         <v>95</v>
       </c>
       <c r="C74" s="80" t="s">
@@ -26022,7 +26102,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="55" t="s">
+      <c r="B75" s="56" t="s">
         <v>305</v>
       </c>
       <c r="C75" s="80" t="s">
@@ -26038,31 +26118,31 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="55" t="s">
+      <c r="B77" s="56" t="s">
         <v>364</v>
       </c>
-      <c r="C77" s="55" t="s">
+      <c r="C77" s="56" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="55" t="s">
+      <c r="B78" s="56" t="s">
         <v>224</v>
       </c>
-      <c r="C78" s="55" t="s">
+      <c r="C78" s="56" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="55" t="s">
+      <c r="B79" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="C79" s="55" t="s">
+      <c r="C79" s="56" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="55" t="s">
+      <c r="B80" s="56" t="s">
         <v>260</v>
       </c>
       <c r="C80" s="81" t="s">
@@ -26070,15 +26150,15 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="55" t="s">
+      <c r="B81" s="56" t="s">
         <v>379</v>
       </c>
-      <c r="C81" s="55" t="s">
+      <c r="C81" s="56" t="s">
         <v>680</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="55" t="s">
+      <c r="B82" s="56" t="s">
         <v>263</v>
       </c>
       <c r="C82" s="0" t="s">
@@ -26089,15 +26169,15 @@
       <c r="B83" s="0" t="s">
         <v>793</v>
       </c>
-      <c r="C83" s="55" t="s">
+      <c r="C83" s="56" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="55" t="s">
+      <c r="B84" s="56" t="s">
         <v>459</v>
       </c>
-      <c r="C84" s="55" t="s">
+      <c r="C84" s="56" t="s">
         <v>168</v>
       </c>
     </row>
@@ -26105,27 +26185,27 @@
       <c r="B85" s="0" t="s">
         <v>864</v>
       </c>
-      <c r="C85" s="55" t="s">
+      <c r="C85" s="56" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C86" s="55" t="s">
+      <c r="C86" s="56" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C87" s="55" t="s">
+      <c r="C87" s="56" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C88" s="55" t="s">
+      <c r="C88" s="56" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C89" s="55" t="s">
+      <c r="C89" s="56" t="s">
         <v>757</v>
       </c>
     </row>
@@ -26140,7 +26220,7 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C92" s="55" t="s">
+      <c r="C92" s="56" t="s">
         <v>386</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working on more issue files
</commit_message>
<xml_diff>
--- a/info/apinet_survey (2).xlsx
+++ b/info/apinet_survey (2).xlsx
@@ -3830,7 +3830,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3918,13 +3918,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4156,7 +4149,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4377,10 +4370,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4389,7 +4378,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4401,7 +4390,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4469,31 +4458,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4581,11 +4570,11 @@
   </sheetPr>
   <dimension ref="A1:AK346"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N289" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S319" activeCellId="0" sqref="S319"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U304" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W326" activeCellId="0" sqref="W326"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.12"/>
@@ -16212,19 +16201,19 @@
       <c r="AA310" s="13" t="s">
         <v>904</v>
       </c>
-      <c r="AB310" s="48" t="s">
+      <c r="AB310" s="13" t="s">
         <v>905</v>
       </c>
       <c r="AC310" s="13" t="s">
         <v>906</v>
       </c>
-      <c r="AD310" s="48" t="s">
+      <c r="AD310" s="13" t="s">
         <v>907</v>
       </c>
       <c r="AE310" s="13" t="s">
         <v>908</v>
       </c>
-      <c r="AF310" s="55" t="s">
+      <c r="AF310" s="44" t="s">
         <v>905</v>
       </c>
       <c r="AK310" s="0" t="n">
@@ -16391,10 +16380,10 @@
       <c r="L314" s="10" t="s">
         <v>933</v>
       </c>
-      <c r="M314" s="56" t="s">
+      <c r="M314" s="55" t="s">
         <v>934</v>
       </c>
-      <c r="N314" s="56" t="s">
+      <c r="N314" s="55" t="s">
         <v>935</v>
       </c>
       <c r="O314" s="13" t="s">
@@ -16409,7 +16398,7 @@
       <c r="R314" s="13" t="s">
         <v>939</v>
       </c>
-      <c r="S314" s="48" t="s">
+      <c r="S314" s="13" t="s">
         <v>940</v>
       </c>
       <c r="T314" s="50" t="s">
@@ -16501,7 +16490,7 @@
       <c r="R315" s="13" t="s">
         <v>939</v>
       </c>
-      <c r="S315" s="48" t="s">
+      <c r="S315" s="13" t="s">
         <v>940</v>
       </c>
       <c r="T315" s="50" t="s">
@@ -16534,7 +16523,7 @@
       <c r="AC315" s="13" t="s">
         <v>950</v>
       </c>
-      <c r="AD315" s="57" t="s">
+      <c r="AD315" s="56" t="s">
         <v>956</v>
       </c>
       <c r="AE315" s="13" t="s">
@@ -16574,7 +16563,7 @@
       <c r="L316" s="54" t="s">
         <v>962</v>
       </c>
-      <c r="M316" s="56" t="s">
+      <c r="M316" s="55" t="s">
         <v>963</v>
       </c>
       <c r="N316" s="13" t="s">
@@ -16703,7 +16692,7 @@
       <c r="L318" s="11" t="s">
         <v>812</v>
       </c>
-      <c r="M318" s="56" t="s">
+      <c r="M318" s="55" t="s">
         <v>984</v>
       </c>
       <c r="O318" s="26"/>
@@ -16726,10 +16715,10 @@
       <c r="F319" s="0" t="s">
         <v>511</v>
       </c>
-      <c r="G319" s="58" t="s">
+      <c r="G319" s="57" t="s">
         <v>985</v>
       </c>
-      <c r="H319" s="58" t="s">
+      <c r="H319" s="57" t="s">
         <v>986</v>
       </c>
       <c r="I319" s="0" t="str">
@@ -16905,7 +16894,7 @@
       <c r="L323" s="11" t="s">
         <v>812</v>
       </c>
-      <c r="M323" s="56" t="s">
+      <c r="M323" s="55" t="s">
         <v>1004</v>
       </c>
       <c r="N323" s="7"/>
@@ -17089,7 +17078,7 @@
       <c r="S326" s="13" t="s">
         <v>1046</v>
       </c>
-      <c r="T326" s="59" t="s">
+      <c r="T326" s="58" t="s">
         <v>1043</v>
       </c>
       <c r="U326" s="13" t="s">
@@ -17098,7 +17087,7 @@
       <c r="V326" s="13" t="s">
         <v>1048</v>
       </c>
-      <c r="W326" s="48" t="s">
+      <c r="W326" s="13" t="s">
         <v>1049</v>
       </c>
       <c r="X326" s="13" t="s">
@@ -17110,19 +17099,19 @@
       <c r="Z326" s="13" t="s">
         <v>1052</v>
       </c>
-      <c r="AE326" s="60"/>
+      <c r="AE326" s="59"/>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B327" s="61"/>
+      <c r="B327" s="60"/>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B328" s="61"/>
+      <c r="B328" s="60"/>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B329" s="61"/>
+      <c r="B329" s="60"/>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B330" s="61"/>
+      <c r="B330" s="60"/>
       <c r="D330" s="1"/>
       <c r="E330" s="0" t="s">
         <v>1053</v>
@@ -17133,13 +17122,13 @@
       <c r="E331" s="0" t="s">
         <v>1054</v>
       </c>
-      <c r="L331" s="62"/>
+      <c r="L331" s="61"/>
       <c r="M331" s="0" t="s">
         <v>1055</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D332" s="63"/>
+      <c r="D332" s="62"/>
       <c r="E332" s="0" t="s">
         <v>1056</v>
       </c>
@@ -17149,7 +17138,7 @@
       </c>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D333" s="64"/>
+      <c r="D333" s="63"/>
       <c r="E333" s="0" t="s">
         <v>1058</v>
       </c>
@@ -17159,79 +17148,79 @@
       </c>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L334" s="65"/>
+      <c r="L334" s="64"/>
       <c r="M334" s="0" t="s">
         <v>1060</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L335" s="66"/>
+      <c r="L335" s="65"/>
       <c r="M335" s="0" t="s">
         <v>1061</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L336" s="67"/>
+      <c r="L336" s="66"/>
       <c r="M336" s="0" t="s">
         <v>1062</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L337" s="68"/>
+      <c r="L337" s="67"/>
       <c r="M337" s="0" t="s">
         <v>1063</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L338" s="69"/>
+      <c r="L338" s="68"/>
       <c r="M338" s="0" t="s">
         <v>1064</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L339" s="70"/>
+      <c r="L339" s="69"/>
       <c r="M339" s="0" t="s">
         <v>1065</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L340" s="71"/>
+      <c r="L340" s="70"/>
       <c r="M340" s="0" t="s">
         <v>1066</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L341" s="72"/>
+      <c r="L341" s="71"/>
       <c r="M341" s="0" t="s">
         <v>1067</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L342" s="73"/>
+      <c r="L342" s="72"/>
       <c r="M342" s="0" t="s">
         <v>1068</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L343" s="74"/>
+      <c r="L343" s="73"/>
       <c r="M343" s="0" t="s">
         <v>1069</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L344" s="75"/>
+      <c r="L344" s="74"/>
       <c r="M344" s="0" t="s">
         <v>1070</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L345" s="76"/>
+      <c r="L345" s="75"/>
       <c r="M345" s="0" t="s">
         <v>1071</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L346" s="77"/>
+      <c r="L346" s="76"/>
       <c r="M346" s="0" t="s">
         <v>1072</v>
       </c>
@@ -17883,7 +17872,7 @@
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.11"/>
@@ -17911,7 +17900,7 @@
       <c r="F1" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="J1" s="78" t="str">
+      <c r="J1" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K1)),RIGHT(K1,LEN(K1)-FIND(" ",K1)))</f>
         <v>aalternata</v>
       </c>
@@ -17945,7 +17934,7 @@
       <c r="F2" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="J2" s="78" t="str">
+      <c r="J2" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K2)),RIGHT(K2,LEN(K2)-FIND(" ",K2)))</f>
         <v>aalternata</v>
       </c>
@@ -17972,7 +17961,7 @@
       <c r="F3" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="J3" s="78" t="str">
+      <c r="J3" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K3)),RIGHT(K3,LEN(K3)-FIND(" ",K3)))</f>
         <v>aalternata</v>
       </c>
@@ -17999,7 +17988,7 @@
       <c r="F4" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="J4" s="78" t="str">
+      <c r="J4" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K4)),RIGHT(K4,LEN(K4)-FIND(" ",K4)))</f>
         <v>aapis</v>
       </c>
@@ -18033,7 +18022,7 @@
       <c r="F5" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="J5" s="79" t="s">
+      <c r="J5" s="78" t="s">
         <v>1073</v>
       </c>
       <c r="K5" s="7" t="s">
@@ -18066,7 +18055,7 @@
       <c r="F6" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="J6" s="78" t="str">
+      <c r="J6" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K6)),RIGHT(K6,LEN(K6)-FIND(" ",K6)))</f>
         <v>acoronavirus</v>
       </c>
@@ -18100,7 +18089,7 @@
       <c r="F7" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="J7" s="78" t="str">
+      <c r="J7" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K7)),RIGHT(K7,LEN(K7)-FIND(" ",K7)))</f>
         <v>aflavus</v>
       </c>
@@ -18134,7 +18123,7 @@
       <c r="F8" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="J8" s="78" t="str">
+      <c r="J8" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K8)),RIGHT(K8,LEN(K8)-FIND(" ",K8)))</f>
         <v>afumigatus</v>
       </c>
@@ -18168,7 +18157,7 @@
       <c r="F9" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="J9" s="78" t="str">
+      <c r="J9" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K9)),RIGHT(K9,LEN(K9)-FIND(" ",K9)))</f>
         <v>aflavus</v>
       </c>
@@ -18195,7 +18184,7 @@
       <c r="F10" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="J10" s="79" t="s">
+      <c r="J10" s="78" t="s">
         <v>1074</v>
       </c>
       <c r="K10" s="6" t="s">
@@ -18228,7 +18217,7 @@
       <c r="F11" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="J11" s="78" t="str">
+      <c r="J11" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K11)),RIGHT(K11,LEN(K11)-FIND(" ",K11)))</f>
         <v>afumigatus</v>
       </c>
@@ -18255,7 +18244,7 @@
       <c r="F12" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="J12" s="78" t="str">
+      <c r="J12" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K12)),RIGHT(K12,LEN(K12)-FIND(" ",K12)))</f>
         <v>afumigatus</v>
       </c>
@@ -18276,7 +18265,7 @@
         <f aca="false">SUM(F1:F12)</f>
         <v>106</v>
       </c>
-      <c r="J13" s="78" t="str">
+      <c r="J13" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K13)),RIGHT(K13,LEN(K13)-FIND(" ",K13)))</f>
         <v>afumigatus</v>
       </c>
@@ -18285,7 +18274,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J14" s="78" t="str">
+      <c r="J14" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K14)),RIGHT(K14,LEN(K14)-FIND(" ",K14)))</f>
         <v>afumigatus</v>
       </c>
@@ -18294,7 +18283,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J15" s="78" t="str">
+      <c r="J15" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K15)),RIGHT(K15,LEN(K15)-FIND(" ",K15)))</f>
         <v>afumigatus</v>
       </c>
@@ -18303,7 +18292,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J16" s="78" t="str">
+      <c r="J16" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K16)),RIGHT(K16,LEN(K16)-FIND(" ",K16)))</f>
         <v>afumigatus</v>
       </c>
@@ -18312,7 +18301,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J17" s="78" t="str">
+      <c r="J17" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K17)),RIGHT(K17,LEN(K17)-FIND(" ",K17)))</f>
         <v>amarginale</v>
       </c>
@@ -18328,7 +18317,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J18" s="78" t="str">
+      <c r="J18" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K18)),RIGHT(K18,LEN(K18)-FIND(" ",K18)))</f>
         <v>aniger</v>
       </c>
@@ -18344,7 +18333,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J19" s="78" t="str">
+      <c r="J19" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K19)),RIGHT(K19,LEN(K19)-FIND(" ",K19)))</f>
         <v>aparasiticus</v>
       </c>
@@ -18360,7 +18349,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J20" s="79" t="s">
+      <c r="J20" s="78" t="s">
         <v>1075</v>
       </c>
       <c r="K20" s="6" t="s">
@@ -18375,7 +18364,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J21" s="78" t="str">
+      <c r="J21" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K21)),RIGHT(K21,LEN(K21)-FIND(" ",K21)))</f>
         <v>aterreus</v>
       </c>
@@ -18391,7 +18380,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J22" s="78" t="str">
+      <c r="J22" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K22)),RIGHT(K22,LEN(K22)-FIND(" ",K22)))</f>
         <v>aviscosus</v>
       </c>
@@ -18407,7 +18396,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J23" s="78" t="str">
+      <c r="J23" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K23)),RIGHT(K23,LEN(K23)-FIND(" ",K23)))</f>
         <v>babortus</v>
       </c>
@@ -18423,7 +18412,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J24" s="79" t="s">
+      <c r="J24" s="78" t="s">
         <v>1076</v>
       </c>
       <c r="K24" s="6" t="s">
@@ -18438,7 +18427,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J25" s="78" t="str">
+      <c r="J25" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K25)),RIGHT(K25,LEN(K25)-FIND(" ",K25)))</f>
         <v>babortus</v>
       </c>
@@ -18447,7 +18436,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J26" s="78" t="str">
+      <c r="J26" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K26)),RIGHT(K26,LEN(K26)-FIND(" ",K26)))</f>
         <v>babortus</v>
       </c>
@@ -18456,7 +18445,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J27" s="78" t="str">
+      <c r="J27" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K27)),RIGHT(K27,LEN(K27)-FIND(" ",K27)))</f>
         <v>banthracis</v>
       </c>
@@ -18472,7 +18461,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J28" s="78" t="str">
+      <c r="J28" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K28)),RIGHT(K28,LEN(K28)-FIND(" ",K28)))</f>
         <v>balphaherpesvirus 1</v>
       </c>
@@ -18481,7 +18470,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J29" s="78" t="str">
+      <c r="J29" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K29)),RIGHT(K29,LEN(K29)-FIND(" ",K29)))</f>
         <v>bbronchiseptica</v>
       </c>
@@ -18497,7 +18486,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J30" s="78" t="str">
+      <c r="J30" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K30)),RIGHT(K30,LEN(K30)-FIND(" ",K30)))</f>
         <v>banthracis</v>
       </c>
@@ -18506,7 +18495,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J31" s="78" t="str">
+      <c r="J31" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K31)),RIGHT(K31,LEN(K31)-FIND(" ",K31)))</f>
         <v>banthracis</v>
       </c>
@@ -18515,7 +18504,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J32" s="78" t="str">
+      <c r="J32" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K32)),RIGHT(K32,LEN(K32)-FIND(" ",K32)))</f>
         <v>bdermatitidis</v>
       </c>
@@ -18531,7 +18520,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J33" s="78" t="str">
+      <c r="J33" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K33)),RIGHT(K33,LEN(K33)-FIND(" ",K33)))</f>
         <v>bbronchiseptica</v>
       </c>
@@ -18540,7 +18529,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J34" s="78" t="str">
+      <c r="J34" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K34)),RIGHT(K34,LEN(K34)-FIND(" ",K34)))</f>
         <v>bbronchiseptica</v>
       </c>
@@ -18549,7 +18538,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J35" s="79" t="s">
+      <c r="J35" s="78" t="s">
         <v>1077</v>
       </c>
       <c r="K35" s="6" t="s">
@@ -18564,7 +18553,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J36" s="78" t="str">
+      <c r="J36" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K36)),RIGHT(K36,LEN(K36)-FIND(" ",K36)))</f>
         <v>bdermatitidis</v>
       </c>
@@ -18573,7 +18562,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J37" s="78" t="str">
+      <c r="J37" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K37)),RIGHT(K37,LEN(K37)-FIND(" ",K37)))</f>
         <v>bdermatitidis</v>
       </c>
@@ -18582,7 +18571,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J38" s="78" t="str">
+      <c r="J38" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K38)),RIGHT(K38,LEN(K38)-FIND(" ",K38)))</f>
         <v>bhyodysenteriae</v>
       </c>
@@ -18598,7 +18587,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J39" s="79" t="s">
+      <c r="J39" s="78" t="s">
         <v>1078</v>
       </c>
       <c r="K39" s="7" t="s">
@@ -18613,7 +18602,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J40" s="78" t="str">
+      <c r="J40" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K40)),RIGHT(K40,LEN(K40)-FIND(" ",K40)))</f>
         <v>bmelitensis</v>
       </c>
@@ -18629,7 +18618,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J41" s="79" t="s">
+      <c r="J41" s="78" t="s">
         <v>1079</v>
       </c>
       <c r="K41" s="6" t="s">
@@ -18644,7 +18633,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J42" s="78" t="str">
+      <c r="J42" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K42)),RIGHT(K42,LEN(K42)-FIND(" ",K42)))</f>
         <v>bmelitensis</v>
       </c>
@@ -18653,7 +18642,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J43" s="79" t="s">
+      <c r="J43" s="78" t="s">
         <v>1080</v>
       </c>
       <c r="K43" s="7" t="s">
@@ -18668,7 +18657,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J44" s="78" t="str">
+      <c r="J44" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K44)),RIGHT(K44,LEN(K44)-FIND(" ",K44)))</f>
         <v>branarum</v>
       </c>
@@ -18684,7 +18673,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J45" s="78" t="str">
+      <c r="J45" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K45)),RIGHT(K45,LEN(K45)-FIND(" ",K45)))</f>
         <v>bsuis</v>
       </c>
@@ -18700,7 +18689,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J46" s="79" t="s">
+      <c r="J46" s="78" t="s">
         <v>1081</v>
       </c>
       <c r="K46" s="7" t="s">
@@ -18715,7 +18704,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J47" s="79" t="s">
+      <c r="J47" s="78" t="s">
         <v>1082</v>
       </c>
       <c r="K47" s="6" t="s">
@@ -18730,7 +18719,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J48" s="78" t="str">
+      <c r="J48" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K48)),RIGHT(K48,LEN(K48)-FIND(" ",K48)))</f>
         <v>bviral diarrhea virus 1</v>
       </c>
@@ -18739,7 +18728,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J49" s="78" t="str">
+      <c r="J49" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K49)),RIGHT(K49,LEN(K49)-FIND(" ",K49)))</f>
         <v>bviral diarrhea virus 1</v>
       </c>
@@ -18748,7 +18737,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J50" s="78" t="str">
+      <c r="J50" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K50)),RIGHT(K50,LEN(K50)-FIND(" ",K50)))</f>
         <v>bvirus</v>
       </c>
@@ -18764,7 +18753,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J51" s="78" t="str">
+      <c r="J51" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K51)),RIGHT(K51,LEN(K51)-FIND(" ",K51)))</f>
         <v>bviral diarrhea virus 2</v>
       </c>
@@ -18773,7 +18762,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J52" s="78" t="str">
+      <c r="J52" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K52)),RIGHT(K52,LEN(K52)-FIND(" ",K52)))</f>
         <v>cabortus</v>
       </c>
@@ -18789,7 +18778,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J53" s="78" t="str">
+      <c r="J53" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K53)),RIGHT(K53,LEN(K53)-FIND(" ",K53)))</f>
         <v>bvirus</v>
       </c>
@@ -18798,7 +18787,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J54" s="79" t="s">
+      <c r="J54" s="78" t="s">
         <v>1083</v>
       </c>
       <c r="K54" s="7" t="s">
@@ -18813,7 +18802,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J55" s="78" t="str">
+      <c r="J55" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K55)),RIGHT(K55,LEN(K55)-FIND(" ",K55)))</f>
         <v>cabortus</v>
       </c>
@@ -18822,7 +18811,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J56" s="79" t="s">
+      <c r="J56" s="78" t="s">
         <v>1084</v>
       </c>
       <c r="K56" s="7" t="s">
@@ -18837,7 +18826,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J57" s="78" t="str">
+      <c r="J57" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K57)),RIGHT(K57,LEN(K57)-FIND(" ",K57)))</f>
         <v>calbicans</v>
       </c>
@@ -18853,7 +18842,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J58" s="78" t="str">
+      <c r="J58" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K58)),RIGHT(K58,LEN(K58)-FIND(" ",K58)))</f>
         <v>candersoni</v>
       </c>
@@ -18869,7 +18858,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J59" s="78" t="str">
+      <c r="J59" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K59)),RIGHT(K59,LEN(K59)-FIND(" ",K59)))</f>
         <v>calbicans</v>
       </c>
@@ -18878,7 +18867,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J60" s="78" t="str">
+      <c r="J60" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K60)),RIGHT(K60,LEN(K60)-FIND(" ",K60)))</f>
         <v>calbicans</v>
       </c>
@@ -18887,7 +18876,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J61" s="78" t="str">
+      <c r="J61" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K61)),RIGHT(K61,LEN(K61)-FIND(" ",K61)))</f>
         <v>calbicans</v>
       </c>
@@ -18896,7 +18885,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J62" s="78" t="str">
+      <c r="J62" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K62)),RIGHT(K62,LEN(K62)-FIND(" ",K62)))</f>
         <v>calbicans</v>
       </c>
@@ -18905,7 +18894,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J63" s="78" t="str">
+      <c r="J63" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K63)),RIGHT(K63,LEN(K63)-FIND(" ",K63)))</f>
         <v>calbicans</v>
       </c>
@@ -18914,7 +18903,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J64" s="78" t="str">
+      <c r="J64" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K64)),RIGHT(K64,LEN(K64)-FIND(" ",K64)))</f>
         <v>calbicans</v>
       </c>
@@ -18923,7 +18912,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J65" s="78" t="str">
+      <c r="J65" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K65)),RIGHT(K65,LEN(K65)-FIND(" ",K65)))</f>
         <v>calbicans</v>
       </c>
@@ -18932,7 +18921,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J66" s="79" t="s">
+      <c r="J66" s="78" t="s">
         <v>1085</v>
       </c>
       <c r="K66" s="7" t="s">
@@ -18947,7 +18936,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J67" s="78" t="str">
+      <c r="J67" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K67)),RIGHT(K67,LEN(K67)-FIND(" ",K67)))</f>
         <v>cauris</v>
       </c>
@@ -18963,7 +18952,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J68" s="78" t="str">
+      <c r="J68" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K68)),RIGHT(K68,LEN(K68)-FIND(" ",K68)))</f>
         <v>cbantiana</v>
       </c>
@@ -18979,7 +18968,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J69" s="79" t="s">
+      <c r="J69" s="78" t="s">
         <v>1086</v>
       </c>
       <c r="K69" s="7" t="s">
@@ -18994,7 +18983,7 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J70" s="78" t="str">
+      <c r="J70" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K70)),RIGHT(K70,LEN(K70)-FIND(" ",K70)))</f>
         <v>cbantiana</v>
       </c>
@@ -19003,7 +18992,7 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J71" s="78" t="str">
+      <c r="J71" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K71)),RIGHT(K71,LEN(K71)-FIND(" ",K71)))</f>
         <v>cbantiana</v>
       </c>
@@ -19012,7 +19001,7 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J72" s="78" t="str">
+      <c r="J72" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K72)),RIGHT(K72,LEN(K72)-FIND(" ",K72)))</f>
         <v>cbovis</v>
       </c>
@@ -19028,7 +19017,7 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J73" s="78" t="str">
+      <c r="J73" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K73)),RIGHT(K73,LEN(K73)-FIND(" ",K73)))</f>
         <v>cburnetii</v>
       </c>
@@ -19044,7 +19033,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J74" s="78" t="str">
+      <c r="J74" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K74)),RIGHT(K74,LEN(K74)-FIND(" ",K74)))</f>
         <v>ccoronatus</v>
       </c>
@@ -19060,7 +19049,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J75" s="78" t="str">
+      <c r="J75" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K75)),RIGHT(K75,LEN(K75)-FIND(" ",K75)))</f>
         <v>cburnetii</v>
       </c>
@@ -19069,7 +19058,7 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J76" s="78" t="str">
+      <c r="J76" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K76)),RIGHT(K76,LEN(K76)-FIND(" ",K76)))</f>
         <v>ccoronavirus</v>
       </c>
@@ -19085,7 +19074,7 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J77" s="78" t="str">
+      <c r="J77" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K77)),RIGHT(K77,LEN(K77)-FIND(" ",K77)))</f>
         <v>cdifficile</v>
       </c>
@@ -19101,7 +19090,7 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J78" s="78" t="str">
+      <c r="J78" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K78)),RIGHT(K78,LEN(K78)-FIND(" ",K78)))</f>
         <v>cfelis</v>
       </c>
@@ -19117,7 +19106,7 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J79" s="78" t="str">
+      <c r="J79" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K79)),RIGHT(K79,LEN(K79)-FIND(" ",K79)))</f>
         <v>cgattii</v>
       </c>
@@ -19133,7 +19122,7 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J80" s="79" t="s">
+      <c r="J80" s="78" t="s">
         <v>1087</v>
       </c>
       <c r="K80" s="7" t="s">
@@ -19148,7 +19137,7 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J81" s="78" t="str">
+      <c r="J81" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K81)),RIGHT(K81,LEN(K81)-FIND(" ",K81)))</f>
         <v>cgattii</v>
       </c>
@@ -19157,7 +19146,7 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J82" s="78" t="str">
+      <c r="J82" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K82)),RIGHT(K82,LEN(K82)-FIND(" ",K82)))</f>
         <v>cgattii</v>
       </c>
@@ -19166,7 +19155,7 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J83" s="78" t="str">
+      <c r="J83" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K83)),RIGHT(K83,LEN(K83)-FIND(" ",K83)))</f>
         <v>cgattii</v>
       </c>
@@ -19175,7 +19164,7 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J84" s="78" t="str">
+      <c r="J84" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K84)),RIGHT(K84,LEN(K84)-FIND(" ",K84)))</f>
         <v>cgattii</v>
       </c>
@@ -19184,7 +19173,7 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J85" s="78" t="str">
+      <c r="J85" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K85)),RIGHT(K85,LEN(K85)-FIND(" ",K85)))</f>
         <v>cimmitis</v>
       </c>
@@ -19200,7 +19189,7 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J86" s="78" t="str">
+      <c r="J86" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K86)),RIGHT(K86,LEN(K86)-FIND(" ",K86)))</f>
         <v>cjejuni</v>
       </c>
@@ -19216,7 +19205,7 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J87" s="78" t="str">
+      <c r="J87" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K87)),RIGHT(K87,LEN(K87)-FIND(" ",K87)))</f>
         <v>cimmitis</v>
       </c>
@@ -19225,7 +19214,7 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J88" s="78" t="str">
+      <c r="J88" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K88)),RIGHT(K88,LEN(K88)-FIND(" ",K88)))</f>
         <v>cneoformans</v>
       </c>
@@ -19241,7 +19230,7 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J89" s="78" t="str">
+      <c r="J89" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K89)),RIGHT(K89,LEN(K89)-FIND(" ",K89)))</f>
         <v>cjejuni</v>
       </c>
@@ -19250,7 +19239,7 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J90" s="79" t="s">
+      <c r="J90" s="78" t="s">
         <v>1089</v>
       </c>
       <c r="K90" s="7" t="s">
@@ -19265,7 +19254,7 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J91" s="78" t="str">
+      <c r="J91" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K91)),RIGHT(K91,LEN(K91)-FIND(" ",K91)))</f>
         <v>cneoformans</v>
       </c>
@@ -19274,7 +19263,7 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J92" s="78" t="str">
+      <c r="J92" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K92)),RIGHT(K92,LEN(K92)-FIND(" ",K92)))</f>
         <v>cneoformans</v>
       </c>
@@ -19283,7 +19272,7 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J93" s="78" t="str">
+      <c r="J93" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K93)),RIGHT(K93,LEN(K93)-FIND(" ",K93)))</f>
         <v>cneoformans</v>
       </c>
@@ -19292,7 +19281,7 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J94" s="78" t="str">
+      <c r="J94" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K94)),RIGHT(K94,LEN(K94)-FIND(" ",K94)))</f>
         <v>cparvovirus</v>
       </c>
@@ -19308,7 +19297,7 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J95" s="78" t="str">
+      <c r="J95" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K95)),RIGHT(K95,LEN(K95)-FIND(" ",K95)))</f>
         <v>cparvum</v>
       </c>
@@ -19324,7 +19313,7 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J96" s="79" t="s">
+      <c r="J96" s="78" t="s">
         <v>1090</v>
       </c>
       <c r="K96" s="7" t="s">
@@ -19339,7 +19328,7 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J97" s="79" t="s">
+      <c r="J97" s="78" t="s">
         <v>1091</v>
       </c>
       <c r="K97" s="7" t="s">
@@ -19354,7 +19343,7 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J98" s="79" t="s">
+      <c r="J98" s="78" t="s">
         <v>1092</v>
       </c>
       <c r="K98" s="7" t="s">
@@ -19369,7 +19358,7 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J99" s="79" t="s">
+      <c r="J99" s="78" t="s">
         <v>1093</v>
       </c>
       <c r="K99" s="7" t="s">
@@ -19384,7 +19373,7 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J100" s="79" t="s">
+      <c r="J100" s="78" t="s">
         <v>1094</v>
       </c>
       <c r="K100" s="7" t="s">
@@ -19399,7 +19388,7 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J101" s="78" t="str">
+      <c r="J101" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K101)),RIGHT(K101,LEN(K101)-FIND(" ",K101)))</f>
         <v>cperfringens C</v>
       </c>
@@ -19408,7 +19397,7 @@
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J102" s="78" t="str">
+      <c r="J102" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K102)),RIGHT(K102,LEN(K102)-FIND(" ",K102)))</f>
         <v>cpseudotuberculosis</v>
       </c>
@@ -19424,7 +19413,7 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J103" s="78" t="str">
+      <c r="J103" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K103)),RIGHT(K103,LEN(K103)-FIND(" ",K103)))</f>
         <v>cpsittaci</v>
       </c>
@@ -19440,7 +19429,7 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J104" s="78" t="str">
+      <c r="J104" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K104)),RIGHT(K104,LEN(K104)-FIND(" ",K104)))</f>
         <v>cpseudotuberculosis</v>
       </c>
@@ -19449,7 +19438,7 @@
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J105" s="78" t="str">
+      <c r="J105" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K105)),RIGHT(K105,LEN(K105)-FIND(" ",K105)))</f>
         <v>cpurpurea</v>
       </c>
@@ -19465,7 +19454,7 @@
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J106" s="78" t="str">
+      <c r="J106" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K106)),RIGHT(K106,LEN(K106)-FIND(" ",K106)))</f>
         <v>cryanae</v>
       </c>
@@ -19481,7 +19470,7 @@
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J107" s="79" t="s">
+      <c r="J107" s="78" t="s">
         <v>1095</v>
       </c>
       <c r="K107" s="6" t="s">
@@ -19496,7 +19485,7 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J108" s="78" t="str">
+      <c r="J108" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K108)),RIGHT(K108,LEN(K108)-FIND(" ",K108)))</f>
         <v>ctetani</v>
       </c>
@@ -19512,7 +19501,7 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J109" s="78" t="str">
+      <c r="J109" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K109)),RIGHT(K109,LEN(K109)-FIND(" ",K109)))</f>
         <v>ctrachomatis</v>
       </c>
@@ -19528,7 +19517,7 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J110" s="78" t="str">
+      <c r="J110" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K110)),RIGHT(K110,LEN(K110)-FIND(" ",K110)))</f>
         <v>ctetani</v>
       </c>
@@ -19537,7 +19526,7 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J111" s="78" t="str">
+      <c r="J111" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K111)),RIGHT(K111,LEN(K111)-FIND(" ",K111)))</f>
         <v>ctetani</v>
       </c>
@@ -19546,7 +19535,7 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J112" s="78" t="str">
+      <c r="J112" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K112)),RIGHT(K112,LEN(K112)-FIND(" ",K112)))</f>
         <v>ctetani</v>
       </c>
@@ -19555,7 +19544,7 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J113" s="79" t="s">
+      <c r="J113" s="78" t="s">
         <v>1096</v>
       </c>
       <c r="K113" s="7" t="s">
@@ -19570,7 +19559,7 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J114" s="78" t="str">
+      <c r="J114" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K114)),RIGHT(K114,LEN(K114)-FIND(" ",K114)))</f>
         <v>dcongolensis</v>
       </c>
@@ -19586,7 +19575,7 @@
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J115" s="78" t="str">
+      <c r="J115" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K115)),RIGHT(K115,LEN(K115)-FIND(" ",K115)))</f>
         <v>dnodosus</v>
       </c>
@@ -19602,7 +19591,7 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J116" s="79" t="s">
+      <c r="J116" s="78" t="s">
         <v>1100</v>
       </c>
       <c r="K116" s="7" t="s">
@@ -19617,7 +19606,7 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J117" s="78" t="str">
+      <c r="J117" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K117)),RIGHT(K117,LEN(K117)-FIND(" ",K117)))</f>
         <v>dnodosus</v>
       </c>
@@ -19626,7 +19615,7 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J118" s="79" t="s">
+      <c r="J118" s="78" t="s">
         <v>1101</v>
       </c>
       <c r="K118" s="7" t="s">
@@ -19641,7 +19630,7 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J119" s="79" t="s">
+      <c r="J119" s="78" t="s">
         <v>1102</v>
       </c>
       <c r="K119" s="7" t="s">
@@ -19656,7 +19645,7 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J120" s="79" t="s">
+      <c r="J120" s="78" t="s">
         <v>1103</v>
       </c>
       <c r="K120" s="7" t="s">
@@ -19671,7 +19660,7 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J121" s="78" t="str">
+      <c r="J121" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K121)),RIGHT(K121,LEN(K121)-FIND(" ",K121)))</f>
         <v>ecoli</v>
       </c>
@@ -19687,7 +19676,7 @@
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J122" s="79" t="s">
+      <c r="J122" s="78" t="s">
         <v>1104</v>
       </c>
       <c r="K122" s="0" t="s">
@@ -19702,7 +19691,7 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J123" s="78" t="str">
+      <c r="J123" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K123)),RIGHT(K123,LEN(K123)-FIND(" ",K123)))</f>
         <v>ecoli</v>
       </c>
@@ -19711,7 +19700,7 @@
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J124" s="78" t="str">
+      <c r="J124" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K124)),RIGHT(K124,LEN(K124)-FIND(" ",K124)))</f>
         <v>ecoli</v>
       </c>
@@ -19720,7 +19709,7 @@
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J125" s="78" t="str">
+      <c r="J125" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K125)),RIGHT(K125,LEN(K125)-FIND(" ",K125)))</f>
         <v>ecoli</v>
       </c>
@@ -19729,7 +19718,7 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J126" s="78" t="str">
+      <c r="J126" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K126)),RIGHT(K126,LEN(K126)-FIND(" ",K126)))</f>
         <v>ecoli</v>
       </c>
@@ -19738,7 +19727,7 @@
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J127" s="78" t="str">
+      <c r="J127" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K127)),RIGHT(K127,LEN(K127)-FIND(" ",K127)))</f>
         <v>ecoli</v>
       </c>
@@ -19747,7 +19736,7 @@
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J128" s="78" t="str">
+      <c r="J128" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K128)),RIGHT(K128,LEN(K128)-FIND(" ",K128)))</f>
         <v>ecoli</v>
       </c>
@@ -19756,7 +19745,7 @@
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J129" s="78" t="str">
+      <c r="J129" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K129)),RIGHT(K129,LEN(K129)-FIND(" ",K129)))</f>
         <v>edermatitidis</v>
       </c>
@@ -19772,7 +19761,7 @@
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J130" s="79" t="s">
+      <c r="J130" s="78" t="s">
         <v>1105</v>
       </c>
       <c r="K130" s="7" t="s">
@@ -19787,7 +19776,7 @@
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J131" s="78" t="str">
+      <c r="J131" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K131)),RIGHT(K131,LEN(K131)-FIND(" ",K131)))</f>
         <v>edermatitidis</v>
       </c>
@@ -19796,7 +19785,7 @@
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J132" s="78" t="str">
+      <c r="J132" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K132)),RIGHT(K132,LEN(K132)-FIND(" ",K132)))</f>
         <v>edermatitidis</v>
       </c>
@@ -19805,7 +19794,7 @@
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J133" s="79" t="s">
+      <c r="J133" s="78" t="s">
         <v>1106</v>
       </c>
       <c r="K133" s="6" t="s">
@@ -19820,7 +19809,7 @@
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J134" s="79" t="s">
+      <c r="J134" s="78" t="s">
         <v>1107</v>
       </c>
       <c r="K134" s="6" t="s">
@@ -19835,7 +19824,7 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J135" s="78" t="str">
+      <c r="J135" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K135)),RIGHT(K135,LEN(K135)-FIND(" ",K135)))</f>
         <v>ehemorrhagic disease virus</v>
       </c>
@@ -19844,7 +19833,7 @@
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J136" s="79" t="s">
+      <c r="J136" s="78" t="s">
         <v>1108</v>
       </c>
       <c r="K136" s="7" t="s">
@@ -19859,7 +19848,7 @@
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J137" s="79" t="s">
+      <c r="J137" s="78" t="s">
         <v>1109</v>
       </c>
       <c r="K137" s="7" t="s">
@@ -19874,7 +19863,7 @@
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J138" s="78" t="str">
+      <c r="J138" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K138)),RIGHT(K138,LEN(K138)-FIND(" ",K138)))</f>
         <v>erhusiopathiae</v>
       </c>
@@ -19890,7 +19879,7 @@
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J139" s="78" t="str">
+      <c r="J139" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K139)),RIGHT(K139,LEN(K139)-FIND(" ",K139)))</f>
         <v>erotavirus</v>
       </c>
@@ -19906,7 +19895,7 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J140" s="79" t="s">
+      <c r="J140" s="78" t="s">
         <v>1110</v>
       </c>
       <c r="K140" s="7" t="s">
@@ -19921,7 +19910,7 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J141" s="78" t="str">
+      <c r="J141" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K141)),RIGHT(K141,LEN(K141)-FIND(" ",K141)))</f>
         <v>fcalicivirus</v>
       </c>
@@ -19937,7 +19926,7 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J142" s="79" t="s">
+      <c r="J142" s="78" t="s">
         <v>1111</v>
       </c>
       <c r="K142" s="7" t="s">
@@ -19952,7 +19941,7 @@
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J143" s="78" t="str">
+      <c r="J143" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K143)),RIGHT(K143,LEN(K143)-FIND(" ",K143)))</f>
         <v>fgraminearum</v>
       </c>
@@ -19968,7 +19957,7 @@
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J144" s="78" t="str">
+      <c r="J144" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K144)),RIGHT(K144,LEN(K144)-FIND(" ",K144)))</f>
         <v>fdisease virus</v>
       </c>
@@ -19977,7 +19966,7 @@
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J145" s="78" t="str">
+      <c r="J145" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K145)),RIGHT(K145,LEN(K145)-FIND(" ",K145)))</f>
         <v>fdisease virus</v>
       </c>
@@ -19986,7 +19975,7 @@
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J146" s="78" t="str">
+      <c r="J146" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K146)),RIGHT(K146,LEN(K146)-FIND(" ",K146)))</f>
         <v>fdisease virus</v>
       </c>
@@ -19995,7 +19984,7 @@
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J147" s="78" t="str">
+      <c r="J147" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K147)),RIGHT(K147,LEN(K147)-FIND(" ",K147)))</f>
         <v>fdisease virus</v>
       </c>
@@ -20004,7 +19993,7 @@
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J148" s="78" t="str">
+      <c r="J148" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K148)),RIGHT(K148,LEN(K148)-FIND(" ",K148)))</f>
         <v>fdisease virus</v>
       </c>
@@ -20013,7 +20002,7 @@
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J149" s="79" t="s">
+      <c r="J149" s="78" t="s">
         <v>1112</v>
       </c>
       <c r="K149" s="7" t="s">
@@ -20028,7 +20017,7 @@
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J150" s="79" t="s">
+      <c r="J150" s="78" t="s">
         <v>1113</v>
       </c>
       <c r="K150" s="7" t="s">
@@ -20043,7 +20032,7 @@
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J151" s="79" t="s">
+      <c r="J151" s="78" t="s">
         <v>1114</v>
       </c>
       <c r="K151" s="7" t="s">
@@ -20058,7 +20047,7 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J152" s="78" t="str">
+      <c r="J152" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K152)),RIGHT(K152,LEN(K152)-FIND(" ",K152)))</f>
         <v>fnecrophorum</v>
       </c>
@@ -20074,7 +20063,7 @@
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J153" s="79" t="s">
+      <c r="J153" s="78" t="s">
         <v>1115</v>
       </c>
       <c r="K153" s="7" t="s">
@@ -20089,7 +20078,7 @@
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J154" s="78" t="str">
+      <c r="J154" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K154)),RIGHT(K154,LEN(K154)-FIND(" ",K154)))</f>
         <v>fnecrophorum</v>
       </c>
@@ -20098,7 +20087,7 @@
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J155" s="78" t="str">
+      <c r="J155" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K155)),RIGHT(K155,LEN(K155)-FIND(" ",K155)))</f>
         <v>fproliferatum</v>
       </c>
@@ -20114,7 +20103,7 @@
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J156" s="78" t="str">
+      <c r="J156" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K156)),RIGHT(K156,LEN(K156)-FIND(" ",K156)))</f>
         <v>fverticillioides</v>
       </c>
@@ -20130,7 +20119,7 @@
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J157" s="78" t="str">
+      <c r="J157" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K157)),RIGHT(K157,LEN(K157)-FIND(" ",K157)))</f>
         <v>fproliferatum</v>
       </c>
@@ -20139,7 +20128,7 @@
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J158" s="78" t="str">
+      <c r="J158" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K158)),RIGHT(K158,LEN(K158)-FIND(" ",K158)))</f>
         <v>fvirus</v>
       </c>
@@ -20155,7 +20144,7 @@
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J159" s="78" t="str">
+      <c r="J159" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K159)),RIGHT(K159,LEN(K159)-FIND(" ",K159)))</f>
         <v>fverticillioides (moniliforme)</v>
       </c>
@@ -20164,7 +20153,7 @@
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J160" s="79" t="s">
+      <c r="J160" s="78" t="s">
         <v>1118</v>
       </c>
       <c r="K160" s="7" t="s">
@@ -20179,7 +20168,7 @@
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J161" s="79" t="s">
+      <c r="J161" s="78" t="s">
         <v>1119</v>
       </c>
       <c r="K161" s="0" t="s">
@@ -20194,7 +20183,7 @@
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J162" s="79" t="s">
+      <c r="J162" s="78" t="s">
         <v>1120</v>
       </c>
       <c r="K162" s="0" t="s">
@@ -20209,7 +20198,7 @@
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J163" s="79" t="s">
+      <c r="J163" s="78" t="s">
         <v>1121</v>
       </c>
       <c r="K163" s="0" t="s">
@@ -20224,7 +20213,7 @@
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J164" s="78" t="str">
+      <c r="J164" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K164)),RIGHT(K164,LEN(K164)-FIND(" ",K164)))</f>
         <v>hcapsulatum</v>
       </c>
@@ -20240,7 +20229,7 @@
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J165" s="79" t="s">
+      <c r="J165" s="78" t="s">
         <v>1122</v>
       </c>
       <c r="K165" s="7" t="s">
@@ -20255,7 +20244,7 @@
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J166" s="78" t="str">
+      <c r="J166" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K166)),RIGHT(K166,LEN(K166)-FIND(" ",K166)))</f>
         <v>hcapsulatum</v>
       </c>
@@ -20264,7 +20253,7 @@
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J167" s="78" t="str">
+      <c r="J167" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K167)),RIGHT(K167,LEN(K167)-FIND(" ",K167)))</f>
         <v>hcapsulatum</v>
       </c>
@@ -20273,7 +20262,7 @@
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J168" s="79" t="s">
+      <c r="J168" s="78" t="s">
         <v>1125</v>
       </c>
       <c r="K168" s="0" t="s">
@@ -20288,7 +20277,7 @@
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J169" s="79" t="s">
+      <c r="J169" s="78" t="s">
         <v>1126</v>
       </c>
       <c r="K169" s="0" t="s">
@@ -20303,7 +20292,7 @@
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J170" s="79" t="s">
+      <c r="J170" s="78" t="s">
         <v>1127</v>
       </c>
       <c r="K170" s="0" t="s">
@@ -20318,7 +20307,7 @@
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J171" s="79" t="s">
+      <c r="J171" s="78" t="s">
         <v>1128</v>
       </c>
       <c r="K171" s="0" t="s">
@@ -20333,13 +20322,13 @@
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J172" s="79" t="s">
+      <c r="J172" s="78" t="s">
         <v>1129</v>
       </c>
-      <c r="K172" s="58" t="s">
+      <c r="K172" s="57" t="s">
         <v>985</v>
       </c>
-      <c r="L172" s="58" t="s">
+      <c r="L172" s="57" t="s">
         <v>986</v>
       </c>
       <c r="M172" s="0" t="str">
@@ -20348,7 +20337,7 @@
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J173" s="79" t="s">
+      <c r="J173" s="78" t="s">
         <v>1130</v>
       </c>
       <c r="K173" s="0" t="s">
@@ -20363,7 +20352,7 @@
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J174" s="79" t="s">
+      <c r="J174" s="78" t="s">
         <v>1131</v>
       </c>
       <c r="K174" s="0" t="s">
@@ -20378,7 +20367,7 @@
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J175" s="79" t="s">
+      <c r="J175" s="78" t="s">
         <v>1132</v>
       </c>
       <c r="K175" s="0" t="s">
@@ -20393,7 +20382,7 @@
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J176" s="79" t="s">
+      <c r="J176" s="78" t="s">
         <v>1133</v>
       </c>
       <c r="K176" s="7" t="s">
@@ -20408,7 +20397,7 @@
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J177" s="79" t="s">
+      <c r="J177" s="78" t="s">
         <v>1134</v>
       </c>
       <c r="K177" s="0" t="s">
@@ -20423,7 +20412,7 @@
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J178" s="79" t="s">
+      <c r="J178" s="78" t="s">
         <v>1135</v>
       </c>
       <c r="K178" s="7" t="s">
@@ -20438,7 +20427,7 @@
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J179" s="79" t="s">
+      <c r="J179" s="78" t="s">
         <v>1136</v>
       </c>
       <c r="K179" s="0" t="s">
@@ -20453,7 +20442,7 @@
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J180" s="78" t="str">
+      <c r="J180" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K180)),RIGHT(K180,LEN(K180)-FIND(" ",K180)))</f>
         <v>iA (H3N2)</v>
       </c>
@@ -20462,7 +20451,7 @@
       </c>
     </row>
     <row r="181" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J181" s="78" t="str">
+      <c r="J181" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K181)),RIGHT(K181,LEN(K181)-FIND(" ",K181)))</f>
         <v>lautumnalis</v>
       </c>
@@ -20478,7 +20467,7 @@
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J182" s="78" t="str">
+      <c r="J182" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K182)),RIGHT(K182,LEN(K182)-FIND(" ",K182)))</f>
         <v>lborgpetersenii</v>
       </c>
@@ -20494,7 +20483,7 @@
       </c>
     </row>
     <row r="183" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J183" s="78" t="str">
+      <c r="J183" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K183)),RIGHT(K183,LEN(K183)-FIND(" ",K183)))</f>
         <v>lgrippothyphosa</v>
       </c>
@@ -20510,7 +20499,7 @@
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J184" s="78" t="str">
+      <c r="J184" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K184)),RIGHT(K184,LEN(K184)-FIND(" ",K184)))</f>
         <v>lborgpetersenii</v>
       </c>
@@ -20519,7 +20508,7 @@
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J185" s="78" t="str">
+      <c r="J185" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K185)),RIGHT(K185,LEN(K185)-FIND(" ",K185)))</f>
         <v>lhyos</v>
       </c>
@@ -20535,7 +20524,7 @@
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J186" s="78" t="str">
+      <c r="J186" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K186)),RIGHT(K186,LEN(K186)-FIND(" ",K186)))</f>
         <v>linterrogans</v>
       </c>
@@ -20551,7 +20540,7 @@
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J187" s="78" t="str">
+      <c r="J187" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K187)),RIGHT(K187,LEN(K187)-FIND(" ",K187)))</f>
         <v>lintracellularis</v>
       </c>
@@ -20567,7 +20556,7 @@
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J188" s="78" t="str">
+      <c r="J188" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K188)),RIGHT(K188,LEN(K188)-FIND(" ",K188)))</f>
         <v>linterrogans</v>
       </c>
@@ -20576,7 +20565,7 @@
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J189" s="78" t="str">
+      <c r="J189" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K189)),RIGHT(K189,LEN(K189)-FIND(" ",K189)))</f>
         <v>linterrogans</v>
       </c>
@@ -20585,7 +20574,7 @@
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J190" s="78" t="str">
+      <c r="J190" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K190)),RIGHT(K190,LEN(K190)-FIND(" ",K190)))</f>
         <v>linterrogans</v>
       </c>
@@ -20594,7 +20583,7 @@
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J191" s="78" t="str">
+      <c r="J191" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K191)),RIGHT(K191,LEN(K191)-FIND(" ",K191)))</f>
         <v>lkirschneri</v>
       </c>
@@ -20610,7 +20599,7 @@
       </c>
     </row>
     <row r="192" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J192" s="78" t="str">
+      <c r="J192" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K192)),RIGHT(K192,LEN(K192)-FIND(" ",K192)))</f>
         <v>lmonocytogenes</v>
       </c>
@@ -20626,7 +20615,7 @@
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J193" s="78" t="str">
+      <c r="J193" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K193)),RIGHT(K193,LEN(K193)-FIND(" ",K193)))</f>
         <v>lkirschneri</v>
       </c>
@@ -20635,7 +20624,7 @@
       </c>
     </row>
     <row r="194" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J194" s="78" t="str">
+      <c r="J194" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K194)),RIGHT(K194,LEN(K194)-FIND(" ",K194)))</f>
         <v>lpomona</v>
       </c>
@@ -20651,7 +20640,7 @@
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J195" s="78" t="str">
+      <c r="J195" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K195)),RIGHT(K195,LEN(K195)-FIND(" ",K195)))</f>
         <v>lrabies</v>
       </c>
@@ -20667,7 +20656,7 @@
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J196" s="79" t="s">
+      <c r="J196" s="78" t="s">
         <v>1138</v>
       </c>
       <c r="K196" s="6" t="s">
@@ -20682,7 +20671,7 @@
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J197" s="78" t="str">
+      <c r="J197" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K197)),RIGHT(K197,LEN(K197)-FIND(" ",K197)))</f>
         <v>lrabies</v>
       </c>
@@ -20691,7 +20680,7 @@
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J198" s="78" t="str">
+      <c r="J198" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K198)),RIGHT(K198,LEN(K198)-FIND(" ",K198)))</f>
         <v>lrabies</v>
       </c>
@@ -20700,7 +20689,7 @@
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J199" s="79" t="s">
+      <c r="J199" s="78" t="s">
         <v>1139</v>
       </c>
       <c r="K199" s="7" t="s">
@@ -20715,7 +20704,7 @@
       </c>
     </row>
     <row r="200" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J200" s="78" t="str">
+      <c r="J200" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K200)),RIGHT(K200,LEN(K200)-FIND(" ",K200)))</f>
         <v>lskin disease virus</v>
       </c>
@@ -20724,7 +20713,7 @@
       </c>
     </row>
     <row r="201" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J201" s="78" t="str">
+      <c r="J201" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K201)),RIGHT(K201,LEN(K201)-FIND(" ",K201)))</f>
         <v>malcelaphinegamma1</v>
       </c>
@@ -20740,7 +20729,7 @@
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J202" s="79" t="s">
+      <c r="J202" s="78" t="s">
         <v>1140</v>
       </c>
       <c r="K202" s="7" t="s">
@@ -20755,7 +20744,7 @@
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J203" s="78" t="str">
+      <c r="J203" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K203)),RIGHT(K203,LEN(K203)-FIND(" ",K203)))</f>
         <v>mbovis</v>
       </c>
@@ -20771,7 +20760,7 @@
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J204" s="78" t="str">
+      <c r="J204" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K204)),RIGHT(K204,LEN(K204)-FIND(" ",K204)))</f>
         <v>mavium subsp. Paratuberculosis</v>
       </c>
@@ -20780,7 +20769,7 @@
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J205" s="78" t="str">
+      <c r="J205" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K205)),RIGHT(K205,LEN(K205)-FIND(" ",K205)))</f>
         <v>mavium subsp. Paratuberculosis</v>
       </c>
@@ -20789,7 +20778,7 @@
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J206" s="78" t="str">
+      <c r="J206" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K206)),RIGHT(K206,LEN(K206)-FIND(" ",K206)))</f>
         <v>mcanis</v>
       </c>
@@ -20805,7 +20794,7 @@
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J207" s="78" t="str">
+      <c r="J207" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K207)),RIGHT(K207,LEN(K207)-FIND(" ",K207)))</f>
         <v>mbovis</v>
       </c>
@@ -20814,7 +20803,7 @@
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J208" s="78" t="str">
+      <c r="J208" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K208)),RIGHT(K208,LEN(K208)-FIND(" ",K208)))</f>
         <v>mbovis</v>
       </c>
@@ -20823,7 +20812,7 @@
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J209" s="78" t="str">
+      <c r="J209" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K209)),RIGHT(K209,LEN(K209)-FIND(" ",K209)))</f>
         <v>mcanis</v>
       </c>
@@ -20839,7 +20828,7 @@
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J210" s="79" t="s">
+      <c r="J210" s="78" t="s">
         <v>1143</v>
       </c>
       <c r="K210" s="7" t="s">
@@ -20854,7 +20843,7 @@
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J211" s="78" t="str">
+      <c r="J211" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K211)),RIGHT(K211,LEN(K211)-FIND(" ",K211)))</f>
         <v>mcanis</v>
       </c>
@@ -20863,7 +20852,7 @@
       </c>
     </row>
     <row r="212" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J212" s="78" t="str">
+      <c r="J212" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K212)),RIGHT(K212,LEN(K212)-FIND(" ",K212)))</f>
         <v>mcaprinegamma2</v>
       </c>
@@ -20879,7 +20868,7 @@
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J213" s="78" t="str">
+      <c r="J213" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K213)),RIGHT(K213,LEN(K213)-FIND(" ",K213)))</f>
         <v>mconjunctivae</v>
       </c>
@@ -20895,7 +20884,7 @@
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J214" s="79" t="s">
+      <c r="J214" s="78" t="s">
         <v>1144</v>
       </c>
       <c r="K214" s="7" t="s">
@@ -20910,7 +20899,7 @@
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J215" s="78" t="str">
+      <c r="J215" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K215)),RIGHT(K215,LEN(K215)-FIND(" ",K215)))</f>
         <v>mgallisepticum</v>
       </c>
@@ -20926,7 +20915,7 @@
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J216" s="78" t="str">
+      <c r="J216" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K216)),RIGHT(K216,LEN(K216)-FIND(" ",K216)))</f>
         <v>mhaemolytica</v>
       </c>
@@ -20942,7 +20931,7 @@
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J217" s="78" t="str">
+      <c r="J217" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K217)),RIGHT(K217,LEN(K217)-FIND(" ",K217)))</f>
         <v>mmycoides</v>
       </c>
@@ -20958,7 +20947,7 @@
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J218" s="78" t="str">
+      <c r="J218" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K218)),RIGHT(K218,LEN(K218)-FIND(" ",K218)))</f>
         <v>mhaemolytica</v>
       </c>
@@ -20967,7 +20956,7 @@
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J219" s="78" t="str">
+      <c r="J219" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K219)),RIGHT(K219,LEN(K219)-FIND(" ",K219)))</f>
         <v>mnanum</v>
       </c>
@@ -20983,7 +20972,7 @@
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J220" s="78" t="str">
+      <c r="J220" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K220)),RIGHT(K220,LEN(K220)-FIND(" ",K220)))</f>
         <v>movinegamma2</v>
       </c>
@@ -20999,7 +20988,7 @@
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J221" s="78" t="str">
+      <c r="J221" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K221)),RIGHT(K221,LEN(K221)-FIND(" ",K221)))</f>
         <v>movis</v>
       </c>
@@ -21015,7 +21004,7 @@
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J222" s="78" t="str">
+      <c r="J222" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K222)),RIGHT(K222,LEN(K222)-FIND(" ",K222)))</f>
         <v>mpachydermatis</v>
       </c>
@@ -21031,7 +21020,7 @@
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J223" s="78" t="str">
+      <c r="J223" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K223)),RIGHT(K223,LEN(K223)-FIND(" ",K223)))</f>
         <v>movis</v>
       </c>
@@ -21040,7 +21029,7 @@
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J224" s="78" t="str">
+      <c r="J224" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K224)),RIGHT(K224,LEN(K224)-FIND(" ",K224)))</f>
         <v>mplutonius</v>
       </c>
@@ -21056,7 +21045,7 @@
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J225" s="78" t="str">
+      <c r="J225" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K225)),RIGHT(K225,LEN(K225)-FIND(" ",K225)))</f>
         <v>mpachydermatis</v>
       </c>
@@ -21065,7 +21054,7 @@
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J226" s="78" t="str">
+      <c r="J226" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K226)),RIGHT(K226,LEN(K226)-FIND(" ",K226)))</f>
         <v>mtuberculosis</v>
       </c>
@@ -21081,7 +21070,7 @@
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J227" s="78" t="str">
+      <c r="J227" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K227)),RIGHT(K227,LEN(K227)-FIND(" ",K227)))</f>
         <v>napis</v>
       </c>
@@ -21097,7 +21086,7 @@
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J228" s="78" t="str">
+      <c r="J228" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K228)),RIGHT(K228,LEN(K228)-FIND(" ",K228)))</f>
         <v>nasteroides</v>
       </c>
@@ -21113,7 +21102,7 @@
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J229" s="78" t="str">
+      <c r="J229" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K229)),RIGHT(K229,LEN(K229)-FIND(" ",K229)))</f>
         <v>nbrasiliensis</v>
       </c>
@@ -21129,7 +21118,7 @@
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J230" s="79" t="s">
+      <c r="J230" s="78" t="s">
         <v>1149</v>
       </c>
       <c r="K230" s="7" t="s">
@@ -21144,7 +21133,7 @@
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J231" s="79" t="s">
+      <c r="J231" s="78" t="s">
         <v>1150</v>
       </c>
       <c r="K231" s="0" t="s">
@@ -21159,7 +21148,7 @@
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J232" s="78" t="str">
+      <c r="J232" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K232)),RIGHT(K232,LEN(K232)-FIND(" ",K232)))</f>
         <v>ngonorrhoeae</v>
       </c>
@@ -21175,7 +21164,7 @@
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J233" s="79" t="s">
+      <c r="J233" s="78" t="s">
         <v>1151</v>
       </c>
       <c r="K233" s="0" t="s">
@@ -21190,7 +21179,7 @@
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J234" s="78" t="str">
+      <c r="J234" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K234)),RIGHT(K234,LEN(K234)-FIND(" ",K234)))</f>
         <v>nmeningitidis</v>
       </c>
@@ -21206,7 +21195,7 @@
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J235" s="78" t="str">
+      <c r="J235" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K235)),RIGHT(K235,LEN(K235)-FIND(" ",K235)))</f>
         <v>nristicii</v>
       </c>
@@ -21222,7 +21211,7 @@
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J236" s="78" t="str">
+      <c r="J236" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K236)),RIGHT(K236,LEN(K236)-FIND(" ",K236)))</f>
         <v>ovirus</v>
       </c>
@@ -21238,7 +21227,7 @@
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J237" s="78" t="str">
+      <c r="J237" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K237)),RIGHT(K237,LEN(K237)-FIND(" ",K237)))</f>
         <v>paeruginosa</v>
       </c>
@@ -21254,7 +21243,7 @@
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J238" s="78" t="str">
+      <c r="J238" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K238)),RIGHT(K238,LEN(K238)-FIND(" ",K238)))</f>
         <v>ovirus</v>
       </c>
@@ -21263,7 +21252,7 @@
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J239" s="78" t="str">
+      <c r="J239" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K239)),RIGHT(K239,LEN(K239)-FIND(" ",K239)))</f>
         <v>pchartarum</v>
       </c>
@@ -21279,7 +21268,7 @@
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J240" s="78" t="str">
+      <c r="J240" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K240)),RIGHT(K240,LEN(K240)-FIND(" ",K240)))</f>
         <v>paeruginosa</v>
       </c>
@@ -21288,7 +21277,7 @@
       </c>
     </row>
     <row r="241" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J241" s="79" t="s">
+      <c r="J241" s="78" t="s">
         <v>1152</v>
       </c>
       <c r="K241" s="6" t="s">
@@ -21303,7 +21292,7 @@
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J242" s="79" t="s">
+      <c r="J242" s="78" t="s">
         <v>1154</v>
       </c>
       <c r="K242" s="7" t="s">
@@ -21318,7 +21307,7 @@
       </c>
     </row>
     <row r="243" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J243" s="79" t="s">
+      <c r="J243" s="78" t="s">
         <v>1155</v>
       </c>
       <c r="K243" s="6" t="s">
@@ -21333,7 +21322,7 @@
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J244" s="78" t="str">
+      <c r="J244" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K244)),RIGHT(K244,LEN(K244)-FIND(" ",K244)))</f>
         <v>plarvae</v>
       </c>
@@ -21349,7 +21338,7 @@
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J245" s="78" t="str">
+      <c r="J245" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K245)),RIGHT(K245,LEN(K245)-FIND(" ",K245)))</f>
         <v>pmultocida</v>
       </c>
@@ -21365,7 +21354,7 @@
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J246" s="78" t="str">
+      <c r="J246" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K246)),RIGHT(K246,LEN(K246)-FIND(" ",K246)))</f>
         <v>ppuberulum</v>
       </c>
@@ -21381,7 +21370,7 @@
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J247" s="78" t="str">
+      <c r="J247" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K247)),RIGHT(K247,LEN(K247)-FIND(" ",K247)))</f>
         <v>pmultocida</v>
       </c>
@@ -21390,7 +21379,7 @@
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J248" s="78" t="str">
+      <c r="J248" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K248)),RIGHT(K248,LEN(K248)-FIND(" ",K248)))</f>
         <v>pmultocida</v>
       </c>
@@ -21399,7 +21388,7 @@
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J249" s="78" t="str">
+      <c r="J249" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K249)),RIGHT(K249,LEN(K249)-FIND(" ",K249)))</f>
         <v>pmultocida</v>
       </c>
@@ -21408,7 +21397,7 @@
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J250" s="78" t="str">
+      <c r="J250" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K250)),RIGHT(K250,LEN(K250)-FIND(" ",K250)))</f>
         <v>pmultocida</v>
       </c>
@@ -21417,7 +21406,7 @@
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J251" s="78" t="str">
+      <c r="J251" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K251)),RIGHT(K251,LEN(K251)-FIND(" ",K251)))</f>
         <v>pmultocida</v>
       </c>
@@ -21426,7 +21415,7 @@
       </c>
     </row>
     <row r="252" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J252" s="79" t="s">
+      <c r="J252" s="78" t="s">
         <v>1156</v>
       </c>
       <c r="K252" s="6" t="s">
@@ -21441,7 +21430,7 @@
       </c>
     </row>
     <row r="253" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J253" s="79" t="s">
+      <c r="J253" s="78" t="s">
         <v>1157</v>
       </c>
       <c r="K253" s="6" t="s">
@@ -21456,7 +21445,7 @@
       </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J254" s="79" t="s">
+      <c r="J254" s="78" t="s">
         <v>1158</v>
       </c>
       <c r="K254" s="7" t="s">
@@ -21471,7 +21460,7 @@
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J255" s="79" t="s">
+      <c r="J255" s="78" t="s">
         <v>1159</v>
       </c>
       <c r="K255" s="7" t="s">
@@ -21486,7 +21475,7 @@
       </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J256" s="79" t="s">
+      <c r="J256" s="78" t="s">
         <v>1160</v>
       </c>
       <c r="K256" s="7" t="s">
@@ -21501,7 +21490,7 @@
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J257" s="79" t="s">
+      <c r="J257" s="78" t="s">
         <v>1161</v>
       </c>
       <c r="K257" s="7" t="s">
@@ -21516,7 +21505,7 @@
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J258" s="79" t="s">
+      <c r="J258" s="78" t="s">
         <v>1162</v>
       </c>
       <c r="K258" s="7" t="s">
@@ -21531,7 +21520,7 @@
       </c>
     </row>
     <row r="259" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J259" s="78" t="str">
+      <c r="J259" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K259)),RIGHT(K259,LEN(K259)-FIND(" ",K259)))</f>
         <v>rvirus</v>
       </c>
@@ -21547,7 +21536,7 @@
       </c>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J260" s="78" t="str">
+      <c r="J260" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K260)),RIGHT(K260,LEN(K260)-FIND(" ",K260)))</f>
         <v>sagalactiae</v>
       </c>
@@ -21563,7 +21552,7 @@
       </c>
     </row>
     <row r="261" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J261" s="78" t="str">
+      <c r="J261" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K261)),RIGHT(K261,LEN(K261)-FIND(" ",K261)))</f>
         <v>rvirus</v>
       </c>
@@ -21572,7 +21561,7 @@
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J262" s="78" t="str">
+      <c r="J262" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K262)),RIGHT(K262,LEN(K262)-FIND(" ",K262)))</f>
         <v>sagona</v>
       </c>
@@ -21588,7 +21577,7 @@
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J263" s="79" t="s">
+      <c r="J263" s="78" t="s">
         <v>1163</v>
       </c>
       <c r="K263" s="7" t="s">
@@ -21603,7 +21592,7 @@
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J264" s="78" t="str">
+      <c r="J264" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K264)),RIGHT(K264,LEN(K264)-FIND(" ",K264)))</f>
         <v>saureus</v>
       </c>
@@ -21619,7 +21608,7 @@
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J265" s="78" t="str">
+      <c r="J265" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K265)),RIGHT(K265,LEN(K265)-FIND(" ",K265)))</f>
         <v>scanis</v>
       </c>
@@ -21635,7 +21624,7 @@
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J266" s="78" t="str">
+      <c r="J266" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K266)),RIGHT(K266,LEN(K266)-FIND(" ",K266)))</f>
         <v>saureus</v>
       </c>
@@ -21644,7 +21633,7 @@
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J267" s="78" t="str">
+      <c r="J267" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K267)),RIGHT(K267,LEN(K267)-FIND(" ",K267)))</f>
         <v>saureus</v>
       </c>
@@ -21653,7 +21642,7 @@
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J268" s="78" t="str">
+      <c r="J268" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K268)),RIGHT(K268,LEN(K268)-FIND(" ",K268)))</f>
         <v>saureus</v>
       </c>
@@ -21662,7 +21651,7 @@
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J269" s="78" t="str">
+      <c r="J269" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K269)),RIGHT(K269,LEN(K269)-FIND(" ",K269)))</f>
         <v>saureus</v>
       </c>
@@ -21671,7 +21660,7 @@
       </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J270" s="79" t="s">
+      <c r="J270" s="78" t="s">
         <v>1164</v>
       </c>
       <c r="K270" s="7" t="s">
@@ -21686,7 +21675,7 @@
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J271" s="78" t="str">
+      <c r="J271" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K271)),RIGHT(K271,LEN(K271)-FIND(" ",K271)))</f>
         <v>scanis</v>
       </c>
@@ -21695,7 +21684,7 @@
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J272" s="78" t="str">
+      <c r="J272" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K272)),RIGHT(K272,LEN(K272)-FIND(" ",K272)))</f>
         <v>scholeraesuis</v>
       </c>
@@ -21711,7 +21700,7 @@
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J273" s="78" t="str">
+      <c r="J273" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K273)),RIGHT(K273,LEN(K273)-FIND(" ",K273)))</f>
         <v>sdublin</v>
       </c>
@@ -21727,7 +21716,7 @@
       </c>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J274" s="78" t="str">
+      <c r="J274" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K274)),RIGHT(K274,LEN(K274)-FIND(" ",K274)))</f>
         <v>sdysenteriae</v>
       </c>
@@ -21743,7 +21732,7 @@
       </c>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J275" s="78" t="str">
+      <c r="J275" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K275)),RIGHT(K275,LEN(K275)-FIND(" ",K275)))</f>
         <v>senteritidis</v>
       </c>
@@ -21759,7 +21748,7 @@
       </c>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J276" s="79" t="s">
+      <c r="J276" s="78" t="s">
         <v>1166</v>
       </c>
       <c r="K276" s="7" t="s">
@@ -21774,7 +21763,7 @@
       </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J277" s="79" t="s">
+      <c r="J277" s="78" t="s">
         <v>1169</v>
       </c>
       <c r="K277" s="7" t="s">
@@ -21789,7 +21778,7 @@
       </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J278" s="78" t="str">
+      <c r="J278" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K278)),RIGHT(K278,LEN(K278)-FIND(" ",K278)))</f>
         <v>sfelis</v>
       </c>
@@ -21805,7 +21794,7 @@
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J279" s="78" t="str">
+      <c r="J279" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K279)),RIGHT(K279,LEN(K279)-FIND(" ",K279)))</f>
         <v>sequi subsp. Zooepidemicus</v>
       </c>
@@ -21814,7 +21803,7 @@
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J280" s="78" t="str">
+      <c r="J280" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K280)),RIGHT(K280,LEN(K280)-FIND(" ",K280)))</f>
         <v>sequi subsp. Zooepidemicus</v>
       </c>
@@ -21823,7 +21812,7 @@
       </c>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J281" s="78" t="str">
+      <c r="J281" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K281)),RIGHT(K281,LEN(K281)-FIND(" ",K281)))</f>
         <v>sflexneri</v>
       </c>
@@ -21839,7 +21828,7 @@
       </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J282" s="78" t="str">
+      <c r="J282" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K282)),RIGHT(K282,LEN(K282)-FIND(" ",K282)))</f>
         <v>sgallinarum</v>
       </c>
@@ -21855,7 +21844,7 @@
       </c>
     </row>
     <row r="283" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J283" s="78" t="str">
+      <c r="J283" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K283)),RIGHT(K283,LEN(K283)-FIND(" ",K283)))</f>
         <v>shyicus</v>
       </c>
@@ -21871,7 +21860,7 @@
       </c>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J284" s="79" t="s">
+      <c r="J284" s="78" t="s">
         <v>1174</v>
       </c>
       <c r="K284" s="7" t="s">
@@ -21886,7 +21875,7 @@
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J285" s="79" t="s">
+      <c r="J285" s="78" t="s">
         <v>1175</v>
       </c>
       <c r="K285" s="7" t="s">
@@ -21901,7 +21890,7 @@
       </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J286" s="78" t="str">
+      <c r="J286" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K286)),RIGHT(K286,LEN(K286)-FIND(" ",K286)))</f>
         <v>sintermedius</v>
       </c>
@@ -21917,7 +21906,7 @@
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J287" s="78" t="str">
+      <c r="J287" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K287)),RIGHT(K287,LEN(K287)-FIND(" ",K287)))</f>
         <v>snewport</v>
       </c>
@@ -21933,7 +21922,7 @@
       </c>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J288" s="78" t="str">
+      <c r="J288" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K288)),RIGHT(K288,LEN(K288)-FIND(" ",K288)))</f>
         <v>spneumoniae</v>
       </c>
@@ -21949,7 +21938,7 @@
       </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J289" s="78" t="str">
+      <c r="J289" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K289)),RIGHT(K289,LEN(K289)-FIND(" ",K289)))</f>
         <v>spseudintermedius</v>
       </c>
@@ -21965,7 +21954,7 @@
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J290" s="78" t="str">
+      <c r="J290" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K290)),RIGHT(K290,LEN(K290)-FIND(" ",K290)))</f>
         <v>spullorum</v>
       </c>
@@ -21981,7 +21970,7 @@
       </c>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J291" s="78" t="str">
+      <c r="J291" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K291)),RIGHT(K291,LEN(K291)-FIND(" ",K291)))</f>
         <v>spseudintermedius</v>
       </c>
@@ -21990,7 +21979,7 @@
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J292" s="78" t="str">
+      <c r="J292" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K292)),RIGHT(K292,LEN(K292)-FIND(" ",K292)))</f>
         <v>spseudintermedius</v>
       </c>
@@ -21999,7 +21988,7 @@
       </c>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J293" s="78" t="str">
+      <c r="J293" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K293)),RIGHT(K293,LEN(K293)-FIND(" ",K293)))</f>
         <v>sschenckii</v>
       </c>
@@ -22015,7 +22004,7 @@
       </c>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J294" s="78" t="str">
+      <c r="J294" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K294)),RIGHT(K294,LEN(K294)-FIND(" ",K294)))</f>
         <v>ssonnei</v>
       </c>
@@ -22031,7 +22020,7 @@
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J295" s="78" t="str">
+      <c r="J295" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K295)),RIGHT(K295,LEN(K295)-FIND(" ",K295)))</f>
         <v>sschenckii</v>
       </c>
@@ -22040,7 +22029,7 @@
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J296" s="78" t="str">
+      <c r="J296" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K296)),RIGHT(K296,LEN(K296)-FIND(" ",K296)))</f>
         <v>sschenckii</v>
       </c>
@@ -22049,7 +22038,7 @@
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J297" s="79" t="s">
+      <c r="J297" s="78" t="s">
         <v>1178</v>
       </c>
       <c r="K297" s="7" t="s">
@@ -22064,7 +22053,7 @@
       </c>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J298" s="78" t="str">
+      <c r="J298" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K298)),RIGHT(K298,LEN(K298)-FIND(" ",K298)))</f>
         <v>styphimurium</v>
       </c>
@@ -22080,7 +22069,7 @@
       </c>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J299" s="78" t="str">
+      <c r="J299" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K299)),RIGHT(K299,LEN(K299)-FIND(" ",K299)))</f>
         <v>styphimurium</v>
       </c>
@@ -22096,7 +22085,7 @@
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J300" s="78" t="str">
+      <c r="J300" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K300)),RIGHT(K300,LEN(K300)-FIND(" ",K300)))</f>
         <v>styphimurium</v>
       </c>
@@ -22105,7 +22094,7 @@
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J301" s="78" t="str">
+      <c r="J301" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K301)),RIGHT(K301,LEN(K301)-FIND(" ",K301)))</f>
         <v>styphimurium</v>
       </c>
@@ -22114,7 +22103,7 @@
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J302" s="78" t="str">
+      <c r="J302" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K302)),RIGHT(K302,LEN(K302)-FIND(" ",K302)))</f>
         <v>styphimurium</v>
       </c>
@@ -22123,7 +22112,7 @@
       </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J303" s="78" t="str">
+      <c r="J303" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K303)),RIGHT(K303,LEN(K303)-FIND(" ",K303)))</f>
         <v>styphimurium</v>
       </c>
@@ -22132,7 +22121,7 @@
       </c>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J304" s="79" t="s">
+      <c r="J304" s="78" t="s">
         <v>1180</v>
       </c>
       <c r="K304" s="7" t="s">
@@ -22147,7 +22136,7 @@
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J305" s="79" t="s">
+      <c r="J305" s="78" t="s">
         <v>1181</v>
       </c>
       <c r="K305" s="7" t="s">
@@ -22162,7 +22151,7 @@
       </c>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J306" s="79" t="s">
+      <c r="J306" s="78" t="s">
         <v>1182</v>
       </c>
       <c r="K306" s="7" t="s">
@@ -22177,7 +22166,7 @@
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J307" s="78" t="str">
+      <c r="J307" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K307)),RIGHT(K307,LEN(K307)-FIND(" ",K307)))</f>
         <v>svirus</v>
       </c>
@@ -22186,7 +22175,7 @@
       </c>
     </row>
     <row r="308" customFormat="false" ht="14.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J308" s="78" t="str">
+      <c r="J308" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K308)),RIGHT(K308,LEN(K308)-FIND(" ",K308)))</f>
         <v>svirus</v>
       </c>
@@ -22195,7 +22184,7 @@
       </c>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J309" s="79" t="s">
+      <c r="J309" s="78" t="s">
         <v>1183</v>
       </c>
       <c r="K309" s="7" t="s">
@@ -22210,7 +22199,7 @@
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J310" s="78" t="str">
+      <c r="J310" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K310)),RIGHT(K310,LEN(K310)-FIND(" ",K310)))</f>
         <v>tequinum</v>
       </c>
@@ -22226,7 +22215,7 @@
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J311" s="79" t="s">
+      <c r="J311" s="78" t="s">
         <v>1184</v>
       </c>
       <c r="K311" s="7" t="s">
@@ -22241,7 +22230,7 @@
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J312" s="78" t="str">
+      <c r="J312" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K312)),RIGHT(K312,LEN(K312)-FIND(" ",K312)))</f>
         <v>tmentagrophytes</v>
       </c>
@@ -22257,7 +22246,7 @@
       </c>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J313" s="78" t="str">
+      <c r="J313" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K313)),RIGHT(K313,LEN(K313)-FIND(" ",K313)))</f>
         <v>tpallidum</v>
       </c>
@@ -22273,7 +22262,7 @@
       </c>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J314" s="78" t="str">
+      <c r="J314" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K314)),RIGHT(K314,LEN(K314)-FIND(" ",K314)))</f>
         <v>tmentagrophytes</v>
       </c>
@@ -22282,7 +22271,7 @@
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J315" s="78" t="str">
+      <c r="J315" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K315)),RIGHT(K315,LEN(K315)-FIND(" ",K315)))</f>
         <v>trubrum</v>
       </c>
@@ -22298,7 +22287,7 @@
       </c>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J316" s="78" t="str">
+      <c r="J316" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K316)),RIGHT(K316,LEN(K316)-FIND(" ",K316)))</f>
         <v>tverrucosum</v>
       </c>
@@ -22314,7 +22303,7 @@
       </c>
     </row>
     <row r="317" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J317" s="79" t="s">
+      <c r="J317" s="78" t="s">
         <v>1185</v>
       </c>
       <c r="K317" s="6" t="s">
@@ -22329,7 +22318,7 @@
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J318" s="78" t="str">
+      <c r="J318" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K318)),RIGHT(K318,LEN(K318)-FIND(" ",K318)))</f>
         <v>tverrucosum</v>
       </c>
@@ -22338,7 +22327,7 @@
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J319" s="78" t="str">
+      <c r="J319" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K319)),RIGHT(K319,LEN(K319)-FIND(" ",K319)))</f>
         <v>tverrucosum</v>
       </c>
@@ -22347,7 +22336,7 @@
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J320" s="78" t="str">
+      <c r="J320" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K320)),RIGHT(K320,LEN(K320)-FIND(" ",K320)))</f>
         <v>tverrucosum</v>
       </c>
@@ -22356,7 +22345,7 @@
       </c>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J321" s="78" t="str">
+      <c r="J321" s="77" t="str">
         <f aca="false">_xlfn.CONCAT(LOWER(LEFT(K321)),RIGHT(K321,LEN(K321)-FIND(" ",K321)))</f>
         <v>tverrucosum</v>
       </c>
@@ -22365,7 +22354,7 @@
       </c>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J322" s="79" t="s">
+      <c r="J322" s="78" t="s">
         <v>1186</v>
       </c>
       <c r="K322" s="0" t="s">
@@ -22380,7 +22369,7 @@
       </c>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J323" s="79" t="s">
+      <c r="J323" s="78" t="s">
         <v>1187</v>
       </c>
       <c r="K323" s="7" t="s">
@@ -22395,7 +22384,7 @@
       </c>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J324" s="79" t="s">
+      <c r="J324" s="78" t="s">
         <v>1188</v>
       </c>
       <c r="K324" s="0" t="s">
@@ -22410,7 +22399,7 @@
       </c>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J325" s="79" t="s">
+      <c r="J325" s="78" t="s">
         <v>1189</v>
       </c>
       <c r="K325" s="0" t="s">
@@ -22425,7 +22414,7 @@
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J326" s="78"/>
+      <c r="J326" s="77"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -22449,7 +22438,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="11.72"/>
   </cols>
@@ -24040,7 +24029,7 @@
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A318" s="58" t="s">
+      <c r="A318" s="57" t="s">
         <v>986</v>
       </c>
     </row>
@@ -24101,7 +24090,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.89"/>
@@ -25469,7 +25458,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.99"/>
@@ -25478,24 +25467,24 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="79" t="s">
         <v>1194</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="79" t="s">
         <v>1195</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="80" t="s">
         <v>1196</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="57" t="s">
         <v>214</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="57" t="s">
         <v>238</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="57" t="s">
         <v>697</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -25504,112 +25493,112 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="57" t="s">
         <v>665</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="81" t="s">
         <v>559</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="81" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="82" t="s">
         <v>185</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="82" t="s">
+      <c r="C4" s="81" t="s">
         <v>575</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="57" t="s">
         <v>419</v>
       </c>
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="57" t="s">
         <v>267</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="57" t="s">
         <v>724</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="81" t="s">
         <v>463</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="57" t="s">
         <v>688</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="57" t="s">
         <v>188</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="57" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="57" t="s">
         <v>422</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="82" t="s">
+      <c r="C8" s="81" t="s">
         <v>590</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="57" t="s">
         <v>182</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="57" t="s">
         <v>442</v>
       </c>
-      <c r="C9" s="82" t="s">
+      <c r="C9" s="81" t="s">
         <v>598</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="57" t="s">
         <v>345</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="57" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="57" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="57" t="s">
         <v>200</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="57" t="s">
         <v>156</v>
       </c>
-      <c r="C11" s="82" t="s">
+      <c r="C11" s="81" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="57" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>843</v>
       </c>
-      <c r="C12" s="58" t="s">
+      <c r="C12" s="57" t="s">
         <v>55</v>
       </c>
     </row>
@@ -25617,117 +25606,117 @@
       <c r="A13" s="0" t="s">
         <v>778</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="57" t="s">
         <v>309</v>
       </c>
-      <c r="C13" s="82" t="s">
+      <c r="C13" s="81" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="57" t="s">
         <v>211</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="57" t="s">
         <v>650</v>
       </c>
-      <c r="C14" s="58" t="s">
+      <c r="C14" s="57" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="57" t="s">
         <v>428</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="57" t="s">
         <v>456</v>
       </c>
-      <c r="C15" s="58" t="s">
+      <c r="C15" s="57" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="58" t="s">
+      <c r="A16" s="57" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="57" t="s">
         <v>450</v>
       </c>
-      <c r="C16" s="58" t="s">
+      <c r="C16" s="57" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="58" t="s">
+      <c r="A17" s="57" t="s">
         <v>348</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="57" t="s">
         <v>617</v>
       </c>
-      <c r="C17" s="58" t="s">
+      <c r="C17" s="57" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="B18" s="58" t="s">
+      <c r="B18" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="58" t="s">
+      <c r="C18" s="57" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="57" t="s">
         <v>453</v>
       </c>
-      <c r="C19" s="58" t="s">
+      <c r="C19" s="57" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="57" t="s">
         <v>706</v>
       </c>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="57" t="s">
         <v>620</v>
       </c>
-      <c r="C20" s="58" t="s">
+      <c r="C20" s="57" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="58" t="s">
+      <c r="A21" s="57" t="s">
         <v>208</v>
       </c>
-      <c r="B21" s="58" t="s">
+      <c r="B21" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="C21" s="57" t="s">
         <v>684</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="58" t="s">
+      <c r="A22" s="57" t="s">
         <v>431</v>
       </c>
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="C22" s="82" t="s">
+      <c r="C22" s="81" t="s">
         <v>502</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="58" t="s">
+      <c r="A23" s="57" t="s">
         <v>361</v>
       </c>
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="57" t="s">
         <v>152</v>
       </c>
       <c r="C23" s="0" t="s">
@@ -25735,21 +25724,21 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="58" t="s">
+      <c r="A24" s="57" t="s">
         <v>358</v>
       </c>
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="57" t="s">
         <v>636</v>
       </c>
-      <c r="C24" s="58" t="s">
+      <c r="C24" s="57" t="s">
         <v>692</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="58" t="s">
+      <c r="A25" s="57" t="s">
         <v>196</v>
       </c>
-      <c r="B25" s="58" t="s">
+      <c r="B25" s="57" t="s">
         <v>633</v>
       </c>
       <c r="C25" s="0" t="s">
@@ -25757,187 +25746,187 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="58" t="s">
+      <c r="A26" s="57" t="s">
         <v>341</v>
       </c>
-      <c r="B26" s="58" t="s">
+      <c r="B26" s="57" t="s">
         <v>639</v>
       </c>
-      <c r="C26" s="82" t="s">
+      <c r="C26" s="81" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="58" t="s">
+      <c r="A27" s="57" t="s">
         <v>217</v>
       </c>
-      <c r="B27" s="58" t="s">
+      <c r="B27" s="57" t="s">
         <v>642</v>
       </c>
-      <c r="C27" s="82" t="s">
+      <c r="C27" s="81" t="s">
         <v>659</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="83" t="s">
+      <c r="A28" s="82" t="s">
         <v>703</v>
       </c>
-      <c r="B28" s="58" t="s">
+      <c r="B28" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="C28" s="58" t="s">
+      <c r="C28" s="57" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="83" t="s">
+      <c r="A29" s="82" t="s">
         <v>416</v>
       </c>
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="C29" s="58" t="s">
+      <c r="C29" s="57" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="58" t="s">
+      <c r="A30" s="57" t="s">
         <v>669</v>
       </c>
-      <c r="B30" s="82" t="s">
+      <c r="B30" s="81" t="s">
         <v>476</v>
       </c>
-      <c r="C30" s="58" t="s">
+      <c r="C30" s="57" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="83" t="s">
+      <c r="A31" s="82" t="s">
         <v>425</v>
       </c>
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="57" t="s">
         <v>257</v>
       </c>
-      <c r="C31" s="58" t="s">
+      <c r="C31" s="57" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="58" t="s">
+      <c r="A32" s="57" t="s">
         <v>608</v>
       </c>
-      <c r="B32" s="58" t="s">
+      <c r="B32" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="58" t="s">
+      <c r="C32" s="57" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="58" t="s">
+      <c r="A33" s="57" t="s">
         <v>204</v>
       </c>
-      <c r="B33" s="82" t="s">
+      <c r="B33" s="81" t="s">
         <v>467</v>
       </c>
-      <c r="C33" s="58" t="s">
+      <c r="C33" s="57" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="58" t="s">
+      <c r="A34" s="57" t="s">
         <v>351</v>
       </c>
-      <c r="B34" s="84" t="s">
+      <c r="B34" s="83" t="s">
         <v>438</v>
       </c>
-      <c r="C34" s="58" t="s">
+      <c r="C34" s="57" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="58" t="s">
+      <c r="A35" s="57" t="s">
         <v>354</v>
       </c>
-      <c r="B35" s="58" t="s">
+      <c r="B35" s="57" t="s">
         <v>312</v>
       </c>
-      <c r="C35" s="58" t="s">
+      <c r="C35" s="57" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="58" t="s">
+      <c r="A36" s="57" t="s">
         <v>763</v>
       </c>
-      <c r="B36" s="84" t="s">
+      <c r="B36" s="83" t="s">
         <v>436</v>
       </c>
-      <c r="C36" s="58" t="s">
+      <c r="C36" s="57" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="58" t="s">
+      <c r="A37" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="83" t="s">
+      <c r="B37" s="82" t="s">
         <v>440</v>
       </c>
-      <c r="C37" s="58" t="s">
+      <c r="C37" s="57" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="58" t="s">
+      <c r="B38" s="57" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="58" t="s">
+      <c r="C38" s="57" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="58" t="s">
+      <c r="B39" s="57" t="s">
         <v>220</v>
       </c>
-      <c r="C39" s="58" t="s">
+      <c r="C39" s="57" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="84" t="s">
+      <c r="B40" s="83" t="s">
         <v>434</v>
       </c>
-      <c r="C40" s="58" t="s">
+      <c r="C40" s="57" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="82" t="s">
+      <c r="B41" s="81" t="s">
         <v>614</v>
       </c>
-      <c r="C41" s="58" t="s">
+      <c r="C41" s="57" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="58" t="s">
+      <c r="B42" s="57" t="s">
         <v>228</v>
       </c>
-      <c r="C42" s="58" t="s">
+      <c r="C42" s="57" t="s">
         <v>728</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="58" t="s">
+      <c r="B43" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="C43" s="58" t="s">
+      <c r="C43" s="57" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="58" t="s">
+      <c r="B44" s="57" t="s">
         <v>677</v>
       </c>
       <c r="C44" s="0" t="s">
@@ -25945,7 +25934,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="58" t="s">
+      <c r="B45" s="57" t="s">
         <v>64</v>
       </c>
       <c r="C45" s="0" t="s">
@@ -25953,7 +25942,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="58" t="s">
+      <c r="B46" s="57" t="s">
         <v>35</v>
       </c>
       <c r="C46" s="0" t="s">
@@ -25969,7 +25958,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="58" t="s">
+      <c r="B48" s="57" t="s">
         <v>117</v>
       </c>
       <c r="C48" s="0" t="s">
@@ -25977,7 +25966,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="58" t="s">
+      <c r="B49" s="57" t="s">
         <v>106</v>
       </c>
       <c r="C49" s="0" t="s">
@@ -25985,7 +25974,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="58" t="s">
+      <c r="B50" s="57" t="s">
         <v>715</v>
       </c>
       <c r="C50" s="0" t="s">
@@ -26001,7 +25990,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="58" t="s">
+      <c r="B52" s="57" t="s">
         <v>140</v>
       </c>
       <c r="C52" s="0" t="s">
@@ -26012,7 +26001,7 @@
       <c r="B53" s="0" t="s">
         <v>868</v>
       </c>
-      <c r="C53" s="58" t="s">
+      <c r="C53" s="57" t="s">
         <v>986</v>
       </c>
     </row>
@@ -26025,15 +26014,15 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="58" t="s">
+      <c r="B55" s="57" t="s">
         <v>373</v>
       </c>
-      <c r="C55" s="58" t="s">
+      <c r="C55" s="57" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="58" t="s">
+      <c r="B56" s="57" t="s">
         <v>242</v>
       </c>
       <c r="C56" s="0" t="s">
@@ -26041,15 +26030,15 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="58" t="s">
+      <c r="B57" s="57" t="s">
         <v>245</v>
       </c>
-      <c r="C57" s="58" t="s">
+      <c r="C57" s="57" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="58" t="s">
+      <c r="B58" s="57" t="s">
         <v>673</v>
       </c>
       <c r="C58" s="0" t="s">
@@ -26057,34 +26046,34 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="58" t="s">
+      <c r="B59" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="C59" s="82" t="s">
+      <c r="C59" s="81" t="s">
         <v>594</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="58" t="s">
+      <c r="B60" s="57" t="s">
         <v>231</v>
       </c>
-      <c r="C60" s="58" t="s">
+      <c r="C60" s="57" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="58" t="s">
+      <c r="B61" s="57" t="s">
         <v>368</v>
       </c>
-      <c r="C61" s="82" t="s">
+      <c r="C61" s="81" t="s">
         <v>572</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="58" t="s">
+      <c r="B62" s="57" t="s">
         <v>376</v>
       </c>
-      <c r="C62" s="82" t="s">
+      <c r="C62" s="81" t="s">
         <v>581</v>
       </c>
     </row>
@@ -26092,15 +26081,15 @@
       <c r="B63" s="0" t="s">
         <v>445</v>
       </c>
-      <c r="C63" s="82" t="s">
+      <c r="C63" s="81" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="58" t="s">
+      <c r="B64" s="57" t="s">
         <v>654</v>
       </c>
-      <c r="C64" s="58" t="s">
+      <c r="C64" s="57" t="s">
         <v>733</v>
       </c>
     </row>
@@ -26108,28 +26097,28 @@
       <c r="B65" s="0" t="s">
         <v>830</v>
       </c>
-      <c r="C65" s="58" t="s">
+      <c r="C65" s="57" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="58" t="s">
+      <c r="B66" s="57" t="s">
         <v>720</v>
       </c>
-      <c r="C66" s="58" t="s">
+      <c r="C66" s="57" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="58" t="s">
+      <c r="B67" s="57" t="s">
         <v>657</v>
       </c>
-      <c r="C67" s="58" t="s">
+      <c r="C67" s="57" t="s">
         <v>741</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="58" t="s">
+      <c r="B68" s="57" t="s">
         <v>718</v>
       </c>
       <c r="C68" s="0" t="s">
@@ -26137,7 +26126,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="58" t="s">
+      <c r="B69" s="57" t="s">
         <v>249</v>
       </c>
       <c r="C69" s="0" t="s">
@@ -26145,10 +26134,10 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="58" t="s">
+      <c r="B70" s="57" t="s">
         <v>235</v>
       </c>
-      <c r="C70" s="58" t="s">
+      <c r="C70" s="57" t="s">
         <v>164</v>
       </c>
     </row>
@@ -26156,7 +26145,7 @@
       <c r="B71" s="0" t="s">
         <v>857</v>
       </c>
-      <c r="C71" s="58" t="s">
+      <c r="C71" s="57" t="s">
         <v>175</v>
       </c>
     </row>
@@ -26164,7 +26153,7 @@
       <c r="B72" s="0" t="s">
         <v>860</v>
       </c>
-      <c r="C72" s="82" t="s">
+      <c r="C72" s="81" t="s">
         <v>535</v>
       </c>
     </row>
@@ -26172,76 +26161,76 @@
       <c r="B73" s="0" t="s">
         <v>854</v>
       </c>
-      <c r="C73" s="82" t="s">
+      <c r="C73" s="81" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="58" t="s">
+      <c r="B74" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="C74" s="82" t="s">
+      <c r="C74" s="81" t="s">
         <v>538</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="58" t="s">
+      <c r="B75" s="57" t="s">
         <v>305</v>
       </c>
-      <c r="C75" s="82" t="s">
+      <c r="C75" s="81" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="82" t="s">
+      <c r="B76" s="81" t="s">
         <v>472</v>
       </c>
-      <c r="C76" s="82" t="s">
+      <c r="C76" s="81" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="58" t="s">
+      <c r="B77" s="57" t="s">
         <v>364</v>
       </c>
-      <c r="C77" s="58" t="s">
+      <c r="C77" s="57" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="58" t="s">
+      <c r="B78" s="57" t="s">
         <v>224</v>
       </c>
-      <c r="C78" s="58" t="s">
+      <c r="C78" s="57" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="58" t="s">
+      <c r="B79" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="C79" s="58" t="s">
+      <c r="C79" s="57" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="58" t="s">
+      <c r="B80" s="57" t="s">
         <v>260</v>
       </c>
-      <c r="C80" s="83" t="s">
+      <c r="C80" s="82" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="58" t="s">
+      <c r="B81" s="57" t="s">
         <v>379</v>
       </c>
-      <c r="C81" s="58" t="s">
+      <c r="C81" s="57" t="s">
         <v>680</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="58" t="s">
+      <c r="B82" s="57" t="s">
         <v>263</v>
       </c>
       <c r="C82" s="0" t="s">
@@ -26252,15 +26241,15 @@
       <c r="B83" s="0" t="s">
         <v>793</v>
       </c>
-      <c r="C83" s="58" t="s">
+      <c r="C83" s="57" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="58" t="s">
+      <c r="B84" s="57" t="s">
         <v>459</v>
       </c>
-      <c r="C84" s="58" t="s">
+      <c r="C84" s="57" t="s">
         <v>168</v>
       </c>
     </row>
@@ -26268,27 +26257,27 @@
       <c r="B85" s="0" t="s">
         <v>864</v>
       </c>
-      <c r="C85" s="58" t="s">
+      <c r="C85" s="57" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C86" s="58" t="s">
+      <c r="C86" s="57" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C87" s="58" t="s">
+      <c r="C87" s="57" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C88" s="58" t="s">
+      <c r="C88" s="57" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C89" s="58" t="s">
+      <c r="C89" s="57" t="s">
         <v>757</v>
       </c>
     </row>
@@ -26298,12 +26287,12 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="82" t="s">
+      <c r="C91" s="81" t="s">
         <v>626</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C92" s="58" t="s">
+      <c r="C92" s="57" t="s">
         <v>386</v>
       </c>
     </row>

</xml_diff>